<commit_message>
model updates for: - attached file model - unique constraints fieldinformation: - names - dataset result columns attached files: - in views - to _static dir, with redirect.  to rework with blobs to handle authorization. - refactor templates for detaillisting
</commit_message>
<xml_diff>
--- a/sampledata/fieldinformation.xlsx
+++ b/sampledata/fieldinformation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1476" uniqueCount="647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1555" uniqueCount="680">
   <si>
     <t>table</t>
   </si>
@@ -605,6 +605,9 @@
     <t>SM_Center_Compound_ID</t>
   </si>
   <si>
+    <t>Small Molecule Facility ID</t>
+  </si>
+  <si>
     <t>Center specific compound ID of the (parent structure) assigned by the center</t>
   </si>
   <si>
@@ -614,7 +617,7 @@
     <t>1003</t>
   </si>
   <si>
-    <t>Facility and Salt ID</t>
+    <t>Small Molecule Facility and Salt ID</t>
   </si>
   <si>
     <t>Combination of HMS Facility ID and Salt ID</t>
@@ -629,7 +632,7 @@
     <t>1004</t>
   </si>
   <si>
-    <t>Facility-Salt-Batch ID</t>
+    <t>Small Molecule Facility-Salt-Batch ID</t>
   </si>
   <si>
     <t>Combination of HMS Facility ID (SM:4 – SM_Center_Compound_ID) , Salt ID, and Batch ID (SM:5 - SM_Center_Sample_ID)</t>
@@ -1037,6 +1040,9 @@
     <t>PP_Name</t>
   </si>
   <si>
+    <t>Protein Name</t>
+  </si>
+  <si>
     <t>canonical protein</t>
   </si>
   <si>
@@ -1419,6 +1425,9 @@
   </si>
   <si>
     <t>CL_Name</t>
+  </si>
+  <si>
+    <t>Cell Name</t>
   </si>
   <si>
     <t>canonical cell line</t>
@@ -1961,6 +1970,96 @@
   </si>
   <si>
     <t>Patient Gender</t>
+  </si>
+  <si>
+    <t>attachedfile</t>
+  </si>
+  <si>
+    <t>filename</t>
+  </si>
+  <si>
+    <t>1008</t>
+  </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>Name portion of the file path</t>
+  </si>
+  <si>
+    <t>1009</t>
+  </si>
+  <si>
+    <t>relative_path</t>
+  </si>
+  <si>
+    <t>1010</t>
+  </si>
+  <si>
+    <t>Relative Path</t>
+  </si>
+  <si>
+    <t>Path relative to the doc root.</t>
+  </si>
+  <si>
+    <t>facility_id_for</t>
+  </si>
+  <si>
+    <t>1011</t>
+  </si>
+  <si>
+    <t>Facility ID for</t>
+  </si>
+  <si>
+    <t>The Facility ID of the entity this attached file is for.</t>
+  </si>
+  <si>
+    <t>salt_id_for</t>
+  </si>
+  <si>
+    <t>1012</t>
+  </si>
+  <si>
+    <t>Salt ID for</t>
+  </si>
+  <si>
+    <t>The Salt ID of the Small Molecule this attached file is for</t>
+  </si>
+  <si>
+    <t>batch_id_for</t>
+  </si>
+  <si>
+    <t>1013</t>
+  </si>
+  <si>
+    <t>Batch ID for</t>
+  </si>
+  <si>
+    <t>The Batch ID of the Entity this attached file is for.</t>
+  </si>
+  <si>
+    <t>file_type</t>
+  </si>
+  <si>
+    <t>1014</t>
+  </si>
+  <si>
+    <t>File Type</t>
+  </si>
+  <si>
+    <t>Type designation</t>
+  </si>
+  <si>
+    <t>file_date</t>
+  </si>
+  <si>
+    <t>1015</t>
+  </si>
+  <si>
+    <t>File Date</t>
+  </si>
+  <si>
+    <t>Date entered for this file</t>
   </si>
 </sst>
 </file>
@@ -1971,7 +2070,7 @@
     <numFmt formatCode="GENERAL" numFmtId="164"/>
     <numFmt formatCode="@" numFmtId="165"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -2075,6 +2174,13 @@
       <color rgb="00A6A6A6"/>
       <sz val="9"/>
     </font>
+    <font>
+      <name val="Monospace"/>
+      <charset val="1"/>
+      <family val="0"/>
+      <color rgb="00000000"/>
+      <sz val="10"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2129,7 +2235,7 @@
       <protection hidden="false" locked="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="20">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
@@ -2205,6 +2311,12 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="14" numFmtId="165" xfId="20">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
     </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="20">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="16" numFmtId="164" xfId="20">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -2213,7 +2325,7 @@
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -2283,31 +2395,35 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X126"/>
+  <dimension ref="A1:X134"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <pane activePane="bottomRight" topLeftCell="B98" xSplit="2556" ySplit="2250"/>
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="B1" activeCellId="0" pane="topRight" sqref="B1"/>
+      <selection activeCell="A98" activeCellId="0" pane="bottomLeft" sqref="A98"/>
+      <selection activeCell="M102" activeCellId="0" pane="bottomRight" sqref="M102"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.5450980392157"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.1333333333333"/>
-    <col collapsed="false" hidden="false" max="9" min="3" style="1" width="10.7882352941176"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="10.7882352941176"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.7882352941176"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="27.8313725490196"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="1" width="25.6509803921569"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="55.2235294117647"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="14.9960784313725"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="44.4509803921569"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="13.8470588235294"/>
-    <col collapsed="false" hidden="false" max="20" min="19" style="1" width="21.4274509803922"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="21.2823529411765"/>
-    <col collapsed="false" hidden="false" max="24" min="22" style="1" width="9.32549019607843"/>
-    <col collapsed="false" hidden="false" max="1025" min="25" style="0" width="9.32549019607843"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.6509803921569"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.1960784313725"/>
+    <col collapsed="false" hidden="false" max="9" min="3" style="1" width="10.8352941176471"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="10.8352941176471"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.8352941176471"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="27.9725490196078"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="1" width="25.7843137254902"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="55.4941176470588"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="15.0666666666667"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="44.6705882352941"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="13.9176470588235"/>
+    <col collapsed="false" hidden="false" max="20" min="19" style="1" width="21.5333333333333"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="21.3882352941176"/>
+    <col collapsed="false" hidden="false" max="24" min="22" style="1" width="9.36862745098039"/>
+    <col collapsed="false" hidden="false" max="1025" min="25" style="0" width="9.36862745098039"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="100.7" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="86.55" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3304,7 +3420,9 @@
         <v>111</v>
       </c>
       <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
+      <c r="D27" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="E27" s="3" t="s">
         <v>22</v>
       </c>
@@ -4128,13 +4246,13 @@
         <v>195</v>
       </c>
       <c r="M51" s="8" t="s">
-        <v>99</v>
+        <v>196</v>
       </c>
       <c r="N51" s="8" t="s">
         <v>180</v>
       </c>
       <c r="O51" s="8" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="P51" s="11" t="n">
         <v>1</v>
@@ -4148,10 +4266,10 @@
       <c r="W51" s="7"/>
       <c r="X51" s="7"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.2" outlineLevel="0" r="52">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.85" outlineLevel="0" r="52">
       <c r="A52" s="7"/>
       <c r="B52" s="7" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C52" s="7"/>
       <c r="D52" s="7" t="s">
@@ -4174,15 +4292,15 @@
       </c>
       <c r="J52" s="9"/>
       <c r="K52" s="10" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="L52" s="8"/>
       <c r="M52" s="8" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="N52" s="8"/>
       <c r="O52" s="8" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="P52" s="11"/>
       <c r="Q52" s="8"/>
@@ -4195,13 +4313,11 @@
       <c r="X52" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="39.55" outlineLevel="0" r="53">
-      <c r="A53" s="0"/>
       <c r="B53" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="C53" s="0"/>
+        <v>202</v>
+      </c>
       <c r="D53" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E53" s="7" t="s">
         <v>22</v>
@@ -4220,15 +4336,15 @@
       </c>
       <c r="J53" s="9"/>
       <c r="K53" s="10" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="L53" s="8"/>
       <c r="M53" s="8" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="N53" s="8"/>
       <c r="O53" s="8" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="P53" s="11"/>
       <c r="Q53" s="8"/>
@@ -4242,13 +4358,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="39.55" outlineLevel="0" r="54">
       <c r="A54" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D54" s="7"/>
       <c r="E54" s="7" t="s">
@@ -4270,25 +4386,25 @@
         <v>177</v>
       </c>
       <c r="K54" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="L54" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="M54" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="N54" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="L54" s="8" t="s">
-        <v>209</v>
-      </c>
-      <c r="M54" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="N54" s="8" t="s">
-        <v>207</v>
-      </c>
       <c r="O54" s="8" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="P54" s="11" t="n">
         <v>1</v>
       </c>
       <c r="Q54" s="8" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="R54" s="8"/>
       <c r="S54" s="8"/>
@@ -4300,10 +4416,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.2" outlineLevel="0" r="55">
       <c r="A55" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
@@ -4326,23 +4442,23 @@
         <v>177</v>
       </c>
       <c r="K55" s="10" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="L55" s="8" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="M55" s="8"/>
       <c r="N55" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O55" s="8" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="P55" s="11" t="n">
         <v>1</v>
       </c>
       <c r="Q55" s="8" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="R55" s="8"/>
       <c r="S55" s="8"/>
@@ -4354,10 +4470,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.85" outlineLevel="0" r="56">
       <c r="A56" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
@@ -4380,17 +4496,17 @@
         <v>177</v>
       </c>
       <c r="K56" s="10" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="L56" s="8" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="M56" s="8"/>
       <c r="N56" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O56" s="8" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="P56" s="11" t="n">
         <v>1</v>
@@ -4406,10 +4522,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="39.55" outlineLevel="0" r="57">
       <c r="A57" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
@@ -4432,17 +4548,17 @@
         <v>177</v>
       </c>
       <c r="K57" s="10" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L57" s="8" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="M57" s="8"/>
       <c r="N57" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O57" s="8" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="P57" s="11" t="n">
         <v>2</v>
@@ -4461,7 +4577,7 @@
         <v>175</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
@@ -4484,30 +4600,30 @@
         <v>177</v>
       </c>
       <c r="K58" s="10" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="L58" s="8" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="M58" s="8" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="N58" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O58" s="8" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="P58" s="11" t="n">
         <v>1</v>
       </c>
       <c r="Q58" s="8" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="R58" s="8"/>
       <c r="S58" s="8"/>
       <c r="T58" s="13" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="U58" s="7"/>
       <c r="V58" s="7"/>
@@ -4519,7 +4635,7 @@
         <v>175</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
@@ -4542,32 +4658,32 @@
         <v>177</v>
       </c>
       <c r="K59" s="10" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="L59" s="8" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="M59" s="8"/>
       <c r="N59" s="8" t="s">
         <v>180</v>
       </c>
       <c r="O59" s="8" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="P59" s="11" t="n">
         <v>1</v>
       </c>
       <c r="Q59" s="8" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="R59" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="S59" s="14" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="T59" s="13" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="U59" s="7"/>
       <c r="V59" s="7"/>
@@ -4579,7 +4695,7 @@
         <v>175</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
@@ -4602,29 +4718,29 @@
         <v>177</v>
       </c>
       <c r="K60" s="10" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="L60" s="8" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="M60" s="8"/>
       <c r="N60" s="8" t="s">
         <v>180</v>
       </c>
       <c r="O60" s="8" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="P60" s="11" t="n">
         <v>2</v>
       </c>
       <c r="Q60" s="8" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="R60" s="8" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="S60" s="14" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="T60" s="13"/>
       <c r="U60" s="7"/>
@@ -4637,7 +4753,7 @@
         <v>175</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
@@ -4658,23 +4774,23 @@
         <v>177</v>
       </c>
       <c r="K61" s="10" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L61" s="8" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="M61" s="8"/>
       <c r="N61" s="8" t="s">
         <v>180</v>
       </c>
       <c r="O61" s="8" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="P61" s="11" t="n">
         <v>2</v>
       </c>
       <c r="Q61" s="8" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="R61" s="8"/>
       <c r="S61" s="8"/>
@@ -4689,7 +4805,7 @@
         <v>175</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
@@ -4710,17 +4826,17 @@
         <v>177</v>
       </c>
       <c r="K62" s="10" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="L62" s="8" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="M62" s="8"/>
       <c r="N62" s="8" t="s">
         <v>180</v>
       </c>
       <c r="O62" s="8" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="P62" s="11" t="n">
         <v>2</v>
@@ -4729,7 +4845,7 @@
       <c r="R62" s="8"/>
       <c r="S62" s="8"/>
       <c r="T62" s="13" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="U62" s="7"/>
       <c r="V62" s="7"/>
@@ -4741,7 +4857,7 @@
         <v>175</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
@@ -4762,23 +4878,23 @@
         <v>177</v>
       </c>
       <c r="K63" s="10" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="L63" s="8" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="M63" s="8"/>
       <c r="N63" s="8" t="s">
         <v>180</v>
       </c>
       <c r="O63" s="8" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="P63" s="11" t="n">
         <v>1</v>
       </c>
       <c r="Q63" s="8" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="R63" s="8"/>
       <c r="S63" s="8"/>
@@ -4791,11 +4907,11 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.85" outlineLevel="0" r="64">
       <c r="A64" s="7"/>
       <c r="B64" s="7" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C64" s="7"/>
       <c r="D64" s="7" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E64" s="7"/>
       <c r="F64" s="7"/>
@@ -4812,23 +4928,23 @@
         <v>177</v>
       </c>
       <c r="K64" s="10" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="L64" s="8" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="M64" s="8"/>
       <c r="N64" s="8" t="s">
         <v>180</v>
       </c>
       <c r="O64" s="8" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="P64" s="11" t="n">
         <v>1</v>
       </c>
       <c r="Q64" s="8" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="R64" s="8"/>
       <c r="S64" s="8"/>
@@ -4840,10 +4956,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.85" outlineLevel="0" r="65">
       <c r="A65" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
@@ -4864,23 +4980,23 @@
         <v>177</v>
       </c>
       <c r="K65" s="10" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="L65" s="8" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="M65" s="8"/>
       <c r="N65" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O65" s="8" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="P65" s="11" t="n">
         <v>2</v>
       </c>
       <c r="Q65" s="8" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="R65" s="8"/>
       <c r="S65" s="8"/>
@@ -4892,10 +5008,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.2" outlineLevel="0" r="66">
       <c r="A66" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
@@ -4916,17 +5032,17 @@
         <v>177</v>
       </c>
       <c r="K66" s="10" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="L66" s="8" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="M66" s="8"/>
       <c r="N66" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O66" s="8" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="P66" s="11" t="n">
         <v>2</v>
@@ -4935,7 +5051,7 @@
       <c r="R66" s="8"/>
       <c r="S66" s="8"/>
       <c r="T66" s="13" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="U66" s="7"/>
       <c r="V66" s="7"/>
@@ -4944,10 +5060,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.85" outlineLevel="0" r="67">
       <c r="A67" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
@@ -4968,23 +5084,23 @@
         <v>177</v>
       </c>
       <c r="K67" s="10" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="L67" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="M67" s="8"/>
       <c r="N67" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O67" s="8" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="P67" s="11" t="n">
         <v>1</v>
       </c>
       <c r="Q67" s="8" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="R67" s="8"/>
       <c r="S67" s="8"/>
@@ -4999,7 +5115,7 @@
         <v>175</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
@@ -5020,15 +5136,15 @@
         <v>177</v>
       </c>
       <c r="K68" s="10" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="L68" s="8" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="M68" s="8"/>
       <c r="N68" s="8"/>
       <c r="O68" s="8" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="P68" s="11" t="n">
         <v>2</v>
@@ -5037,7 +5153,7 @@
       <c r="R68" s="8"/>
       <c r="S68" s="8"/>
       <c r="T68" s="12" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="U68" s="7"/>
       <c r="V68" s="7"/>
@@ -5047,11 +5163,11 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="90.25" outlineLevel="0" r="69">
       <c r="A69" s="7"/>
       <c r="B69" s="7" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C69" s="7"/>
       <c r="D69" s="7" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E69" s="7"/>
       <c r="F69" s="7"/>
@@ -5068,28 +5184,28 @@
         <v>177</v>
       </c>
       <c r="K69" s="10" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="L69" s="8" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="M69" s="8"/>
       <c r="N69" s="8" t="s">
         <v>180</v>
       </c>
       <c r="O69" s="8" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="P69" s="11" t="n">
         <v>2</v>
       </c>
       <c r="Q69" s="8" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="R69" s="8"/>
       <c r="S69" s="8"/>
       <c r="T69" s="13" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="U69" s="7"/>
       <c r="V69" s="7"/>
@@ -5098,10 +5214,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.85" outlineLevel="0" r="70">
       <c r="A70" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
@@ -5113,7 +5229,7 @@
         <v>22</v>
       </c>
       <c r="H70" s="7" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="I70" s="3" t="s">
         <v>22</v>
@@ -5122,23 +5238,23 @@
         <v>177</v>
       </c>
       <c r="K70" s="10" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="L70" s="8" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="M70" s="8"/>
       <c r="N70" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O70" s="8" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="P70" s="11" t="n">
         <v>1</v>
       </c>
       <c r="Q70" s="8" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="R70" s="8"/>
       <c r="S70" s="8"/>
@@ -5150,10 +5266,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="39.55" outlineLevel="0" r="71">
       <c r="A71" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
@@ -5165,7 +5281,7 @@
         <v>22</v>
       </c>
       <c r="H71" s="7" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="I71" s="3" t="s">
         <v>22</v>
@@ -5174,23 +5290,23 @@
         <v>177</v>
       </c>
       <c r="K71" s="10" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="L71" s="8" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="M71" s="8"/>
       <c r="N71" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O71" s="8" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="P71" s="11" t="n">
         <v>2</v>
       </c>
       <c r="Q71" s="8" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="R71" s="8"/>
       <c r="S71" s="8"/>
@@ -5202,10 +5318,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.85" outlineLevel="0" r="72">
       <c r="A72" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
@@ -5217,7 +5333,7 @@
         <v>22</v>
       </c>
       <c r="H72" s="7" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="I72" s="3" t="s">
         <v>22</v>
@@ -5226,23 +5342,23 @@
         <v>177</v>
       </c>
       <c r="K72" s="10" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="L72" s="8" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="M72" s="8"/>
       <c r="N72" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O72" s="8" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="P72" s="11" t="n">
         <v>3</v>
       </c>
       <c r="Q72" s="8" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="R72" s="8"/>
       <c r="S72" s="8"/>
@@ -5254,10 +5370,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.2" outlineLevel="0" r="73">
       <c r="A73" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C73" s="7"/>
       <c r="D73" s="7"/>
@@ -5269,7 +5385,7 @@
         <v>22</v>
       </c>
       <c r="H73" s="7" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="I73" s="3" t="s">
         <v>22</v>
@@ -5278,23 +5394,23 @@
         <v>177</v>
       </c>
       <c r="K73" s="10" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="L73" s="8" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="M73" s="8"/>
       <c r="N73" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O73" s="8" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="P73" s="11" t="n">
         <v>3</v>
       </c>
       <c r="Q73" s="8" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="R73" s="8"/>
       <c r="S73" s="8"/>
@@ -5306,10 +5422,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.2" outlineLevel="0" r="74">
       <c r="A74" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C74" s="7"/>
       <c r="D74" s="7"/>
@@ -5321,7 +5437,7 @@
         <v>22</v>
       </c>
       <c r="H74" s="7" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="I74" s="3" t="s">
         <v>22</v>
@@ -5330,17 +5446,17 @@
         <v>177</v>
       </c>
       <c r="K74" s="10" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="L74" s="8" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="M74" s="8"/>
       <c r="N74" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O74" s="8" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="P74" s="11" t="n">
         <v>3</v>
@@ -5356,10 +5472,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.85" outlineLevel="0" r="75">
       <c r="A75" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
@@ -5371,7 +5487,7 @@
         <v>22</v>
       </c>
       <c r="H75" s="7" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="I75" s="3" t="s">
         <v>22</v>
@@ -5380,23 +5496,23 @@
         <v>177</v>
       </c>
       <c r="K75" s="10" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="L75" s="8" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="M75" s="8"/>
       <c r="N75" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O75" s="8" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="P75" s="11" t="n">
         <v>3</v>
       </c>
       <c r="Q75" s="8" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="R75" s="8"/>
       <c r="S75" s="8"/>
@@ -5408,7 +5524,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="76">
       <c r="A76" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>142</v>
@@ -5432,7 +5548,7 @@
         <v>23</v>
       </c>
       <c r="K76" s="4" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="M76" s="7" t="s">
         <v>144</v>
@@ -5443,7 +5559,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="77">
       <c r="A77" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>146</v>
@@ -5467,7 +5583,7 @@
         <v>23</v>
       </c>
       <c r="K77" s="4" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="M77" s="7" t="s">
         <v>147</v>
@@ -5478,7 +5594,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="78">
       <c r="A78" s="7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>149</v>
@@ -5502,7 +5618,7 @@
         <v>23</v>
       </c>
       <c r="K78" s="4" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="M78" s="7" t="s">
         <v>150</v>
@@ -5514,11 +5630,11 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.85" outlineLevel="0" r="79">
       <c r="A79" s="7"/>
       <c r="B79" s="7" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C79" s="7"/>
       <c r="D79" s="7" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E79" s="7" t="s">
         <v>22</v>
@@ -5528,7 +5644,7 @@
         <v>22</v>
       </c>
       <c r="H79" s="7" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="I79" s="3" t="s">
         <v>22</v>
@@ -5537,23 +5653,23 @@
         <v>177</v>
       </c>
       <c r="K79" s="10" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="L79" s="8" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="M79" s="8"/>
       <c r="N79" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O79" s="8" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="P79" s="11" t="n">
         <v>3</v>
       </c>
       <c r="Q79" s="8" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="R79" s="8"/>
       <c r="S79" s="8"/>
@@ -5568,7 +5684,7 @@
         <v>175</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
@@ -5578,7 +5694,7 @@
         <v>23</v>
       </c>
       <c r="H80" s="7" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="I80" s="3" t="s">
         <v>23</v>
@@ -5589,13 +5705,13 @@
       </c>
       <c r="L80" s="7"/>
       <c r="M80" s="7" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="N80" s="7" t="s">
         <v>180</v>
       </c>
       <c r="O80" s="7" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="P80" s="7"/>
       <c r="Q80" s="7"/>
@@ -5612,7 +5728,7 @@
         <v>175</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C81" s="7"/>
       <c r="D81" s="7"/>
@@ -5624,7 +5740,7 @@
         <v>23</v>
       </c>
       <c r="H81" s="7" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="I81" s="3" t="s">
         <v>23</v>
@@ -5635,11 +5751,11 @@
       </c>
       <c r="L81" s="7"/>
       <c r="M81" s="7" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="N81" s="7"/>
       <c r="O81" s="7" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="P81" s="7"/>
       <c r="Q81" s="7"/>
@@ -5651,15 +5767,15 @@
       <c r="W81" s="7"/>
       <c r="X81" s="7"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="114.9" outlineLevel="0" r="82">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="100.7" outlineLevel="0" r="82">
       <c r="A82" s="7" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B82" s="7" t="s">
         <v>132</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D82" s="7"/>
       <c r="E82" s="7" t="s">
@@ -5678,29 +5794,31 @@
         <v>22</v>
       </c>
       <c r="J82" s="15" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K82" s="16" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="L82" s="16" t="s">
-        <v>339</v>
-      </c>
-      <c r="M82" s="16"/>
+        <v>340</v>
+      </c>
+      <c r="M82" s="16" t="s">
+        <v>341</v>
+      </c>
       <c r="N82" s="16" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="O82" s="16" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="P82" s="5" t="n">
         <v>1</v>
       </c>
       <c r="Q82" s="16" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="R82" s="16" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="S82" s="16"/>
       <c r="T82" s="17"/>
@@ -5708,7 +5826,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="29.85" outlineLevel="0" r="83">
       <c r="A83" s="7" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B83" s="7" t="s">
         <v>184</v>
@@ -5731,26 +5849,26 @@
         <v>22</v>
       </c>
       <c r="J83" s="15" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K83" s="16" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="L83" s="16" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="M83" s="16"/>
       <c r="N83" s="16" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="O83" s="16" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="P83" s="5" t="n">
         <v>1</v>
       </c>
       <c r="Q83" s="16" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="R83" s="16"/>
       <c r="S83" s="16"/>
@@ -5759,10 +5877,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="58.2" outlineLevel="0" r="84">
       <c r="A84" s="7" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="C84" s="7"/>
       <c r="D84" s="7"/>
@@ -5782,44 +5900,44 @@
         <v>22</v>
       </c>
       <c r="J84" s="15" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K84" s="16" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="L84" s="16" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="M84" s="16"/>
       <c r="N84" s="16" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="O84" s="16" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="P84" s="5" t="n">
         <v>1</v>
       </c>
       <c r="Q84" s="16" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="R84" s="16" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="S84" s="16" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="T84" s="17" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="U84" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="72.35" outlineLevel="0" r="85">
       <c r="A85" s="7" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="C85" s="7"/>
       <c r="D85" s="7"/>
@@ -5839,44 +5957,44 @@
         <v>22</v>
       </c>
       <c r="J85" s="15" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K85" s="16" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="L85" s="16" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="M85" s="16"/>
       <c r="N85" s="16" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="O85" s="16" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="P85" s="5" t="n">
         <v>1</v>
       </c>
       <c r="Q85" s="16" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="R85" s="16" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="S85" s="16" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="T85" s="17" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="U85" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="86">
       <c r="A86" s="7" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C86" s="7"/>
       <c r="D86" s="7"/>
@@ -5896,20 +6014,20 @@
         <v>22</v>
       </c>
       <c r="J86" s="15" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K86" s="16" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="L86" s="16" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="M86" s="16"/>
       <c r="N86" s="16" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O86" s="16" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="P86" s="5" t="n">
         <v>1</v>
@@ -5917,17 +6035,17 @@
       <c r="Q86" s="16"/>
       <c r="R86" s="16"/>
       <c r="S86" s="16" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="T86" s="17"/>
       <c r="U86" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="29.85" outlineLevel="0" r="87">
       <c r="A87" s="7" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C87" s="7"/>
       <c r="D87" s="7"/>
@@ -5947,20 +6065,20 @@
         <v>22</v>
       </c>
       <c r="J87" s="15" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K87" s="16" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="L87" s="16" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="M87" s="16"/>
       <c r="N87" s="16" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O87" s="16" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="P87" s="5" t="n">
         <v>1</v>
@@ -5968,17 +6086,17 @@
       <c r="Q87" s="16"/>
       <c r="R87" s="16"/>
       <c r="S87" s="16" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="T87" s="17"/>
       <c r="U87" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="29.85" outlineLevel="0" r="88">
       <c r="A88" s="7" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="C88" s="7"/>
       <c r="D88" s="7"/>
@@ -5998,40 +6116,40 @@
         <v>22</v>
       </c>
       <c r="J88" s="15" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K88" s="16" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="L88" s="16" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="M88" s="16"/>
       <c r="N88" s="16" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O88" s="16" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="P88" s="5" t="n">
         <v>1</v>
       </c>
       <c r="Q88" s="16" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="R88" s="16"/>
       <c r="S88" s="16" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="T88" s="17"/>
       <c r="U88" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="72.35" outlineLevel="0" r="89">
       <c r="A89" s="7" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="C89" s="7"/>
       <c r="D89" s="7"/>
@@ -6049,44 +6167,44 @@
         <v>22</v>
       </c>
       <c r="J89" s="15" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K89" s="16" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="L89" s="16" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="M89" s="16"/>
       <c r="N89" s="16" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="O89" s="16" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="P89" s="5" t="n">
         <v>2</v>
       </c>
       <c r="Q89" s="16" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="R89" s="16" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="S89" s="16" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="T89" s="17" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="U89" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="58.2" outlineLevel="0" r="90">
       <c r="A90" s="7" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="C90" s="7"/>
       <c r="D90" s="7"/>
@@ -6104,44 +6222,44 @@
         <v>22</v>
       </c>
       <c r="J90" s="15" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K90" s="16" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="L90" s="16" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="M90" s="16"/>
       <c r="N90" s="16" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="O90" s="16" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="P90" s="5" t="n">
         <v>2</v>
       </c>
       <c r="Q90" s="16" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="R90" s="16" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="S90" s="16" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="T90" s="17" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="U90" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="91">
       <c r="A91" s="7" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="C91" s="7"/>
       <c r="D91" s="7"/>
@@ -6159,42 +6277,42 @@
         <v>22</v>
       </c>
       <c r="J91" s="15" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K91" s="16" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="L91" s="16" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="M91" s="16"/>
       <c r="N91" s="16" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="O91" s="16" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="P91" s="5" t="n">
         <v>2</v>
       </c>
       <c r="Q91" s="16"/>
       <c r="R91" s="16" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="S91" s="16" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="T91" s="17" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="U91" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="44" outlineLevel="0" r="92">
       <c r="A92" s="7" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="C92" s="7"/>
       <c r="D92" s="7"/>
@@ -6212,42 +6330,42 @@
         <v>22</v>
       </c>
       <c r="J92" s="15" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K92" s="16" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="L92" s="16" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="M92" s="16"/>
       <c r="N92" s="16" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O92" s="16" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="P92" s="5" t="n">
         <v>1</v>
       </c>
       <c r="Q92" s="16"/>
       <c r="R92" s="16" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="S92" s="16" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="T92" s="17" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="U92" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="86.55" outlineLevel="0" r="93">
       <c r="A93" s="7" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="C93" s="7"/>
       <c r="D93" s="7"/>
@@ -6265,44 +6383,44 @@
         <v>22</v>
       </c>
       <c r="J93" s="15" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K93" s="16" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="L93" s="16" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="M93" s="16"/>
       <c r="N93" s="16" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O93" s="16" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="P93" s="5" t="n">
         <v>2</v>
       </c>
       <c r="Q93" s="16" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="R93" s="16" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="S93" s="16" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="T93" s="17" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="U93" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="44" outlineLevel="0" r="94">
       <c r="A94" s="7" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C94" s="7"/>
       <c r="D94" s="7"/>
@@ -6320,44 +6438,44 @@
         <v>22</v>
       </c>
       <c r="J94" s="15" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K94" s="16" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="L94" s="16" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="M94" s="16"/>
       <c r="N94" s="16" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O94" s="16" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="P94" s="5" t="n">
         <v>2</v>
       </c>
       <c r="Q94" s="16" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="R94" s="16" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="S94" s="16" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="T94" s="17" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="U94" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="114.9" outlineLevel="0" r="95">
       <c r="A95" s="7" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="C95" s="7"/>
       <c r="D95" s="7"/>
@@ -6375,44 +6493,44 @@
         <v>22</v>
       </c>
       <c r="J95" s="15" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K95" s="16" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="L95" s="16" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="M95" s="16"/>
       <c r="N95" s="16" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="O95" s="16" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="P95" s="5" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="Q95" s="16" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="R95" s="16" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="S95" s="16" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="T95" s="17" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="U95" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="100.7" outlineLevel="0" r="96">
       <c r="A96" s="7" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="C96" s="7"/>
       <c r="D96" s="7"/>
@@ -6430,44 +6548,44 @@
         <v>22</v>
       </c>
       <c r="J96" s="15" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K96" s="16" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="L96" s="16" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="M96" s="16"/>
       <c r="N96" s="16" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="O96" s="16" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="P96" s="5" t="n">
         <v>2</v>
       </c>
       <c r="Q96" s="16" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="R96" s="16" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="S96" s="16" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="T96" s="17" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="U96" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="157.45" outlineLevel="0" r="97">
       <c r="A97" s="7" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="C97" s="7"/>
       <c r="D97" s="7"/>
@@ -6485,44 +6603,44 @@
         <v>22</v>
       </c>
       <c r="J97" s="15" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K97" s="16" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="L97" s="16" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="M97" s="16"/>
       <c r="N97" s="16" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="O97" s="16" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="P97" s="5" t="n">
         <v>3</v>
       </c>
       <c r="Q97" s="16" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="R97" s="16" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="S97" s="16" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="T97" s="17" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="U97" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="44" outlineLevel="0" r="98">
       <c r="A98" s="7" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="C98" s="7"/>
       <c r="D98" s="7"/>
@@ -6540,42 +6658,42 @@
         <v>22</v>
       </c>
       <c r="J98" s="15" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K98" s="16" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="L98" s="16" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="M98" s="16"/>
       <c r="N98" s="16" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O98" s="16" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="P98" s="5" t="n">
         <v>2</v>
       </c>
       <c r="Q98" s="16"/>
       <c r="R98" s="16" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="S98" s="16" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="T98" s="17" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="U98" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="29.85" outlineLevel="0" r="99">
       <c r="A99" s="7" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="C99" s="7"/>
       <c r="D99" s="7"/>
@@ -6593,42 +6711,42 @@
         <v>22</v>
       </c>
       <c r="J99" s="15" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K99" s="16" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="L99" s="16" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="M99" s="16"/>
       <c r="N99" s="16"/>
       <c r="O99" s="16" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="P99" s="5" t="n">
         <v>2</v>
       </c>
       <c r="Q99" s="16"/>
       <c r="R99" s="16" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="S99" s="16" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="T99" s="17" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="U99" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="44" outlineLevel="0" r="100">
       <c r="A100" s="7"/>
       <c r="B100" s="7" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C100" s="7"/>
       <c r="D100" s="7" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E100" s="7"/>
       <c r="F100" s="7"/>
@@ -6642,44 +6760,44 @@
         <v>22</v>
       </c>
       <c r="J100" s="15" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K100" s="16" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="L100" s="16" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="M100" s="16"/>
       <c r="N100" s="16" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="O100" s="16" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="P100" s="5" t="n">
         <v>1</v>
       </c>
       <c r="Q100" s="16"/>
       <c r="R100" s="16" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="S100" s="16" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="T100" s="17" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="U100" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="29.85" outlineLevel="0" r="101">
       <c r="A101" s="7"/>
       <c r="B101" s="7" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="C101" s="7"/>
       <c r="D101" s="7" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E101" s="7"/>
       <c r="F101" s="7"/>
@@ -6693,45 +6811,45 @@
         <v>22</v>
       </c>
       <c r="J101" s="15" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K101" s="16" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="L101" s="16" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="M101" s="16"/>
       <c r="N101" s="16" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="O101" s="16" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="P101" s="5" t="n">
         <v>1</v>
       </c>
       <c r="Q101" s="16"/>
       <c r="R101" s="16" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="S101" s="16" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="T101" s="18" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="U101" s="16"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="43.25" outlineLevel="0" r="102">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="32.8" outlineLevel="0" r="102">
       <c r="A102" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>132</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="E102" s="7" t="s">
         <v>22</v>
@@ -6749,51 +6867,53 @@
         <v>22</v>
       </c>
       <c r="J102" s="7" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="K102" s="19" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="L102" s="19" t="s">
-        <v>467</v>
-      </c>
-      <c r="M102" s="19"/>
+        <v>469</v>
+      </c>
+      <c r="M102" s="19" t="s">
+        <v>470</v>
+      </c>
       <c r="N102" s="19" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="O102" s="19" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="P102" s="19" t="n">
         <v>1</v>
       </c>
       <c r="Q102" s="19" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="R102" s="19" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="S102" s="20"/>
       <c r="T102" s="21"/>
       <c r="U102" s="22" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="V102" s="22" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="W102" s="22" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="X102" s="22" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="22.35" outlineLevel="0" r="103">
       <c r="A103" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="E103" s="7" t="s">
         <v>22</v>
@@ -6811,28 +6931,28 @@
         <v>22</v>
       </c>
       <c r="J103" s="7" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="K103" s="19" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="L103" s="19" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="M103" s="19" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
       <c r="N103" s="19" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="O103" s="19" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="P103" s="19" t="n">
         <v>1</v>
       </c>
       <c r="Q103" s="19" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="R103" s="19"/>
       <c r="S103" s="20"/>
@@ -6844,10 +6964,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="22.35" outlineLevel="0" r="104">
       <c r="A104" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E104" s="7" t="s">
         <v>22</v>
@@ -6865,26 +6985,26 @@
         <v>22</v>
       </c>
       <c r="J104" s="7" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="K104" s="19" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="L104" s="19" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="M104" s="19"/>
       <c r="N104" s="19" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="O104" s="19" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="P104" s="19" t="n">
         <v>2</v>
       </c>
       <c r="Q104" s="19" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="R104" s="19"/>
       <c r="S104" s="20"/>
@@ -6896,10 +7016,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="105">
       <c r="A105" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="E105" s="7" t="s">
         <v>22</v>
@@ -6914,26 +7034,26 @@
         <v>22</v>
       </c>
       <c r="J105" s="7" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="K105" s="19" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="L105" s="19" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="M105" s="19"/>
       <c r="N105" s="19" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="O105" s="19" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="P105" s="19" t="n">
         <v>2</v>
       </c>
       <c r="Q105" s="19" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="R105" s="19"/>
       <c r="S105" s="20"/>
@@ -6945,10 +7065,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="106">
       <c r="A106" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="E106" s="7" t="s">
         <v>22</v>
@@ -6963,24 +7083,24 @@
         <v>22</v>
       </c>
       <c r="J106" s="7" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="K106" s="19" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="L106" s="19" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="M106" s="19"/>
       <c r="N106" s="19" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="O106" s="19"/>
       <c r="P106" s="19" t="n">
         <v>1</v>
       </c>
       <c r="Q106" s="19" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="R106" s="19"/>
       <c r="S106" s="20"/>
@@ -6992,7 +7112,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="107">
       <c r="A107" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>98</v>
@@ -7013,28 +7133,28 @@
         <v>22</v>
       </c>
       <c r="J107" s="7" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="K107" s="19" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="L107" s="19" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="M107" s="19" t="s">
         <v>99</v>
       </c>
       <c r="N107" s="19" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="O107" s="19" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
       <c r="P107" s="19" t="n">
         <v>1</v>
       </c>
       <c r="Q107" s="19" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
       <c r="R107" s="19"/>
       <c r="S107" s="20"/>
@@ -7046,10 +7166,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="53.7" outlineLevel="0" r="108">
       <c r="A108" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="E108" s="7" t="s">
         <v>22</v>
@@ -7064,51 +7184,51 @@
         <v>22</v>
       </c>
       <c r="J108" s="7" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="K108" s="19" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
       <c r="L108" s="19" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="M108" s="19"/>
       <c r="N108" s="19" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="O108" s="19" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="P108" s="19" t="n">
         <v>1</v>
       </c>
       <c r="Q108" s="19" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
       <c r="R108" s="19" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="S108" s="20"/>
       <c r="T108" s="21"/>
       <c r="U108" s="22" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
       <c r="V108" s="22" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
       <c r="W108" s="22" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="X108" s="22" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="53.7" outlineLevel="0" r="109">
       <c r="A109" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E109" s="7" t="s">
         <v>22</v>
@@ -7123,43 +7243,43 @@
         <v>22</v>
       </c>
       <c r="J109" s="7" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="K109" s="19" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="L109" s="19" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="M109" s="19"/>
       <c r="N109" s="19" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="O109" s="19" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="P109" s="19" t="n">
         <v>1</v>
       </c>
       <c r="Q109" s="23" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
       <c r="R109" s="19"/>
       <c r="S109" s="20"/>
       <c r="T109" s="21"/>
       <c r="U109" s="22"/>
       <c r="V109" s="22" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="W109" s="22"/>
       <c r="X109" s="22"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="22.35" outlineLevel="0" r="110">
       <c r="A110" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="E110" s="7" t="s">
         <v>22</v>
@@ -7174,31 +7294,31 @@
         <v>22</v>
       </c>
       <c r="J110" s="7" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="K110" s="19" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="L110" s="19" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="M110" s="19"/>
       <c r="N110" s="19" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="O110" s="19" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="P110" s="19" t="n">
         <v>1</v>
       </c>
       <c r="Q110" s="19" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="R110" s="19"/>
       <c r="S110" s="20"/>
       <c r="T110" s="21" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="U110" s="22"/>
       <c r="V110" s="22"/>
@@ -7207,10 +7327,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="32.8" outlineLevel="0" r="111">
       <c r="A111" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="E111" s="7" t="s">
         <v>22</v>
@@ -7228,36 +7348,36 @@
         <v>22</v>
       </c>
       <c r="J111" s="7" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="K111" s="19" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="L111" s="19" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="M111" s="19"/>
       <c r="N111" s="19" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="O111" s="19" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="P111" s="19" t="n">
         <v>1</v>
       </c>
       <c r="Q111" s="19" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="R111" s="19" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="S111" s="20" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="T111" s="21"/>
       <c r="U111" s="22" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="V111" s="22"/>
       <c r="W111" s="22"/>
@@ -7265,10 +7385,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="22.35" outlineLevel="0" r="112">
       <c r="A112" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="E112" s="7" t="s">
         <v>22</v>
@@ -7286,30 +7406,30 @@
         <v>22</v>
       </c>
       <c r="J112" s="7" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="K112" s="19" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="L112" s="19" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="M112" s="19"/>
       <c r="N112" s="19" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="O112" s="19" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="P112" s="19" t="n">
         <v>1</v>
       </c>
       <c r="Q112" s="19"/>
       <c r="R112" s="19" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="S112" s="20" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="T112" s="21"/>
       <c r="U112" s="22"/>
@@ -7319,10 +7439,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="22.35" outlineLevel="0" r="113">
       <c r="A113" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="E113" s="7" t="s">
         <v>22</v>
@@ -7340,53 +7460,53 @@
         <v>22</v>
       </c>
       <c r="J113" s="7" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="K113" s="19" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="L113" s="19" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="M113" s="19"/>
       <c r="N113" s="19" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="O113" s="19" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
       <c r="P113" s="19" t="n">
         <v>1</v>
       </c>
       <c r="Q113" s="19" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="R113" s="19" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="S113" s="20" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="T113" s="21"/>
       <c r="U113" s="22" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="V113" s="22" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="W113" s="22" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="X113" s="22" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="43.25" outlineLevel="0" r="114">
       <c r="A114" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
       <c r="E114" s="7" t="s">
         <v>22</v>
@@ -7404,49 +7524,49 @@
         <v>22</v>
       </c>
       <c r="J114" s="7" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="K114" s="19" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="L114" s="19" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="M114" s="19"/>
       <c r="N114" s="19" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="O114" s="19" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="P114" s="19" t="n">
         <v>1</v>
       </c>
       <c r="Q114" s="24" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="R114" s="19" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="S114" s="20" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="T114" s="21" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="U114" s="22"/>
       <c r="V114" s="22" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="W114" s="22"/>
       <c r="X114" s="22"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="22.35" outlineLevel="0" r="115">
       <c r="A115" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="E115" s="7" t="s">
         <v>22</v>
@@ -7461,31 +7581,31 @@
         <v>22</v>
       </c>
       <c r="J115" s="7" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="K115" s="24" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="L115" s="24" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="M115" s="24"/>
       <c r="N115" s="24" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="O115" s="24" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="P115" s="24" t="n">
         <v>2</v>
       </c>
       <c r="Q115" s="24" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="R115" s="24"/>
       <c r="S115" s="25"/>
       <c r="T115" s="26" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="U115" s="22"/>
       <c r="V115" s="22"/>
@@ -7494,10 +7614,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="64.15" outlineLevel="0" r="116">
       <c r="A116" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="E116" s="7" t="s">
         <v>22</v>
@@ -7515,53 +7635,53 @@
         <v>22</v>
       </c>
       <c r="J116" s="7" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="K116" s="19" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
       <c r="L116" s="19" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="M116" s="19"/>
       <c r="N116" s="19" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="O116" s="19" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="P116" s="19" t="n">
         <v>1</v>
       </c>
       <c r="Q116" s="19" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
       <c r="R116" s="19" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="S116" s="20" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="T116" s="21" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="U116" s="22" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="V116" s="22" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="W116" s="22"/>
       <c r="X116" s="22" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="22.35" outlineLevel="0" r="117">
       <c r="A117" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="E117" s="7" t="s">
         <v>22</v>
@@ -7576,33 +7696,33 @@
         <v>22</v>
       </c>
       <c r="J117" s="7" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="K117" s="19" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="L117" s="19" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="M117" s="19"/>
       <c r="N117" s="19" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="O117" s="19" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="P117" s="19" t="n">
         <v>2</v>
       </c>
       <c r="Q117" s="19" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="R117" s="19" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="S117" s="20"/>
       <c r="T117" s="21" t="s">
-        <v>576</v>
+        <v>579</v>
       </c>
       <c r="U117" s="22"/>
       <c r="V117" s="22"/>
@@ -7611,10 +7731,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="85.05" outlineLevel="0" r="118">
       <c r="A118" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="E118" s="7" t="s">
         <v>22</v>
@@ -7629,51 +7749,51 @@
         <v>22</v>
       </c>
       <c r="J118" s="7" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="K118" s="19" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
       <c r="L118" s="19" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
       <c r="M118" s="19"/>
       <c r="N118" s="19" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="O118" s="19" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
       <c r="P118" s="19" t="n">
         <v>1</v>
       </c>
       <c r="Q118" s="19"/>
       <c r="R118" s="19" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
       <c r="S118" s="20" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="T118" s="21" t="s">
-        <v>582</v>
+        <v>585</v>
       </c>
       <c r="U118" s="22" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
       <c r="V118" s="22" t="s">
-        <v>584</v>
+        <v>587</v>
       </c>
       <c r="W118" s="22"/>
       <c r="X118" s="22" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="179.1" outlineLevel="0" r="119">
       <c r="A119" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>586</v>
+        <v>589</v>
       </c>
       <c r="E119" s="7" t="s">
         <v>22</v>
@@ -7688,35 +7808,35 @@
         <v>22</v>
       </c>
       <c r="J119" s="7" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="K119" s="19" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="L119" s="19" t="s">
-        <v>588</v>
+        <v>591</v>
       </c>
       <c r="M119" s="19"/>
       <c r="N119" s="19" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="O119" s="19" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="P119" s="19" t="n">
         <v>1</v>
       </c>
       <c r="Q119" s="19" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
       <c r="R119" s="19" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="S119" s="20" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="T119" s="21" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
       <c r="U119" s="22"/>
       <c r="V119" s="22"/>
@@ -7725,10 +7845,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="32.8" outlineLevel="0" r="120">
       <c r="A120" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="E120" s="7" t="s">
         <v>22</v>
@@ -7743,36 +7863,36 @@
         <v>22</v>
       </c>
       <c r="J120" s="7" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="K120" s="19" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
       <c r="L120" s="19" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="M120" s="19"/>
       <c r="N120" s="19" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="O120" s="19" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
       <c r="P120" s="19" t="n">
         <v>2</v>
       </c>
       <c r="Q120" s="19" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="R120" s="19" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
       <c r="S120" s="20"/>
       <c r="T120" s="21" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="U120" s="22" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
       <c r="V120" s="22"/>
       <c r="W120" s="22"/>
@@ -7780,10 +7900,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="137.3" outlineLevel="0" r="121">
       <c r="A121" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="E121" s="7" t="s">
         <v>22</v>
@@ -7798,49 +7918,49 @@
         <v>22</v>
       </c>
       <c r="J121" s="7" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="K121" s="19" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="L121" s="19" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="M121" s="19"/>
       <c r="N121" s="19" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="O121" s="19" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
       <c r="P121" s="19" t="n">
         <v>2</v>
       </c>
       <c r="Q121" s="19" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="R121" s="19" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="S121" s="20" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="T121" s="21" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="U121" s="22"/>
       <c r="V121" s="22"/>
       <c r="W121" s="22"/>
       <c r="X121" s="22" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="64.15" outlineLevel="0" r="122">
       <c r="A122" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
       <c r="E122" s="7" t="s">
         <v>22</v>
@@ -7849,53 +7969,53 @@
         <v>22</v>
       </c>
       <c r="H122" s="7" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="I122" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J122" s="7" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="K122" s="19" t="s">
-        <v>609</v>
+        <v>612</v>
       </c>
       <c r="L122" s="19" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="M122" s="19"/>
       <c r="N122" s="19" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="O122" s="19" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="P122" s="19" t="n">
         <v>1</v>
       </c>
       <c r="Q122" s="19" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="R122" s="19" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
       <c r="S122" s="20"/>
       <c r="T122" s="21" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
       <c r="U122" s="22"/>
       <c r="V122" s="22" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
       <c r="W122" s="22"/>
       <c r="X122" s="22"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="22.35" outlineLevel="0" r="123">
       <c r="A123" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
       <c r="E123" s="7" t="s">
         <v>22</v>
@@ -7904,37 +8024,37 @@
         <v>22</v>
       </c>
       <c r="H123" s="7" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="I123" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J123" s="7" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="K123" s="19" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
       <c r="L123" s="24" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="M123" s="24"/>
       <c r="N123" s="19" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="O123" s="19" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
       <c r="P123" s="19" t="n">
         <v>2</v>
       </c>
       <c r="Q123" s="19" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
       <c r="R123" s="19"/>
       <c r="S123" s="20"/>
       <c r="T123" s="21" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
       <c r="U123" s="22"/>
       <c r="V123" s="22"/>
@@ -7943,10 +8063,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="43.25" outlineLevel="0" r="124">
       <c r="A124" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
       <c r="E124" s="7" t="s">
         <v>22</v>
@@ -7955,41 +8075,41 @@
         <v>22</v>
       </c>
       <c r="H124" s="7" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="I124" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J124" s="7" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="K124" s="19" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
       <c r="L124" s="19" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="M124" s="19"/>
       <c r="N124" s="19" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="O124" s="19" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
       <c r="P124" s="19" t="n">
         <v>1</v>
       </c>
       <c r="Q124" s="24" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
       <c r="R124" s="24" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="S124" s="24" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="T124" s="26" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="U124" s="22"/>
       <c r="V124" s="22"/>
@@ -7998,10 +8118,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="53.7" outlineLevel="0" r="125">
       <c r="A125" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>630</v>
+        <v>633</v>
       </c>
       <c r="E125" s="7" t="s">
         <v>22</v>
@@ -8010,44 +8130,44 @@
         <v>22</v>
       </c>
       <c r="H125" s="7" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="I125" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J125" s="7" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="K125" s="19" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
       <c r="L125" s="19" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="M125" s="19"/>
       <c r="N125" s="19" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="O125" s="19" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="P125" s="19" t="n">
         <v>2</v>
       </c>
       <c r="Q125" s="19" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
       <c r="R125" s="19" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="S125" s="20" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="T125" s="21" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
       <c r="U125" s="22" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
       <c r="V125" s="22"/>
       <c r="W125" s="22"/>
@@ -8055,10 +8175,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="32.8" outlineLevel="0" r="126">
       <c r="A126" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="E126" s="7" t="s">
         <v>22</v>
@@ -8067,47 +8187,291 @@
         <v>22</v>
       </c>
       <c r="H126" s="7" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="I126" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J126" s="7" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="K126" s="19" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
       <c r="L126" s="19" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
       <c r="M126" s="19"/>
       <c r="N126" s="19" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="O126" s="19" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="P126" s="19" t="n">
         <v>2</v>
       </c>
       <c r="Q126" s="19" t="s">
-        <v>642</v>
+        <v>645</v>
       </c>
       <c r="R126" s="19" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="S126" s="20"/>
       <c r="T126" s="21" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
       <c r="U126" s="22" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
       <c r="V126" s="22"/>
       <c r="W126" s="22"/>
       <c r="X126" s="22" t="s">
-        <v>646</v>
+        <v>649</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="127">
+      <c r="A127" s="27" t="s">
+        <v>650</v>
+      </c>
+      <c r="B127" s="28" t="s">
+        <v>651</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G127" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H127" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I127" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K127" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="M127" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="O127" s="1" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="128">
+      <c r="A128" s="27" t="s">
+        <v>650</v>
+      </c>
+      <c r="B128" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G128" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H128" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I128" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K128" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="M128" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O128" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="129">
+      <c r="A129" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="B129" s="27" t="s">
+        <v>656</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G129" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H129" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I129" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K129" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="M129" s="27" t="s">
+        <v>658</v>
+      </c>
+      <c r="O129" s="1" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="130">
+      <c r="A130" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="B130" s="27" t="s">
+        <v>660</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G130" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H130" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I130" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K130" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="M130" s="27" t="s">
+        <v>662</v>
+      </c>
+      <c r="O130" s="1" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="131">
+      <c r="A131" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="B131" s="27" t="s">
+        <v>664</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G131" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H131" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I131" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K131" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="M131" s="27" t="s">
+        <v>666</v>
+      </c>
+      <c r="O131" s="1" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="132">
+      <c r="A132" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="B132" s="27" t="s">
+        <v>668</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G132" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H132" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I132" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K132" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="M132" s="27" t="s">
+        <v>670</v>
+      </c>
+      <c r="O132" s="1" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="133">
+      <c r="A133" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="B133" s="27" t="s">
+        <v>672</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G133" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H133" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I133" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K133" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="M133" s="27" t="s">
+        <v>674</v>
+      </c>
+      <c r="O133" s="1" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="134">
+      <c r="A134" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="B134" s="27" t="s">
+        <v>676</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G134" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H134" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I134" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K134" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="M134" s="27" t="s">
+        <v>678</v>
+      </c>
+      <c r="O134" s="1" t="s">
+        <v>679</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
layout and css tweaks
</commit_message>
<xml_diff>
--- a/sampledata/fieldinformation.xlsx
+++ b/sampledata/fieldinformation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1583" uniqueCount="683">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1585" uniqueCount="684">
   <si>
     <t>table</t>
   </si>
@@ -1194,6 +1194,9 @@
   </si>
   <si>
     <t>PP_Alternate_Name</t>
+  </si>
+  <si>
+    <t>Alternate Names</t>
   </si>
   <si>
     <t>List of synonymous protein names</t>
@@ -2407,11 +2410,11 @@
   <dimension ref="A1:X138"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <pane activePane="bottomRight" topLeftCell="C34" xSplit="2556" ySplit="2250"/>
+      <pane activePane="bottomRight" topLeftCell="A1" xSplit="2556" ySplit="2250"/>
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-      <selection activeCell="C1" activeCellId="0" pane="topRight" sqref="C1"/>
-      <selection activeCell="A34" activeCellId="0" pane="bottomLeft" sqref="A34"/>
-      <selection activeCell="C60" activeCellId="0" pane="bottomRight" sqref="C60"/>
+      <selection activeCell="A1" activeCellId="0" pane="topRight" sqref="A1"/>
+      <selection activeCell="A1" activeCellId="0" pane="bottomLeft" sqref="A1"/>
+      <selection activeCell="B117" activeCellId="0" pane="bottomRight" sqref="B117"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -6346,24 +6349,26 @@
       <c r="L97" s="18" t="s">
         <v>392</v>
       </c>
-      <c r="M97" s="18"/>
+      <c r="M97" s="18" t="s">
+        <v>393</v>
+      </c>
       <c r="N97" s="18" t="s">
         <v>375</v>
       </c>
       <c r="O97" s="18" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="P97" s="5" t="n">
         <v>1</v>
       </c>
       <c r="Q97" s="18" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="R97" s="18" t="s">
         <v>378</v>
       </c>
       <c r="S97" s="18" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="T97" s="19" t="s">
         <v>389</v>
@@ -6398,17 +6403,17 @@
         <v>371</v>
       </c>
       <c r="K98" s="18" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="L98" s="18" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="M98" s="18"/>
       <c r="N98" s="18" t="s">
         <v>241</v>
       </c>
       <c r="O98" s="18" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="P98" s="5" t="n">
         <v>1</v>
@@ -6416,7 +6421,7 @@
       <c r="Q98" s="18"/>
       <c r="R98" s="18"/>
       <c r="S98" s="18" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="T98" s="19"/>
       <c r="U98" s="18"/>
@@ -6449,17 +6454,17 @@
         <v>371</v>
       </c>
       <c r="K99" s="18" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="L99" s="18" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="M99" s="18"/>
       <c r="N99" s="18" t="s">
         <v>241</v>
       </c>
       <c r="O99" s="18" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="P99" s="5" t="n">
         <v>1</v>
@@ -6467,7 +6472,7 @@
       <c r="Q99" s="18"/>
       <c r="R99" s="18"/>
       <c r="S99" s="18" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="T99" s="19"/>
       <c r="U99" s="18"/>
@@ -6477,7 +6482,7 @@
         <v>369</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C100" s="7"/>
       <c r="D100" s="7"/>
@@ -6500,27 +6505,27 @@
         <v>371</v>
       </c>
       <c r="K100" s="18" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="L100" s="18" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="M100" s="18"/>
       <c r="N100" s="18" t="s">
         <v>241</v>
       </c>
       <c r="O100" s="18" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="P100" s="5" t="n">
         <v>1</v>
       </c>
       <c r="Q100" s="18" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="R100" s="18"/>
       <c r="S100" s="18" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="T100" s="19"/>
       <c r="U100" s="18"/>
@@ -6530,7 +6535,7 @@
         <v>369</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C101" s="7"/>
       <c r="D101" s="7"/>
@@ -6551,32 +6556,32 @@
         <v>371</v>
       </c>
       <c r="K101" s="18" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="L101" s="18" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="M101" s="18"/>
       <c r="N101" s="18" t="s">
         <v>375</v>
       </c>
       <c r="O101" s="18" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="P101" s="5" t="n">
         <v>2</v>
       </c>
       <c r="Q101" s="18" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="R101" s="18" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="S101" s="18" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="T101" s="19" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="U101" s="18"/>
     </row>
@@ -6585,7 +6590,7 @@
         <v>369</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C102" s="7"/>
       <c r="D102" s="7"/>
@@ -6606,32 +6611,32 @@
         <v>371</v>
       </c>
       <c r="K102" s="18" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="L102" s="18" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="M102" s="18"/>
       <c r="N102" s="18" t="s">
         <v>375</v>
       </c>
       <c r="O102" s="18" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="P102" s="5" t="n">
         <v>2</v>
       </c>
       <c r="Q102" s="18" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="R102" s="18" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="S102" s="18" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="T102" s="19" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="U102" s="18"/>
     </row>
@@ -6640,7 +6645,7 @@
         <v>369</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C103" s="7"/>
       <c r="D103" s="7"/>
@@ -6661,30 +6666,30 @@
         <v>371</v>
       </c>
       <c r="K103" s="18" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="L103" s="18" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="M103" s="18"/>
       <c r="N103" s="18" t="s">
         <v>375</v>
       </c>
       <c r="O103" s="18" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="P103" s="5" t="n">
         <v>2</v>
       </c>
       <c r="Q103" s="18"/>
       <c r="R103" s="18" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="S103" s="18" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="T103" s="19" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="U103" s="18"/>
     </row>
@@ -6693,7 +6698,7 @@
         <v>369</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C104" s="7"/>
       <c r="D104" s="7"/>
@@ -6714,30 +6719,30 @@
         <v>371</v>
       </c>
       <c r="K104" s="18" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="L104" s="18" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="M104" s="18"/>
       <c r="N104" s="18" t="s">
         <v>241</v>
       </c>
       <c r="O104" s="18" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="P104" s="5" t="n">
         <v>1</v>
       </c>
       <c r="Q104" s="18"/>
       <c r="R104" s="18" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="S104" s="18" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="T104" s="19" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="U104" s="18"/>
     </row>
@@ -6746,7 +6751,7 @@
         <v>369</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C105" s="7"/>
       <c r="D105" s="7"/>
@@ -6767,32 +6772,32 @@
         <v>371</v>
       </c>
       <c r="K105" s="18" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="L105" s="18" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="M105" s="18"/>
       <c r="N105" s="18" t="s">
         <v>241</v>
       </c>
       <c r="O105" s="18" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="P105" s="5" t="n">
         <v>2</v>
       </c>
       <c r="Q105" s="18" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="R105" s="18" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="S105" s="18" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="T105" s="19" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="U105" s="18"/>
     </row>
@@ -6801,7 +6806,7 @@
         <v>369</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C106" s="7"/>
       <c r="D106" s="7"/>
@@ -6822,32 +6827,32 @@
         <v>371</v>
       </c>
       <c r="K106" s="18" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="L106" s="18" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="M106" s="18"/>
       <c r="N106" s="18" t="s">
         <v>241</v>
       </c>
       <c r="O106" s="18" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="P106" s="5" t="n">
         <v>2</v>
       </c>
       <c r="Q106" s="18" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="R106" s="18" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="S106" s="18" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="T106" s="19" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="U106" s="18"/>
     </row>
@@ -6856,7 +6861,7 @@
         <v>369</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C107" s="7"/>
       <c r="D107" s="7"/>
@@ -6877,32 +6882,32 @@
         <v>371</v>
       </c>
       <c r="K107" s="18" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="L107" s="18" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="M107" s="18"/>
       <c r="N107" s="18" t="s">
         <v>375</v>
       </c>
       <c r="O107" s="18" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="P107" s="5" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="Q107" s="18" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="R107" s="18" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="S107" s="18" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="T107" s="19" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="U107" s="18"/>
     </row>
@@ -6911,7 +6916,7 @@
         <v>369</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C108" s="7"/>
       <c r="D108" s="7"/>
@@ -6932,29 +6937,29 @@
         <v>371</v>
       </c>
       <c r="K108" s="18" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="L108" s="18" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="M108" s="18"/>
       <c r="N108" s="18" t="s">
         <v>375</v>
       </c>
       <c r="O108" s="18" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="P108" s="5" t="n">
         <v>2</v>
       </c>
       <c r="Q108" s="18" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="R108" s="18" t="s">
         <v>378</v>
       </c>
       <c r="S108" s="18" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="T108" s="19" t="s">
         <v>389</v>
@@ -6966,7 +6971,7 @@
         <v>369</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C109" s="7"/>
       <c r="D109" s="7"/>
@@ -6987,32 +6992,32 @@
         <v>371</v>
       </c>
       <c r="K109" s="18" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="L109" s="18" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="M109" s="18"/>
       <c r="N109" s="18" t="s">
         <v>375</v>
       </c>
       <c r="O109" s="18" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="P109" s="5" t="n">
         <v>3</v>
       </c>
       <c r="Q109" s="18" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="R109" s="18" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="S109" s="18" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="T109" s="19" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="U109" s="18"/>
     </row>
@@ -7021,7 +7026,7 @@
         <v>369</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C110" s="7"/>
       <c r="D110" s="7"/>
@@ -7042,30 +7047,30 @@
         <v>371</v>
       </c>
       <c r="K110" s="18" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="L110" s="18" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="M110" s="18"/>
       <c r="N110" s="18" t="s">
         <v>241</v>
       </c>
       <c r="O110" s="18" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="P110" s="5" t="n">
         <v>2</v>
       </c>
       <c r="Q110" s="18"/>
       <c r="R110" s="18" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="S110" s="18" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="T110" s="19" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="U110" s="18"/>
     </row>
@@ -7074,7 +7079,7 @@
         <v>369</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="C111" s="7"/>
       <c r="D111" s="7"/>
@@ -7095,35 +7100,35 @@
         <v>371</v>
       </c>
       <c r="K111" s="18" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="L111" s="18" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="M111" s="18"/>
       <c r="N111" s="18"/>
       <c r="O111" s="18" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="P111" s="5" t="n">
         <v>2</v>
       </c>
       <c r="Q111" s="18"/>
       <c r="R111" s="18" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="S111" s="18" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="T111" s="19" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="U111" s="18"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="44" outlineLevel="0" r="112">
       <c r="A112" s="7"/>
       <c r="B112" s="7" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C112" s="7"/>
       <c r="D112" s="7" t="s">
@@ -7144,37 +7149,37 @@
         <v>371</v>
       </c>
       <c r="K112" s="18" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="L112" s="18" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="M112" s="18"/>
       <c r="N112" s="18" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="O112" s="18" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="P112" s="5" t="n">
         <v>1</v>
       </c>
       <c r="Q112" s="18"/>
       <c r="R112" s="18" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="S112" s="18" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="T112" s="19" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="U112" s="18"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="29.85" outlineLevel="0" r="113">
       <c r="A113" s="7"/>
       <c r="B113" s="7" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C113" s="7"/>
       <c r="D113" s="7" t="s">
@@ -7195,42 +7200,42 @@
         <v>371</v>
       </c>
       <c r="K113" s="18" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="L113" s="18" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="M113" s="18"/>
       <c r="N113" s="18" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="O113" s="18" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="P113" s="5" t="n">
         <v>1</v>
       </c>
       <c r="Q113" s="18"/>
       <c r="R113" s="18" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="S113" s="18" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="T113" s="20" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="U113" s="18"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="32.8" outlineLevel="0" r="114">
       <c r="A114" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>132</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="E114" s="7" t="s">
         <v>22</v>
@@ -7248,53 +7253,53 @@
         <v>22</v>
       </c>
       <c r="J114" s="7" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="K114" s="21" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="L114" s="21" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="M114" s="21" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="N114" s="21" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="O114" s="21" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="P114" s="21" t="n">
         <v>1</v>
       </c>
       <c r="Q114" s="21" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="R114" s="21" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="S114" s="22"/>
       <c r="T114" s="23"/>
       <c r="U114" s="24" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="V114" s="24" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="W114" s="24" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="X114" s="24" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="22.35" outlineLevel="0" r="115">
       <c r="A115" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="E115" s="7" t="s">
         <v>22</v>
@@ -7312,19 +7317,19 @@
         <v>22</v>
       </c>
       <c r="J115" s="7" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="K115" s="21" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="L115" s="21" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="M115" s="21" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="N115" s="21" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="O115" s="21" t="s">
         <v>381</v>
@@ -7333,7 +7338,7 @@
         <v>1</v>
       </c>
       <c r="Q115" s="21" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="R115" s="21"/>
       <c r="S115" s="22"/>
@@ -7345,7 +7350,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="22.35" outlineLevel="0" r="116">
       <c r="A116" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>390</v>
@@ -7366,26 +7371,28 @@
         <v>22</v>
       </c>
       <c r="J116" s="7" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="K116" s="21" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="L116" s="21" t="s">
-        <v>518</v>
-      </c>
-      <c r="M116" s="21"/>
+        <v>519</v>
+      </c>
+      <c r="M116" s="21" t="s">
+        <v>393</v>
+      </c>
       <c r="N116" s="21" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="O116" s="21" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="P116" s="21" t="n">
         <v>2</v>
       </c>
       <c r="Q116" s="21" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="R116" s="21"/>
       <c r="S116" s="22"/>
@@ -7397,10 +7404,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="117">
       <c r="A117" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="E117" s="7" t="s">
         <v>22</v>
@@ -7415,26 +7422,26 @@
         <v>22</v>
       </c>
       <c r="J117" s="7" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="K117" s="21" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="L117" s="21" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="M117" s="21"/>
       <c r="N117" s="21" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="O117" s="21" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="P117" s="21" t="n">
         <v>2</v>
       </c>
       <c r="Q117" s="21" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="R117" s="21"/>
       <c r="S117" s="22"/>
@@ -7446,10 +7453,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="118">
       <c r="A118" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="E118" s="7" t="s">
         <v>22</v>
@@ -7464,24 +7471,24 @@
         <v>22</v>
       </c>
       <c r="J118" s="7" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="K118" s="21" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="L118" s="21" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="M118" s="21"/>
       <c r="N118" s="21" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="O118" s="21"/>
       <c r="P118" s="21" t="n">
         <v>1</v>
       </c>
       <c r="Q118" s="21" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="R118" s="21"/>
       <c r="S118" s="22"/>
@@ -7493,7 +7500,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="119">
       <c r="A119" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>98</v>
@@ -7514,28 +7521,28 @@
         <v>22</v>
       </c>
       <c r="J119" s="7" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="K119" s="21" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="L119" s="21" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="M119" s="21" t="s">
         <v>99</v>
       </c>
       <c r="N119" s="21" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="O119" s="21" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="P119" s="21" t="n">
         <v>1</v>
       </c>
       <c r="Q119" s="21" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="R119" s="21"/>
       <c r="S119" s="22"/>
@@ -7547,10 +7554,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="53.7" outlineLevel="0" r="120">
       <c r="A120" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="E120" s="7" t="s">
         <v>22</v>
@@ -7565,48 +7572,48 @@
         <v>22</v>
       </c>
       <c r="J120" s="7" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="K120" s="21" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="L120" s="21" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="M120" s="21"/>
       <c r="N120" s="21" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="O120" s="21" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="P120" s="21" t="n">
         <v>1</v>
       </c>
       <c r="Q120" s="21" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="R120" s="21" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="S120" s="22"/>
       <c r="T120" s="23"/>
       <c r="U120" s="24" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="V120" s="24" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="W120" s="24" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="X120" s="24" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="53.7" outlineLevel="0" r="121">
       <c r="A121" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>252</v>
@@ -7624,43 +7631,43 @@
         <v>22</v>
       </c>
       <c r="J121" s="7" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="K121" s="21" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="L121" s="21" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="M121" s="21"/>
       <c r="N121" s="21" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="O121" s="21" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="P121" s="21" t="n">
         <v>1</v>
       </c>
       <c r="Q121" s="25" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="R121" s="21"/>
       <c r="S121" s="22"/>
       <c r="T121" s="23"/>
       <c r="U121" s="24"/>
       <c r="V121" s="24" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="W121" s="24"/>
       <c r="X121" s="24"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="22.35" outlineLevel="0" r="122">
       <c r="A122" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="E122" s="7" t="s">
         <v>22</v>
@@ -7675,31 +7682,31 @@
         <v>22</v>
       </c>
       <c r="J122" s="7" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="K122" s="21" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="L122" s="21" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="M122" s="21"/>
       <c r="N122" s="21" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="O122" s="21" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="P122" s="21" t="n">
         <v>1</v>
       </c>
       <c r="Q122" s="21" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="R122" s="21"/>
       <c r="S122" s="22"/>
       <c r="T122" s="23" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="U122" s="24"/>
       <c r="V122" s="24"/>
@@ -7708,10 +7715,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="32.8" outlineLevel="0" r="123">
       <c r="A123" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="E123" s="7" t="s">
         <v>22</v>
@@ -7729,36 +7736,36 @@
         <v>22</v>
       </c>
       <c r="J123" s="7" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="K123" s="21" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="L123" s="21" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="M123" s="21"/>
       <c r="N123" s="21" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="O123" s="21" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="P123" s="21" t="n">
         <v>1</v>
       </c>
       <c r="Q123" s="21" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="R123" s="21" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="S123" s="22" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="T123" s="23"/>
       <c r="U123" s="24" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="V123" s="24"/>
       <c r="W123" s="24"/>
@@ -7766,10 +7773,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="22.35" outlineLevel="0" r="124">
       <c r="A124" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="E124" s="7" t="s">
         <v>22</v>
@@ -7787,30 +7794,30 @@
         <v>22</v>
       </c>
       <c r="J124" s="7" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="K124" s="21" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="L124" s="21" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="M124" s="21"/>
       <c r="N124" s="21" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="O124" s="21" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="P124" s="21" t="n">
         <v>1</v>
       </c>
       <c r="Q124" s="21"/>
       <c r="R124" s="21" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="S124" s="22" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="T124" s="23"/>
       <c r="U124" s="24"/>
@@ -7820,10 +7827,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="22.35" outlineLevel="0" r="125">
       <c r="A125" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="E125" s="7" t="s">
         <v>22</v>
@@ -7841,53 +7848,53 @@
         <v>22</v>
       </c>
       <c r="J125" s="7" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="K125" s="21" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="L125" s="21" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="M125" s="21"/>
       <c r="N125" s="21" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="O125" s="21" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="P125" s="21" t="n">
         <v>1</v>
       </c>
       <c r="Q125" s="21" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="R125" s="21" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="S125" s="22" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="T125" s="23"/>
       <c r="U125" s="24" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="V125" s="24" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="W125" s="24" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="X125" s="24" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="43.25" outlineLevel="0" r="126">
       <c r="A126" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="E126" s="7" t="s">
         <v>22</v>
@@ -7905,49 +7912,49 @@
         <v>22</v>
       </c>
       <c r="J126" s="7" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="K126" s="21" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="L126" s="21" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="M126" s="21"/>
       <c r="N126" s="21" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="O126" s="21" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="P126" s="21" t="n">
         <v>1</v>
       </c>
       <c r="Q126" s="26" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="R126" s="21" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="S126" s="22" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="T126" s="23" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="U126" s="24"/>
       <c r="V126" s="24" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="W126" s="24"/>
       <c r="X126" s="24"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="22.35" outlineLevel="0" r="127">
       <c r="A127" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="E127" s="7" t="s">
         <v>22</v>
@@ -7962,31 +7969,31 @@
         <v>22</v>
       </c>
       <c r="J127" s="7" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="K127" s="26" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="L127" s="26" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="M127" s="26"/>
       <c r="N127" s="26" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="O127" s="26" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="P127" s="26" t="n">
         <v>2</v>
       </c>
       <c r="Q127" s="26" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="R127" s="26"/>
       <c r="S127" s="27"/>
       <c r="T127" s="28" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="U127" s="24"/>
       <c r="V127" s="24"/>
@@ -7995,10 +8002,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="64.15" outlineLevel="0" r="128">
       <c r="A128" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="E128" s="7" t="s">
         <v>22</v>
@@ -8016,53 +8023,53 @@
         <v>22</v>
       </c>
       <c r="J128" s="7" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="K128" s="21" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="L128" s="21" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="M128" s="21"/>
       <c r="N128" s="21" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="O128" s="21" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="P128" s="21" t="n">
         <v>1</v>
       </c>
       <c r="Q128" s="21" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="R128" s="21" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="S128" s="22" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="T128" s="23" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="U128" s="24" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="V128" s="24" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="W128" s="24"/>
       <c r="X128" s="24" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="22.35" outlineLevel="0" r="129">
       <c r="A129" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E129" s="7" t="s">
         <v>22</v>
@@ -8077,33 +8084,33 @@
         <v>22</v>
       </c>
       <c r="J129" s="7" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="K129" s="21" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="L129" s="21" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="M129" s="21"/>
       <c r="N129" s="21" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="O129" s="21" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="P129" s="21" t="n">
         <v>2</v>
       </c>
       <c r="Q129" s="21" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="R129" s="21" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="S129" s="22"/>
       <c r="T129" s="23" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="U129" s="24"/>
       <c r="V129" s="24"/>
@@ -8112,10 +8119,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="85.05" outlineLevel="0" r="130">
       <c r="A130" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="E130" s="7" t="s">
         <v>22</v>
@@ -8130,51 +8137,51 @@
         <v>22</v>
       </c>
       <c r="J130" s="7" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="K130" s="21" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="L130" s="21" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="M130" s="21"/>
       <c r="N130" s="21" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="O130" s="21" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="P130" s="21" t="n">
         <v>1</v>
       </c>
       <c r="Q130" s="21"/>
       <c r="R130" s="21" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="S130" s="22" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="T130" s="23" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="U130" s="24" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="V130" s="24" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="W130" s="24"/>
       <c r="X130" s="24" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="179.1" outlineLevel="0" r="131">
       <c r="A131" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="E131" s="7" t="s">
         <v>22</v>
@@ -8189,35 +8196,35 @@
         <v>22</v>
       </c>
       <c r="J131" s="7" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="K131" s="21" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="L131" s="21" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="M131" s="21"/>
       <c r="N131" s="21" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="O131" s="21" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="P131" s="21" t="n">
         <v>1</v>
       </c>
       <c r="Q131" s="21" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="R131" s="21" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="S131" s="22" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="T131" s="23" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="U131" s="24"/>
       <c r="V131" s="24"/>
@@ -8226,10 +8233,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="32.8" outlineLevel="0" r="132">
       <c r="A132" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="E132" s="7" t="s">
         <v>22</v>
@@ -8244,36 +8251,36 @@
         <v>22</v>
       </c>
       <c r="J132" s="7" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="K132" s="21" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="L132" s="21" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="M132" s="21"/>
       <c r="N132" s="21" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="O132" s="21" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="P132" s="21" t="n">
         <v>2</v>
       </c>
       <c r="Q132" s="21" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="R132" s="21" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="S132" s="22"/>
       <c r="T132" s="23" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="U132" s="24" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="V132" s="24"/>
       <c r="W132" s="24"/>
@@ -8281,10 +8288,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="137.3" outlineLevel="0" r="133">
       <c r="A133" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="E133" s="7" t="s">
         <v>22</v>
@@ -8299,49 +8306,49 @@
         <v>22</v>
       </c>
       <c r="J133" s="7" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="K133" s="21" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="L133" s="21" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="M133" s="21"/>
       <c r="N133" s="21" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="O133" s="21" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="P133" s="21" t="n">
         <v>2</v>
       </c>
       <c r="Q133" s="21" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="R133" s="21" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="S133" s="22" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="T133" s="23" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="U133" s="24"/>
       <c r="V133" s="24"/>
       <c r="W133" s="24"/>
       <c r="X133" s="24" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="64.15" outlineLevel="0" r="134">
       <c r="A134" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="E134" s="7" t="s">
         <v>22</v>
@@ -8356,47 +8363,47 @@
         <v>22</v>
       </c>
       <c r="J134" s="7" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="K134" s="21" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="L134" s="21" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="M134" s="21"/>
       <c r="N134" s="21" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="O134" s="21" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="P134" s="21" t="n">
         <v>1</v>
       </c>
       <c r="Q134" s="21" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="R134" s="21" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="S134" s="22"/>
       <c r="T134" s="23" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="U134" s="24"/>
       <c r="V134" s="24" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="W134" s="24"/>
       <c r="X134" s="24"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="22.35" outlineLevel="0" r="135">
       <c r="A135" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="E135" s="7" t="s">
         <v>22</v>
@@ -8411,31 +8418,31 @@
         <v>22</v>
       </c>
       <c r="J135" s="7" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="K135" s="21" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="L135" s="26" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="M135" s="26"/>
       <c r="N135" s="21" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="O135" s="21" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="P135" s="21" t="n">
         <v>2</v>
       </c>
       <c r="Q135" s="21" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="R135" s="21"/>
       <c r="S135" s="22"/>
       <c r="T135" s="23" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="U135" s="24"/>
       <c r="V135" s="24"/>
@@ -8444,10 +8451,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="43.25" outlineLevel="0" r="136">
       <c r="A136" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="E136" s="7" t="s">
         <v>22</v>
@@ -8462,35 +8469,35 @@
         <v>22</v>
       </c>
       <c r="J136" s="7" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="K136" s="21" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="L136" s="21" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="M136" s="21"/>
       <c r="N136" s="21" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="O136" s="21" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="P136" s="21" t="n">
         <v>1</v>
       </c>
       <c r="Q136" s="26" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="R136" s="26" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="S136" s="26" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="T136" s="28" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="U136" s="24"/>
       <c r="V136" s="24"/>
@@ -8499,10 +8506,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="53.7" outlineLevel="0" r="137">
       <c r="A137" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="E137" s="7" t="s">
         <v>22</v>
@@ -8517,38 +8524,38 @@
         <v>22</v>
       </c>
       <c r="J137" s="7" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="K137" s="21" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="L137" s="21" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="M137" s="21"/>
       <c r="N137" s="21" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="O137" s="21" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="P137" s="21" t="n">
         <v>2</v>
       </c>
       <c r="Q137" s="21" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="R137" s="21" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="S137" s="22" t="s">
         <v>389</v>
       </c>
       <c r="T137" s="23" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="U137" s="24" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="V137" s="24"/>
       <c r="W137" s="24"/>
@@ -8556,10 +8563,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="32.8" outlineLevel="0" r="138">
       <c r="A138" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="E138" s="7" t="s">
         <v>22</v>
@@ -8574,41 +8581,41 @@
         <v>22</v>
       </c>
       <c r="J138" s="7" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="K138" s="21" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="L138" s="21" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="M138" s="21"/>
       <c r="N138" s="21" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="O138" s="21" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="P138" s="21" t="n">
         <v>2</v>
       </c>
       <c r="Q138" s="21" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="R138" s="21" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="S138" s="22"/>
       <c r="T138" s="23" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="U138" s="24" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="V138" s="24"/>
       <c r="W138" s="24"/>
       <c r="X138" s="24" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- add datasets to the small molecule page - UI tweaks: -- image styling -- field order
</commit_message>
<xml_diff>
--- a/sampledata/fieldinformation.xlsx
+++ b/sampledata/fieldinformation.xlsx
@@ -2349,7 +2349,7 @@
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -2422,29 +2422,29 @@
   <dimension ref="A1:X139"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <pane activePane="bottomRight" topLeftCell="C49" xSplit="2369" ySplit="2250"/>
+      <pane activePane="bottomRight" topLeftCell="A61" xSplit="2195" ySplit="2250"/>
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-      <selection activeCell="C1" activeCellId="0" pane="topRight" sqref="C1"/>
-      <selection activeCell="A49" activeCellId="0" pane="bottomLeft" sqref="A49"/>
-      <selection activeCell="O61" activeCellId="0" pane="bottomRight" sqref="O61"/>
+      <selection activeCell="A1" activeCellId="0" pane="topRight" sqref="A1"/>
+      <selection activeCell="A61" activeCellId="0" pane="bottomLeft" sqref="A61"/>
+      <selection activeCell="H69" activeCellId="0" pane="bottomRight" sqref="H69"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.7607843137255"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.2588235294118"/>
-    <col collapsed="false" hidden="false" max="9" min="3" style="1" width="10.8901960784314"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="10.8901960784314"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.8901960784314"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="28.1098039215686"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="1" width="25.9137254901961"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="55.7686274509804"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="15.1411764705882"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="44.8862745098039"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="13.9921568627451"/>
-    <col collapsed="false" hidden="false" max="20" min="19" style="1" width="21.643137254902"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="21.4980392156863"/>
-    <col collapsed="false" hidden="false" max="24" min="22" style="1" width="9.4156862745098"/>
-    <col collapsed="false" hidden="false" max="1025" min="25" style="0" width="9.4156862745098"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.8705882352941"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.321568627451"/>
+    <col collapsed="false" hidden="false" max="9" min="3" style="1" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.9450980392157"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="28.2549019607843"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="1" width="26.0392156862745"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="56.0470588235294"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="15.2235294117647"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="45.1137254901961"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="14.0627450980392"/>
+    <col collapsed="false" hidden="false" max="20" min="19" style="1" width="21.7529411764706"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="21.6078431372549"/>
+    <col collapsed="false" hidden="false" max="24" min="22" style="1" width="9.45882352941177"/>
+    <col collapsed="false" hidden="false" max="1025" min="25" style="0" width="9.45882352941177"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="86.55" outlineLevel="0" r="1">
@@ -3963,7 +3963,7 @@
         <v>23</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="I44" s="3" t="s">
         <v>23</v>
@@ -3995,7 +3995,7 @@
         <v>23</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="I45" s="3" t="s">
         <v>23</v>
@@ -4861,7 +4861,7 @@
         <v>22</v>
       </c>
       <c r="H68" s="7" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="I68" s="3" t="s">
         <v>22</v>
@@ -7757,7 +7757,7 @@
       <c r="W123" s="24"/>
       <c r="X123" s="24"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="32.8" outlineLevel="0" r="124">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="22.35" outlineLevel="0" r="124">
       <c r="A124" s="1" t="s">
         <v>503</v>
       </c>

</xml_diff>

<commit_message>
- loop batch save optimization for import_datasets - hide summary field
</commit_message>
<xml_diff>
--- a/sampledata/fieldinformation.xlsx
+++ b/sampledata/fieldinformation.xlsx
@@ -2452,11 +2452,11 @@
   <dimension ref="A1:X140"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <pane activePane="bottomRight" topLeftCell="A54" xSplit="2195" ySplit="2250"/>
+      <pane activePane="bottomRight" topLeftCell="A16" xSplit="2195" ySplit="2250"/>
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
       <selection activeCell="A1" activeCellId="0" pane="topRight" sqref="A1"/>
-      <selection activeCell="A54" activeCellId="0" pane="bottomLeft" sqref="A54"/>
-      <selection activeCell="M67" activeCellId="0" pane="bottomRight" sqref="M67"/>
+      <selection activeCell="A16" activeCellId="0" pane="bottomLeft" sqref="A16"/>
+      <selection activeCell="F32" activeCellId="0" pane="bottomRight" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -3633,7 +3633,7 @@
         <v>22</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
- ordering for dataset columns (closes #57)
</commit_message>
<xml_diff>
--- a/sampledata/fieldinformation.xlsx
+++ b/sampledata/fieldinformation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1607" uniqueCount="698">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1607" uniqueCount="697">
   <si>
     <t>table</t>
   </si>
@@ -912,9 +912,6 @@
   </si>
   <si>
     <t>chembl_id</t>
-  </si>
-  <si>
-    <t>34</t>
   </si>
   <si>
     <t>ChEMBL ID</t>
@@ -2452,11 +2449,11 @@
   <dimension ref="A1:X140"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <pane activePane="bottomRight" topLeftCell="A16" xSplit="2195" ySplit="2250"/>
+      <pane activePane="bottomRight" topLeftCell="A66" xSplit="2195" ySplit="2250"/>
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
       <selection activeCell="A1" activeCellId="0" pane="topRight" sqref="A1"/>
-      <selection activeCell="A16" activeCellId="0" pane="bottomLeft" sqref="A16"/>
-      <selection activeCell="F32" activeCellId="0" pane="bottomRight" sqref="F32"/>
+      <selection activeCell="A66" activeCellId="0" pane="bottomLeft" sqref="A66"/>
+      <selection activeCell="H77" activeCellId="0" pane="bottomRight" sqref="H77"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -5306,7 +5303,7 @@
         <v>23</v>
       </c>
       <c r="H76" s="7" t="s">
-        <v>299</v>
+        <v>79</v>
       </c>
       <c r="I76" s="3" t="s">
         <v>23</v>
@@ -5317,11 +5314,11 @@
       </c>
       <c r="L76" s="7"/>
       <c r="M76" s="7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="N76" s="7"/>
       <c r="O76" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="P76" s="7"/>
       <c r="Q76" s="7"/>
@@ -5338,7 +5335,7 @@
         <v>216</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
@@ -5359,13 +5356,13 @@
       </c>
       <c r="L77" s="7"/>
       <c r="M77" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="N77" s="7" t="s">
         <v>221</v>
       </c>
       <c r="O77" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="P77" s="7"/>
       <c r="Q77" s="7"/>
@@ -5380,11 +5377,11 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.85" outlineLevel="0" r="78">
       <c r="A78" s="7"/>
       <c r="B78" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C78" s="7"/>
       <c r="D78" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E78" s="7"/>
       <c r="F78" s="7"/>
@@ -5401,17 +5398,17 @@
         <v>218</v>
       </c>
       <c r="K78" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="L78" s="8" t="s">
         <v>307</v>
-      </c>
-      <c r="L78" s="8" t="s">
-        <v>308</v>
       </c>
       <c r="M78" s="8"/>
       <c r="N78" s="8" t="s">
         <v>221</v>
       </c>
       <c r="O78" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="P78" s="13" t="n">
         <v>1</v>
@@ -5432,7 +5429,7 @@
         <v>216</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C79" s="7"/>
       <c r="D79" s="7"/>
@@ -5453,15 +5450,15 @@
         <v>218</v>
       </c>
       <c r="K79" s="12" t="s">
+        <v>310</v>
+      </c>
+      <c r="L79" s="8" t="s">
         <v>311</v>
-      </c>
-      <c r="L79" s="8" t="s">
-        <v>312</v>
       </c>
       <c r="M79" s="8"/>
       <c r="N79" s="8"/>
       <c r="O79" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="P79" s="13" t="n">
         <v>2</v>
@@ -5470,7 +5467,7 @@
       <c r="R79" s="8"/>
       <c r="S79" s="8"/>
       <c r="T79" s="14" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="U79" s="7"/>
       <c r="V79" s="7"/>
@@ -5480,11 +5477,11 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="90.25" outlineLevel="0" r="80">
       <c r="A80" s="7"/>
       <c r="B80" s="7" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C80" s="7"/>
       <c r="D80" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E80" s="7"/>
       <c r="F80" s="7"/>
@@ -5501,28 +5498,28 @@
         <v>218</v>
       </c>
       <c r="K80" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="L80" s="8" t="s">
         <v>316</v>
-      </c>
-      <c r="L80" s="8" t="s">
-        <v>317</v>
       </c>
       <c r="M80" s="8"/>
       <c r="N80" s="8" t="s">
         <v>221</v>
       </c>
       <c r="O80" s="8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="P80" s="13" t="n">
         <v>2</v>
       </c>
       <c r="Q80" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="R80" s="8"/>
       <c r="S80" s="8"/>
       <c r="T80" s="15" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="U80" s="7"/>
       <c r="V80" s="7"/>
@@ -5534,7 +5531,7 @@
         <v>244</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C81" s="7" t="s">
         <v>251</v>
@@ -5559,25 +5556,25 @@
         <v>218</v>
       </c>
       <c r="K81" s="12" t="s">
+        <v>321</v>
+      </c>
+      <c r="L81" s="8" t="s">
         <v>322</v>
       </c>
-      <c r="L81" s="8" t="s">
+      <c r="M81" s="8" t="s">
         <v>323</v>
-      </c>
-      <c r="M81" s="8" t="s">
-        <v>324</v>
       </c>
       <c r="N81" s="8" t="s">
         <v>251</v>
       </c>
       <c r="O81" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="P81" s="13" t="n">
         <v>1</v>
       </c>
       <c r="Q81" s="8" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="R81" s="8"/>
       <c r="S81" s="8"/>
@@ -5592,7 +5589,7 @@
         <v>244</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C82" s="7"/>
       <c r="D82" s="7"/>
@@ -5615,23 +5612,23 @@
         <v>218</v>
       </c>
       <c r="K82" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="L82" s="8" t="s">
         <v>328</v>
-      </c>
-      <c r="L82" s="8" t="s">
-        <v>329</v>
       </c>
       <c r="M82" s="8"/>
       <c r="N82" s="8" t="s">
         <v>251</v>
       </c>
       <c r="O82" s="8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P82" s="13" t="n">
         <v>1</v>
       </c>
       <c r="Q82" s="8" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="R82" s="8"/>
       <c r="S82" s="8"/>
@@ -5646,7 +5643,7 @@
         <v>244</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C83" s="7"/>
       <c r="D83" s="7"/>
@@ -5669,17 +5666,17 @@
         <v>218</v>
       </c>
       <c r="K83" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="L83" s="8" t="s">
         <v>333</v>
-      </c>
-      <c r="L83" s="8" t="s">
-        <v>334</v>
       </c>
       <c r="M83" s="8"/>
       <c r="N83" s="8" t="s">
         <v>251</v>
       </c>
       <c r="O83" s="8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="P83" s="13" t="n">
         <v>1</v>
@@ -5698,7 +5695,7 @@
         <v>244</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C84" s="7"/>
       <c r="D84" s="7"/>
@@ -5721,19 +5718,19 @@
         <v>218</v>
       </c>
       <c r="K84" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="L84" s="8" t="s">
         <v>337</v>
       </c>
-      <c r="L84" s="8" t="s">
+      <c r="M84" s="8" t="s">
         <v>338</v>
-      </c>
-      <c r="M84" s="8" t="s">
-        <v>339</v>
       </c>
       <c r="N84" s="8" t="s">
         <v>251</v>
       </c>
       <c r="O84" s="8" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="P84" s="13" t="n">
         <v>2</v>
@@ -5764,7 +5761,7 @@
         <v>22</v>
       </c>
       <c r="H85" s="7" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I85" s="3" t="s">
         <v>23</v>
@@ -5773,17 +5770,17 @@
         <v>218</v>
       </c>
       <c r="K85" s="12" t="s">
+        <v>341</v>
+      </c>
+      <c r="L85" s="8" t="s">
         <v>342</v>
-      </c>
-      <c r="L85" s="8" t="s">
-        <v>343</v>
       </c>
       <c r="M85" s="8"/>
       <c r="N85" s="8" t="s">
         <v>251</v>
       </c>
       <c r="O85" s="8" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="P85" s="13" t="n">
         <v>2</v>
@@ -5816,7 +5813,7 @@
         <v>22</v>
       </c>
       <c r="H86" s="7" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="I86" s="3" t="s">
         <v>23</v>
@@ -5825,17 +5822,17 @@
         <v>218</v>
       </c>
       <c r="K86" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="L86" s="8" t="s">
         <v>346</v>
-      </c>
-      <c r="L86" s="8" t="s">
-        <v>347</v>
       </c>
       <c r="M86" s="8"/>
       <c r="N86" s="8" t="s">
         <v>251</v>
       </c>
       <c r="O86" s="8" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="P86" s="13" t="n">
         <v>2</v>
@@ -5868,7 +5865,7 @@
         <v>22</v>
       </c>
       <c r="H87" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I87" s="3" t="s">
         <v>23</v>
@@ -5877,17 +5874,17 @@
         <v>218</v>
       </c>
       <c r="K87" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="L87" s="8" t="s">
         <v>350</v>
-      </c>
-      <c r="L87" s="8" t="s">
-        <v>351</v>
       </c>
       <c r="M87" s="8"/>
       <c r="N87" s="8" t="s">
         <v>251</v>
       </c>
       <c r="O87" s="8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="P87" s="13" t="n">
         <v>1</v>
@@ -5908,7 +5905,7 @@
         <v>244</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C88" s="7"/>
       <c r="D88" s="7"/>
@@ -5920,7 +5917,7 @@
         <v>22</v>
       </c>
       <c r="H88" s="7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I88" s="3" t="s">
         <v>22</v>
@@ -5929,23 +5926,23 @@
         <v>218</v>
       </c>
       <c r="K88" s="12" t="s">
+        <v>354</v>
+      </c>
+      <c r="L88" s="8" t="s">
         <v>355</v>
-      </c>
-      <c r="L88" s="8" t="s">
-        <v>356</v>
       </c>
       <c r="M88" s="8"/>
       <c r="N88" s="8" t="s">
         <v>251</v>
       </c>
       <c r="O88" s="8" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="P88" s="13" t="n">
         <v>3</v>
       </c>
       <c r="Q88" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="R88" s="8"/>
       <c r="S88" s="8"/>
@@ -5960,7 +5957,7 @@
         <v>244</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C89" s="7"/>
       <c r="D89" s="7"/>
@@ -5972,7 +5969,7 @@
         <v>22</v>
       </c>
       <c r="H89" s="7" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="I89" s="3" t="s">
         <v>22</v>
@@ -5981,23 +5978,23 @@
         <v>218</v>
       </c>
       <c r="K89" s="12" t="s">
+        <v>360</v>
+      </c>
+      <c r="L89" s="8" t="s">
         <v>361</v>
-      </c>
-      <c r="L89" s="8" t="s">
-        <v>362</v>
       </c>
       <c r="M89" s="8"/>
       <c r="N89" s="8" t="s">
         <v>251</v>
       </c>
       <c r="O89" s="8" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="P89" s="13" t="n">
         <v>3</v>
       </c>
       <c r="Q89" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="R89" s="8"/>
       <c r="S89" s="8"/>
@@ -6012,7 +6009,7 @@
         <v>244</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C90" s="7"/>
       <c r="D90" s="7"/>
@@ -6024,7 +6021,7 @@
         <v>22</v>
       </c>
       <c r="H90" s="7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I90" s="3" t="s">
         <v>22</v>
@@ -6033,17 +6030,17 @@
         <v>218</v>
       </c>
       <c r="K90" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="L90" s="8" t="s">
         <v>366</v>
-      </c>
-      <c r="L90" s="8" t="s">
-        <v>367</v>
       </c>
       <c r="M90" s="8"/>
       <c r="N90" s="8" t="s">
         <v>251</v>
       </c>
       <c r="O90" s="8" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="P90" s="13" t="n">
         <v>3</v>
@@ -6062,7 +6059,7 @@
         <v>244</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C91" s="7"/>
       <c r="D91" s="7"/>
@@ -6074,7 +6071,7 @@
         <v>22</v>
       </c>
       <c r="H91" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="I91" s="3" t="s">
         <v>22</v>
@@ -6083,23 +6080,23 @@
         <v>218</v>
       </c>
       <c r="K91" s="12" t="s">
+        <v>370</v>
+      </c>
+      <c r="L91" s="8" t="s">
         <v>371</v>
-      </c>
-      <c r="L91" s="8" t="s">
-        <v>372</v>
       </c>
       <c r="M91" s="8"/>
       <c r="N91" s="8" t="s">
         <v>251</v>
       </c>
       <c r="O91" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="P91" s="13" t="n">
         <v>3</v>
       </c>
       <c r="Q91" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="R91" s="8"/>
       <c r="S91" s="8"/>
@@ -6135,7 +6132,7 @@
         <v>23</v>
       </c>
       <c r="K92" s="4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="M92" s="7" t="s">
         <v>146</v>
@@ -6170,7 +6167,7 @@
         <v>23</v>
       </c>
       <c r="K93" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="M93" s="7" t="s">
         <v>149</v>
@@ -6205,7 +6202,7 @@
         <v>23</v>
       </c>
       <c r="K94" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="M94" s="7" t="s">
         <v>152</v>
@@ -6217,11 +6214,11 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.85" outlineLevel="0" r="95">
       <c r="A95" s="7"/>
       <c r="B95" s="7" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C95" s="7"/>
       <c r="D95" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E95" s="7" t="s">
         <v>22</v>
@@ -6231,7 +6228,7 @@
         <v>22</v>
       </c>
       <c r="H95" s="7" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I95" s="3" t="s">
         <v>22</v>
@@ -6240,23 +6237,23 @@
         <v>218</v>
       </c>
       <c r="K95" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="L95" s="8" t="s">
         <v>379</v>
-      </c>
-      <c r="L95" s="8" t="s">
-        <v>380</v>
       </c>
       <c r="M95" s="8"/>
       <c r="N95" s="8" t="s">
         <v>251</v>
       </c>
       <c r="O95" s="8" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="P95" s="13" t="n">
         <v>3</v>
       </c>
       <c r="Q95" s="8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="R95" s="8"/>
       <c r="S95" s="8"/>
@@ -6268,13 +6265,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="100.7" outlineLevel="0" r="96">
       <c r="A96" s="7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B96" s="7" t="s">
         <v>134</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D96" s="7"/>
       <c r="E96" s="7" t="s">
@@ -6293,31 +6290,31 @@
         <v>22</v>
       </c>
       <c r="J96" s="17" t="s">
+        <v>383</v>
+      </c>
+      <c r="K96" s="18" t="s">
         <v>384</v>
       </c>
-      <c r="K96" s="18" t="s">
+      <c r="L96" s="18" t="s">
         <v>385</v>
       </c>
-      <c r="L96" s="18" t="s">
+      <c r="M96" s="18" t="s">
         <v>386</v>
       </c>
-      <c r="M96" s="18" t="s">
+      <c r="N96" s="18" t="s">
         <v>387</v>
       </c>
-      <c r="N96" s="18" t="s">
+      <c r="O96" s="18" t="s">
         <v>388</v>
-      </c>
-      <c r="O96" s="18" t="s">
-        <v>389</v>
       </c>
       <c r="P96" s="5" t="n">
         <v>1</v>
       </c>
       <c r="Q96" s="18" t="s">
+        <v>389</v>
+      </c>
+      <c r="R96" s="18" t="s">
         <v>390</v>
-      </c>
-      <c r="R96" s="18" t="s">
-        <v>391</v>
       </c>
       <c r="S96" s="18"/>
       <c r="T96" s="19"/>
@@ -6325,7 +6322,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="29.85" outlineLevel="0" r="97">
       <c r="A97" s="7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B97" s="7" t="s">
         <v>225</v>
@@ -6348,26 +6345,26 @@
         <v>22</v>
       </c>
       <c r="J97" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K97" s="18" t="s">
+        <v>391</v>
+      </c>
+      <c r="L97" s="18" t="s">
         <v>392</v>
-      </c>
-      <c r="L97" s="18" t="s">
-        <v>393</v>
       </c>
       <c r="M97" s="18"/>
       <c r="N97" s="18" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O97" s="18" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="P97" s="5" t="n">
         <v>1</v>
       </c>
       <c r="Q97" s="18" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="R97" s="18"/>
       <c r="S97" s="18"/>
@@ -6376,10 +6373,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="58.2" outlineLevel="0" r="98">
       <c r="A98" s="7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C98" s="7"/>
       <c r="D98" s="7"/>
@@ -6399,44 +6396,44 @@
         <v>22</v>
       </c>
       <c r="J98" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K98" s="18" t="s">
+        <v>396</v>
+      </c>
+      <c r="L98" s="18" t="s">
         <v>397</v>
-      </c>
-      <c r="L98" s="18" t="s">
-        <v>398</v>
       </c>
       <c r="M98" s="18"/>
       <c r="N98" s="18" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O98" s="18" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="P98" s="5" t="n">
         <v>1</v>
       </c>
       <c r="Q98" s="18" t="s">
+        <v>399</v>
+      </c>
+      <c r="R98" s="18" t="s">
+        <v>390</v>
+      </c>
+      <c r="S98" s="18" t="s">
         <v>400</v>
       </c>
-      <c r="R98" s="18" t="s">
-        <v>391</v>
-      </c>
-      <c r="S98" s="18" t="s">
+      <c r="T98" s="19" t="s">
         <v>401</v>
-      </c>
-      <c r="T98" s="19" t="s">
-        <v>402</v>
       </c>
       <c r="U98" s="18"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="72.35" outlineLevel="0" r="99">
       <c r="A99" s="7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C99" s="7"/>
       <c r="D99" s="7"/>
@@ -6456,46 +6453,46 @@
         <v>22</v>
       </c>
       <c r="J99" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K99" s="18" t="s">
+        <v>403</v>
+      </c>
+      <c r="L99" s="18" t="s">
         <v>404</v>
       </c>
-      <c r="L99" s="18" t="s">
+      <c r="M99" s="18" t="s">
         <v>405</v>
       </c>
-      <c r="M99" s="18" t="s">
+      <c r="N99" s="18" t="s">
+        <v>387</v>
+      </c>
+      <c r="O99" s="18" t="s">
         <v>406</v>
-      </c>
-      <c r="N99" s="18" t="s">
-        <v>388</v>
-      </c>
-      <c r="O99" s="18" t="s">
-        <v>407</v>
       </c>
       <c r="P99" s="5" t="n">
         <v>1</v>
       </c>
       <c r="Q99" s="18" t="s">
+        <v>407</v>
+      </c>
+      <c r="R99" s="18" t="s">
+        <v>390</v>
+      </c>
+      <c r="S99" s="18" t="s">
         <v>408</v>
       </c>
-      <c r="R99" s="18" t="s">
-        <v>391</v>
-      </c>
-      <c r="S99" s="18" t="s">
-        <v>409</v>
-      </c>
       <c r="T99" s="19" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="U99" s="18"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="100">
       <c r="A100" s="7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C100" s="7"/>
       <c r="D100" s="7"/>
@@ -6515,20 +6512,20 @@
         <v>22</v>
       </c>
       <c r="J100" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K100" s="18" t="s">
+        <v>409</v>
+      </c>
+      <c r="L100" s="18" t="s">
         <v>410</v>
-      </c>
-      <c r="L100" s="18" t="s">
-        <v>411</v>
       </c>
       <c r="M100" s="18"/>
       <c r="N100" s="18" t="s">
         <v>251</v>
       </c>
       <c r="O100" s="18" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="P100" s="5" t="n">
         <v>1</v>
@@ -6536,17 +6533,17 @@
       <c r="Q100" s="18"/>
       <c r="R100" s="18"/>
       <c r="S100" s="18" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="T100" s="19"/>
       <c r="U100" s="18"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="29.85" outlineLevel="0" r="101">
       <c r="A101" s="7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C101" s="7"/>
       <c r="D101" s="7"/>
@@ -6566,20 +6563,20 @@
         <v>22</v>
       </c>
       <c r="J101" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K101" s="18" t="s">
+        <v>413</v>
+      </c>
+      <c r="L101" s="18" t="s">
         <v>414</v>
-      </c>
-      <c r="L101" s="18" t="s">
-        <v>415</v>
       </c>
       <c r="M101" s="18"/>
       <c r="N101" s="18" t="s">
         <v>251</v>
       </c>
       <c r="O101" s="18" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="P101" s="5" t="n">
         <v>1</v>
@@ -6587,17 +6584,17 @@
       <c r="Q101" s="18"/>
       <c r="R101" s="18"/>
       <c r="S101" s="18" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="T101" s="19"/>
       <c r="U101" s="18"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="29.85" outlineLevel="0" r="102">
       <c r="A102" s="7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C102" s="7"/>
       <c r="D102" s="7"/>
@@ -6617,40 +6614,40 @@
         <v>22</v>
       </c>
       <c r="J102" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K102" s="18" t="s">
+        <v>418</v>
+      </c>
+      <c r="L102" s="18" t="s">
         <v>419</v>
-      </c>
-      <c r="L102" s="18" t="s">
-        <v>420</v>
       </c>
       <c r="M102" s="18"/>
       <c r="N102" s="18" t="s">
         <v>251</v>
       </c>
       <c r="O102" s="18" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="P102" s="5" t="n">
         <v>1</v>
       </c>
       <c r="Q102" s="18" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="R102" s="18"/>
       <c r="S102" s="18" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="T102" s="19"/>
       <c r="U102" s="18"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="58.2" outlineLevel="0" r="103">
       <c r="A103" s="7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C103" s="7"/>
       <c r="D103" s="7"/>
@@ -6668,44 +6665,44 @@
         <v>22</v>
       </c>
       <c r="J103" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K103" s="18" t="s">
+        <v>424</v>
+      </c>
+      <c r="L103" s="18" t="s">
         <v>425</v>
-      </c>
-      <c r="L103" s="18" t="s">
-        <v>426</v>
       </c>
       <c r="M103" s="18"/>
       <c r="N103" s="18" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O103" s="18" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="P103" s="5" t="n">
         <v>2</v>
       </c>
       <c r="Q103" s="18" t="s">
+        <v>427</v>
+      </c>
+      <c r="R103" s="18" t="s">
         <v>428</v>
       </c>
-      <c r="R103" s="18" t="s">
+      <c r="S103" s="18" t="s">
         <v>429</v>
       </c>
-      <c r="S103" s="18" t="s">
+      <c r="T103" s="19" t="s">
         <v>430</v>
-      </c>
-      <c r="T103" s="19" t="s">
-        <v>431</v>
       </c>
       <c r="U103" s="18"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="58.2" outlineLevel="0" r="104">
       <c r="A104" s="7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C104" s="7"/>
       <c r="D104" s="7"/>
@@ -6723,44 +6720,44 @@
         <v>22</v>
       </c>
       <c r="J104" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K104" s="18" t="s">
+        <v>432</v>
+      </c>
+      <c r="L104" s="18" t="s">
         <v>433</v>
-      </c>
-      <c r="L104" s="18" t="s">
-        <v>434</v>
       </c>
       <c r="M104" s="18"/>
       <c r="N104" s="18" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O104" s="18" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="P104" s="5" t="n">
         <v>2</v>
       </c>
       <c r="Q104" s="18" t="s">
+        <v>435</v>
+      </c>
+      <c r="R104" s="18" t="s">
         <v>436</v>
       </c>
-      <c r="R104" s="18" t="s">
+      <c r="S104" s="18" t="s">
         <v>437</v>
       </c>
-      <c r="S104" s="18" t="s">
+      <c r="T104" s="19" t="s">
         <v>438</v>
-      </c>
-      <c r="T104" s="19" t="s">
-        <v>439</v>
       </c>
       <c r="U104" s="18"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="105">
       <c r="A105" s="7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C105" s="7"/>
       <c r="D105" s="7"/>
@@ -6778,42 +6775,42 @@
         <v>22</v>
       </c>
       <c r="J105" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K105" s="18" t="s">
+        <v>440</v>
+      </c>
+      <c r="L105" s="18" t="s">
         <v>441</v>
-      </c>
-      <c r="L105" s="18" t="s">
-        <v>442</v>
       </c>
       <c r="M105" s="18"/>
       <c r="N105" s="18" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O105" s="18" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="P105" s="5" t="n">
         <v>2</v>
       </c>
       <c r="Q105" s="18"/>
       <c r="R105" s="18" t="s">
+        <v>443</v>
+      </c>
+      <c r="S105" s="18" t="s">
         <v>444</v>
       </c>
-      <c r="S105" s="18" t="s">
-        <v>445</v>
-      </c>
       <c r="T105" s="19" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="U105" s="18"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="44" outlineLevel="0" r="106">
       <c r="A106" s="7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C106" s="7"/>
       <c r="D106" s="7"/>
@@ -6831,42 +6828,42 @@
         <v>22</v>
       </c>
       <c r="J106" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K106" s="18" t="s">
+        <v>446</v>
+      </c>
+      <c r="L106" s="18" t="s">
         <v>447</v>
-      </c>
-      <c r="L106" s="18" t="s">
-        <v>448</v>
       </c>
       <c r="M106" s="18"/>
       <c r="N106" s="18" t="s">
         <v>251</v>
       </c>
       <c r="O106" s="18" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="P106" s="5" t="n">
         <v>1</v>
       </c>
       <c r="Q106" s="18"/>
       <c r="R106" s="18" t="s">
+        <v>449</v>
+      </c>
+      <c r="S106" s="18" t="s">
         <v>450</v>
       </c>
-      <c r="S106" s="18" t="s">
+      <c r="T106" s="19" t="s">
         <v>451</v>
-      </c>
-      <c r="T106" s="19" t="s">
-        <v>452</v>
       </c>
       <c r="U106" s="18"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="86.55" outlineLevel="0" r="107">
       <c r="A107" s="7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C107" s="7"/>
       <c r="D107" s="7"/>
@@ -6884,44 +6881,44 @@
         <v>22</v>
       </c>
       <c r="J107" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K107" s="18" t="s">
+        <v>453</v>
+      </c>
+      <c r="L107" s="18" t="s">
         <v>454</v>
-      </c>
-      <c r="L107" s="18" t="s">
-        <v>455</v>
       </c>
       <c r="M107" s="18"/>
       <c r="N107" s="18" t="s">
         <v>251</v>
       </c>
       <c r="O107" s="18" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="P107" s="5" t="n">
         <v>2</v>
       </c>
       <c r="Q107" s="18" t="s">
+        <v>456</v>
+      </c>
+      <c r="R107" s="18" t="s">
+        <v>449</v>
+      </c>
+      <c r="S107" s="18" t="s">
         <v>457</v>
       </c>
-      <c r="R107" s="18" t="s">
-        <v>450</v>
-      </c>
-      <c r="S107" s="18" t="s">
-        <v>458</v>
-      </c>
       <c r="T107" s="19" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="U107" s="18"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="44" outlineLevel="0" r="108">
       <c r="A108" s="7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C108" s="7"/>
       <c r="D108" s="7"/>
@@ -6939,44 +6936,44 @@
         <v>22</v>
       </c>
       <c r="J108" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K108" s="18" t="s">
+        <v>459</v>
+      </c>
+      <c r="L108" s="18" t="s">
         <v>460</v>
-      </c>
-      <c r="L108" s="18" t="s">
-        <v>461</v>
       </c>
       <c r="M108" s="18"/>
       <c r="N108" s="18" t="s">
         <v>251</v>
       </c>
       <c r="O108" s="18" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="P108" s="5" t="n">
         <v>2</v>
       </c>
       <c r="Q108" s="18" t="s">
+        <v>462</v>
+      </c>
+      <c r="R108" s="18" t="s">
+        <v>449</v>
+      </c>
+      <c r="S108" s="18" t="s">
         <v>463</v>
       </c>
-      <c r="R108" s="18" t="s">
-        <v>450</v>
-      </c>
-      <c r="S108" s="18" t="s">
-        <v>464</v>
-      </c>
       <c r="T108" s="19" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="U108" s="18"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="114.9" outlineLevel="0" r="109">
       <c r="A109" s="7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C109" s="7"/>
       <c r="D109" s="7"/>
@@ -6994,44 +6991,44 @@
         <v>22</v>
       </c>
       <c r="J109" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K109" s="18" t="s">
+        <v>465</v>
+      </c>
+      <c r="L109" s="18" t="s">
         <v>466</v>
-      </c>
-      <c r="L109" s="18" t="s">
-        <v>467</v>
       </c>
       <c r="M109" s="18"/>
       <c r="N109" s="18" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O109" s="18" t="s">
+        <v>467</v>
+      </c>
+      <c r="P109" s="5" t="s">
         <v>468</v>
       </c>
-      <c r="P109" s="5" t="s">
+      <c r="Q109" s="18" t="s">
         <v>469</v>
       </c>
-      <c r="Q109" s="18" t="s">
+      <c r="R109" s="18" t="s">
         <v>470</v>
       </c>
-      <c r="R109" s="18" t="s">
+      <c r="S109" s="18" t="s">
         <v>471</v>
       </c>
-      <c r="S109" s="18" t="s">
+      <c r="T109" s="19" t="s">
         <v>472</v>
-      </c>
-      <c r="T109" s="19" t="s">
-        <v>473</v>
       </c>
       <c r="U109" s="18"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="100.7" outlineLevel="0" r="110">
       <c r="A110" s="7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C110" s="7"/>
       <c r="D110" s="7"/>
@@ -7049,44 +7046,44 @@
         <v>22</v>
       </c>
       <c r="J110" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K110" s="18" t="s">
+        <v>474</v>
+      </c>
+      <c r="L110" s="18" t="s">
         <v>475</v>
-      </c>
-      <c r="L110" s="18" t="s">
-        <v>476</v>
       </c>
       <c r="M110" s="18"/>
       <c r="N110" s="18" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O110" s="18" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="P110" s="5" t="n">
         <v>2</v>
       </c>
       <c r="Q110" s="18" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="R110" s="18" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="S110" s="18" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="T110" s="19" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="U110" s="18"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="157.45" outlineLevel="0" r="111">
       <c r="A111" s="7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C111" s="7"/>
       <c r="D111" s="7"/>
@@ -7104,44 +7101,44 @@
         <v>22</v>
       </c>
       <c r="J111" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K111" s="18" t="s">
+        <v>479</v>
+      </c>
+      <c r="L111" s="18" t="s">
         <v>480</v>
-      </c>
-      <c r="L111" s="18" t="s">
-        <v>481</v>
       </c>
       <c r="M111" s="18"/>
       <c r="N111" s="18" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O111" s="18" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="P111" s="5" t="n">
         <v>3</v>
       </c>
       <c r="Q111" s="18" t="s">
+        <v>482</v>
+      </c>
+      <c r="R111" s="18" t="s">
         <v>483</v>
       </c>
-      <c r="R111" s="18" t="s">
+      <c r="S111" s="18" t="s">
         <v>484</v>
       </c>
-      <c r="S111" s="18" t="s">
+      <c r="T111" s="19" t="s">
         <v>485</v>
-      </c>
-      <c r="T111" s="19" t="s">
-        <v>486</v>
       </c>
       <c r="U111" s="18"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="29.85" outlineLevel="0" r="112">
       <c r="A112" s="7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C112" s="7"/>
       <c r="D112" s="7"/>
@@ -7159,42 +7156,42 @@
         <v>22</v>
       </c>
       <c r="J112" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K112" s="18" t="s">
+        <v>487</v>
+      </c>
+      <c r="L112" s="18" t="s">
         <v>488</v>
-      </c>
-      <c r="L112" s="18" t="s">
-        <v>489</v>
       </c>
       <c r="M112" s="18"/>
       <c r="N112" s="18" t="s">
         <v>251</v>
       </c>
       <c r="O112" s="18" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="P112" s="5" t="n">
         <v>2</v>
       </c>
       <c r="Q112" s="18"/>
       <c r="R112" s="18" t="s">
+        <v>490</v>
+      </c>
+      <c r="S112" s="18" t="s">
         <v>491</v>
       </c>
-      <c r="S112" s="18" t="s">
+      <c r="T112" s="19" t="s">
         <v>492</v>
-      </c>
-      <c r="T112" s="19" t="s">
-        <v>493</v>
       </c>
       <c r="U112" s="18"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="29.85" outlineLevel="0" r="113">
       <c r="A113" s="7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C113" s="7"/>
       <c r="D113" s="7"/>
@@ -7212,42 +7209,42 @@
         <v>22</v>
       </c>
       <c r="J113" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K113" s="18" t="s">
+        <v>494</v>
+      </c>
+      <c r="L113" s="18" t="s">
         <v>495</v>
-      </c>
-      <c r="L113" s="18" t="s">
-        <v>496</v>
       </c>
       <c r="M113" s="18"/>
       <c r="N113" s="18"/>
       <c r="O113" s="18" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="P113" s="5" t="n">
         <v>2</v>
       </c>
       <c r="Q113" s="18"/>
       <c r="R113" s="18" t="s">
+        <v>497</v>
+      </c>
+      <c r="S113" s="18" t="s">
         <v>498</v>
       </c>
-      <c r="S113" s="18" t="s">
+      <c r="T113" s="19" t="s">
         <v>499</v>
-      </c>
-      <c r="T113" s="19" t="s">
-        <v>500</v>
       </c>
       <c r="U113" s="18"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="44" outlineLevel="0" r="114">
       <c r="A114" s="7"/>
       <c r="B114" s="7" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C114" s="7"/>
       <c r="D114" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E114" s="7"/>
       <c r="F114" s="7"/>
@@ -7261,44 +7258,44 @@
         <v>22</v>
       </c>
       <c r="J114" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K114" s="18" t="s">
+        <v>501</v>
+      </c>
+      <c r="L114" s="18" t="s">
         <v>502</v>
-      </c>
-      <c r="L114" s="18" t="s">
-        <v>503</v>
       </c>
       <c r="M114" s="18"/>
       <c r="N114" s="18" t="s">
+        <v>503</v>
+      </c>
+      <c r="O114" s="18" t="s">
         <v>504</v>
-      </c>
-      <c r="O114" s="18" t="s">
-        <v>505</v>
       </c>
       <c r="P114" s="5" t="n">
         <v>1</v>
       </c>
       <c r="Q114" s="18"/>
       <c r="R114" s="18" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="S114" s="18" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="T114" s="19" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="U114" s="18"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="29.85" outlineLevel="0" r="115">
       <c r="A115" s="7"/>
       <c r="B115" s="7" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C115" s="7"/>
       <c r="D115" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E115" s="7"/>
       <c r="F115" s="7"/>
@@ -7312,45 +7309,45 @@
         <v>22</v>
       </c>
       <c r="J115" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K115" s="18" t="s">
+        <v>507</v>
+      </c>
+      <c r="L115" s="18" t="s">
         <v>508</v>
-      </c>
-      <c r="L115" s="18" t="s">
-        <v>509</v>
       </c>
       <c r="M115" s="18"/>
       <c r="N115" s="18" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="O115" s="18" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="P115" s="5" t="n">
         <v>1</v>
       </c>
       <c r="Q115" s="18"/>
       <c r="R115" s="18" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="S115" s="18" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="T115" s="20" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="U115" s="18"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="32.8" outlineLevel="0" r="116">
       <c r="A116" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>134</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E116" s="7" t="s">
         <v>22</v>
@@ -7368,53 +7365,53 @@
         <v>22</v>
       </c>
       <c r="J116" s="7" t="s">
+        <v>513</v>
+      </c>
+      <c r="K116" s="21" t="s">
         <v>514</v>
       </c>
-      <c r="K116" s="21" t="s">
+      <c r="L116" s="21" t="s">
         <v>515</v>
       </c>
-      <c r="L116" s="21" t="s">
+      <c r="M116" s="21" t="s">
         <v>516</v>
       </c>
-      <c r="M116" s="21" t="s">
+      <c r="N116" s="21" t="s">
         <v>517</v>
       </c>
-      <c r="N116" s="21" t="s">
+      <c r="O116" s="21" t="s">
         <v>518</v>
-      </c>
-      <c r="O116" s="21" t="s">
-        <v>519</v>
       </c>
       <c r="P116" s="21" t="n">
         <v>1</v>
       </c>
       <c r="Q116" s="21" t="s">
+        <v>519</v>
+      </c>
+      <c r="R116" s="21" t="s">
         <v>520</v>
-      </c>
-      <c r="R116" s="21" t="s">
-        <v>521</v>
       </c>
       <c r="S116" s="22"/>
       <c r="T116" s="23"/>
       <c r="U116" s="24" t="s">
+        <v>521</v>
+      </c>
+      <c r="V116" s="24" t="s">
         <v>522</v>
       </c>
-      <c r="V116" s="24" t="s">
+      <c r="W116" s="24" t="s">
         <v>523</v>
       </c>
-      <c r="W116" s="24" t="s">
+      <c r="X116" s="24" t="s">
         <v>524</v>
-      </c>
-      <c r="X116" s="24" t="s">
-        <v>525</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="22.35" outlineLevel="0" r="117">
       <c r="A117" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E117" s="7" t="s">
         <v>23</v>
@@ -7432,28 +7429,28 @@
         <v>22</v>
       </c>
       <c r="J117" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="K117" s="21" t="s">
+        <v>526</v>
+      </c>
+      <c r="L117" s="21" t="s">
         <v>527</v>
       </c>
-      <c r="L117" s="21" t="s">
+      <c r="M117" s="21" t="s">
         <v>528</v>
       </c>
-      <c r="M117" s="21" t="s">
-        <v>529</v>
-      </c>
       <c r="N117" s="21" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="O117" s="21" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="P117" s="21" t="n">
         <v>1</v>
       </c>
       <c r="Q117" s="21" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="R117" s="21"/>
       <c r="S117" s="22"/>
@@ -7465,10 +7462,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="22.35" outlineLevel="0" r="118">
       <c r="A118" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E118" s="7" t="s">
         <v>22</v>
@@ -7486,28 +7483,28 @@
         <v>22</v>
       </c>
       <c r="J118" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="K118" s="21" t="s">
+        <v>530</v>
+      </c>
+      <c r="L118" s="21" t="s">
         <v>531</v>
       </c>
-      <c r="L118" s="21" t="s">
+      <c r="M118" s="21" t="s">
+        <v>405</v>
+      </c>
+      <c r="N118" s="21" t="s">
+        <v>517</v>
+      </c>
+      <c r="O118" s="21" t="s">
         <v>532</v>
-      </c>
-      <c r="M118" s="21" t="s">
-        <v>406</v>
-      </c>
-      <c r="N118" s="21" t="s">
-        <v>518</v>
-      </c>
-      <c r="O118" s="21" t="s">
-        <v>533</v>
       </c>
       <c r="P118" s="21" t="n">
         <v>2</v>
       </c>
       <c r="Q118" s="21" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="R118" s="21"/>
       <c r="S118" s="22"/>
@@ -7519,10 +7516,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="119">
       <c r="A119" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E119" s="7" t="s">
         <v>22</v>
@@ -7537,26 +7534,26 @@
         <v>22</v>
       </c>
       <c r="J119" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="K119" s="21" t="s">
+        <v>535</v>
+      </c>
+      <c r="L119" s="21" t="s">
         <v>536</v>
-      </c>
-      <c r="L119" s="21" t="s">
-        <v>537</v>
       </c>
       <c r="M119" s="21"/>
       <c r="N119" s="21" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="O119" s="21" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="P119" s="21" t="n">
         <v>2</v>
       </c>
       <c r="Q119" s="21" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="R119" s="21"/>
       <c r="S119" s="22"/>
@@ -7568,10 +7565,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="120">
       <c r="A120" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="E120" s="7" t="s">
         <v>22</v>
@@ -7586,24 +7583,24 @@
         <v>22</v>
       </c>
       <c r="J120" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="K120" s="21" t="s">
+        <v>540</v>
+      </c>
+      <c r="L120" s="21" t="s">
         <v>541</v>
-      </c>
-      <c r="L120" s="21" t="s">
-        <v>542</v>
       </c>
       <c r="M120" s="21"/>
       <c r="N120" s="21" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="O120" s="21"/>
       <c r="P120" s="21" t="n">
         <v>1</v>
       </c>
       <c r="Q120" s="21" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="R120" s="21"/>
       <c r="S120" s="22"/>
@@ -7615,7 +7612,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="121">
       <c r="A121" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>98</v>
@@ -7636,28 +7633,28 @@
         <v>22</v>
       </c>
       <c r="J121" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="K121" s="21" t="s">
+        <v>544</v>
+      </c>
+      <c r="L121" s="21" t="s">
         <v>545</v>
       </c>
-      <c r="L121" s="21" t="s">
+      <c r="M121" s="21" t="s">
         <v>546</v>
       </c>
-      <c r="M121" s="21" t="s">
+      <c r="N121" s="21" t="s">
+        <v>542</v>
+      </c>
+      <c r="O121" s="21" t="s">
         <v>547</v>
-      </c>
-      <c r="N121" s="21" t="s">
-        <v>543</v>
-      </c>
-      <c r="O121" s="21" t="s">
-        <v>548</v>
       </c>
       <c r="P121" s="21" t="n">
         <v>1</v>
       </c>
       <c r="Q121" s="21" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="R121" s="21"/>
       <c r="S121" s="22"/>
@@ -7669,10 +7666,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="53.7" outlineLevel="0" r="122">
       <c r="A122" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="E122" s="7" t="s">
         <v>22</v>
@@ -7687,51 +7684,51 @@
         <v>22</v>
       </c>
       <c r="J122" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="K122" s="21" t="s">
+        <v>550</v>
+      </c>
+      <c r="L122" s="21" t="s">
         <v>551</v>
-      </c>
-      <c r="L122" s="21" t="s">
-        <v>552</v>
       </c>
       <c r="M122" s="21"/>
       <c r="N122" s="21" t="s">
+        <v>552</v>
+      </c>
+      <c r="O122" s="21" t="s">
         <v>553</v>
-      </c>
-      <c r="O122" s="21" t="s">
-        <v>554</v>
       </c>
       <c r="P122" s="21" t="n">
         <v>1</v>
       </c>
       <c r="Q122" s="21" t="s">
+        <v>554</v>
+      </c>
+      <c r="R122" s="21" t="s">
         <v>555</v>
-      </c>
-      <c r="R122" s="21" t="s">
-        <v>556</v>
       </c>
       <c r="S122" s="22"/>
       <c r="T122" s="23"/>
       <c r="U122" s="24" t="s">
+        <v>556</v>
+      </c>
+      <c r="V122" s="24" t="s">
         <v>557</v>
       </c>
-      <c r="V122" s="24" t="s">
+      <c r="W122" s="24" t="s">
         <v>558</v>
       </c>
-      <c r="W122" s="24" t="s">
+      <c r="X122" s="24" t="s">
         <v>559</v>
-      </c>
-      <c r="X122" s="24" t="s">
-        <v>560</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="53.7" outlineLevel="0" r="123">
       <c r="A123" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E123" s="7" t="s">
         <v>22</v>
@@ -7746,43 +7743,43 @@
         <v>22</v>
       </c>
       <c r="J123" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="K123" s="21" t="s">
+        <v>560</v>
+      </c>
+      <c r="L123" s="21" t="s">
         <v>561</v>
-      </c>
-      <c r="L123" s="21" t="s">
-        <v>562</v>
       </c>
       <c r="M123" s="21"/>
       <c r="N123" s="21" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="O123" s="21" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="P123" s="21" t="n">
         <v>1</v>
       </c>
       <c r="Q123" s="25" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="R123" s="21"/>
       <c r="S123" s="22"/>
       <c r="T123" s="23"/>
       <c r="U123" s="24"/>
       <c r="V123" s="24" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="W123" s="24"/>
       <c r="X123" s="24"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="22.35" outlineLevel="0" r="124">
       <c r="A124" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E124" s="7" t="s">
         <v>22</v>
@@ -7797,31 +7794,31 @@
         <v>22</v>
       </c>
       <c r="J124" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="K124" s="21" t="s">
+        <v>565</v>
+      </c>
+      <c r="L124" s="21" t="s">
         <v>566</v>
-      </c>
-      <c r="L124" s="21" t="s">
-        <v>567</v>
       </c>
       <c r="M124" s="21"/>
       <c r="N124" s="21" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="O124" s="21" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="P124" s="21" t="n">
         <v>1</v>
       </c>
       <c r="Q124" s="21" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="R124" s="21"/>
       <c r="S124" s="22"/>
       <c r="T124" s="23" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="U124" s="24"/>
       <c r="V124" s="24"/>
@@ -7830,10 +7827,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="22.35" outlineLevel="0" r="125">
       <c r="A125" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="E125" s="7" t="s">
         <v>22</v>
@@ -7851,36 +7848,36 @@
         <v>22</v>
       </c>
       <c r="J125" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="K125" s="21" t="s">
+        <v>571</v>
+      </c>
+      <c r="L125" s="21" t="s">
         <v>572</v>
-      </c>
-      <c r="L125" s="21" t="s">
-        <v>573</v>
       </c>
       <c r="M125" s="21"/>
       <c r="N125" s="21" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="O125" s="21" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="P125" s="21" t="n">
         <v>1</v>
       </c>
       <c r="Q125" s="21" t="s">
+        <v>574</v>
+      </c>
+      <c r="R125" s="21" t="s">
         <v>575</v>
       </c>
-      <c r="R125" s="21" t="s">
+      <c r="S125" s="22" t="s">
         <v>576</v>
-      </c>
-      <c r="S125" s="22" t="s">
-        <v>577</v>
       </c>
       <c r="T125" s="23"/>
       <c r="U125" s="24" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="V125" s="24"/>
       <c r="W125" s="24"/>
@@ -7888,10 +7885,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="22.35" outlineLevel="0" r="126">
       <c r="A126" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="E126" s="7" t="s">
         <v>22</v>
@@ -7909,30 +7906,30 @@
         <v>22</v>
       </c>
       <c r="J126" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="K126" s="21" t="s">
+        <v>579</v>
+      </c>
+      <c r="L126" s="21" t="s">
         <v>580</v>
-      </c>
-      <c r="L126" s="21" t="s">
-        <v>581</v>
       </c>
       <c r="M126" s="21"/>
       <c r="N126" s="21" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="O126" s="21" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="P126" s="21" t="n">
         <v>1</v>
       </c>
       <c r="Q126" s="21"/>
       <c r="R126" s="21" t="s">
+        <v>582</v>
+      </c>
+      <c r="S126" s="22" t="s">
         <v>583</v>
-      </c>
-      <c r="S126" s="22" t="s">
-        <v>584</v>
       </c>
       <c r="T126" s="23"/>
       <c r="U126" s="24"/>
@@ -7942,10 +7939,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="22.35" outlineLevel="0" r="127">
       <c r="A127" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E127" s="7" t="s">
         <v>22</v>
@@ -7963,53 +7960,53 @@
         <v>22</v>
       </c>
       <c r="J127" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="K127" s="21" t="s">
+        <v>585</v>
+      </c>
+      <c r="L127" s="21" t="s">
         <v>586</v>
-      </c>
-      <c r="L127" s="21" t="s">
-        <v>587</v>
       </c>
       <c r="M127" s="21"/>
       <c r="N127" s="21" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="O127" s="21" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="P127" s="21" t="n">
         <v>1</v>
       </c>
       <c r="Q127" s="21" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="R127" s="21" t="s">
+        <v>582</v>
+      </c>
+      <c r="S127" s="22" t="s">
         <v>583</v>
-      </c>
-      <c r="S127" s="22" t="s">
-        <v>584</v>
       </c>
       <c r="T127" s="23"/>
       <c r="U127" s="24" t="s">
+        <v>589</v>
+      </c>
+      <c r="V127" s="24" t="s">
         <v>590</v>
       </c>
-      <c r="V127" s="24" t="s">
+      <c r="W127" s="24" t="s">
         <v>591</v>
       </c>
-      <c r="W127" s="24" t="s">
+      <c r="X127" s="24" t="s">
         <v>592</v>
-      </c>
-      <c r="X127" s="24" t="s">
-        <v>593</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="43.25" outlineLevel="0" r="128">
       <c r="A128" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E128" s="7" t="s">
         <v>22</v>
@@ -8027,49 +8024,49 @@
         <v>22</v>
       </c>
       <c r="J128" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="K128" s="21" t="s">
+        <v>594</v>
+      </c>
+      <c r="L128" s="21" t="s">
         <v>595</v>
-      </c>
-      <c r="L128" s="21" t="s">
-        <v>596</v>
       </c>
       <c r="M128" s="21"/>
       <c r="N128" s="21" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="O128" s="21" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="P128" s="21" t="n">
         <v>1</v>
       </c>
       <c r="Q128" s="26" t="s">
+        <v>597</v>
+      </c>
+      <c r="R128" s="21" t="s">
         <v>598</v>
       </c>
-      <c r="R128" s="21" t="s">
+      <c r="S128" s="22" t="s">
         <v>599</v>
       </c>
-      <c r="S128" s="22" t="s">
+      <c r="T128" s="23" t="s">
         <v>600</v>
-      </c>
-      <c r="T128" s="23" t="s">
-        <v>601</v>
       </c>
       <c r="U128" s="24"/>
       <c r="V128" s="24" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="W128" s="24"/>
       <c r="X128" s="24"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="22.35" outlineLevel="0" r="129">
       <c r="A129" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E129" s="7" t="s">
         <v>22</v>
@@ -8084,31 +8081,31 @@
         <v>22</v>
       </c>
       <c r="J129" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="K129" s="26" t="s">
+        <v>603</v>
+      </c>
+      <c r="L129" s="26" t="s">
         <v>604</v>
-      </c>
-      <c r="L129" s="26" t="s">
-        <v>605</v>
       </c>
       <c r="M129" s="26"/>
       <c r="N129" s="26" t="s">
+        <v>605</v>
+      </c>
+      <c r="O129" s="26" t="s">
         <v>606</v>
-      </c>
-      <c r="O129" s="26" t="s">
-        <v>607</v>
       </c>
       <c r="P129" s="26" t="n">
         <v>2</v>
       </c>
       <c r="Q129" s="26" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="R129" s="26"/>
       <c r="S129" s="27"/>
       <c r="T129" s="28" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="U129" s="24"/>
       <c r="V129" s="24"/>
@@ -8117,10 +8114,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="64.15" outlineLevel="0" r="130">
       <c r="A130" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E130" s="7" t="s">
         <v>22</v>
@@ -8138,53 +8135,53 @@
         <v>22</v>
       </c>
       <c r="J130" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="K130" s="21" t="s">
+        <v>610</v>
+      </c>
+      <c r="L130" s="21" t="s">
         <v>611</v>
-      </c>
-      <c r="L130" s="21" t="s">
-        <v>612</v>
       </c>
       <c r="M130" s="21"/>
       <c r="N130" s="21" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="O130" s="21" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="P130" s="21" t="n">
         <v>1</v>
       </c>
       <c r="Q130" s="21" t="s">
+        <v>613</v>
+      </c>
+      <c r="R130" s="21" t="s">
         <v>614</v>
       </c>
-      <c r="R130" s="21" t="s">
+      <c r="S130" s="22" t="s">
         <v>615</v>
       </c>
-      <c r="S130" s="22" t="s">
+      <c r="T130" s="23" t="s">
         <v>616</v>
       </c>
-      <c r="T130" s="23" t="s">
+      <c r="U130" s="24" t="s">
         <v>617</v>
       </c>
-      <c r="U130" s="24" t="s">
+      <c r="V130" s="24" t="s">
         <v>618</v>
-      </c>
-      <c r="V130" s="24" t="s">
-        <v>619</v>
       </c>
       <c r="W130" s="24"/>
       <c r="X130" s="24" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="22.35" outlineLevel="0" r="131">
       <c r="A131" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="E131" s="7" t="s">
         <v>22</v>
@@ -8199,33 +8196,33 @@
         <v>22</v>
       </c>
       <c r="J131" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="K131" s="21" t="s">
+        <v>621</v>
+      </c>
+      <c r="L131" s="21" t="s">
         <v>622</v>
-      </c>
-      <c r="L131" s="21" t="s">
-        <v>623</v>
       </c>
       <c r="M131" s="21"/>
       <c r="N131" s="21" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="O131" s="21" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="P131" s="21" t="n">
         <v>2</v>
       </c>
       <c r="Q131" s="21" t="s">
+        <v>624</v>
+      </c>
+      <c r="R131" s="21" t="s">
         <v>625</v>
-      </c>
-      <c r="R131" s="21" t="s">
-        <v>626</v>
       </c>
       <c r="S131" s="22"/>
       <c r="T131" s="23" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="U131" s="24"/>
       <c r="V131" s="24"/>
@@ -8234,10 +8231,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="85.05" outlineLevel="0" r="132">
       <c r="A132" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="E132" s="7" t="s">
         <v>22</v>
@@ -8252,51 +8249,51 @@
         <v>22</v>
       </c>
       <c r="J132" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="K132" s="21" t="s">
+        <v>628</v>
+      </c>
+      <c r="L132" s="21" t="s">
         <v>629</v>
-      </c>
-      <c r="L132" s="21" t="s">
-        <v>630</v>
       </c>
       <c r="M132" s="21"/>
       <c r="N132" s="21" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="O132" s="21" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="P132" s="21" t="n">
         <v>1</v>
       </c>
       <c r="Q132" s="21"/>
       <c r="R132" s="21" t="s">
+        <v>631</v>
+      </c>
+      <c r="S132" s="22" t="s">
+        <v>451</v>
+      </c>
+      <c r="T132" s="23" t="s">
         <v>632</v>
       </c>
-      <c r="S132" s="22" t="s">
-        <v>452</v>
-      </c>
-      <c r="T132" s="23" t="s">
+      <c r="U132" s="24" t="s">
         <v>633</v>
       </c>
-      <c r="U132" s="24" t="s">
+      <c r="V132" s="24" t="s">
         <v>634</v>
-      </c>
-      <c r="V132" s="24" t="s">
-        <v>635</v>
       </c>
       <c r="W132" s="24"/>
       <c r="X132" s="24" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="179.1" outlineLevel="0" r="133">
       <c r="A133" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="E133" s="7" t="s">
         <v>22</v>
@@ -8311,35 +8308,35 @@
         <v>22</v>
       </c>
       <c r="J133" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="K133" s="21" t="s">
+        <v>637</v>
+      </c>
+      <c r="L133" s="21" t="s">
         <v>638</v>
-      </c>
-      <c r="L133" s="21" t="s">
-        <v>639</v>
       </c>
       <c r="M133" s="21"/>
       <c r="N133" s="21" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="O133" s="21" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="P133" s="21" t="n">
         <v>1</v>
       </c>
       <c r="Q133" s="21" t="s">
+        <v>640</v>
+      </c>
+      <c r="R133" s="21" t="s">
         <v>641</v>
       </c>
-      <c r="R133" s="21" t="s">
+      <c r="S133" s="22" t="s">
+        <v>451</v>
+      </c>
+      <c r="T133" s="23" t="s">
         <v>642</v>
-      </c>
-      <c r="S133" s="22" t="s">
-        <v>452</v>
-      </c>
-      <c r="T133" s="23" t="s">
-        <v>643</v>
       </c>
       <c r="U133" s="24"/>
       <c r="V133" s="24"/>
@@ -8348,10 +8345,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="32.8" outlineLevel="0" r="134">
       <c r="A134" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="E134" s="7" t="s">
         <v>22</v>
@@ -8366,36 +8363,36 @@
         <v>22</v>
       </c>
       <c r="J134" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="K134" s="21" t="s">
+        <v>644</v>
+      </c>
+      <c r="L134" s="21" t="s">
         <v>645</v>
-      </c>
-      <c r="L134" s="21" t="s">
-        <v>646</v>
       </c>
       <c r="M134" s="21"/>
       <c r="N134" s="21" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="O134" s="21" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="P134" s="21" t="n">
         <v>2</v>
       </c>
       <c r="Q134" s="21" t="s">
+        <v>647</v>
+      </c>
+      <c r="R134" s="21" t="s">
         <v>648</v>
-      </c>
-      <c r="R134" s="21" t="s">
-        <v>649</v>
       </c>
       <c r="S134" s="22"/>
       <c r="T134" s="23" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="U134" s="24" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="V134" s="24"/>
       <c r="W134" s="24"/>
@@ -8403,10 +8400,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="137.3" outlineLevel="0" r="135">
       <c r="A135" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="E135" s="7" t="s">
         <v>22</v>
@@ -8421,49 +8418,49 @@
         <v>22</v>
       </c>
       <c r="J135" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="K135" s="21" t="s">
+        <v>651</v>
+      </c>
+      <c r="L135" s="21" t="s">
         <v>652</v>
-      </c>
-      <c r="L135" s="21" t="s">
-        <v>653</v>
       </c>
       <c r="M135" s="21"/>
       <c r="N135" s="21" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="O135" s="21" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="P135" s="21" t="n">
         <v>2</v>
       </c>
       <c r="Q135" s="21" t="s">
+        <v>654</v>
+      </c>
+      <c r="R135" s="21" t="s">
         <v>655</v>
       </c>
-      <c r="R135" s="21" t="s">
+      <c r="S135" s="22" t="s">
+        <v>451</v>
+      </c>
+      <c r="T135" s="23" t="s">
         <v>656</v>
-      </c>
-      <c r="S135" s="22" t="s">
-        <v>452</v>
-      </c>
-      <c r="T135" s="23" t="s">
-        <v>657</v>
       </c>
       <c r="U135" s="24"/>
       <c r="V135" s="24"/>
       <c r="W135" s="24"/>
       <c r="X135" s="24" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="64.15" outlineLevel="0" r="136">
       <c r="A136" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="E136" s="7" t="s">
         <v>22</v>
@@ -8478,47 +8475,47 @@
         <v>22</v>
       </c>
       <c r="J136" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="K136" s="21" t="s">
+        <v>659</v>
+      </c>
+      <c r="L136" s="21" t="s">
         <v>660</v>
-      </c>
-      <c r="L136" s="21" t="s">
-        <v>661</v>
       </c>
       <c r="M136" s="21"/>
       <c r="N136" s="21" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="O136" s="21" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="P136" s="21" t="n">
         <v>1</v>
       </c>
       <c r="Q136" s="21" t="s">
+        <v>662</v>
+      </c>
+      <c r="R136" s="21" t="s">
         <v>663</v>
-      </c>
-      <c r="R136" s="21" t="s">
-        <v>664</v>
       </c>
       <c r="S136" s="22"/>
       <c r="T136" s="23" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="U136" s="24"/>
       <c r="V136" s="24" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="W136" s="24"/>
       <c r="X136" s="24"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="22.35" outlineLevel="0" r="137">
       <c r="A137" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="E137" s="7" t="s">
         <v>22</v>
@@ -8533,31 +8530,31 @@
         <v>22</v>
       </c>
       <c r="J137" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="K137" s="21" t="s">
+        <v>667</v>
+      </c>
+      <c r="L137" s="26" t="s">
         <v>668</v>
-      </c>
-      <c r="L137" s="26" t="s">
-        <v>669</v>
       </c>
       <c r="M137" s="26"/>
       <c r="N137" s="21" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="O137" s="21" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="P137" s="21" t="n">
         <v>2</v>
       </c>
       <c r="Q137" s="21" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="R137" s="21"/>
       <c r="S137" s="22"/>
       <c r="T137" s="23" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="U137" s="24"/>
       <c r="V137" s="24"/>
@@ -8566,53 +8563,53 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="43.25" outlineLevel="0" r="138">
       <c r="A138" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B138" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="E138" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G138" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H138" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="I138" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J138" s="7" t="s">
+        <v>513</v>
+      </c>
+      <c r="K138" s="21" t="s">
         <v>673</v>
       </c>
-      <c r="E138" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G138" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H138" s="7" t="s">
-        <v>354</v>
-      </c>
-      <c r="I138" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J138" s="7" t="s">
-        <v>514</v>
-      </c>
-      <c r="K138" s="21" t="s">
+      <c r="L138" s="21" t="s">
         <v>674</v>
-      </c>
-      <c r="L138" s="21" t="s">
-        <v>675</v>
       </c>
       <c r="M138" s="21"/>
       <c r="N138" s="21" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="O138" s="21" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="P138" s="21" t="n">
         <v>1</v>
       </c>
       <c r="Q138" s="26" t="s">
+        <v>676</v>
+      </c>
+      <c r="R138" s="26" t="s">
         <v>677</v>
       </c>
-      <c r="R138" s="26" t="s">
+      <c r="S138" s="26" t="s">
         <v>678</v>
       </c>
-      <c r="S138" s="26" t="s">
+      <c r="T138" s="28" t="s">
         <v>679</v>
-      </c>
-      <c r="T138" s="28" t="s">
-        <v>680</v>
       </c>
       <c r="U138" s="24"/>
       <c r="V138" s="24"/>
@@ -8621,56 +8618,56 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="53.7" outlineLevel="0" r="139">
       <c r="A139" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B139" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="E139" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G139" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H139" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="I139" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J139" s="7" t="s">
+        <v>513</v>
+      </c>
+      <c r="K139" s="21" t="s">
         <v>681</v>
       </c>
-      <c r="E139" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G139" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H139" s="7" t="s">
-        <v>360</v>
-      </c>
-      <c r="I139" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J139" s="7" t="s">
-        <v>514</v>
-      </c>
-      <c r="K139" s="21" t="s">
+      <c r="L139" s="21" t="s">
         <v>682</v>
-      </c>
-      <c r="L139" s="21" t="s">
-        <v>683</v>
       </c>
       <c r="M139" s="21"/>
       <c r="N139" s="21" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="O139" s="21" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="P139" s="21" t="n">
         <v>2</v>
       </c>
       <c r="Q139" s="21" t="s">
+        <v>684</v>
+      </c>
+      <c r="R139" s="21" t="s">
         <v>685</v>
       </c>
-      <c r="R139" s="21" t="s">
+      <c r="S139" s="22" t="s">
+        <v>401</v>
+      </c>
+      <c r="T139" s="23" t="s">
         <v>686</v>
       </c>
-      <c r="S139" s="22" t="s">
-        <v>402</v>
-      </c>
-      <c r="T139" s="23" t="s">
+      <c r="U139" s="24" t="s">
         <v>687</v>
-      </c>
-      <c r="U139" s="24" t="s">
-        <v>688</v>
       </c>
       <c r="V139" s="24"/>
       <c r="W139" s="24"/>
@@ -8678,59 +8675,59 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="32.8" outlineLevel="0" r="140">
       <c r="A140" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B140" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="E140" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G140" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H140" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="I140" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J140" s="7" t="s">
+        <v>513</v>
+      </c>
+      <c r="K140" s="21" t="s">
         <v>689</v>
       </c>
-      <c r="E140" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G140" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H140" s="7" t="s">
-        <v>365</v>
-      </c>
-      <c r="I140" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J140" s="7" t="s">
-        <v>514</v>
-      </c>
-      <c r="K140" s="21" t="s">
+      <c r="L140" s="21" t="s">
         <v>690</v>
-      </c>
-      <c r="L140" s="21" t="s">
-        <v>691</v>
       </c>
       <c r="M140" s="21"/>
       <c r="N140" s="21" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="O140" s="21" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="P140" s="21" t="n">
         <v>2</v>
       </c>
       <c r="Q140" s="21" t="s">
+        <v>692</v>
+      </c>
+      <c r="R140" s="21" t="s">
         <v>693</v>
-      </c>
-      <c r="R140" s="21" t="s">
-        <v>694</v>
       </c>
       <c r="S140" s="22"/>
       <c r="T140" s="23" t="s">
+        <v>694</v>
+      </c>
+      <c r="U140" s="24" t="s">
         <v>695</v>
-      </c>
-      <c r="U140" s="24" t="s">
-        <v>696</v>
       </c>
       <c r="V140" s="24"/>
       <c r="W140" s="24"/>
       <c r="X140" s="24" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- update library details concentration fields to show value and units together - export lincs and search for library details, closes #85 - fix dataset facility-salt id, closes #82 - fix nominal target information in small molecule view - closes #84 - fix db: omero id's importing as floats, closes #83
</commit_message>
<xml_diff>
--- a/sampledata/fieldinformation.xlsx
+++ b/sampledata/fieldinformation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1616" uniqueCount="700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1615" uniqueCount="700">
   <si>
     <t>table</t>
   </si>
@@ -575,6 +575,15 @@
     <t>Number of distinct small molecules in this library</t>
   </si>
   <si>
+    <t>display_concentration</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Concentration (nM,uM,mM)</t>
+  </si>
+  <si>
     <t>attachedfile</t>
   </si>
   <si>
@@ -663,15 +672,6 @@
   </si>
   <si>
     <t>The type of Control Well recorded for this Datarecord</t>
-  </si>
-  <si>
-    <t>omero_image_id</t>
-  </si>
-  <si>
-    <t>Image</t>
-  </si>
-  <si>
-    <t>The image recorded for this Datarecord</t>
   </si>
   <si>
     <t>smallmolecule</t>
@@ -2385,7 +2385,7 @@
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -2458,29 +2458,29 @@
   <dimension ref="A1:X141"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <pane activePane="bottomRight" topLeftCell="A25" xSplit="2036" ySplit="2250"/>
+      <pane activePane="bottomRight" topLeftCell="C27" xSplit="1892" ySplit="2250"/>
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-      <selection activeCell="A1" activeCellId="0" pane="topRight" sqref="A1"/>
-      <selection activeCell="A25" activeCellId="0" pane="bottomLeft" sqref="A25"/>
-      <selection activeCell="F49" activeCellId="0" pane="bottomRight" sqref="F49"/>
+      <selection activeCell="C1" activeCellId="0" pane="topRight" sqref="C1"/>
+      <selection activeCell="A27" activeCellId="0" pane="bottomLeft" sqref="A27"/>
+      <selection activeCell="O51" activeCellId="0" pane="bottomRight" sqref="O51"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.9764705882353"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.3843137254902"/>
-    <col collapsed="false" hidden="false" max="9" min="3" style="1" width="10.9960784313726"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="10.9960784313726"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.9960784313726"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="28.4"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="1" width="26.1725490196078"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="56.3294117647059"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="15.3019607843137"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="45.3411764705882"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="14.1254901960784"/>
-    <col collapsed="false" hidden="false" max="20" min="19" style="1" width="21.8588235294118"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="21.7137254901961"/>
-    <col collapsed="false" hidden="false" max="24" min="22" style="1" width="9.50588235294118"/>
-    <col collapsed="false" hidden="false" max="1025" min="25" style="0" width="9.50588235294118"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.0862745098039"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.4470588235294"/>
+    <col collapsed="false" hidden="false" max="9" min="3" style="1" width="11.0509803921569"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="11.0509803921569"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.0509803921569"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="28.5450980392157"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="1" width="26.3019607843137"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="56.6078431372549"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="15.3764705882353"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="45.5647058823529"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="14.2"/>
+    <col collapsed="false" hidden="false" max="20" min="19" style="1" width="21.9686274509804"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="21.8235294117647"/>
+    <col collapsed="false" hidden="false" max="24" min="22" style="1" width="9.54901960784314"/>
+    <col collapsed="false" hidden="false" max="1025" min="25" style="0" width="9.54901960784314"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="86.55" outlineLevel="0" r="1">
@@ -4054,10 +4054,10 @@
         <v>171</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G46" s="7" t="s">
         <v>23</v>
@@ -4086,10 +4086,10 @@
         <v>174</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G47" s="7" t="s">
         <v>23</v>
@@ -4199,43 +4199,41 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="51">
-      <c r="A51" s="9" t="s">
+      <c r="A51" s="7"/>
+      <c r="B51" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B51" s="10" t="s">
+      <c r="E51" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G51" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="E51" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>22</v>
+      <c r="H51" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="K51" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="M51" s="1" t="s">
+      <c r="M51" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="O51" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="O51" s="1" t="s">
-        <v>189</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="52">
       <c r="A52" s="9" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>75</v>
+        <v>190</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>22</v>
@@ -4247,7 +4245,7 @@
         <v>23</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="I52" s="1" t="s">
         <v>22</v>
@@ -4256,44 +4254,47 @@
         <v>51</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>14</v>
+        <v>191</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>14</v>
+        <v>192</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="53">
-      <c r="A53" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B53" s="9" t="s">
-        <v>190</v>
+      <c r="A53" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>75</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="F53" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="G53" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K53" s="4" t="n">
         <v>52</v>
       </c>
-      <c r="M53" s="9" t="s">
-        <v>191</v>
+      <c r="M53" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="O53" s="1" t="s">
-        <v>192</v>
+        <v>14</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="54">
       <c r="A54" s="1" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B54" s="9" t="s">
         <v>193</v>
@@ -4305,7 +4306,7 @@
         <v>23</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>23</v>
@@ -4322,7 +4323,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="55">
       <c r="A55" s="1" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B55" s="9" t="s">
         <v>196</v>
@@ -4334,7 +4335,7 @@
         <v>23</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>23</v>
@@ -4351,7 +4352,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="56">
       <c r="A56" s="1" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B56" s="9" t="s">
         <v>199</v>
@@ -4363,7 +4364,7 @@
         <v>23</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="I56" s="1" t="s">
         <v>23</v>
@@ -4380,7 +4381,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="57">
       <c r="A57" s="1" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B57" s="9" t="s">
         <v>202</v>
@@ -4388,17 +4389,14 @@
       <c r="E57" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F57" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G57" s="1" t="s">
         <v>23</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K57" s="4" t="n">
         <v>56</v>
@@ -4412,7 +4410,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="58">
       <c r="A58" s="1" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B58" s="9" t="s">
         <v>205</v>
@@ -4427,10 +4425,10 @@
         <v>23</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K58" s="4" t="n">
         <v>57</v>
@@ -4444,11 +4442,11 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="59">
       <c r="A59" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B59" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="B59" s="9" t="s">
-        <v>162</v>
-      </c>
       <c r="E59" s="1" t="s">
         <v>22</v>
       </c>
@@ -4459,7 +4457,7 @@
         <v>23</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="I59" s="1" t="s">
         <v>23</v>
@@ -4476,10 +4474,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="60">
       <c r="A60" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>22</v>
@@ -4491,7 +4489,7 @@
         <v>23</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="I60" s="1" t="s">
         <v>23</v>
@@ -4500,18 +4498,18 @@
         <v>59</v>
       </c>
       <c r="M60" s="9" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="O60" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="61">
       <c r="A61" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>213</v>
+        <v>165</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>22</v>
@@ -4523,7 +4521,7 @@
         <v>23</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I61" s="1" t="s">
         <v>23</v>
@@ -4540,7 +4538,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="62">
       <c r="A62" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B62" s="9" t="s">
         <v>216</v>
@@ -4555,7 +4553,7 @@
         <v>23</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="I62" s="1" t="s">
         <v>23</v>
@@ -4790,7 +4788,7 @@
       <c r="W66" s="7"/>
       <c r="X66" s="7"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="26.85" outlineLevel="0" r="67">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.2" outlineLevel="0" r="67">
       <c r="A67" s="7"/>
       <c r="B67" s="7" t="s">
         <v>242</v>
@@ -8328,7 +8326,7 @@
         <v>638</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="179.1" outlineLevel="0" r="134">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="168.65" outlineLevel="0" r="134">
       <c r="A134" s="1" t="s">
         <v>514</v>
       </c>
@@ -8438,7 +8436,7 @@
       <c r="W135" s="24"/>
       <c r="X135" s="24"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="137.3" outlineLevel="0" r="136">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="126.85" outlineLevel="0" r="136">
       <c r="A136" s="1" t="s">
         <v>514</v>
       </c>

</xml_diff>

<commit_message>
resolves issue #126 db: remove SM Facility ID as separate field in the detail view
</commit_message>
<xml_diff>
--- a/sampledata/fieldinformation.xlsx
+++ b/sampledata/fieldinformation.xlsx
@@ -2418,7 +2418,7 @@
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -2491,29 +2491,29 @@
   <dimension ref="A1:Y144"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <pane activePane="bottomRight" topLeftCell="K37" xSplit="4189" ySplit="2250"/>
+      <pane activePane="bottomRight" topLeftCell="A64" xSplit="2802" ySplit="1980"/>
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-      <selection activeCell="K1" activeCellId="0" pane="topRight" sqref="K1"/>
-      <selection activeCell="A37" activeCellId="0" pane="bottomLeft" sqref="A37"/>
-      <selection activeCell="L37" activeCellId="0" pane="bottomRight" sqref="L37:L65"/>
+      <selection activeCell="A1" activeCellId="0" pane="topRight" sqref="A1"/>
+      <selection activeCell="A64" activeCellId="0" pane="bottomLeft" sqref="A64"/>
+      <selection activeCell="E70" activeCellId="0" pane="bottomRight" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.1960784313725"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.5137254901961"/>
-    <col collapsed="false" hidden="false" max="9" min="3" style="1" width="11.1058823529412"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="2" width="11.1058823529412"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.1058823529412"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="28.6901960784314"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="1" width="26.4352941176471"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="56.8901960784314"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="15.4549019607843"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="45.7921568627451"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="14.2705882352941"/>
-    <col collapsed="false" hidden="false" max="21" min="20" style="1" width="22.078431372549"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="21.9333333333333"/>
-    <col collapsed="false" hidden="false" max="25" min="23" style="1" width="9.59607843137255"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="9.59607843137255"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.3019607843137"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.5843137254902"/>
+    <col collapsed="false" hidden="false" max="9" min="3" style="1" width="11.1607843137255"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="2" width="11.1607843137255"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.1607843137255"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="28.8352941176471"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="1" width="26.5647058823529"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="57.1686274509804"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="15.5294117647059"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="46.0156862745098"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="14.3450980392157"/>
+    <col collapsed="false" hidden="false" max="21" min="20" style="1" width="22.1843137254902"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="22.0392156862745"/>
+    <col collapsed="false" hidden="false" max="25" min="23" style="1" width="9.64313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="9.64313725490196"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="86.55" outlineLevel="0" r="1">
@@ -4898,7 +4898,7 @@
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
       <c r="E69" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>24</v>
@@ -5658,7 +5658,7 @@
       <c r="X82" s="7"/>
       <c r="Y82" s="7"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="52.2" outlineLevel="0" r="83">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="39.55" outlineLevel="0" r="83">
       <c r="A83" s="7" t="s">
         <v>229</v>
       </c>

</xml_diff>

<commit_message>
show an "Endpoints" tab in the Dataset page - fixes #158
</commit_message>
<xml_diff>
--- a/sampledata/fieldinformation.xlsx
+++ b/sampledata/fieldinformation.xlsx
@@ -2500,7 +2500,7 @@
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -2513,29 +2513,29 @@
   <dimension ref="A1:AQ163"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <pane activePane="bottomRight" topLeftCell="K65" xSplit="3053" ySplit="1978"/>
+      <pane activePane="bottomRight" topLeftCell="A62" xSplit="3128" ySplit="1978"/>
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-      <selection activeCell="K1" activeCellId="0" pane="topRight" sqref="K1"/>
-      <selection activeCell="A65" activeCellId="0" pane="bottomLeft" sqref="A65"/>
-      <selection activeCell="P82" activeCellId="0" pane="bottomRight" sqref="P82"/>
+      <selection activeCell="A1" activeCellId="0" pane="topRight" sqref="A1"/>
+      <selection activeCell="A62" activeCellId="0" pane="bottomLeft" sqref="A62"/>
+      <selection activeCell="H77" activeCellId="0" pane="bottomRight" sqref="H77"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.7647058823529"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.8745098039216"/>
-    <col collapsed="false" hidden="false" max="9" min="3" style="1" width="11.3764705882353"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="2" width="11.3764705882353"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.3764705882353"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="29.4117647058823"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="1" width="27.1058823529412"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="58.3176470588235"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="15.8470588235294"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="46.9490196078431"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="14.6352941176471"/>
-    <col collapsed="false" hidden="false" max="21" min="20" style="1" width="22.6196078431373"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="22.4941176470588"/>
-    <col collapsed="false" hidden="false" max="25" min="23" style="1" width="9.83137254901961"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="9.83137254901961"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.8823529411765"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.9372549019608"/>
+    <col collapsed="false" hidden="false" max="9" min="3" style="1" width="11.4313725490196"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="2" width="11.4313725490196"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.4313725490196"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="29.556862745098"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="1" width="27.243137254902"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="58.6078431372549"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="15.9254901960784"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="47.1843137254902"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="14.7137254901961"/>
+    <col collapsed="false" hidden="false" max="21" min="20" style="1" width="22.7294117647059"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="22.6117647058824"/>
+    <col collapsed="false" hidden="false" max="25" min="23" style="1" width="9.87450980392157"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="9.87450980392157"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="67.5" outlineLevel="0" r="1" s="6">
@@ -3535,7 +3535,7 @@
       <c r="AF24" s="1"/>
       <c r="AG24" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.1" outlineLevel="0" r="25">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
       <c r="A25" s="9" t="s">
         <v>101</v>
       </c>
@@ -3573,7 +3573,7 @@
       <c r="AF25" s="1"/>
       <c r="AG25" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.1" outlineLevel="0" r="26">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="A26" s="9" t="s">
         <v>101</v>
       </c>
@@ -3689,7 +3689,7 @@
       <c r="AF28" s="1"/>
       <c r="AG28" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.1" outlineLevel="0" r="29">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
       <c r="A29" s="9" t="s">
         <v>101</v>
       </c>
@@ -3727,7 +3727,7 @@
       <c r="AF29" s="1"/>
       <c r="AG29" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.1" outlineLevel="0" r="30">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
       <c r="A30" s="9" t="s">
         <v>101</v>
       </c>
@@ -5187,7 +5187,7 @@
         <v>24</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="I67" s="1" t="s">
         <v>23</v>
@@ -5233,7 +5233,7 @@
         <v>24</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="I68" s="1" t="s">
         <v>23</v>
@@ -5279,7 +5279,7 @@
         <v>24</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="I69" s="1" t="s">
         <v>23</v>
@@ -5322,7 +5322,7 @@
         <v>24</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="I70" s="1" t="s">
         <v>23</v>
@@ -5365,7 +5365,7 @@
         <v>24</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="I71" s="1" t="s">
         <v>23</v>
@@ -5408,7 +5408,7 @@
         <v>24</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="I72" s="1" t="s">
         <v>23</v>
@@ -5451,7 +5451,7 @@
         <v>24</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="I73" s="1" t="s">
         <v>23</v>
@@ -5494,7 +5494,7 @@
         <v>24</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="I74" s="1" t="s">
         <v>23</v>
@@ -5580,7 +5580,7 @@
         <v>24</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="I76" s="1" t="s">
         <v>24</v>
@@ -5828,7 +5828,6 @@
       <c r="M82" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="N82" s="0"/>
       <c r="P82" s="1" t="s">
         <v>282</v>
       </c>
@@ -5864,7 +5863,6 @@
       <c r="M83" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="N83" s="0"/>
       <c r="P83" s="1" t="s">
         <v>287</v>
       </c>
@@ -5900,7 +5898,6 @@
       <c r="M84" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="N84" s="0"/>
       <c r="P84" s="1" t="s">
         <v>292</v>
       </c>
@@ -10455,7 +10452,7 @@
       <c r="AP154" s="1"/>
       <c r="AQ154" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="33.1" outlineLevel="0" r="155">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="86.25" outlineLevel="0" r="155">
       <c r="A155" s="1" t="s">
         <v>587</v>
       </c>
@@ -10530,7 +10527,7 @@
       <c r="AP155" s="1"/>
       <c r="AQ155" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="54.35" outlineLevel="0" r="156">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="150" outlineLevel="0" r="156">
       <c r="A156" s="1" t="s">
         <v>587</v>
       </c>
@@ -10668,7 +10665,7 @@
       <c r="AP157" s="1"/>
       <c r="AQ157" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="33.1" outlineLevel="0" r="158">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="96.85" outlineLevel="0" r="158">
       <c r="A158" s="1" t="s">
         <v>587</v>
       </c>

</xml_diff>

<commit_message>
implement authorization check in API, resolve #170
</commit_message>
<xml_diff>
--- a/sampledata/fieldinformation.xlsx
+++ b/sampledata/fieldinformation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1876" uniqueCount="773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1982" uniqueCount="773">
   <si>
     <t>table</t>
   </si>
@@ -2500,7 +2500,7 @@
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -2513,29 +2513,29 @@
   <dimension ref="A1:AQ163"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <pane activePane="bottomRight" topLeftCell="A62" xSplit="3128" ySplit="1978"/>
+      <pane activePane="bottomRight" topLeftCell="A42" xSplit="3204" ySplit="1978"/>
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
       <selection activeCell="A1" activeCellId="0" pane="topRight" sqref="A1"/>
-      <selection activeCell="A62" activeCellId="0" pane="bottomLeft" sqref="A62"/>
-      <selection activeCell="H77" activeCellId="0" pane="bottomRight" sqref="H77"/>
+      <selection activeCell="A42" activeCellId="0" pane="bottomLeft" sqref="A42"/>
+      <selection activeCell="K59" activeCellId="0" pane="bottomRight" sqref="K59"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.8823529411765"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.9372549019608"/>
-    <col collapsed="false" hidden="false" max="9" min="3" style="1" width="11.4313725490196"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="2" width="11.4313725490196"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.4313725490196"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="29.556862745098"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="1" width="27.243137254902"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="58.6078431372549"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="15.9254901960784"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="47.1843137254902"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="14.7137254901961"/>
-    <col collapsed="false" hidden="false" max="21" min="20" style="1" width="22.7294117647059"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="22.6117647058824"/>
-    <col collapsed="false" hidden="false" max="25" min="23" style="1" width="9.87450980392157"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="9.87450980392157"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.0078431372549"/>
+    <col collapsed="false" hidden="false" max="9" min="3" style="1" width="11.4862745098039"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="2" width="11.4862745098039"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.4862745098039"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="29.7019607843137"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="1" width="27.3764705882353"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="58.8980392156863"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="16"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="47.4196078431373"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="14.7882352941176"/>
+    <col collapsed="false" hidden="false" max="21" min="20" style="1" width="22.8470588235294"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="22.7294117647059"/>
+    <col collapsed="false" hidden="false" max="25" min="23" style="1" width="9.92156862745098"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="9.92156862745098"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="67.5" outlineLevel="0" r="1" s="6">
@@ -2639,6 +2639,9 @@
       <c r="I2" s="7" t="s">
         <v>23</v>
       </c>
+      <c r="K2" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L2" s="1" t="n">
         <v>1</v>
       </c>
@@ -2682,6 +2685,9 @@
       <c r="I3" s="7" t="s">
         <v>23</v>
       </c>
+      <c r="K3" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L3" s="1" t="n">
         <v>2</v>
       </c>
@@ -2725,6 +2731,9 @@
       <c r="I4" s="7" t="s">
         <v>23</v>
       </c>
+      <c r="K4" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L4" s="1" t="n">
         <v>3</v>
       </c>
@@ -2768,6 +2777,9 @@
       <c r="I5" s="7" t="s">
         <v>23</v>
       </c>
+      <c r="K5" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L5" s="1" t="n">
         <v>4</v>
       </c>
@@ -2811,6 +2823,9 @@
       <c r="I6" s="7" t="s">
         <v>23</v>
       </c>
+      <c r="K6" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L6" s="1" t="n">
         <v>5</v>
       </c>
@@ -2848,6 +2863,9 @@
       <c r="I7" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="K7" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L7" s="1" t="n">
         <v>6</v>
       </c>
@@ -2885,6 +2903,9 @@
       <c r="I8" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="K8" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L8" s="1" t="n">
         <v>7</v>
       </c>
@@ -2922,6 +2943,9 @@
       <c r="I9" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="K9" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L9" s="1" t="n">
         <v>8</v>
       </c>
@@ -2959,6 +2983,9 @@
       <c r="I10" s="7" t="s">
         <v>23</v>
       </c>
+      <c r="K10" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L10" s="1" t="n">
         <v>9</v>
       </c>
@@ -2999,6 +3026,9 @@
       <c r="I11" s="7" t="s">
         <v>23</v>
       </c>
+      <c r="K11" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L11" s="1" t="n">
         <v>10</v>
       </c>
@@ -3039,6 +3069,9 @@
       <c r="I12" s="7" t="s">
         <v>23</v>
       </c>
+      <c r="K12" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L12" s="1" t="n">
         <v>11</v>
       </c>
@@ -3082,6 +3115,9 @@
       <c r="I13" s="7" t="s">
         <v>23</v>
       </c>
+      <c r="K13" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L13" s="1" t="n">
         <v>12</v>
       </c>
@@ -3122,6 +3158,9 @@
       <c r="I14" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="K14" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L14" s="1" t="n">
         <v>13</v>
       </c>
@@ -3162,6 +3201,9 @@
       <c r="I15" s="7" t="s">
         <v>23</v>
       </c>
+      <c r="K15" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L15" s="1" t="n">
         <v>14</v>
       </c>
@@ -3199,6 +3241,9 @@
       <c r="I16" s="7" t="s">
         <v>23</v>
       </c>
+      <c r="K16" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L16" s="1" t="n">
         <v>15</v>
       </c>
@@ -3242,6 +3287,9 @@
       <c r="I17" s="7" t="s">
         <v>23</v>
       </c>
+      <c r="K17" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L17" s="1" t="n">
         <v>16</v>
       </c>
@@ -3282,6 +3330,9 @@
       <c r="I18" s="7" t="s">
         <v>23</v>
       </c>
+      <c r="K18" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L18" s="1" t="n">
         <v>17</v>
       </c>
@@ -3322,6 +3373,9 @@
       <c r="I19" s="7" t="s">
         <v>23</v>
       </c>
+      <c r="K19" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L19" s="1" t="n">
         <v>18</v>
       </c>
@@ -3359,6 +3413,9 @@
       <c r="I20" s="7" t="s">
         <v>23</v>
       </c>
+      <c r="K20" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L20" s="1" t="n">
         <v>19</v>
       </c>
@@ -3396,6 +3453,9 @@
       <c r="I21" s="7" t="s">
         <v>23</v>
       </c>
+      <c r="K21" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L21" s="1" t="n">
         <v>20</v>
       </c>
@@ -3433,6 +3493,9 @@
       <c r="I22" s="7" t="s">
         <v>23</v>
       </c>
+      <c r="K22" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L22" s="1" t="n">
         <v>21</v>
       </c>
@@ -3475,6 +3538,9 @@
       <c r="I23" s="7" t="s">
         <v>23</v>
       </c>
+      <c r="K23" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L23" s="1" t="n">
         <v>22</v>
       </c>
@@ -3517,6 +3583,9 @@
       <c r="I24" s="7" t="s">
         <v>23</v>
       </c>
+      <c r="K24" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L24" s="1" t="n">
         <v>23</v>
       </c>
@@ -3535,7 +3604,7 @@
       <c r="AF24" s="1"/>
       <c r="AG24" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.1" outlineLevel="0" r="25">
       <c r="A25" s="9" t="s">
         <v>101</v>
       </c>
@@ -3553,6 +3622,9 @@
         <v>32</v>
       </c>
       <c r="I25" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="L25" s="1" t="n">
@@ -3573,7 +3645,7 @@
       <c r="AF25" s="1"/>
       <c r="AG25" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.1" outlineLevel="0" r="26">
       <c r="A26" s="9" t="s">
         <v>101</v>
       </c>
@@ -3591,6 +3663,9 @@
         <v>36</v>
       </c>
       <c r="I26" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K26" s="2" t="s">
         <v>23</v>
       </c>
       <c r="L26" s="1" t="n">
@@ -3631,6 +3706,9 @@
       <c r="I27" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="K27" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L27" s="1" t="n">
         <v>26</v>
       </c>
@@ -3671,6 +3749,9 @@
       <c r="I28" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="K28" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L28" s="1" t="n">
         <v>27</v>
       </c>
@@ -3689,7 +3770,7 @@
       <c r="AF28" s="1"/>
       <c r="AG28" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.1" outlineLevel="0" r="29">
       <c r="A29" s="9" t="s">
         <v>101</v>
       </c>
@@ -3707,6 +3788,9 @@
         <v>48</v>
       </c>
       <c r="I29" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K29" s="2" t="s">
         <v>23</v>
       </c>
       <c r="L29" s="1" t="n">
@@ -3727,7 +3811,7 @@
       <c r="AF29" s="1"/>
       <c r="AG29" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.1" outlineLevel="0" r="30">
       <c r="A30" s="9" t="s">
         <v>101</v>
       </c>
@@ -3745,6 +3829,9 @@
         <v>51</v>
       </c>
       <c r="I30" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K30" s="2" t="s">
         <v>23</v>
       </c>
       <c r="L30" s="1" t="n">
@@ -3785,6 +3872,9 @@
       <c r="I31" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="K31" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L31" s="1" t="n">
         <v>30</v>
       </c>
@@ -3823,6 +3913,9 @@
       <c r="I32" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="K32" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L32" s="1" t="n">
         <v>31</v>
       </c>
@@ -3865,6 +3958,9 @@
       <c r="I33" s="7" t="s">
         <v>23</v>
       </c>
+      <c r="K33" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L33" s="1" t="n">
         <v>32</v>
       </c>
@@ -3905,6 +4001,9 @@
       <c r="I34" s="7" t="s">
         <v>23</v>
       </c>
+      <c r="K34" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L34" s="1" t="n">
         <v>33</v>
       </c>
@@ -3945,6 +4044,9 @@
       <c r="I35" s="7" t="s">
         <v>23</v>
       </c>
+      <c r="K35" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L35" s="1" t="n">
         <v>34</v>
       </c>
@@ -3987,6 +4089,9 @@
       <c r="I36" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="K36" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L36" s="1" t="n">
         <v>35</v>
       </c>
@@ -4032,6 +4137,9 @@
       <c r="I37" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="K37" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L37" s="1" t="n">
         <v>36</v>
       </c>
@@ -4072,6 +4180,9 @@
       <c r="I38" s="7" t="s">
         <v>23</v>
       </c>
+      <c r="K38" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L38" s="1" t="n">
         <v>37</v>
       </c>
@@ -4112,6 +4223,9 @@
       <c r="I39" s="7" t="s">
         <v>23</v>
       </c>
+      <c r="K39" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L39" s="1" t="n">
         <v>38</v>
       </c>
@@ -4149,6 +4263,9 @@
       <c r="I40" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="K40" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L40" s="1" t="n">
         <v>39</v>
       </c>
@@ -4189,6 +4306,9 @@
       <c r="I41" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="K41" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L41" s="1" t="n">
         <v>40</v>
       </c>
@@ -4223,6 +4343,9 @@
       <c r="I42" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="K42" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L42" s="1" t="n">
         <v>41</v>
       </c>
@@ -4257,6 +4380,9 @@
       <c r="I43" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="K43" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L43" s="1" t="n">
         <v>42</v>
       </c>
@@ -4291,6 +4417,9 @@
       <c r="I44" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="K44" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L44" s="1" t="n">
         <v>43</v>
       </c>
@@ -4322,6 +4451,9 @@
       <c r="I45" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="K45" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L45" s="1" t="n">
         <v>44</v>
       </c>
@@ -4362,6 +4494,9 @@
       <c r="I46" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="K46" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L46" s="1" t="n">
         <v>45</v>
       </c>
@@ -4402,6 +4537,9 @@
       <c r="I47" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="K47" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L47" s="1" t="n">
         <v>46</v>
       </c>
@@ -4442,6 +4580,9 @@
       <c r="I48" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="K48" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L48" s="1" t="n">
         <v>47</v>
       </c>
@@ -4482,6 +4623,9 @@
       <c r="I49" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="K49" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L49" s="1" t="n">
         <v>48</v>
       </c>
@@ -4522,6 +4666,9 @@
       <c r="I50" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="K50" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L50" s="1" t="n">
         <v>49</v>
       </c>
@@ -4560,6 +4707,9 @@
       <c r="I51" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="K51" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L51" s="1" t="n">
         <v>50</v>
       </c>
@@ -4598,6 +4748,9 @@
       <c r="I52" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="K52" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L52" s="1" t="n">
         <v>51</v>
       </c>
@@ -4634,6 +4787,9 @@
         <v>54</v>
       </c>
       <c r="I53" s="7"/>
+      <c r="K53" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L53" s="1" t="n">
         <v>52</v>
       </c>
@@ -4672,6 +4828,9 @@
       <c r="I54" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="K54" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L54" s="1" t="n">
         <v>53</v>
       </c>
@@ -4712,6 +4871,9 @@
       <c r="I55" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="K55" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L55" s="1" t="n">
         <v>54</v>
       </c>
@@ -4752,6 +4914,9 @@
       <c r="I56" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="K56" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L56" s="1" t="n">
         <v>55</v>
       </c>
@@ -4789,6 +4954,9 @@
       <c r="I57" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="K57" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L57" s="1" t="n">
         <v>56</v>
       </c>
@@ -4826,6 +4994,9 @@
       <c r="I58" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="K58" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L58" s="1" t="n">
         <v>57</v>
       </c>
@@ -4863,6 +5034,9 @@
       <c r="I59" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="K59" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L59" s="1" t="n">
         <v>58</v>
       </c>
@@ -4900,6 +5074,9 @@
       <c r="I60" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="K60" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L60" s="1" t="n">
         <v>59</v>
       </c>
@@ -4940,6 +5117,9 @@
       <c r="I61" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="K61" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L61" s="1" t="n">
         <v>60</v>
       </c>
@@ -4979,6 +5159,9 @@
       </c>
       <c r="I62" s="1" t="s">
         <v>24</v>
+      </c>
+      <c r="K62" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="L62" s="1" t="n">
         <v>61</v>
@@ -7976,7 +8159,9 @@
       <c r="J119" s="13" t="s">
         <v>458</v>
       </c>
-      <c r="K119" s="13"/>
+      <c r="K119" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L119" s="1" t="s">
         <v>459</v>
       </c>
@@ -8047,7 +8232,9 @@
       <c r="J120" s="13" t="s">
         <v>458</v>
       </c>
-      <c r="K120" s="13"/>
+      <c r="K120" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L120" s="1" t="s">
         <v>466</v>
       </c>
@@ -8115,7 +8302,9 @@
       <c r="J121" s="13" t="s">
         <v>458</v>
       </c>
-      <c r="K121" s="13"/>
+      <c r="K121" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L121" s="1" t="s">
         <v>472</v>
       </c>
@@ -8189,7 +8378,9 @@
       <c r="J122" s="13" t="s">
         <v>458</v>
       </c>
-      <c r="K122" s="13"/>
+      <c r="K122" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L122" s="1" t="s">
         <v>479</v>
       </c>
@@ -8266,7 +8457,9 @@
       <c r="J123" s="13" t="s">
         <v>458</v>
       </c>
-      <c r="K123" s="13"/>
+      <c r="K123" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L123" s="1" t="s">
         <v>485</v>
       </c>
@@ -8331,7 +8524,9 @@
       <c r="J124" s="13" t="s">
         <v>458</v>
       </c>
-      <c r="K124" s="13"/>
+      <c r="K124" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L124" s="1" t="s">
         <v>489</v>
       </c>
@@ -8396,7 +8591,9 @@
       <c r="J125" s="13" t="s">
         <v>458</v>
       </c>
-      <c r="K125" s="13"/>
+      <c r="K125" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L125" s="1" t="s">
         <v>494</v>
       </c>
@@ -8462,7 +8659,9 @@
       <c r="J126" s="13" t="s">
         <v>458</v>
       </c>
-      <c r="K126" s="13"/>
+      <c r="K126" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L126" s="1" t="s">
         <v>500</v>
       </c>
@@ -8534,7 +8733,9 @@
       <c r="J127" s="13" t="s">
         <v>458</v>
       </c>
-      <c r="K127" s="13"/>
+      <c r="K127" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L127" s="1" t="s">
         <v>508</v>
       </c>
@@ -8606,7 +8807,9 @@
       <c r="J128" s="13" t="s">
         <v>458</v>
       </c>
-      <c r="K128" s="13"/>
+      <c r="K128" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L128" s="1" t="s">
         <v>516</v>
       </c>
@@ -8675,7 +8878,9 @@
       <c r="J129" s="13" t="s">
         <v>458</v>
       </c>
-      <c r="K129" s="13"/>
+      <c r="K129" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L129" s="1" t="s">
         <v>522</v>
       </c>
@@ -8744,7 +8949,9 @@
       <c r="J130" s="13" t="s">
         <v>458</v>
       </c>
-      <c r="K130" s="13"/>
+      <c r="K130" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L130" s="1" t="s">
         <v>529</v>
       </c>
@@ -8816,7 +9023,9 @@
       <c r="J131" s="13" t="s">
         <v>458</v>
       </c>
-      <c r="K131" s="13"/>
+      <c r="K131" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L131" s="1" t="s">
         <v>535</v>
       </c>
@@ -8888,7 +9097,9 @@
       <c r="J132" s="13" t="s">
         <v>458</v>
       </c>
-      <c r="K132" s="13"/>
+      <c r="K132" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L132" s="1" t="s">
         <v>541</v>
       </c>
@@ -8960,7 +9171,9 @@
       <c r="J133" s="13" t="s">
         <v>458</v>
       </c>
-      <c r="K133" s="13"/>
+      <c r="K133" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L133" s="1" t="s">
         <v>550</v>
       </c>
@@ -9032,7 +9245,9 @@
       <c r="J134" s="13" t="s">
         <v>458</v>
       </c>
-      <c r="K134" s="13"/>
+      <c r="K134" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L134" s="1" t="s">
         <v>555</v>
       </c>
@@ -9104,7 +9319,9 @@
       <c r="J135" s="13" t="s">
         <v>458</v>
       </c>
-      <c r="K135" s="13"/>
+      <c r="K135" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L135" s="1" t="s">
         <v>563</v>
       </c>
@@ -9173,7 +9390,9 @@
       <c r="J136" s="13" t="s">
         <v>458</v>
       </c>
-      <c r="K136" s="13"/>
+      <c r="K136" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L136" s="1" t="s">
         <v>570</v>
       </c>
@@ -9237,7 +9456,9 @@
       <c r="J137" s="13" t="s">
         <v>458</v>
       </c>
-      <c r="K137" s="13"/>
+      <c r="K137" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L137" s="1" t="s">
         <v>577</v>
       </c>
@@ -9304,7 +9525,9 @@
       <c r="J138" s="13" t="s">
         <v>458</v>
       </c>
-      <c r="K138" s="13"/>
+      <c r="K138" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L138" s="1" t="s">
         <v>583</v>
       </c>
@@ -9376,7 +9599,9 @@
       <c r="J139" s="9" t="s">
         <v>589</v>
       </c>
-      <c r="K139" s="9"/>
+      <c r="K139" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L139" s="1" t="s">
         <v>590</v>
       </c>
@@ -9457,7 +9682,9 @@
       <c r="J140" s="9" t="s">
         <v>589</v>
       </c>
-      <c r="K140" s="9"/>
+      <c r="K140" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L140" s="1" t="s">
         <v>602</v>
       </c>
@@ -9523,7 +9750,9 @@
       <c r="J141" s="9" t="s">
         <v>589</v>
       </c>
-      <c r="K141" s="9"/>
+      <c r="K141" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L141" s="1" t="s">
         <v>606</v>
       </c>
@@ -9586,7 +9815,9 @@
       <c r="J142" s="9" t="s">
         <v>589</v>
       </c>
-      <c r="K142" s="9"/>
+      <c r="K142" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L142" s="1" t="s">
         <v>611</v>
       </c>
@@ -9646,7 +9877,9 @@
       <c r="J143" s="9" t="s">
         <v>589</v>
       </c>
-      <c r="K143" s="9"/>
+      <c r="K143" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L143" s="1" t="s">
         <v>616</v>
       </c>
@@ -9706,7 +9939,9 @@
       <c r="J144" s="9" t="s">
         <v>589</v>
       </c>
-      <c r="K144" s="9"/>
+      <c r="K144" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L144" s="1" t="s">
         <v>620</v>
       </c>
@@ -9769,7 +10004,9 @@
       <c r="J145" s="9" t="s">
         <v>589</v>
       </c>
-      <c r="K145" s="9"/>
+      <c r="K145" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L145" s="1" t="s">
         <v>626</v>
       </c>
@@ -9844,7 +10081,9 @@
       <c r="J146" s="9" t="s">
         <v>589</v>
       </c>
-      <c r="K146" s="9"/>
+      <c r="K146" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L146" s="1" t="s">
         <v>636</v>
       </c>
@@ -9907,7 +10146,9 @@
       <c r="J147" s="9" t="s">
         <v>589</v>
       </c>
-      <c r="K147" s="9"/>
+      <c r="K147" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L147" s="1" t="s">
         <v>641</v>
       </c>
@@ -9973,7 +10214,9 @@
       <c r="J148" s="9" t="s">
         <v>589</v>
       </c>
-      <c r="K148" s="9"/>
+      <c r="K148" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L148" s="1" t="s">
         <v>647</v>
       </c>
@@ -10045,7 +10288,9 @@
       <c r="J149" s="9" t="s">
         <v>589</v>
       </c>
-      <c r="K149" s="9"/>
+      <c r="K149" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L149" s="1" t="s">
         <v>655</v>
       </c>
@@ -10111,7 +10356,9 @@
       <c r="J150" s="9" t="s">
         <v>589</v>
       </c>
-      <c r="K150" s="9"/>
+      <c r="K150" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L150" s="1" t="s">
         <v>661</v>
       </c>
@@ -10192,7 +10439,9 @@
       <c r="J151" s="9" t="s">
         <v>589</v>
       </c>
-      <c r="K151" s="9"/>
+      <c r="K151" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L151" s="1" t="s">
         <v>670</v>
       </c>
@@ -10264,7 +10513,9 @@
       <c r="J152" s="9" t="s">
         <v>589</v>
       </c>
-      <c r="K152" s="9"/>
+      <c r="K152" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L152" s="1" t="s">
         <v>679</v>
       </c>
@@ -10330,7 +10581,9 @@
       <c r="J153" s="9" t="s">
         <v>589</v>
       </c>
-      <c r="K153" s="9"/>
+      <c r="K153" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L153" s="1" t="s">
         <v>686</v>
       </c>
@@ -10408,7 +10661,9 @@
       <c r="J154" s="9" t="s">
         <v>589</v>
       </c>
-      <c r="K154" s="9"/>
+      <c r="K154" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L154" s="1" t="s">
         <v>697</v>
       </c>
@@ -10474,7 +10729,9 @@
       <c r="J155" s="9" t="s">
         <v>589</v>
       </c>
-      <c r="K155" s="9"/>
+      <c r="K155" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L155" s="1" t="s">
         <v>704</v>
       </c>
@@ -10549,7 +10806,9 @@
       <c r="J156" s="9" t="s">
         <v>589</v>
       </c>
-      <c r="K156" s="9"/>
+      <c r="K156" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L156" s="1" t="s">
         <v>713</v>
       </c>
@@ -10618,7 +10877,9 @@
       <c r="J157" s="9" t="s">
         <v>589</v>
       </c>
-      <c r="K157" s="9"/>
+      <c r="K157" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L157" s="1" t="s">
         <v>720</v>
       </c>
@@ -10687,7 +10948,9 @@
       <c r="J158" s="9" t="s">
         <v>589</v>
       </c>
-      <c r="K158" s="9"/>
+      <c r="K158" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L158" s="1" t="s">
         <v>727</v>
       </c>
@@ -10759,7 +11022,9 @@
       <c r="J159" s="9" t="s">
         <v>589</v>
       </c>
-      <c r="K159" s="9"/>
+      <c r="K159" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L159" s="1" t="s">
         <v>735</v>
       </c>
@@ -10828,7 +11093,9 @@
       <c r="J160" s="9" t="s">
         <v>589</v>
       </c>
-      <c r="K160" s="9"/>
+      <c r="K160" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L160" s="1" t="s">
         <v>743</v>
       </c>
@@ -10891,7 +11158,9 @@
       <c r="J161" s="9" t="s">
         <v>589</v>
       </c>
-      <c r="K161" s="9"/>
+      <c r="K161" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L161" s="1" t="s">
         <v>749</v>
       </c>
@@ -10960,7 +11229,9 @@
       <c r="J162" s="9" t="s">
         <v>589</v>
       </c>
-      <c r="K162" s="9"/>
+      <c r="K162" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L162" s="1" t="s">
         <v>757</v>
       </c>
@@ -11032,7 +11303,9 @@
       <c r="J163" s="9" t="s">
         <v>589</v>
       </c>
-      <c r="K163" s="9"/>
+      <c r="K163" s="13" t="s">
+        <v>23</v>
+      </c>
       <c r="L163" s="1" t="s">
         <v>765</v>
       </c>

</xml_diff>

<commit_message>
fix code issue with restricted filter for api, #170
</commit_message>
<xml_diff>
--- a/sampledata/fieldinformation.xlsx
+++ b/sampledata/fieldinformation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1982" uniqueCount="773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1998" uniqueCount="776">
   <si>
     <t>table</t>
   </si>
@@ -1185,6 +1185,15 @@
   </si>
   <si>
     <t>The software versions are available from IUPAC</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>SM:28</t>
+  </si>
+  <si>
+    <t>Is restricted molecule: only available to staff</t>
   </si>
   <si>
     <t>target_information_references</t>
@@ -2510,14 +2519,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AQ163"/>
+  <dimension ref="A1:AQ164"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <pane activePane="bottomRight" topLeftCell="A42" xSplit="3204" ySplit="1978"/>
+      <pane activePane="bottomRight" topLeftCell="A93" xSplit="3204" ySplit="1978"/>
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
       <selection activeCell="A1" activeCellId="0" pane="topRight" sqref="A1"/>
-      <selection activeCell="A42" activeCellId="0" pane="bottomLeft" sqref="A42"/>
-      <selection activeCell="K59" activeCellId="0" pane="bottomRight" sqref="K59"/>
+      <selection activeCell="A93" activeCellId="0" pane="bottomLeft" sqref="A93"/>
+      <selection activeCell="E103" activeCellId="0" pane="bottomRight" sqref="E103"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -4442,6 +4451,9 @@
       <c r="B45" s="1" t="s">
         <v>168</v>
       </c>
+      <c r="E45" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="G45" s="9" t="s">
         <v>24</v>
       </c>
@@ -7004,7 +7016,9 @@
       </c>
       <c r="C100" s="9"/>
       <c r="D100" s="9"/>
-      <c r="E100" s="9"/>
+      <c r="E100" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="F100" s="9"/>
       <c r="G100" s="9" t="s">
         <v>24</v>
@@ -7053,7 +7067,9 @@
       <c r="D101" s="9" t="s">
         <v>381</v>
       </c>
-      <c r="E101" s="9"/>
+      <c r="E101" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="F101" s="9"/>
       <c r="G101" s="9" t="s">
         <v>23</v>
@@ -7158,21 +7174,23 @@
       <c r="AK102" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="103">
-      <c r="A103" s="9"/>
+      <c r="A103" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="B103" s="9" t="s">
-        <v>390</v>
+        <v>168</v>
       </c>
       <c r="C103" s="9"/>
-      <c r="D103" s="9" t="s">
-        <v>381</v>
-      </c>
-      <c r="E103" s="9"/>
+      <c r="D103" s="9"/>
+      <c r="E103" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="F103" s="9"/>
       <c r="G103" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H103" s="9" t="s">
-        <v>159</v>
+        <v>390</v>
       </c>
       <c r="I103" s="7" t="s">
         <v>24</v>
@@ -7181,28 +7199,22 @@
         <v>295</v>
       </c>
       <c r="K103" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L103" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="M103" s="1" t="s">
+      <c r="N103" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="P103" s="1" t="s">
         <v>392</v>
-      </c>
-      <c r="O103" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="P103" s="1" t="s">
-        <v>393</v>
       </c>
       <c r="Q103" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="R103" s="1" t="s">
-        <v>394</v>
-      </c>
       <c r="U103" s="1" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="Z103" s="1"/>
       <c r="AA103" s="1"/>
@@ -7218,57 +7230,53 @@
       <c r="AK103" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="104">
-      <c r="A104" s="9" t="s">
-        <v>322</v>
-      </c>
+      <c r="A104" s="9"/>
       <c r="B104" s="9" t="s">
-        <v>396</v>
-      </c>
-      <c r="C104" s="9" t="s">
-        <v>329</v>
-      </c>
-      <c r="D104" s="9"/>
+        <v>393</v>
+      </c>
+      <c r="C104" s="9"/>
+      <c r="D104" s="9" t="s">
+        <v>381</v>
+      </c>
       <c r="E104" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F104" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="F104" s="9"/>
       <c r="G104" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H104" s="9" t="s">
-        <v>40</v>
+        <v>159</v>
       </c>
       <c r="I104" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J104" s="12" t="s">
         <v>295</v>
       </c>
       <c r="K104" s="12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L104" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="M104" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="O104" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="P104" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="Q104" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="R104" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="M104" s="1" t="s">
+      <c r="U104" s="1" t="s">
         <v>398</v>
-      </c>
-      <c r="N104" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="O104" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="P104" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="Q104" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="R104" s="1" t="s">
-        <v>401</v>
       </c>
       <c r="Z104" s="1"/>
       <c r="AA104" s="1"/>
@@ -7288,21 +7296,23 @@
         <v>322</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>402</v>
-      </c>
-      <c r="C105" s="9"/>
+        <v>399</v>
+      </c>
+      <c r="C105" s="9" t="s">
+        <v>329</v>
+      </c>
       <c r="D105" s="9"/>
       <c r="E105" s="9" t="s">
         <v>23</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G105" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H105" s="9" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="I105" s="7" t="s">
         <v>23</v>
@@ -7314,22 +7324,25 @@
         <v>23</v>
       </c>
       <c r="L105" s="1" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="M105" s="1" t="s">
-        <v>404</v>
+        <v>401</v>
+      </c>
+      <c r="N105" s="1" t="s">
+        <v>402</v>
       </c>
       <c r="O105" s="1" t="s">
         <v>329</v>
       </c>
       <c r="P105" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="Q105" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R105" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="Z105" s="1"/>
       <c r="AA105" s="1"/>
@@ -7349,7 +7362,7 @@
         <v>322</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C106" s="9"/>
       <c r="D106" s="9"/>
@@ -7363,7 +7376,7 @@
         <v>23</v>
       </c>
       <c r="H106" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I106" s="7" t="s">
         <v>23</v>
@@ -7375,19 +7388,22 @@
         <v>23</v>
       </c>
       <c r="L106" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="M106" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="O106" s="1" t="s">
         <v>329</v>
       </c>
       <c r="P106" s="1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="Q106" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="R106" s="1" t="s">
+        <v>409</v>
       </c>
       <c r="Z106" s="1"/>
       <c r="AA106" s="1"/>
@@ -7407,7 +7423,7 @@
         <v>322</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C107" s="9"/>
       <c r="D107" s="9"/>
@@ -7421,7 +7437,7 @@
         <v>23</v>
       </c>
       <c r="H107" s="9" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="I107" s="7" t="s">
         <v>23</v>
@@ -7433,22 +7449,19 @@
         <v>23</v>
       </c>
       <c r="L107" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="M107" s="1" t="s">
         <v>412</v>
-      </c>
-      <c r="M107" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="N107" s="1" t="s">
-        <v>414</v>
       </c>
       <c r="O107" s="1" t="s">
         <v>329</v>
       </c>
       <c r="P107" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="Q107" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z107" s="1"/>
       <c r="AA107" s="1"/>
@@ -7468,46 +7481,48 @@
         <v>322</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>363</v>
+        <v>414</v>
       </c>
       <c r="C108" s="9"/>
       <c r="D108" s="9"/>
       <c r="E108" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F108" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="G108" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H108" s="9" t="s">
-        <v>416</v>
+        <v>58</v>
       </c>
       <c r="I108" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J108" s="12" t="s">
         <v>295</v>
       </c>
       <c r="K108" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L108" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="M108" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="N108" s="1" t="s">
         <v>417</v>
-      </c>
-      <c r="M108" s="1" t="s">
-        <v>418</v>
       </c>
       <c r="O108" s="1" t="s">
         <v>329</v>
       </c>
       <c r="P108" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="Q108" s="1" t="n">
         <v>2</v>
-      </c>
-      <c r="R108" s="1" t="s">
-        <v>352</v>
       </c>
       <c r="Z108" s="1"/>
       <c r="AA108" s="1"/>
@@ -7527,7 +7542,7 @@
         <v>322</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="C109" s="9"/>
       <c r="D109" s="9"/>
@@ -7539,7 +7554,7 @@
         <v>23</v>
       </c>
       <c r="H109" s="9" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="I109" s="7" t="s">
         <v>24</v>
@@ -7551,22 +7566,22 @@
         <v>24</v>
       </c>
       <c r="L109" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="M109" s="1" t="s">
         <v>421</v>
-      </c>
-      <c r="M109" s="1" t="s">
-        <v>422</v>
       </c>
       <c r="O109" s="1" t="s">
         <v>329</v>
       </c>
       <c r="P109" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="Q109" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="U109" s="1" t="s">
-        <v>373</v>
+      <c r="R109" s="1" t="s">
+        <v>352</v>
       </c>
       <c r="Z109" s="1"/>
       <c r="AA109" s="1"/>
@@ -7586,7 +7601,7 @@
         <v>322</v>
       </c>
       <c r="B110" s="9" t="s">
-        <v>357</v>
+        <v>368</v>
       </c>
       <c r="C110" s="9"/>
       <c r="D110" s="9"/>
@@ -7598,7 +7613,7 @@
         <v>23</v>
       </c>
       <c r="H110" s="9" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="I110" s="7" t="s">
         <v>24</v>
@@ -7610,22 +7625,22 @@
         <v>24</v>
       </c>
       <c r="L110" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="M110" s="1" t="s">
         <v>425</v>
-      </c>
-      <c r="M110" s="1" t="s">
-        <v>426</v>
       </c>
       <c r="O110" s="1" t="s">
         <v>329</v>
       </c>
       <c r="P110" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="Q110" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="R110" s="1" t="s">
-        <v>352</v>
+        <v>2</v>
+      </c>
+      <c r="U110" s="1" t="s">
+        <v>373</v>
       </c>
       <c r="Z110" s="1"/>
       <c r="AA110" s="1"/>
@@ -7645,22 +7660,22 @@
         <v>322</v>
       </c>
       <c r="B111" s="9" t="s">
-        <v>428</v>
+        <v>357</v>
       </c>
       <c r="C111" s="9"/>
       <c r="D111" s="9"/>
       <c r="E111" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F111" s="9"/>
       <c r="G111" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H111" s="9" t="s">
-        <v>290</v>
+        <v>427</v>
       </c>
       <c r="I111" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J111" s="12" t="s">
         <v>295</v>
@@ -7669,22 +7684,22 @@
         <v>24</v>
       </c>
       <c r="L111" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="M111" s="1" t="s">
         <v>429</v>
-      </c>
-      <c r="M111" s="1" t="s">
-        <v>430</v>
       </c>
       <c r="O111" s="1" t="s">
         <v>329</v>
       </c>
       <c r="P111" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Q111" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R111" s="1" t="s">
-        <v>432</v>
+        <v>352</v>
       </c>
       <c r="Z111" s="1"/>
       <c r="AA111" s="1"/>
@@ -7698,19 +7713,13 @@
       <c r="AI111" s="1"/>
       <c r="AJ111" s="1"/>
       <c r="AK111" s="1"/>
-      <c r="AL111" s="1"/>
-      <c r="AM111" s="1"/>
-      <c r="AN111" s="1"/>
-      <c r="AO111" s="1"/>
-      <c r="AP111" s="1"/>
-      <c r="AQ111" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="112">
       <c r="A112" s="9" t="s">
         <v>322</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C112" s="9"/>
       <c r="D112" s="9"/>
@@ -7722,7 +7731,7 @@
         <v>23</v>
       </c>
       <c r="H112" s="9" t="s">
-        <v>434</v>
+        <v>290</v>
       </c>
       <c r="I112" s="7" t="s">
         <v>23</v>
@@ -7734,22 +7743,22 @@
         <v>24</v>
       </c>
       <c r="L112" s="1" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="M112" s="1" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="O112" s="1" t="s">
         <v>329</v>
       </c>
       <c r="P112" s="1" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="Q112" s="1" t="n">
         <v>3</v>
       </c>
       <c r="R112" s="1" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="Z112" s="1"/>
       <c r="AA112" s="1"/>
@@ -7775,7 +7784,7 @@
         <v>322</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C113" s="9"/>
       <c r="D113" s="9"/>
@@ -7787,7 +7796,7 @@
         <v>23</v>
       </c>
       <c r="H113" s="9" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="I113" s="7" t="s">
         <v>23</v>
@@ -7799,19 +7808,22 @@
         <v>24</v>
       </c>
       <c r="L113" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="M113" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="O113" s="1" t="s">
         <v>329</v>
       </c>
       <c r="P113" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="Q113" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="R113" s="1" t="s">
+        <v>435</v>
       </c>
       <c r="Z113" s="1"/>
       <c r="AA113" s="1"/>
@@ -7837,19 +7849,19 @@
         <v>322</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C114" s="9"/>
       <c r="D114" s="9"/>
       <c r="E114" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F114" s="9"/>
       <c r="G114" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H114" s="9" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="I114" s="7" t="s">
         <v>23</v>
@@ -7861,22 +7873,19 @@
         <v>24</v>
       </c>
       <c r="L114" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="M114" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="O114" s="1" t="s">
         <v>329</v>
       </c>
       <c r="P114" s="1" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="Q114" s="1" t="n">
         <v>3</v>
-      </c>
-      <c r="R114" s="1" t="s">
-        <v>432</v>
       </c>
       <c r="Z114" s="1"/>
       <c r="AA114" s="1"/>
@@ -7901,38 +7910,47 @@
       <c r="A115" s="9" t="s">
         <v>322</v>
       </c>
-      <c r="B115" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="E115" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="B115" s="9" t="s">
+        <v>446</v>
+      </c>
+      <c r="C115" s="9"/>
+      <c r="D115" s="9"/>
+      <c r="E115" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F115" s="9"/>
       <c r="G115" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H115" s="9" t="s">
-        <v>159</v>
+        <v>447</v>
       </c>
       <c r="I115" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K115" s="2" t="s">
-        <v>23</v>
+        <v>23</v>
+      </c>
+      <c r="J115" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="K115" s="12" t="s">
+        <v>24</v>
       </c>
       <c r="L115" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="N115" s="1" t="s">
-        <v>160</v>
+      <c r="M115" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="O115" s="1" t="s">
+        <v>329</v>
       </c>
       <c r="P115" s="1" t="s">
-        <v>161</v>
+        <v>450</v>
+      </c>
+      <c r="Q115" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="R115" s="1" t="s">
+        <v>435</v>
       </c>
       <c r="Z115" s="1"/>
       <c r="AA115" s="1"/>
@@ -7958,7 +7976,7 @@
         <v>322</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>172</v>
@@ -7982,13 +8000,13 @@
         <v>23</v>
       </c>
       <c r="L116" s="1" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="N116" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="P116" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="Z116" s="1"/>
       <c r="AA116" s="1"/>
@@ -8014,7 +8032,7 @@
         <v>322</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>172</v>
@@ -8038,13 +8056,13 @@
         <v>23</v>
       </c>
       <c r="L117" s="1" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="N117" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="P117" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="Z117" s="1"/>
       <c r="AA117" s="1"/>
@@ -8066,50 +8084,41 @@
       <c r="AQ117" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="118">
-      <c r="A118" s="9"/>
-      <c r="B118" s="9" t="s">
-        <v>451</v>
-      </c>
-      <c r="C118" s="9"/>
-      <c r="D118" s="9" t="s">
-        <v>381</v>
-      </c>
-      <c r="E118" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F118" s="9"/>
+      <c r="A118" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="G118" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H118" s="9" t="s">
-        <v>452</v>
+        <v>159</v>
       </c>
       <c r="I118" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J118" s="12" t="s">
-        <v>295</v>
-      </c>
-      <c r="K118" s="12" t="s">
-        <v>24</v>
+        <v>24</v>
+      </c>
+      <c r="K118" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="L118" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="M118" s="1" t="s">
-        <v>454</v>
-      </c>
-      <c r="O118" s="1" t="s">
-        <v>329</v>
+      <c r="N118" s="1" t="s">
+        <v>166</v>
       </c>
       <c r="P118" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="Q118" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="R118" s="1" t="s">
-        <v>432</v>
+        <v>167</v>
       </c>
       <c r="Z118" s="1"/>
       <c r="AA118" s="1"/>
@@ -8131,60 +8140,50 @@
       <c r="AQ118" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="119">
-      <c r="A119" s="9" t="s">
+      <c r="A119" s="9"/>
+      <c r="B119" s="9" t="s">
+        <v>454</v>
+      </c>
+      <c r="C119" s="9"/>
+      <c r="D119" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="E119" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F119" s="9"/>
+      <c r="G119" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H119" s="9" t="s">
+        <v>455</v>
+      </c>
+      <c r="I119" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J119" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="K119" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="L119" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="B119" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="C119" s="9" t="s">
+      <c r="M119" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="D119" s="9"/>
-      <c r="E119" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F119" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G119" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H119" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I119" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J119" s="13" t="s">
+      <c r="O119" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="P119" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="K119" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="L119" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="M119" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="N119" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="O119" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="P119" s="1" t="s">
-        <v>463</v>
-      </c>
       <c r="Q119" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R119" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="S119" s="1" t="s">
-        <v>465</v>
+        <v>435</v>
       </c>
       <c r="Z119" s="1"/>
       <c r="AA119" s="1"/>
@@ -8207,12 +8206,14 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="120">
       <c r="A120" s="9" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>303</v>
-      </c>
-      <c r="C120" s="9"/>
+        <v>145</v>
+      </c>
+      <c r="C120" s="9" t="s">
+        <v>460</v>
+      </c>
       <c r="D120" s="9"/>
       <c r="E120" s="9" t="s">
         <v>23</v>
@@ -8224,37 +8225,40 @@
         <v>23</v>
       </c>
       <c r="H120" s="9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="I120" s="7" t="s">
         <v>23</v>
       </c>
       <c r="J120" s="13" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="K120" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L120" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="M120" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="N120" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="O120" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="P120" s="1" t="s">
         <v>466</v>
-      </c>
-      <c r="M120" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="N120" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="O120" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="P120" s="1" t="s">
-        <v>469</v>
       </c>
       <c r="Q120" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R120" s="1" t="s">
-        <v>470</v>
+        <v>467</v>
+      </c>
+      <c r="S120" s="1" t="s">
+        <v>468</v>
       </c>
       <c r="Z120" s="1"/>
       <c r="AA120" s="1"/>
@@ -8277,10 +8281,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="121">
       <c r="A121" s="9" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>471</v>
+        <v>303</v>
       </c>
       <c r="C121" s="9"/>
       <c r="D121" s="9"/>
@@ -8294,43 +8298,37 @@
         <v>23</v>
       </c>
       <c r="H121" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I121" s="7" t="s">
         <v>23</v>
       </c>
       <c r="J121" s="13" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="K121" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L121" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="M121" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="N121" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="O121" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="P121" s="1" t="s">
         <v>472</v>
-      </c>
-      <c r="M121" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="O121" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="P121" s="1" t="s">
-        <v>474</v>
       </c>
       <c r="Q121" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R121" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="S121" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="T121" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="U121" s="1" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="Z121" s="1"/>
       <c r="AA121" s="1"/>
@@ -8353,10 +8351,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="122">
       <c r="A122" s="9" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="B122" s="9" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="C122" s="9"/>
       <c r="D122" s="9"/>
@@ -8370,46 +8368,43 @@
         <v>23</v>
       </c>
       <c r="H122" s="9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="I122" s="7" t="s">
         <v>23</v>
       </c>
       <c r="J122" s="13" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="K122" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L122" s="1" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="M122" s="1" t="s">
-        <v>480</v>
-      </c>
-      <c r="N122" s="1" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="O122" s="1" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="P122" s="1" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="Q122" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R122" s="1" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="S122" s="1" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="T122" s="1" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="U122" s="1" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="Z122" s="1"/>
       <c r="AA122" s="1"/>
@@ -8432,10 +8427,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="123">
       <c r="A123" s="9" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>402</v>
+        <v>481</v>
       </c>
       <c r="C123" s="9"/>
       <c r="D123" s="9"/>
@@ -8449,34 +8444,46 @@
         <v>23</v>
       </c>
       <c r="H123" s="9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="I123" s="7" t="s">
         <v>23</v>
       </c>
       <c r="J123" s="13" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="K123" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L123" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="M123" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="N123" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="O123" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="P123" s="1" t="s">
         <v>485</v>
-      </c>
-      <c r="M123" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="O123" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="P123" s="1" t="s">
-        <v>487</v>
       </c>
       <c r="Q123" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="R123" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="S123" s="1" t="s">
+        <v>468</v>
+      </c>
       <c r="T123" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
+      </c>
+      <c r="U123" s="1" t="s">
+        <v>480</v>
       </c>
       <c r="Z123" s="1"/>
       <c r="AA123" s="1"/>
@@ -8499,10 +8506,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="124">
       <c r="A124" s="9" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="B124" s="9" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C124" s="9"/>
       <c r="D124" s="9"/>
@@ -8510,40 +8517,40 @@
         <v>23</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G124" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H124" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I124" s="7" t="s">
         <v>23</v>
       </c>
       <c r="J124" s="13" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="K124" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L124" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="M124" s="1" t="s">
         <v>489</v>
-      </c>
-      <c r="M124" s="1" t="s">
-        <v>490</v>
       </c>
       <c r="O124" s="1" t="s">
         <v>329</v>
       </c>
       <c r="P124" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="Q124" s="1" t="n">
         <v>1</v>
       </c>
       <c r="T124" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="Z124" s="1"/>
       <c r="AA124" s="1"/>
@@ -8566,10 +8573,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="125">
       <c r="A125" s="9" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>493</v>
+        <v>410</v>
       </c>
       <c r="C125" s="9"/>
       <c r="D125" s="9"/>
@@ -8583,37 +8590,34 @@
         <v>23</v>
       </c>
       <c r="H125" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I125" s="7" t="s">
         <v>23</v>
       </c>
       <c r="J125" s="13" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="K125" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L125" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="M125" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="O125" s="1" t="s">
         <v>329</v>
       </c>
       <c r="P125" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="Q125" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="R125" s="1" t="s">
-        <v>497</v>
-      </c>
       <c r="T125" s="1" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="Z125" s="1"/>
       <c r="AA125" s="1"/>
@@ -8636,58 +8640,54 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="126">
       <c r="A126" s="9" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="C126" s="9"/>
       <c r="D126" s="9"/>
       <c r="E126" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F126" s="9"/>
+      <c r="F126" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="G126" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H126" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I126" s="7" t="s">
         <v>23</v>
       </c>
       <c r="J126" s="13" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="K126" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L126" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="M126" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="O126" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="P126" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q126" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R126" s="1" t="s">
         <v>500</v>
       </c>
-      <c r="M126" s="1" t="s">
+      <c r="T126" s="1" t="s">
         <v>501</v>
-      </c>
-      <c r="O126" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="P126" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="Q126" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="R126" s="1" t="s">
-        <v>503</v>
-      </c>
-      <c r="S126" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="T126" s="1" t="s">
-        <v>505</v>
-      </c>
-      <c r="U126" s="1" t="s">
-        <v>506</v>
       </c>
       <c r="Z126" s="1"/>
       <c r="AA126" s="1"/>
@@ -8710,10 +8710,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="127">
       <c r="A127" s="9" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="C127" s="9"/>
       <c r="D127" s="9"/>
@@ -8725,43 +8725,43 @@
         <v>23</v>
       </c>
       <c r="H127" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I127" s="7" t="s">
         <v>23</v>
       </c>
       <c r="J127" s="13" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="K127" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L127" s="1" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="M127" s="1" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="O127" s="1" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="P127" s="1" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="Q127" s="1" t="n">
         <v>2</v>
       </c>
       <c r="R127" s="1" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="S127" s="1" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="T127" s="1" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="U127" s="1" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="Z127" s="1"/>
       <c r="AA127" s="1"/>
@@ -8784,10 +8784,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="128">
       <c r="A128" s="9" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="B128" s="9" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="C128" s="9"/>
       <c r="D128" s="9"/>
@@ -8799,40 +8799,43 @@
         <v>23</v>
       </c>
       <c r="H128" s="9" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="I128" s="7" t="s">
         <v>23</v>
       </c>
       <c r="J128" s="13" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="K128" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L128" s="1" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="M128" s="1" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="O128" s="1" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="P128" s="1" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="Q128" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="R128" s="1" t="s">
+        <v>514</v>
+      </c>
       <c r="S128" s="1" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="T128" s="1" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="U128" s="1" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="Z128" s="1"/>
       <c r="AA128" s="1"/>
@@ -8855,10 +8858,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="129">
       <c r="A129" s="9" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="C129" s="9"/>
       <c r="D129" s="9"/>
@@ -8870,40 +8873,40 @@
         <v>23</v>
       </c>
       <c r="H129" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I129" s="7" t="s">
         <v>23</v>
       </c>
       <c r="J129" s="13" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="K129" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L129" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="M129" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="O129" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="P129" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="Q129" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="S129" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="M129" s="1" t="s">
+      <c r="T129" s="1" t="s">
         <v>523</v>
       </c>
-      <c r="O129" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="P129" s="1" t="s">
-        <v>524</v>
-      </c>
-      <c r="Q129" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="S129" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="T129" s="1" t="s">
-        <v>526</v>
-      </c>
       <c r="U129" s="1" t="s">
-        <v>527</v>
+        <v>517</v>
       </c>
       <c r="Z129" s="1"/>
       <c r="AA129" s="1"/>
@@ -8926,10 +8929,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="130">
       <c r="A130" s="9" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="C130" s="9"/>
       <c r="D130" s="9"/>
@@ -8941,43 +8944,40 @@
         <v>23</v>
       </c>
       <c r="H130" s="9" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I130" s="7" t="s">
         <v>23</v>
       </c>
       <c r="J130" s="13" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="K130" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L130" s="1" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="M130" s="1" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="O130" s="1" t="s">
         <v>329</v>
       </c>
       <c r="P130" s="1" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="Q130" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="R130" s="1" t="s">
-        <v>532</v>
+        <v>1</v>
       </c>
       <c r="S130" s="1" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="T130" s="1" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="U130" s="1" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="Z130" s="1"/>
       <c r="AA130" s="1"/>
@@ -9000,10 +9000,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="131">
       <c r="A131" s="9" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="C131" s="9"/>
       <c r="D131" s="9"/>
@@ -9015,43 +9015,43 @@
         <v>23</v>
       </c>
       <c r="H131" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I131" s="7" t="s">
         <v>23</v>
       </c>
       <c r="J131" s="13" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="K131" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L131" s="1" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="M131" s="1" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="O131" s="1" t="s">
         <v>329</v>
       </c>
       <c r="P131" s="1" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="Q131" s="1" t="n">
         <v>2</v>
       </c>
       <c r="R131" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="S131" s="1" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="T131" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="U131" s="1" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="Z131" s="1"/>
       <c r="AA131" s="1"/>
@@ -9074,10 +9074,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="132">
       <c r="A132" s="9" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="C132" s="9"/>
       <c r="D132" s="9"/>
@@ -9089,43 +9089,43 @@
         <v>23</v>
       </c>
       <c r="H132" s="9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I132" s="7" t="s">
         <v>23</v>
       </c>
       <c r="J132" s="13" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="K132" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L132" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="M132" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="O132" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="P132" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="Q132" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="R132" s="1" t="s">
         <v>541</v>
       </c>
-      <c r="M132" s="1" t="s">
+      <c r="S132" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="T132" s="1" t="s">
         <v>542</v>
       </c>
-      <c r="O132" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="P132" s="1" t="s">
-        <v>543</v>
-      </c>
-      <c r="Q132" s="1" t="s">
-        <v>544</v>
-      </c>
-      <c r="R132" s="1" t="s">
-        <v>545</v>
-      </c>
-      <c r="S132" s="1" t="s">
-        <v>546</v>
-      </c>
-      <c r="T132" s="1" t="s">
-        <v>547</v>
-      </c>
       <c r="U132" s="1" t="s">
-        <v>548</v>
+        <v>530</v>
       </c>
       <c r="Z132" s="1"/>
       <c r="AA132" s="1"/>
@@ -9148,10 +9148,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="133">
       <c r="A133" s="9" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="B133" s="9" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
       <c r="C133" s="9"/>
       <c r="D133" s="9"/>
@@ -9163,43 +9163,43 @@
         <v>23</v>
       </c>
       <c r="H133" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I133" s="7" t="s">
         <v>23</v>
       </c>
       <c r="J133" s="13" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="K133" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L133" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="M133" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="O133" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="P133" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="Q133" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="R133" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="S133" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="T133" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="M133" s="1" t="s">
+      <c r="U133" s="1" t="s">
         <v>551</v>
-      </c>
-      <c r="O133" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="P133" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="Q133" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="R133" s="1" t="s">
-        <v>538</v>
-      </c>
-      <c r="S133" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="T133" s="1" t="s">
-        <v>553</v>
-      </c>
-      <c r="U133" s="1" t="s">
-        <v>477</v>
       </c>
       <c r="Z133" s="1"/>
       <c r="AA133" s="1"/>
@@ -9222,10 +9222,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="134">
       <c r="A134" s="9" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="B134" s="9" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C134" s="9"/>
       <c r="D134" s="9"/>
@@ -9237,43 +9237,43 @@
         <v>23</v>
       </c>
       <c r="H134" s="9" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="I134" s="7" t="s">
         <v>23</v>
       </c>
       <c r="J134" s="13" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="K134" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L134" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="M134" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="O134" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="P134" s="1" t="s">
         <v>555</v>
       </c>
-      <c r="M134" s="1" t="s">
+      <c r="Q134" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="R134" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="S134" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="T134" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="O134" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="P134" s="1" t="s">
-        <v>557</v>
-      </c>
-      <c r="Q134" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="R134" s="1" t="s">
-        <v>558</v>
-      </c>
-      <c r="S134" s="1" t="s">
-        <v>559</v>
-      </c>
-      <c r="T134" s="1" t="s">
-        <v>560</v>
-      </c>
       <c r="U134" s="1" t="s">
-        <v>561</v>
+        <v>480</v>
       </c>
       <c r="Z134" s="1"/>
       <c r="AA134" s="1"/>
@@ -9296,10 +9296,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="135">
       <c r="A135" s="9" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="B135" s="9" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="C135" s="9"/>
       <c r="D135" s="9"/>
@@ -9311,40 +9311,43 @@
         <v>23</v>
       </c>
       <c r="H135" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I135" s="7" t="s">
         <v>23</v>
       </c>
       <c r="J135" s="13" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="K135" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L135" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="M135" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="O135" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="P135" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="Q135" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="R135" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="S135" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="T135" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="M135" s="1" t="s">
+      <c r="U135" s="1" t="s">
         <v>564</v>
-      </c>
-      <c r="O135" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="P135" s="1" t="s">
-        <v>565</v>
-      </c>
-      <c r="Q135" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="S135" s="1" t="s">
-        <v>566</v>
-      </c>
-      <c r="T135" s="1" t="s">
-        <v>567</v>
-      </c>
-      <c r="U135" s="1" t="s">
-        <v>568</v>
       </c>
       <c r="Z135" s="1"/>
       <c r="AA135" s="1"/>
@@ -9367,10 +9370,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="136">
       <c r="A136" s="9" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="B136" s="9" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="C136" s="9"/>
       <c r="D136" s="9"/>
@@ -9382,37 +9385,40 @@
         <v>23</v>
       </c>
       <c r="H136" s="9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="I136" s="7" t="s">
         <v>23</v>
       </c>
       <c r="J136" s="13" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="K136" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L136" s="1" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="M136" s="1" t="s">
-        <v>571</v>
+        <v>567</v>
+      </c>
+      <c r="O136" s="1" t="s">
+        <v>329</v>
       </c>
       <c r="P136" s="1" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="Q136" s="1" t="n">
         <v>2</v>
       </c>
       <c r="S136" s="1" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="T136" s="1" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="U136" s="1" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="Z136" s="1"/>
       <c r="AA136" s="1"/>
@@ -9434,54 +9440,53 @@
       <c r="AQ136" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="137">
-      <c r="A137" s="9"/>
+      <c r="A137" s="9" t="s">
+        <v>459</v>
+      </c>
       <c r="B137" s="9" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="C137" s="9"/>
-      <c r="D137" s="9" t="s">
-        <v>381</v>
-      </c>
-      <c r="E137" s="9"/>
+      <c r="D137" s="9"/>
+      <c r="E137" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="F137" s="9"/>
       <c r="G137" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H137" s="9" t="s">
-        <v>169</v>
+        <v>87</v>
       </c>
       <c r="I137" s="7" t="s">
         <v>23</v>
       </c>
       <c r="J137" s="13" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="K137" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L137" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="M137" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="P137" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="Q137" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="S137" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="T137" s="1" t="s">
         <v>577</v>
       </c>
-      <c r="M137" s="1" t="s">
+      <c r="U137" s="1" t="s">
         <v>578</v>
-      </c>
-      <c r="O137" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="P137" s="1" t="s">
-        <v>580</v>
-      </c>
-      <c r="Q137" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="S137" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="T137" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="U137" s="1" t="s">
-        <v>527</v>
       </c>
       <c r="Z137" s="1"/>
       <c r="AA137" s="1"/>
@@ -9505,7 +9510,7 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="138">
       <c r="A138" s="9"/>
       <c r="B138" s="9" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="C138" s="9"/>
       <c r="D138" s="9" t="s">
@@ -9523,34 +9528,34 @@
         <v>23</v>
       </c>
       <c r="J138" s="13" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="K138" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L138" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="M138" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="O138" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="P138" s="1" t="s">
         <v>583</v>
-      </c>
-      <c r="M138" s="1" t="s">
-        <v>584</v>
-      </c>
-      <c r="O138" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="P138" s="1" t="s">
-        <v>585</v>
       </c>
       <c r="Q138" s="1" t="n">
         <v>1</v>
       </c>
       <c r="S138" s="1" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="T138" s="1" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="U138" s="1" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="Z138" s="1"/>
       <c r="AA138" s="1"/>
@@ -9572,71 +9577,54 @@
       <c r="AQ138" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="139">
-      <c r="A139" s="1" t="s">
+      <c r="A139" s="9"/>
+      <c r="B139" s="9" t="s">
+        <v>585</v>
+      </c>
+      <c r="C139" s="9"/>
+      <c r="D139" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="E139" s="9"/>
+      <c r="F139" s="9"/>
+      <c r="G139" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H139" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="I139" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J139" s="13" t="s">
+        <v>461</v>
+      </c>
+      <c r="K139" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L139" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="M139" s="1" t="s">
         <v>587</v>
       </c>
-      <c r="B139" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C139" s="1" t="s">
+      <c r="O139" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="P139" s="1" t="s">
         <v>588</v>
-      </c>
-      <c r="E139" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F139" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G139" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H139" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I139" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J139" s="9" t="s">
-        <v>589</v>
-      </c>
-      <c r="K139" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="L139" s="1" t="s">
-        <v>590</v>
-      </c>
-      <c r="M139" s="1" t="s">
-        <v>591</v>
-      </c>
-      <c r="N139" s="1" t="s">
-        <v>592</v>
-      </c>
-      <c r="O139" s="1" t="s">
-        <v>593</v>
-      </c>
-      <c r="P139" s="1" t="s">
-        <v>594</v>
       </c>
       <c r="Q139" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="R139" s="1" t="s">
-        <v>595</v>
-      </c>
       <c r="S139" s="1" t="s">
-        <v>596</v>
-      </c>
-      <c r="V139" s="1" t="s">
-        <v>597</v>
-      </c>
-      <c r="W139" s="1" t="s">
-        <v>598</v>
-      </c>
-      <c r="X139" s="1" t="s">
-        <v>599</v>
-      </c>
-      <c r="Y139" s="1" t="s">
-        <v>600</v>
+        <v>528</v>
+      </c>
+      <c r="T139" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="U139" s="1" t="s">
+        <v>530</v>
       </c>
       <c r="Z139" s="1"/>
       <c r="AA139" s="1"/>
@@ -9659,52 +9647,70 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="140">
       <c r="A140" s="1" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>601</v>
+        <v>145</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>591</v>
       </c>
       <c r="E140" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G140" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H140" s="9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="I140" s="7" t="s">
         <v>23</v>
       </c>
       <c r="J140" s="9" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="K140" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L140" s="1" t="s">
-        <v>602</v>
+        <v>593</v>
       </c>
       <c r="M140" s="1" t="s">
-        <v>603</v>
+        <v>594</v>
       </c>
       <c r="N140" s="1" t="s">
-        <v>604</v>
+        <v>595</v>
       </c>
       <c r="O140" s="1" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="P140" s="1" t="s">
-        <v>469</v>
+        <v>597</v>
       </c>
       <c r="Q140" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R140" s="1" t="s">
-        <v>605</v>
+        <v>598</v>
+      </c>
+      <c r="S140" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="V140" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="W140" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="X140" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="Y140" s="1" t="s">
+        <v>603</v>
       </c>
       <c r="Z140" s="1"/>
       <c r="AA140" s="1"/>
@@ -9727,52 +9733,52 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="141">
       <c r="A141" s="1" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>478</v>
+        <v>604</v>
       </c>
       <c r="E141" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G141" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H141" s="9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I141" s="7" t="s">
         <v>23</v>
       </c>
       <c r="J141" s="9" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="K141" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L141" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="M141" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="M141" s="1" t="s">
+      <c r="N141" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="N141" s="1" t="s">
-        <v>481</v>
-      </c>
       <c r="O141" s="1" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="P141" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="Q141" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R141" s="1" t="s">
         <v>608</v>
-      </c>
-      <c r="Q141" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="R141" s="1" t="s">
-        <v>609</v>
       </c>
       <c r="Z141" s="1"/>
       <c r="AA141" s="1"/>
@@ -9795,46 +9801,52 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="142">
       <c r="A142" s="1" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="B142" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="E142" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F142" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G142" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H142" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="I142" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J142" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="K142" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L142" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="M142" s="1" t="s">
         <v>610</v>
       </c>
-      <c r="E142" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G142" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H142" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="I142" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J142" s="9" t="s">
-        <v>589</v>
-      </c>
-      <c r="K142" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="L142" s="1" t="s">
+      <c r="N142" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="O142" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="P142" s="1" t="s">
         <v>611</v>
-      </c>
-      <c r="M142" s="1" t="s">
-        <v>612</v>
-      </c>
-      <c r="O142" s="1" t="s">
-        <v>593</v>
-      </c>
-      <c r="P142" s="1" t="s">
-        <v>613</v>
       </c>
       <c r="Q142" s="1" t="n">
         <v>2</v>
       </c>
       <c r="R142" s="1" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="Z142" s="1"/>
       <c r="AA142" s="1"/>
@@ -9857,43 +9869,46 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="143">
       <c r="A143" s="1" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="B143" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="E143" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G143" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H143" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I143" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J143" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="K143" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L143" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="M143" s="1" t="s">
         <v>615</v>
       </c>
-      <c r="E143" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G143" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H143" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="I143" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J143" s="9" t="s">
-        <v>589</v>
-      </c>
-      <c r="K143" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="L143" s="1" t="s">
+      <c r="O143" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="P143" s="1" t="s">
         <v>616</v>
       </c>
-      <c r="M143" s="1" t="s">
+      <c r="Q143" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="R143" s="1" t="s">
         <v>617</v>
-      </c>
-      <c r="O143" s="1" t="s">
-        <v>618</v>
-      </c>
-      <c r="Q143" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="R143" s="1" t="s">
-        <v>619</v>
       </c>
       <c r="Z143" s="1"/>
       <c r="AA143" s="1"/>
@@ -9916,52 +9931,43 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="144">
       <c r="A144" s="1" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>102</v>
+        <v>618</v>
       </c>
       <c r="E144" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F144" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="G144" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H144" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I144" s="7" t="s">
         <v>23</v>
       </c>
       <c r="J144" s="9" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="K144" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L144" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="M144" s="1" t="s">
         <v>620</v>
       </c>
-      <c r="M144" s="1" t="s">
+      <c r="O144" s="1" t="s">
         <v>621</v>
-      </c>
-      <c r="N144" s="1" t="s">
-        <v>622</v>
-      </c>
-      <c r="O144" s="1" t="s">
-        <v>618</v>
-      </c>
-      <c r="P144" s="1" t="s">
-        <v>623</v>
       </c>
       <c r="Q144" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R144" s="1" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="Z144" s="1"/>
       <c r="AA144" s="1"/>
@@ -9984,61 +9990,52 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="145">
       <c r="A145" s="1" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="B145" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E145" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F145" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G145" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H145" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I145" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J145" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="K145" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L145" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="M145" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="N145" s="1" t="s">
         <v>625</v>
       </c>
-      <c r="E145" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G145" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H145" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="I145" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J145" s="9" t="s">
-        <v>589</v>
-      </c>
-      <c r="K145" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="L145" s="1" t="s">
+      <c r="O145" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="P145" s="1" t="s">
         <v>626</v>
-      </c>
-      <c r="M145" s="1" t="s">
-        <v>627</v>
-      </c>
-      <c r="O145" s="1" t="s">
-        <v>628</v>
-      </c>
-      <c r="P145" s="1" t="s">
-        <v>629</v>
       </c>
       <c r="Q145" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R145" s="1" t="s">
-        <v>630</v>
-      </c>
-      <c r="S145" s="1" t="s">
-        <v>631</v>
-      </c>
-      <c r="V145" s="1" t="s">
-        <v>632</v>
-      </c>
-      <c r="W145" s="1" t="s">
-        <v>633</v>
-      </c>
-      <c r="X145" s="1" t="s">
-        <v>634</v>
-      </c>
-      <c r="Y145" s="1" t="s">
-        <v>635</v>
+        <v>627</v>
       </c>
       <c r="Z145" s="1"/>
       <c r="AA145" s="1"/>
@@ -10061,10 +10058,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="146">
       <c r="A146" s="1" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>407</v>
+        <v>628</v>
       </c>
       <c r="E146" s="9" t="s">
         <v>23</v>
@@ -10073,37 +10070,49 @@
         <v>23</v>
       </c>
       <c r="H146" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I146" s="7" t="s">
         <v>23</v>
       </c>
       <c r="J146" s="9" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="K146" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L146" s="1" t="s">
-        <v>636</v>
+        <v>629</v>
       </c>
       <c r="M146" s="1" t="s">
-        <v>637</v>
+        <v>630</v>
       </c>
       <c r="O146" s="1" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="P146" s="1" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
       <c r="Q146" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R146" s="1" t="s">
-        <v>639</v>
+        <v>633</v>
+      </c>
+      <c r="S146" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="V146" s="1" t="s">
+        <v>635</v>
       </c>
       <c r="W146" s="1" t="s">
-        <v>640</v>
+        <v>636</v>
+      </c>
+      <c r="X146" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="Y146" s="1" t="s">
+        <v>638</v>
       </c>
       <c r="Z146" s="1"/>
       <c r="AA146" s="1"/>
@@ -10126,10 +10135,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="147">
       <c r="A147" s="1" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>493</v>
+        <v>410</v>
       </c>
       <c r="E147" s="9" t="s">
         <v>23</v>
@@ -10138,37 +10147,37 @@
         <v>23</v>
       </c>
       <c r="H147" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I147" s="7" t="s">
         <v>23</v>
       </c>
       <c r="J147" s="9" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="K147" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L147" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="M147" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="O147" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="P147" s="1" t="s">
         <v>641</v>
-      </c>
-      <c r="M147" s="1" t="s">
-        <v>642</v>
-      </c>
-      <c r="O147" s="1" t="s">
-        <v>628</v>
-      </c>
-      <c r="P147" s="1" t="s">
-        <v>643</v>
       </c>
       <c r="Q147" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R147" s="1" t="s">
-        <v>644</v>
-      </c>
-      <c r="U147" s="1" t="s">
-        <v>645</v>
+        <v>642</v>
+      </c>
+      <c r="W147" s="1" t="s">
+        <v>643</v>
       </c>
       <c r="Z147" s="1"/>
       <c r="AA147" s="1"/>
@@ -10191,58 +10200,49 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="148">
       <c r="A148" s="1" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="B148" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="E148" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G148" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H148" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="I148" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J148" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="K148" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L148" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="M148" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="O148" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="P148" s="1" t="s">
         <v>646</v>
-      </c>
-      <c r="E148" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F148" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G148" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H148" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="I148" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J148" s="9" t="s">
-        <v>589</v>
-      </c>
-      <c r="K148" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="L148" s="1" t="s">
-        <v>647</v>
-      </c>
-      <c r="M148" s="1" t="s">
-        <v>648</v>
-      </c>
-      <c r="O148" s="1" t="s">
-        <v>593</v>
-      </c>
-      <c r="P148" s="1" t="s">
-        <v>649</v>
       </c>
       <c r="Q148" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R148" s="1" t="s">
-        <v>650</v>
-      </c>
-      <c r="S148" s="1" t="s">
-        <v>651</v>
-      </c>
-      <c r="T148" s="1" t="s">
-        <v>652</v>
-      </c>
-      <c r="V148" s="1" t="s">
-        <v>653</v>
+        <v>647</v>
+      </c>
+      <c r="U148" s="1" t="s">
+        <v>648</v>
       </c>
       <c r="Z148" s="1"/>
       <c r="AA148" s="1"/>
@@ -10265,10 +10265,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="149">
       <c r="A149" s="1" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>654</v>
+        <v>649</v>
       </c>
       <c r="E149" s="9" t="s">
         <v>23</v>
@@ -10280,37 +10280,43 @@
         <v>23</v>
       </c>
       <c r="H149" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I149" s="7" t="s">
         <v>23</v>
       </c>
       <c r="J149" s="9" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="K149" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L149" s="1" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
       <c r="M149" s="1" t="s">
-        <v>656</v>
+        <v>651</v>
       </c>
       <c r="O149" s="1" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="P149" s="1" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="Q149" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="R149" s="1" t="s">
+        <v>653</v>
+      </c>
       <c r="S149" s="1" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="T149" s="1" t="s">
-        <v>659</v>
+        <v>655</v>
+      </c>
+      <c r="V149" s="1" t="s">
+        <v>656</v>
       </c>
       <c r="Z149" s="1"/>
       <c r="AA149" s="1"/>
@@ -10333,67 +10339,52 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="150">
       <c r="A150" s="1" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="B150" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="E150" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F150" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G150" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H150" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="I150" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J150" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="K150" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L150" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="M150" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="O150" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="P150" s="1" t="s">
         <v>660</v>
-      </c>
-      <c r="E150" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F150" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G150" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H150" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="I150" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J150" s="9" t="s">
-        <v>589</v>
-      </c>
-      <c r="K150" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="L150" s="1" t="s">
-        <v>661</v>
-      </c>
-      <c r="M150" s="1" t="s">
-        <v>662</v>
-      </c>
-      <c r="O150" s="1" t="s">
-        <v>593</v>
-      </c>
-      <c r="P150" s="1" t="s">
-        <v>663</v>
       </c>
       <c r="Q150" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="R150" s="1" t="s">
-        <v>664</v>
-      </c>
       <c r="S150" s="1" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
       <c r="T150" s="1" t="s">
-        <v>659</v>
-      </c>
-      <c r="V150" s="1" t="s">
-        <v>665</v>
-      </c>
-      <c r="W150" s="1" t="s">
-        <v>666</v>
-      </c>
-      <c r="X150" s="1" t="s">
-        <v>667</v>
-      </c>
-      <c r="Y150" s="1" t="s">
-        <v>668</v>
+        <v>662</v>
       </c>
       <c r="Z150" s="1"/>
       <c r="AA150" s="1"/>
@@ -10416,10 +10407,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="151">
       <c r="A151" s="1" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
       <c r="E151" s="9" t="s">
         <v>23</v>
@@ -10431,46 +10422,52 @@
         <v>23</v>
       </c>
       <c r="H151" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I151" s="7" t="s">
         <v>23</v>
       </c>
       <c r="J151" s="9" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="K151" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L151" s="1" t="s">
-        <v>670</v>
+        <v>664</v>
       </c>
       <c r="M151" s="1" t="s">
-        <v>671</v>
+        <v>665</v>
       </c>
       <c r="O151" s="1" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="P151" s="1" t="s">
-        <v>672</v>
+        <v>666</v>
       </c>
       <c r="Q151" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R151" s="1" t="s">
-        <v>673</v>
+        <v>667</v>
       </c>
       <c r="S151" s="1" t="s">
-        <v>674</v>
+        <v>661</v>
       </c>
       <c r="T151" s="1" t="s">
-        <v>675</v>
-      </c>
-      <c r="U151" s="1" t="s">
-        <v>676</v>
+        <v>662</v>
+      </c>
+      <c r="V151" s="1" t="s">
+        <v>668</v>
       </c>
       <c r="W151" s="1" t="s">
-        <v>677</v>
+        <v>669</v>
+      </c>
+      <c r="X151" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="Y151" s="1" t="s">
+        <v>671</v>
       </c>
       <c r="Z151" s="1"/>
       <c r="AA151" s="1"/>
@@ -10493,49 +10490,61 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="152">
       <c r="A152" s="1" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="B152" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="E152" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F152" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G152" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H152" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="I152" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J152" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="K152" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L152" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="M152" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="O152" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="P152" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="Q152" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R152" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="S152" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="T152" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="E152" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G152" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H152" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="I152" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J152" s="9" t="s">
-        <v>589</v>
-      </c>
-      <c r="K152" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="L152" s="1" t="s">
+      <c r="U152" s="1" t="s">
         <v>679</v>
       </c>
-      <c r="M152" s="1" t="s">
+      <c r="W152" s="1" t="s">
         <v>680</v>
-      </c>
-      <c r="O152" s="1" t="s">
-        <v>681</v>
-      </c>
-      <c r="P152" s="1" t="s">
-        <v>682</v>
-      </c>
-      <c r="Q152" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="R152" s="1" t="s">
-        <v>683</v>
-      </c>
-      <c r="U152" s="1" t="s">
-        <v>684</v>
       </c>
       <c r="Z152" s="1"/>
       <c r="AA152" s="1"/>
@@ -10558,67 +10567,49 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="153">
       <c r="A153" s="1" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="B153" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="E153" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G153" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H153" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="I153" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J153" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="K153" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L153" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="M153" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="O153" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="P153" s="1" t="s">
         <v>685</v>
       </c>
-      <c r="E153" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F153" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G153" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H153" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="I153" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J153" s="9" t="s">
-        <v>589</v>
-      </c>
-      <c r="K153" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="L153" s="1" t="s">
+      <c r="Q153" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="R153" s="1" t="s">
         <v>686</v>
       </c>
-      <c r="M153" s="1" t="s">
+      <c r="U153" s="1" t="s">
         <v>687</v>
-      </c>
-      <c r="O153" s="1" t="s">
-        <v>593</v>
-      </c>
-      <c r="P153" s="1" t="s">
-        <v>688</v>
-      </c>
-      <c r="Q153" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="R153" s="1" t="s">
-        <v>689</v>
-      </c>
-      <c r="S153" s="1" t="s">
-        <v>690</v>
-      </c>
-      <c r="T153" s="1" t="s">
-        <v>691</v>
-      </c>
-      <c r="U153" s="1" t="s">
-        <v>692</v>
-      </c>
-      <c r="V153" s="1" t="s">
-        <v>693</v>
-      </c>
-      <c r="W153" s="1" t="s">
-        <v>694</v>
-      </c>
-      <c r="Y153" s="1" t="s">
-        <v>695</v>
       </c>
       <c r="Z153" s="1"/>
       <c r="AA153" s="1"/>
@@ -10641,52 +10632,67 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="154">
       <c r="A154" s="1" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="B154" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="E154" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G154" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H154" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="I154" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J154" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="K154" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L154" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="M154" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="O154" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="P154" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="Q154" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R154" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="S154" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="T154" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="U154" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="V154" s="1" t="s">
         <v>696</v>
       </c>
-      <c r="E154" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G154" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H154" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="I154" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J154" s="9" t="s">
-        <v>589</v>
-      </c>
-      <c r="K154" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="L154" s="1" t="s">
+      <c r="W154" s="1" t="s">
         <v>697</v>
       </c>
-      <c r="M154" s="1" t="s">
+      <c r="Y154" s="1" t="s">
         <v>698</v>
-      </c>
-      <c r="O154" s="1" t="s">
-        <v>593</v>
-      </c>
-      <c r="P154" s="1" t="s">
-        <v>699</v>
-      </c>
-      <c r="Q154" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="R154" s="1" t="s">
-        <v>700</v>
-      </c>
-      <c r="S154" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="U154" s="1" t="s">
-        <v>702</v>
       </c>
       <c r="Z154" s="1"/>
       <c r="AA154" s="1"/>
@@ -10707,63 +10713,54 @@
       <c r="AP154" s="1"/>
       <c r="AQ154" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="86.25" outlineLevel="0" r="155">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="155">
       <c r="A155" s="1" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="B155" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="E155" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G155" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H155" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="I155" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J155" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="K155" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L155" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="M155" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="O155" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="P155" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="Q155" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="R155" s="1" t="s">
         <v>703</v>
       </c>
-      <c r="E155" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G155" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H155" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="I155" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J155" s="9" t="s">
-        <v>589</v>
-      </c>
-      <c r="K155" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="L155" s="1" t="s">
+      <c r="S155" s="1" t="s">
         <v>704</v>
       </c>
-      <c r="M155" s="1" t="s">
+      <c r="U155" s="1" t="s">
         <v>705</v>
-      </c>
-      <c r="O155" s="1" t="s">
-        <v>593</v>
-      </c>
-      <c r="P155" s="1" t="s">
-        <v>706</v>
-      </c>
-      <c r="Q155" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="S155" s="14" t="s">
-        <v>707</v>
-      </c>
-      <c r="T155" s="1" t="s">
-        <v>527</v>
-      </c>
-      <c r="U155" s="1" t="s">
-        <v>708</v>
-      </c>
-      <c r="V155" s="1" t="s">
-        <v>709</v>
-      </c>
-      <c r="W155" s="1" t="s">
-        <v>710</v>
-      </c>
-      <c r="Y155" s="1" t="s">
-        <v>711</v>
       </c>
       <c r="Z155" s="1"/>
       <c r="AA155" s="1"/>
@@ -10784,12 +10781,12 @@
       <c r="AP155" s="1"/>
       <c r="AQ155" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="150" outlineLevel="0" r="156">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="86.25" outlineLevel="0" r="156">
       <c r="A156" s="1" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>712</v>
+        <v>706</v>
       </c>
       <c r="E156" s="9" t="s">
         <v>23</v>
@@ -10798,43 +10795,49 @@
         <v>23</v>
       </c>
       <c r="H156" s="9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="I156" s="7" t="s">
         <v>23</v>
       </c>
       <c r="J156" s="9" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="K156" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L156" s="1" t="s">
-        <v>713</v>
+        <v>707</v>
       </c>
       <c r="M156" s="1" t="s">
-        <v>714</v>
+        <v>708</v>
       </c>
       <c r="O156" s="1" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="P156" s="1" t="s">
-        <v>715</v>
+        <v>709</v>
       </c>
       <c r="Q156" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="R156" s="1" t="s">
-        <v>716</v>
-      </c>
       <c r="S156" s="14" t="s">
-        <v>717</v>
+        <v>710</v>
       </c>
       <c r="T156" s="1" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="U156" s="1" t="s">
-        <v>718</v>
+        <v>711</v>
+      </c>
+      <c r="V156" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="W156" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="Y156" s="1" t="s">
+        <v>714</v>
       </c>
       <c r="Z156" s="1"/>
       <c r="AA156" s="1"/>
@@ -10855,57 +10858,57 @@
       <c r="AP156" s="1"/>
       <c r="AQ156" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="157">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="150" outlineLevel="0" r="157">
       <c r="A157" s="1" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="B157" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="E157" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G157" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H157" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="I157" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J157" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="K157" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L157" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="M157" s="1" t="s">
+        <v>717</v>
+      </c>
+      <c r="O157" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="P157" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="Q157" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R157" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="E157" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G157" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H157" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="I157" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J157" s="9" t="s">
-        <v>589</v>
-      </c>
-      <c r="K157" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="L157" s="1" t="s">
+      <c r="S157" s="14" t="s">
         <v>720</v>
       </c>
-      <c r="M157" s="1" t="s">
+      <c r="T157" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="U157" s="1" t="s">
         <v>721</v>
-      </c>
-      <c r="O157" s="1" t="s">
-        <v>593</v>
-      </c>
-      <c r="P157" s="1" t="s">
-        <v>722</v>
-      </c>
-      <c r="Q157" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="R157" s="1" t="s">
-        <v>723</v>
-      </c>
-      <c r="S157" s="1" t="s">
-        <v>724</v>
-      </c>
-      <c r="U157" s="1" t="s">
-        <v>645</v>
-      </c>
-      <c r="V157" s="1" t="s">
-        <v>725</v>
       </c>
       <c r="Z157" s="1"/>
       <c r="AA157" s="1"/>
@@ -10926,12 +10929,12 @@
       <c r="AP157" s="1"/>
       <c r="AQ157" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="96.85" outlineLevel="0" r="158">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="158">
       <c r="A158" s="1" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="E158" s="9" t="s">
         <v>23</v>
@@ -10940,46 +10943,43 @@
         <v>23</v>
       </c>
       <c r="H158" s="9" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I158" s="7" t="s">
         <v>23</v>
       </c>
       <c r="J158" s="9" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="K158" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L158" s="1" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="M158" s="1" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
       <c r="O158" s="1" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="P158" s="1" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="Q158" s="1" t="n">
         <v>2</v>
       </c>
       <c r="R158" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="S158" s="14" t="s">
-        <v>731</v>
-      </c>
-      <c r="T158" s="1" t="s">
-        <v>527</v>
+        <v>726</v>
+      </c>
+      <c r="S158" s="1" t="s">
+        <v>727</v>
       </c>
       <c r="U158" s="1" t="s">
-        <v>732</v>
-      </c>
-      <c r="Y158" s="1" t="s">
-        <v>733</v>
+        <v>648</v>
+      </c>
+      <c r="V158" s="1" t="s">
+        <v>728</v>
       </c>
       <c r="Z158" s="1"/>
       <c r="AA158" s="1"/>
@@ -11000,57 +11000,60 @@
       <c r="AP158" s="1"/>
       <c r="AQ158" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="159">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="96.85" outlineLevel="0" r="159">
       <c r="A159" s="1" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="B159" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="E159" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G159" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H159" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="I159" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J159" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="K159" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L159" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="M159" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="O159" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="P159" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="Q159" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="R159" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="S159" s="14" t="s">
         <v>734</v>
       </c>
-      <c r="E159" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G159" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H159" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="I159" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J159" s="9" t="s">
-        <v>589</v>
-      </c>
-      <c r="K159" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="L159" s="1" t="s">
+      <c r="T159" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="U159" s="1" t="s">
         <v>735</v>
       </c>
-      <c r="M159" s="1" t="s">
+      <c r="Y159" s="1" t="s">
         <v>736</v>
-      </c>
-      <c r="O159" s="1" t="s">
-        <v>628</v>
-      </c>
-      <c r="P159" s="1" t="s">
-        <v>737</v>
-      </c>
-      <c r="Q159" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="R159" s="1" t="s">
-        <v>738</v>
-      </c>
-      <c r="S159" s="1" t="s">
-        <v>739</v>
-      </c>
-      <c r="U159" s="1" t="s">
-        <v>740</v>
-      </c>
-      <c r="W159" s="1" t="s">
-        <v>741</v>
       </c>
       <c r="Z159" s="1"/>
       <c r="AA159" s="1"/>
@@ -11073,49 +11076,55 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="160">
       <c r="A160" s="1" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="B160" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="E160" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G160" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H160" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="I160" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J160" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="K160" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L160" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="M160" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="O160" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="P160" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="Q160" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R160" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="S160" s="1" t="s">
         <v>742</v>
       </c>
-      <c r="E160" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G160" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H160" s="9" t="s">
-        <v>285</v>
-      </c>
-      <c r="I160" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J160" s="9" t="s">
-        <v>589</v>
-      </c>
-      <c r="K160" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="L160" s="1" t="s">
+      <c r="U160" s="1" t="s">
         <v>743</v>
       </c>
-      <c r="M160" s="1" t="s">
+      <c r="W160" s="1" t="s">
         <v>744</v>
-      </c>
-      <c r="O160" s="1" t="s">
-        <v>593</v>
-      </c>
-      <c r="P160" s="1" t="s">
-        <v>745</v>
-      </c>
-      <c r="Q160" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="R160" s="1" t="s">
-        <v>746</v>
-      </c>
-      <c r="U160" s="1" t="s">
-        <v>747</v>
       </c>
       <c r="Z160" s="1"/>
       <c r="AA160" s="1"/>
@@ -11138,55 +11147,49 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="161">
       <c r="A161" s="1" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="B161" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="E161" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G161" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H161" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="I161" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J161" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="K161" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L161" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="M161" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="O161" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="P161" s="1" t="s">
         <v>748</v>
       </c>
-      <c r="E161" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G161" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H161" s="9" t="s">
-        <v>290</v>
-      </c>
-      <c r="I161" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J161" s="9" t="s">
-        <v>589</v>
-      </c>
-      <c r="K161" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="L161" s="1" t="s">
+      <c r="Q161" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="R161" s="1" t="s">
         <v>749</v>
       </c>
-      <c r="M161" s="1" t="s">
+      <c r="U161" s="1" t="s">
         <v>750</v>
-      </c>
-      <c r="O161" s="1" t="s">
-        <v>593</v>
-      </c>
-      <c r="P161" s="1" t="s">
-        <v>751</v>
-      </c>
-      <c r="Q161" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="R161" s="1" t="s">
-        <v>752</v>
-      </c>
-      <c r="S161" s="1" t="s">
-        <v>753</v>
-      </c>
-      <c r="T161" s="1" t="s">
-        <v>754</v>
-      </c>
-      <c r="U161" s="1" t="s">
-        <v>755</v>
       </c>
       <c r="Z161" s="1"/>
       <c r="AA161" s="1"/>
@@ -11209,58 +11212,55 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="162">
       <c r="A162" s="1" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="B162" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="E162" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G162" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H162" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="I162" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J162" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="K162" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L162" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="M162" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="O162" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="P162" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="Q162" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R162" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="S162" s="1" t="s">
         <v>756</v>
       </c>
-      <c r="E162" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G162" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H162" s="9" t="s">
-        <v>434</v>
-      </c>
-      <c r="I162" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J162" s="9" t="s">
-        <v>589</v>
-      </c>
-      <c r="K162" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="L162" s="1" t="s">
+      <c r="T162" s="1" t="s">
         <v>757</v>
       </c>
-      <c r="M162" s="1" t="s">
+      <c r="U162" s="1" t="s">
         <v>758</v>
-      </c>
-      <c r="O162" s="1" t="s">
-        <v>593</v>
-      </c>
-      <c r="P162" s="1" t="s">
-        <v>759</v>
-      </c>
-      <c r="Q162" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="R162" s="1" t="s">
-        <v>760</v>
-      </c>
-      <c r="S162" s="1" t="s">
-        <v>761</v>
-      </c>
-      <c r="T162" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="U162" s="1" t="s">
-        <v>762</v>
-      </c>
-      <c r="V162" s="1" t="s">
-        <v>763</v>
       </c>
       <c r="Z162" s="1"/>
       <c r="AA162" s="1"/>
@@ -11283,10 +11283,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="163">
       <c r="A163" s="1" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>764</v>
+        <v>759</v>
       </c>
       <c r="E163" s="9" t="s">
         <v>23</v>
@@ -11295,46 +11295,46 @@
         <v>23</v>
       </c>
       <c r="H163" s="9" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="I163" s="7" t="s">
         <v>23</v>
       </c>
       <c r="J163" s="9" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="K163" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L163" s="1" t="s">
-        <v>765</v>
+        <v>760</v>
       </c>
       <c r="M163" s="1" t="s">
-        <v>766</v>
+        <v>761</v>
       </c>
       <c r="O163" s="1" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="P163" s="1" t="s">
-        <v>767</v>
+        <v>762</v>
       </c>
       <c r="Q163" s="1" t="n">
         <v>2</v>
       </c>
       <c r="R163" s="1" t="s">
-        <v>768</v>
+        <v>763</v>
       </c>
       <c r="S163" s="1" t="s">
-        <v>769</v>
+        <v>764</v>
+      </c>
+      <c r="T163" s="1" t="s">
+        <v>480</v>
       </c>
       <c r="U163" s="1" t="s">
-        <v>770</v>
+        <v>765</v>
       </c>
       <c r="V163" s="1" t="s">
-        <v>771</v>
-      </c>
-      <c r="Y163" s="1" t="s">
-        <v>772</v>
+        <v>766</v>
       </c>
       <c r="Z163" s="1"/>
       <c r="AA163" s="1"/>
@@ -11355,6 +11355,80 @@
       <c r="AP163" s="1"/>
       <c r="AQ163" s="1"/>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="164">
+      <c r="A164" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="E164" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G164" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H164" s="9" t="s">
+        <v>442</v>
+      </c>
+      <c r="I164" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J164" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="K164" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L164" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="M164" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="O164" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="P164" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="Q164" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="R164" s="1" t="s">
+        <v>771</v>
+      </c>
+      <c r="S164" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="U164" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="V164" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="Y164" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="Z164" s="1"/>
+      <c r="AA164" s="1"/>
+      <c r="AB164" s="1"/>
+      <c r="AC164" s="1"/>
+      <c r="AD164" s="1"/>
+      <c r="AE164" s="1"/>
+      <c r="AF164" s="1"/>
+      <c r="AG164" s="1"/>
+      <c r="AH164" s="1"/>
+      <c r="AI164" s="1"/>
+      <c r="AJ164" s="1"/>
+      <c r="AK164" s="1"/>
+      <c r="AL164" s="1"/>
+      <c r="AM164" s="1"/>
+      <c r="AN164" s="1"/>
+      <c r="AO164" s="1"/>
+      <c r="AP164" s="1"/>
+      <c r="AQ164" s="1"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink display="The version of the LINCS Data Working Group Standards Document from which this column definition was taken.  See https://sites.google.com/site/lincsdwgdevelopment/standards-and-use" ref="P11" r:id="rId1"/>

</xml_diff>

<commit_message>
change "endpoint" terminology for fieldinformation re #175
</commit_message>
<xml_diff>
--- a/sampledata/fieldinformation.xlsx
+++ b/sampledata/fieldinformation.xlsx
@@ -719,19 +719,19 @@
     <t>datacolumn</t>
   </si>
   <si>
-    <t>Endpoint Name</t>
+    <t>Datapoint Name</t>
   </si>
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>The name given to the endpoint</t>
+    <t>The name given to the data point</t>
   </si>
   <si>
     <t>unit</t>
   </si>
   <si>
-    <t>Endpoint Unit</t>
+    <t>Datapoint Unit</t>
   </si>
   <si>
     <t>Unit</t>
@@ -812,16 +812,16 @@
     <t>The order in which this endpoint should be displayed in an ordered list of endpoints</t>
   </si>
   <si>
-    <t>endpoint_value</t>
-  </si>
-  <si>
-    <t>Endpoint Value</t>
+    <t>datapoint_value</t>
+  </si>
+  <si>
+    <t>Datapoint Value</t>
   </si>
   <si>
     <t>Value</t>
   </si>
   <si>
-    <t>The measured or derived value included in the dataset</t>
+    <t>The measured, derived, or recorded value included in the dataset</t>
   </si>
   <si>
     <t>timepoint</t>
@@ -854,16 +854,16 @@
     <t>Description of this timepoint</t>
   </si>
   <si>
-    <t>endpoint_file</t>
-  </si>
-  <si>
-    <t>endpointFile</t>
-  </si>
-  <si>
-    <t>Endpoint File</t>
-  </si>
-  <si>
-    <t>URI for the endpoint (results) resource for this dataset</t>
+    <t>datapoint_file</t>
+  </si>
+  <si>
+    <t>datapointFile</t>
+  </si>
+  <si>
+    <t>Datapoint File</t>
+  </si>
+  <si>
+    <t>URI for the datapoint (results datacolumns and associated data columns) resource for this dataset</t>
   </si>
   <si>
     <t>saf_version</t>
@@ -2509,7 +2509,7 @@
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -2522,29 +2522,29 @@
   <dimension ref="A1:AQ164"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <pane activePane="bottomRight" topLeftCell="A93" xSplit="3204" ySplit="1978"/>
+      <pane activePane="bottomRight" topLeftCell="J67" xSplit="3356" ySplit="1978"/>
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-      <selection activeCell="A1" activeCellId="0" pane="topRight" sqref="A1"/>
-      <selection activeCell="A93" activeCellId="0" pane="bottomLeft" sqref="A93"/>
-      <selection activeCell="E103" activeCellId="0" pane="bottomRight" sqref="E103"/>
+      <selection activeCell="J1" activeCellId="0" pane="topRight" sqref="J1"/>
+      <selection activeCell="A67" activeCellId="0" pane="bottomLeft" sqref="A67"/>
+      <selection activeCell="P68" activeCellId="0" pane="bottomRight" sqref="P68"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.0078431372549"/>
-    <col collapsed="false" hidden="false" max="9" min="3" style="1" width="11.4862745098039"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="2" width="11.4862745098039"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.4862745098039"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="29.7019607843137"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="1" width="27.3764705882353"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="58.8980392156863"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="16"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="47.4196078431373"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="14.7882352941176"/>
-    <col collapsed="false" hidden="false" max="21" min="20" style="1" width="22.8470588235294"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="22.7294117647059"/>
-    <col collapsed="false" hidden="false" max="25" min="23" style="1" width="9.92156862745098"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="9.92156862745098"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.2352941176471"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.1529411764706"/>
+    <col collapsed="false" hidden="false" max="9" min="3" style="1" width="11.5960784313726"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="2" width="11.5960784313726"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.5960784313726"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="30.0078431372549"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="1" width="27.6470588235294"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="59.4941176470588"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="16.1607843137255"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="47.8901960784314"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="14.9333333333333"/>
+    <col collapsed="false" hidden="false" max="21" min="20" style="1" width="23.0823529411765"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="22.9647058823529"/>
+    <col collapsed="false" hidden="false" max="25" min="23" style="1" width="10.0196078431373"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="10.0196078431373"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="67.5" outlineLevel="0" r="1" s="6">
@@ -3613,7 +3613,7 @@
       <c r="AF24" s="1"/>
       <c r="AG24" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.1" outlineLevel="0" r="25">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="25">
       <c r="A25" s="9" t="s">
         <v>101</v>
       </c>
@@ -3654,7 +3654,7 @@
       <c r="AF25" s="1"/>
       <c r="AG25" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.1" outlineLevel="0" r="26">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="A26" s="9" t="s">
         <v>101</v>
       </c>
@@ -3779,7 +3779,7 @@
       <c r="AF28" s="1"/>
       <c r="AG28" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.1" outlineLevel="0" r="29">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
       <c r="A29" s="9" t="s">
         <v>101</v>
       </c>
@@ -3820,7 +3820,7 @@
       <c r="AF29" s="1"/>
       <c r="AG29" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.1" outlineLevel="0" r="30">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
       <c r="A30" s="9" t="s">
         <v>101</v>
       </c>

</xml_diff>

<commit_message>
Show the Library full name instead of the short name
</commit_message>
<xml_diff>
--- a/sampledata/fieldinformation.xlsx
+++ b/sampledata/fieldinformation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2001" uniqueCount="779">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2002" uniqueCount="779">
   <si>
     <t>table</t>
   </si>
@@ -2532,11 +2532,11 @@
   <dimension ref="A1:AQ164"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <pane activePane="bottomLeft" topLeftCell="A39" xSplit="3830" ySplit="1925"/>
+      <pane activePane="bottomRight" topLeftCell="A21" xSplit="3830" ySplit="1925"/>
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
       <selection activeCell="A1" activeCellId="0" pane="topRight" sqref="A1"/>
-      <selection activeCell="A78" activeCellId="0" pane="bottomLeft" sqref="A78"/>
-      <selection activeCell="A39" activeCellId="0" pane="bottomRight" sqref="A39"/>
+      <selection activeCell="A21" activeCellId="0" pane="bottomLeft" sqref="A21"/>
+      <selection activeCell="F40" activeCellId="0" pane="bottomRight" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -4190,6 +4190,9 @@
       <c r="E38" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="F38" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="G38" s="1" t="s">
         <v>24</v>
       </c>
@@ -4231,7 +4234,7 @@
         <v>23</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
dataset UI improvements - download link on detail pages for proteins,cells,sm's,dc's - show the cells, proteins columns only if records have cells, proteins;   but not if cells, proteins are referenced only from a datacolumn - cleanup in api.py only
</commit_message>
<xml_diff>
--- a/sampledata/fieldinformation.xlsx
+++ b/sampledata/fieldinformation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2021" uniqueCount="780">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2022" uniqueCount="780">
   <si>
     <t>table</t>
   </si>
@@ -2521,7 +2521,7 @@
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -2534,29 +2534,29 @@
   <dimension ref="A1:AQ166"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <pane activePane="bottomRight" topLeftCell="A59" xSplit="3336" ySplit="1910"/>
+      <pane activePane="bottomRight" topLeftCell="A26" xSplit="3441" ySplit="1896"/>
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
       <selection activeCell="A1" activeCellId="0" pane="topRight" sqref="A1"/>
-      <selection activeCell="A59" activeCellId="0" pane="bottomLeft" sqref="A59"/>
-      <selection activeCell="B80" activeCellId="0" pane="bottomRight" sqref="B80"/>
+      <selection activeCell="A26" activeCellId="0" pane="bottomLeft" sqref="A26"/>
+      <selection activeCell="F46" activeCellId="0" pane="bottomRight" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.8235294117647"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.5176470588235"/>
-    <col collapsed="false" hidden="false" max="9" min="3" style="1" width="11.8941176470588"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="2" width="11.8941176470588"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.8941176470588"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="30.7764705882353"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="1" width="28.3372549019608"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="60.9960784313726"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="16.5686274509804"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="49.0941176470588"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="15.3019607843137"/>
-    <col collapsed="false" hidden="false" max="21" min="20" style="1" width="23.6705882352941"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="23.5529411764706"/>
-    <col collapsed="false" hidden="false" max="25" min="23" style="1" width="10.2823529411765"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="8.68235294117647"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.9411764705882"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.5882352941176"/>
+    <col collapsed="false" hidden="false" max="9" min="3" style="1" width="11.956862745098"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="2" width="11.956862745098"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.956862745098"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="30.9333333333333"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="1" width="28.4823529411765"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="61.3019607843137"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="16.6509803921569"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="49.3372549019608"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="15.3764705882353"/>
+    <col collapsed="false" hidden="false" max="21" min="20" style="1" width="23.7882352941176"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="23.6705882352941"/>
+    <col collapsed="false" hidden="false" max="25" min="23" style="1" width="10.3294117647059"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="8.72941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="67.5" outlineLevel="0" r="1" s="6">
@@ -4469,6 +4469,9 @@
       <c r="E45" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="F45" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="G45" s="9" t="s">
         <v>24</v>
       </c>
@@ -5337,7 +5340,7 @@
       <c r="AF65" s="1"/>
       <c r="AG65" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="66">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="66">
       <c r="A66" s="1" t="s">
         <v>220</v>
       </c>
@@ -5601,7 +5604,7 @@
       <c r="AF71" s="1"/>
       <c r="AG71" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="72">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="72">
       <c r="A72" s="1" t="s">
         <v>231</v>
       </c>
@@ -5644,7 +5647,7 @@
       <c r="AF72" s="1"/>
       <c r="AG72" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="73">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="73">
       <c r="A73" s="1" t="s">
         <v>231</v>
       </c>
@@ -5687,7 +5690,7 @@
       <c r="AF73" s="1"/>
       <c r="AG73" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="74">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="74">
       <c r="A74" s="1" t="s">
         <v>231</v>
       </c>
@@ -5730,7 +5733,7 @@
       <c r="AF74" s="1"/>
       <c r="AG74" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="75">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="75">
       <c r="A75" s="1" t="s">
         <v>231</v>
       </c>
@@ -5773,7 +5776,7 @@
       <c r="AF75" s="1"/>
       <c r="AG75" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="76">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="76">
       <c r="A76" s="1" t="s">
         <v>231</v>
       </c>
@@ -5816,7 +5819,7 @@
       <c r="AF76" s="1"/>
       <c r="AG76" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="77">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="77">
       <c r="A77" s="1" t="s">
         <v>231</v>
       </c>
@@ -5859,7 +5862,7 @@
       <c r="AF77" s="1"/>
       <c r="AG77" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="78">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="78">
       <c r="A78" s="1" t="s">
         <v>231</v>
       </c>
@@ -5902,7 +5905,7 @@
       <c r="AF78" s="1"/>
       <c r="AG78" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="79">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="79">
       <c r="A79" s="1" t="s">
         <v>231</v>
       </c>
@@ -5945,7 +5948,7 @@
       <c r="AF79" s="1"/>
       <c r="AG79" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="80">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="80">
       <c r="B80" s="1" t="s">
         <v>268</v>
       </c>
@@ -5988,7 +5991,7 @@
       <c r="AF80" s="1"/>
       <c r="AG80" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="81">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="81">
       <c r="B81" s="1" t="s">
         <v>272</v>
       </c>
@@ -6023,7 +6026,7 @@
         <v>274</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="82">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="82">
       <c r="B82" s="1" t="s">
         <v>275</v>
       </c>
@@ -6058,7 +6061,7 @@
         <v>277</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="83">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="83">
       <c r="B83" s="1" t="s">
         <v>278</v>
       </c>
@@ -6093,7 +6096,7 @@
         <v>281</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="84">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="84">
       <c r="B84" s="1" t="s">
         <v>282</v>
       </c>
@@ -6128,7 +6131,7 @@
         <v>285</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="85">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="85">
       <c r="B85" s="1" t="s">
         <v>286</v>
       </c>
@@ -6163,7 +6166,7 @@
         <v>290</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="86">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="86">
       <c r="B86" s="1" t="s">
         <v>291</v>
       </c>

</xml_diff>

<commit_message>
further fix of restricted property visibility - restricted fields not shown by default for all views - use get_property(is_authenticated) for restricted fields on export - fix csv export broken in last commit - fix detail views to show fields in unrestricted instances (or for authenticated users) - update of field information to conform to "private" field naming
</commit_message>
<xml_diff>
--- a/sampledata/fieldinformation.xlsx
+++ b/sampledata/fieldinformation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2022" uniqueCount="780">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2027" uniqueCount="788">
   <si>
     <t>table</t>
   </si>
@@ -1073,7 +1073,10 @@
     <t>http://www.ebi.ac.uk/chebi/</t>
   </si>
   <si>
-    <t>molecular_mass</t>
+    <t>_molecular_mass</t>
+  </si>
+  <si>
+    <t>get_molecular_mass</t>
   </si>
   <si>
     <t>SM:21</t>
@@ -1088,7 +1091,10 @@
     <t>this includes salts and addends and no structure canonicalization; full structure</t>
   </si>
   <si>
-    <t>molecular_formula</t>
+    <t>_molecular_formula</t>
+  </si>
+  <si>
+    <t>get_molecular_formula</t>
   </si>
   <si>
     <t>SM:22</t>
@@ -1100,214 +1106,232 @@
     <t>String representation of the compound with addends; type and number of the different atoms in the compound; without structural details</t>
   </si>
   <si>
+    <t>_smiles</t>
+  </si>
+  <si>
+    <t>get_smiles</t>
+  </si>
+  <si>
+    <t>SM:14</t>
+  </si>
+  <si>
+    <t>SM_SMILES_Parent</t>
+  </si>
+  <si>
+    <t>SMILES</t>
+  </si>
+  <si>
+    <t>Canonical SMILES representation of parent (standardized) chemical structure generated by LINCS business rules</t>
+  </si>
+  <si>
+    <t>standardized small molecule representation; documented standardization protocol</t>
+  </si>
+  <si>
+    <t>_inchi</t>
+  </si>
+  <si>
+    <t>get_inchi</t>
+  </si>
+  <si>
+    <t>SM:12</t>
+  </si>
+  <si>
+    <t>SM_InChi_Parent</t>
+  </si>
+  <si>
+    <t>InChi</t>
+  </si>
+  <si>
+    <t>InChi representation of parent (standardized) chemical structure chemical structure generated by LINCS business rules</t>
+  </si>
+  <si>
+    <t>_inchi_key</t>
+  </si>
+  <si>
+    <t>get_inchi_key</t>
+  </si>
+  <si>
+    <t>SM:13</t>
+  </si>
+  <si>
+    <t>SM_InChi_Key_Parent</t>
+  </si>
+  <si>
+    <t>InChi Key</t>
+  </si>
+  <si>
+    <t>InChi key of parent (standardized) chemical structure generated by LINCS business rules</t>
+  </si>
+  <si>
+    <t>derived from InChi</t>
+  </si>
+  <si>
+    <t>chembl_id</t>
+  </si>
+  <si>
+    <t>ChEMBL ID</t>
+  </si>
+  <si>
+    <t>ChEMBL is a database of bioactive drug-like small molecules, it contains 2-D structures, calculated properties (e.g. logP, Molecular Weight, Lipinski Parameters, etc.) and abstracted bioactivities (e.g. binding constants, pharmacology and ADMET data)</t>
+  </si>
+  <si>
+    <t>molfile</t>
+  </si>
+  <si>
+    <t>Molfile</t>
+  </si>
+  <si>
+    <t>Molfile used to generate smiles/inchi</t>
+  </si>
+  <si>
+    <t>canonical_structure</t>
+  </si>
+  <si>
+    <t>_undefined</t>
+  </si>
+  <si>
+    <t>SM:15</t>
+  </si>
+  <si>
+    <t>SM_Image_Parent</t>
+  </si>
+  <si>
+    <t>An image of the parent (standardized) compound produced using structure rendering software</t>
+  </si>
+  <si>
+    <t>software</t>
+  </si>
+  <si>
+    <t>SM:19</t>
+  </si>
+  <si>
+    <t>SM_Software</t>
+  </si>
+  <si>
+    <t>Name, Version, Link for Software used to generate InChi and SMILES</t>
+  </si>
+  <si>
+    <t>The software versions are available from IUPAC</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>SM:28</t>
+  </si>
+  <si>
+    <t>Is restricted molecule: only available to staff</t>
+  </si>
+  <si>
+    <t>target_information_references</t>
+  </si>
+  <si>
+    <t>SM:20</t>
+  </si>
+  <si>
+    <t>SM_Target Information_References</t>
+  </si>
+  <si>
+    <t>Information about the pharmacological target(s) of the compound in cells, e.g. proteins or other molecules with which the drug interacts to confer its effect. Appropriate literature references should also be provided.</t>
+  </si>
+  <si>
+    <t>this should include references to other databases where such information can be extracted; it appears unrealistic to maintain the available external biological activity data for LINCS compounds; if we create a database we can reference this; this will be implemented in multiple fields</t>
+  </si>
+  <si>
+    <t>it appears that this should be a separate database that links here</t>
+  </si>
+  <si>
+    <t>facility_batch_id</t>
+  </si>
+  <si>
+    <t>SM:5</t>
+  </si>
+  <si>
+    <t>SM_Center_Sample_ID</t>
+  </si>
+  <si>
+    <t>Batch ID</t>
+  </si>
+  <si>
+    <t>Sample ID of the tested compound, referring to  of the tested sample; assigned after local registry of the compound (center specific)</t>
+  </si>
+  <si>
+    <t>assigned by local LINCS center</t>
+  </si>
+  <si>
+    <t>provider</t>
+  </si>
+  <si>
+    <t>SM:6</t>
+  </si>
+  <si>
+    <t>SM_Provider</t>
+  </si>
+  <si>
+    <t>Vendor or lab that supplied the compound</t>
+  </si>
+  <si>
+    <t>list of vendor names and other providers</t>
+  </si>
+  <si>
+    <t>provider_catalog_id</t>
+  </si>
+  <si>
+    <t>SM:7</t>
+  </si>
+  <si>
+    <t>SM_Provider_Catalog_ID</t>
+  </si>
+  <si>
+    <t>ID or catalogue number assigned to the specific supplied sample by the vendor or provider</t>
+  </si>
+  <si>
+    <t>provider_sample_id</t>
+  </si>
+  <si>
+    <t>SM:8</t>
+  </si>
+  <si>
+    <t>SM_Provider_Sample_ID</t>
+  </si>
+  <si>
+    <t>Provider Batch ID</t>
+  </si>
+  <si>
+    <t>Sample ID of the compound obtained from the provider or vendor (if available); this should include batch and / or lot number</t>
+  </si>
+  <si>
+    <t>inchi</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>SM:16</t>
+  </si>
+  <si>
+    <t>SM_InChi_Batch</t>
+  </si>
+  <si>
+    <t>InChi representation of the actual sample (batch) structure</t>
+  </si>
+  <si>
+    <t>inchi_key</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>SM:17</t>
+  </si>
+  <si>
+    <t>SM_InChi_Key_Batch</t>
+  </si>
+  <si>
+    <t>InChi key of the actual sample (batch) structure</t>
+  </si>
+  <si>
     <t>smiles</t>
-  </si>
-  <si>
-    <t>SM:14</t>
-  </si>
-  <si>
-    <t>SM_SMILES_Parent</t>
-  </si>
-  <si>
-    <t>SMILES</t>
-  </si>
-  <si>
-    <t>Canonical SMILES representation of parent (standardized) chemical structure generated by LINCS business rules</t>
-  </si>
-  <si>
-    <t>standardized small molecule representation; documented standardization protocol</t>
-  </si>
-  <si>
-    <t>inchi</t>
-  </si>
-  <si>
-    <t>SM:12</t>
-  </si>
-  <si>
-    <t>SM_InChi_Parent</t>
-  </si>
-  <si>
-    <t>InChi</t>
-  </si>
-  <si>
-    <t>InChi representation of parent (standardized) chemical structure chemical structure generated by LINCS business rules</t>
-  </si>
-  <si>
-    <t>inchi_key</t>
-  </si>
-  <si>
-    <t>SM:13</t>
-  </si>
-  <si>
-    <t>SM_InChi_Key_Parent</t>
-  </si>
-  <si>
-    <t>InChi Key</t>
-  </si>
-  <si>
-    <t>InChi key of parent (standardized) chemical structure generated by LINCS business rules</t>
-  </si>
-  <si>
-    <t>derived from InChi</t>
-  </si>
-  <si>
-    <t>chembl_id</t>
-  </si>
-  <si>
-    <t>ChEMBL ID</t>
-  </si>
-  <si>
-    <t>ChEMBL is a database of bioactive drug-like small molecules, it contains 2-D structures, calculated properties (e.g. logP, Molecular Weight, Lipinski Parameters, etc.) and abstracted bioactivities (e.g. binding constants, pharmacology and ADMET data)</t>
-  </si>
-  <si>
-    <t>molfile</t>
-  </si>
-  <si>
-    <t>Molfile</t>
-  </si>
-  <si>
-    <t>Molfile used to generate smiles/inchi</t>
-  </si>
-  <si>
-    <t>canonical_structure</t>
-  </si>
-  <si>
-    <t>_undefined</t>
-  </si>
-  <si>
-    <t>SM:15</t>
-  </si>
-  <si>
-    <t>SM_Image_Parent</t>
-  </si>
-  <si>
-    <t>An image of the parent (standardized) compound produced using structure rendering software</t>
-  </si>
-  <si>
-    <t>software</t>
-  </si>
-  <si>
-    <t>SM:19</t>
-  </si>
-  <si>
-    <t>SM_Software</t>
-  </si>
-  <si>
-    <t>Name, Version, Link for Software used to generate InChi and SMILES</t>
-  </si>
-  <si>
-    <t>The software versions are available from IUPAC</t>
-  </si>
-  <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>SM:28</t>
-  </si>
-  <si>
-    <t>Is restricted molecule: only available to staff</t>
-  </si>
-  <si>
-    <t>target_information_references</t>
-  </si>
-  <si>
-    <t>SM:20</t>
-  </si>
-  <si>
-    <t>SM_Target Information_References</t>
-  </si>
-  <si>
-    <t>Information about the pharmacological target(s) of the compound in cells, e.g. proteins or other molecules with which the drug interacts to confer its effect. Appropriate literature references should also be provided.</t>
-  </si>
-  <si>
-    <t>this should include references to other databases where such information can be extracted; it appears unrealistic to maintain the available external biological activity data for LINCS compounds; if we create a database we can reference this; this will be implemented in multiple fields</t>
-  </si>
-  <si>
-    <t>it appears that this should be a separate database that links here</t>
-  </si>
-  <si>
-    <t>facility_batch_id</t>
-  </si>
-  <si>
-    <t>SM:5</t>
-  </si>
-  <si>
-    <t>SM_Center_Sample_ID</t>
-  </si>
-  <si>
-    <t>Batch ID</t>
-  </si>
-  <si>
-    <t>Sample ID of the tested compound, referring to  of the tested sample; assigned after local registry of the compound (center specific)</t>
-  </si>
-  <si>
-    <t>assigned by local LINCS center</t>
-  </si>
-  <si>
-    <t>provider</t>
-  </si>
-  <si>
-    <t>SM:6</t>
-  </si>
-  <si>
-    <t>SM_Provider</t>
-  </si>
-  <si>
-    <t>Vendor or lab that supplied the compound</t>
-  </si>
-  <si>
-    <t>list of vendor names and other providers</t>
-  </si>
-  <si>
-    <t>provider_catalog_id</t>
-  </si>
-  <si>
-    <t>SM:7</t>
-  </si>
-  <si>
-    <t>SM_Provider_Catalog_ID</t>
-  </si>
-  <si>
-    <t>ID or catalogue number assigned to the specific supplied sample by the vendor or provider</t>
-  </si>
-  <si>
-    <t>provider_sample_id</t>
-  </si>
-  <si>
-    <t>SM:8</t>
-  </si>
-  <si>
-    <t>SM_Provider_Sample_ID</t>
-  </si>
-  <si>
-    <t>Provider Batch ID</t>
-  </si>
-  <si>
-    <t>Sample ID of the compound obtained from the provider or vendor (if available); this should include batch and / or lot number</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>SM:16</t>
-  </si>
-  <si>
-    <t>SM_InChi_Batch</t>
-  </si>
-  <si>
-    <t>InChi representation of the actual sample (batch) structure</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>SM:17</t>
-  </si>
-  <si>
-    <t>SM_InChi_Key_Batch</t>
-  </si>
-  <si>
-    <t>InChi key of the actual sample (batch) structure</t>
   </si>
   <si>
     <t>42</t>
@@ -2521,7 +2545,7 @@
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -2534,29 +2558,29 @@
   <dimension ref="A1:AQ166"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <pane activePane="bottomRight" topLeftCell="A26" xSplit="3441" ySplit="1896"/>
+      <pane activePane="bottomRight" topLeftCell="A80" xSplit="3560" ySplit="1881"/>
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
       <selection activeCell="A1" activeCellId="0" pane="topRight" sqref="A1"/>
-      <selection activeCell="A26" activeCellId="0" pane="bottomLeft" sqref="A26"/>
-      <selection activeCell="F46" activeCellId="0" pane="bottomRight" sqref="F46"/>
+      <selection activeCell="A80" activeCellId="0" pane="bottomLeft" sqref="A80"/>
+      <selection activeCell="C101" activeCellId="0" pane="bottomRight" sqref="C101"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.9411764705882"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.5882352941176"/>
-    <col collapsed="false" hidden="false" max="9" min="3" style="1" width="11.956862745098"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="2" width="11.956862745098"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.956862745098"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="30.9333333333333"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="1" width="28.4823529411765"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="61.3019607843137"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="16.6509803921569"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="49.3372549019608"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="15.3764705882353"/>
-    <col collapsed="false" hidden="false" max="21" min="20" style="1" width="23.7882352941176"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="23.6705882352941"/>
-    <col collapsed="false" hidden="false" max="25" min="23" style="1" width="10.3294117647059"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="8.72941176470588"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.0588235294118"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.6627450980392"/>
+    <col collapsed="false" hidden="false" max="9" min="3" style="1" width="12.0196078431373"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="2" width="12.0196078431373"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.0196078431373"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="31.0862745098039"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="1" width="28.6235294117647"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="61.6117647058824"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="16.7333333333333"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="49.5803921568627"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="15.4549019607843"/>
+    <col collapsed="false" hidden="false" max="21" min="20" style="1" width="23.9058823529412"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="23.7882352941176"/>
+    <col collapsed="false" hidden="false" max="25" min="23" style="1" width="10.3843137254902"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="8.77254901960784"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="67.5" outlineLevel="0" r="1" s="6">
@@ -6757,14 +6781,16 @@
       <c r="AJ95" s="1"/>
       <c r="AK95" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="96">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="96">
       <c r="A96" s="9" t="s">
         <v>296</v>
       </c>
       <c r="B96" s="9" t="s">
         <v>352</v>
       </c>
-      <c r="C96" s="9"/>
+      <c r="C96" s="9" t="s">
+        <v>353</v>
+      </c>
       <c r="D96" s="9"/>
       <c r="E96" s="9" t="s">
         <v>23</v>
@@ -6788,22 +6814,22 @@
         <v>24</v>
       </c>
       <c r="L96" s="1" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="M96" s="1" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="O96" s="1" t="s">
         <v>333</v>
       </c>
       <c r="P96" s="1" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="Q96" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R96" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="Z96" s="1"/>
       <c r="AA96" s="1"/>
@@ -6818,14 +6844,16 @@
       <c r="AJ96" s="1"/>
       <c r="AK96" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="97">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="97">
       <c r="A97" s="9" t="s">
         <v>296</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>357</v>
-      </c>
-      <c r="C97" s="9"/>
+        <v>358</v>
+      </c>
+      <c r="C97" s="9" t="s">
+        <v>359</v>
+      </c>
       <c r="D97" s="9"/>
       <c r="E97" s="9" t="s">
         <v>23</v>
@@ -6849,22 +6877,22 @@
         <v>24</v>
       </c>
       <c r="L97" s="1" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="M97" s="1" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="O97" s="1" t="s">
         <v>333</v>
       </c>
       <c r="P97" s="1" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="Q97" s="1" t="n">
         <v>2</v>
       </c>
       <c r="R97" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="Z97" s="1"/>
       <c r="AA97" s="1"/>
@@ -6879,14 +6907,16 @@
       <c r="AJ97" s="1"/>
       <c r="AK97" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="98">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="98">
       <c r="A98" s="9" t="s">
         <v>296</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>361</v>
-      </c>
-      <c r="C98" s="9"/>
+        <v>363</v>
+      </c>
+      <c r="C98" s="9" t="s">
+        <v>364</v>
+      </c>
       <c r="D98" s="9"/>
       <c r="E98" s="9" t="s">
         <v>23</v>
@@ -6908,25 +6938,25 @@
         <v>24</v>
       </c>
       <c r="L98" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="M98" s="1" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="N98" s="1" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="O98" s="1" t="s">
         <v>302</v>
       </c>
       <c r="P98" s="1" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="Q98" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R98" s="1" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="Z98" s="1"/>
       <c r="AA98" s="1"/>
@@ -6941,14 +6971,16 @@
       <c r="AJ98" s="1"/>
       <c r="AK98" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="99">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="99">
       <c r="A99" s="9" t="s">
         <v>296</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>367</v>
-      </c>
-      <c r="C99" s="9"/>
+        <v>370</v>
+      </c>
+      <c r="C99" s="9" t="s">
+        <v>371</v>
+      </c>
       <c r="D99" s="9"/>
       <c r="E99" s="9" t="s">
         <v>23</v>
@@ -6970,25 +7002,25 @@
         <v>24</v>
       </c>
       <c r="L99" s="1" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="M99" s="1" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="N99" s="1" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="O99" s="1" t="s">
         <v>302</v>
       </c>
       <c r="P99" s="1" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="Q99" s="1" t="n">
         <v>2</v>
       </c>
       <c r="R99" s="1" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="Z99" s="1"/>
       <c r="AA99" s="1"/>
@@ -7003,14 +7035,16 @@
       <c r="AJ99" s="1"/>
       <c r="AK99" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="100">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="100">
       <c r="A100" s="9" t="s">
         <v>296</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>372</v>
-      </c>
-      <c r="C100" s="9"/>
+        <v>376</v>
+      </c>
+      <c r="C100" s="9" t="s">
+        <v>377</v>
+      </c>
       <c r="D100" s="9"/>
       <c r="E100" s="9" t="s">
         <v>23</v>
@@ -7032,25 +7066,25 @@
         <v>24</v>
       </c>
       <c r="L100" s="1" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
       <c r="M100" s="1" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="N100" s="1" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
       <c r="O100" s="1" t="s">
         <v>302</v>
       </c>
       <c r="P100" s="1" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="Q100" s="1" t="n">
         <v>2</v>
       </c>
       <c r="U100" s="1" t="s">
-        <v>377</v>
+        <v>382</v>
       </c>
       <c r="Z100" s="1"/>
       <c r="AA100" s="1"/>
@@ -7070,7 +7104,7 @@
         <v>296</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>378</v>
+        <v>383</v>
       </c>
       <c r="C101" s="9"/>
       <c r="D101" s="9"/>
@@ -7095,10 +7129,10 @@
         <v>1002</v>
       </c>
       <c r="N101" s="1" t="s">
-        <v>379</v>
+        <v>384</v>
       </c>
       <c r="P101" s="1" t="s">
-        <v>380</v>
+        <v>385</v>
       </c>
       <c r="Z101" s="1"/>
       <c r="AA101" s="1"/>
@@ -7118,7 +7152,7 @@
         <v>296</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>381</v>
+        <v>386</v>
       </c>
       <c r="C102" s="9"/>
       <c r="D102" s="9"/>
@@ -7143,13 +7177,13 @@
         <v>1001</v>
       </c>
       <c r="N102" s="1" t="s">
-        <v>382</v>
+        <v>387</v>
       </c>
       <c r="O102" s="1" t="s">
         <v>302</v>
       </c>
       <c r="P102" s="1" t="s">
-        <v>383</v>
+        <v>388</v>
       </c>
       <c r="Z102" s="1"/>
       <c r="AA102" s="1"/>
@@ -7167,11 +7201,11 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="103">
       <c r="A103" s="9"/>
       <c r="B103" s="9" t="s">
-        <v>384</v>
+        <v>389</v>
       </c>
       <c r="C103" s="9"/>
       <c r="D103" s="9" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
       <c r="E103" s="9" t="s">
         <v>24</v>
@@ -7193,22 +7227,22 @@
         <v>24</v>
       </c>
       <c r="L103" s="1" t="s">
-        <v>386</v>
+        <v>391</v>
       </c>
       <c r="M103" s="1" t="s">
-        <v>387</v>
+        <v>392</v>
       </c>
       <c r="O103" s="1" t="s">
         <v>302</v>
       </c>
       <c r="P103" s="1" t="s">
-        <v>388</v>
+        <v>393</v>
       </c>
       <c r="Q103" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R103" s="1" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="Z103" s="1"/>
       <c r="AA103" s="1"/>
@@ -7228,7 +7262,7 @@
         <v>296</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="C104" s="9"/>
       <c r="D104" s="9"/>
@@ -7252,19 +7286,19 @@
         <v>24</v>
       </c>
       <c r="L104" s="1" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="M104" s="1" t="s">
-        <v>391</v>
+        <v>396</v>
       </c>
       <c r="P104" s="1" t="s">
-        <v>392</v>
+        <v>397</v>
       </c>
       <c r="Q104" s="1" t="n">
         <v>2</v>
       </c>
       <c r="U104" s="1" t="s">
-        <v>393</v>
+        <v>398</v>
       </c>
       <c r="Z104" s="1"/>
       <c r="AA104" s="1"/>
@@ -7296,7 +7330,7 @@
         <v>23</v>
       </c>
       <c r="H105" s="9" t="s">
-        <v>394</v>
+        <v>399</v>
       </c>
       <c r="I105" s="7" t="s">
         <v>24</v>
@@ -7308,19 +7342,19 @@
         <v>23</v>
       </c>
       <c r="L105" s="1" t="s">
-        <v>395</v>
+        <v>400</v>
       </c>
       <c r="N105" s="1" t="s">
         <v>168</v>
       </c>
       <c r="P105" s="1" t="s">
-        <v>396</v>
+        <v>401</v>
       </c>
       <c r="Q105" s="1" t="n">
         <v>2</v>
       </c>
       <c r="U105" s="1" t="s">
-        <v>393</v>
+        <v>398</v>
       </c>
       <c r="Z105" s="1"/>
       <c r="AA105" s="1"/>
@@ -7338,11 +7372,11 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="106">
       <c r="A106" s="9"/>
       <c r="B106" s="9" t="s">
-        <v>397</v>
+        <v>402</v>
       </c>
       <c r="C106" s="9"/>
       <c r="D106" s="9" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
       <c r="E106" s="9" t="s">
         <v>23</v>
@@ -7364,25 +7398,25 @@
         <v>24</v>
       </c>
       <c r="L106" s="1" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="M106" s="1" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="O106" s="1" t="s">
         <v>302</v>
       </c>
       <c r="P106" s="1" t="s">
-        <v>400</v>
+        <v>405</v>
       </c>
       <c r="Q106" s="1" t="n">
         <v>2</v>
       </c>
       <c r="R106" s="1" t="s">
-        <v>401</v>
+        <v>406</v>
       </c>
       <c r="U106" s="1" t="s">
-        <v>402</v>
+        <v>407</v>
       </c>
       <c r="Z106" s="1"/>
       <c r="AA106" s="1"/>
@@ -7402,7 +7436,7 @@
         <v>326</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>403</v>
+        <v>408</v>
       </c>
       <c r="C107" s="9" t="s">
         <v>333</v>
@@ -7430,25 +7464,25 @@
         <v>23</v>
       </c>
       <c r="L107" s="1" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
       <c r="M107" s="1" t="s">
-        <v>405</v>
+        <v>410</v>
       </c>
       <c r="N107" s="1" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
       <c r="O107" s="1" t="s">
         <v>333</v>
       </c>
       <c r="P107" s="1" t="s">
-        <v>407</v>
+        <v>412</v>
       </c>
       <c r="Q107" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R107" s="1" t="s">
-        <v>408</v>
+        <v>413</v>
       </c>
       <c r="Z107" s="1"/>
       <c r="AA107" s="1"/>
@@ -7468,7 +7502,7 @@
         <v>326</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="C108" s="9"/>
       <c r="D108" s="9"/>
@@ -7494,22 +7528,22 @@
         <v>23</v>
       </c>
       <c r="L108" s="1" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="M108" s="1" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
       <c r="O108" s="1" t="s">
         <v>333</v>
       </c>
       <c r="P108" s="1" t="s">
-        <v>412</v>
+        <v>417</v>
       </c>
       <c r="Q108" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R108" s="1" t="s">
-        <v>413</v>
+        <v>418</v>
       </c>
       <c r="Z108" s="1"/>
       <c r="AA108" s="1"/>
@@ -7529,7 +7563,7 @@
         <v>326</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="C109" s="9"/>
       <c r="D109" s="9"/>
@@ -7555,16 +7589,16 @@
         <v>23</v>
       </c>
       <c r="L109" s="1" t="s">
-        <v>415</v>
+        <v>420</v>
       </c>
       <c r="M109" s="1" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="O109" s="1" t="s">
         <v>333</v>
       </c>
       <c r="P109" s="1" t="s">
-        <v>417</v>
+        <v>422</v>
       </c>
       <c r="Q109" s="1" t="n">
         <v>1</v>
@@ -7587,7 +7621,7 @@
         <v>326</v>
       </c>
       <c r="B110" s="9" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="C110" s="9"/>
       <c r="D110" s="9"/>
@@ -7613,19 +7647,19 @@
         <v>23</v>
       </c>
       <c r="L110" s="1" t="s">
-        <v>419</v>
+        <v>424</v>
       </c>
       <c r="M110" s="1" t="s">
-        <v>420</v>
+        <v>425</v>
       </c>
       <c r="N110" s="1" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
       <c r="O110" s="1" t="s">
         <v>333</v>
       </c>
       <c r="P110" s="1" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="Q110" s="1" t="n">
         <v>2</v>
@@ -7648,7 +7682,7 @@
         <v>326</v>
       </c>
       <c r="B111" s="9" t="s">
-        <v>367</v>
+        <v>428</v>
       </c>
       <c r="C111" s="9"/>
       <c r="D111" s="9"/>
@@ -7660,7 +7694,7 @@
         <v>23</v>
       </c>
       <c r="H111" s="9" t="s">
-        <v>423</v>
+        <v>429</v>
       </c>
       <c r="I111" s="7" t="s">
         <v>24</v>
@@ -7672,22 +7706,22 @@
         <v>24</v>
       </c>
       <c r="L111" s="1" t="s">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="M111" s="1" t="s">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="O111" s="1" t="s">
         <v>333</v>
       </c>
       <c r="P111" s="1" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="Q111" s="1" t="n">
         <v>2</v>
       </c>
       <c r="R111" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="Z111" s="1"/>
       <c r="AA111" s="1"/>
@@ -7707,7 +7741,7 @@
         <v>326</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>372</v>
+        <v>433</v>
       </c>
       <c r="C112" s="9"/>
       <c r="D112" s="9"/>
@@ -7719,7 +7753,7 @@
         <v>23</v>
       </c>
       <c r="H112" s="9" t="s">
-        <v>427</v>
+        <v>434</v>
       </c>
       <c r="I112" s="7" t="s">
         <v>24</v>
@@ -7731,22 +7765,22 @@
         <v>24</v>
       </c>
       <c r="L112" s="1" t="s">
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="M112" s="1" t="s">
-        <v>429</v>
+        <v>436</v>
       </c>
       <c r="O112" s="1" t="s">
         <v>333</v>
       </c>
       <c r="P112" s="1" t="s">
-        <v>430</v>
+        <v>437</v>
       </c>
       <c r="Q112" s="1" t="n">
         <v>2</v>
       </c>
       <c r="U112" s="1" t="s">
-        <v>377</v>
+        <v>382</v>
       </c>
       <c r="Z112" s="1"/>
       <c r="AA112" s="1"/>
@@ -7766,7 +7800,7 @@
         <v>326</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>361</v>
+        <v>438</v>
       </c>
       <c r="C113" s="9"/>
       <c r="D113" s="9"/>
@@ -7778,7 +7812,7 @@
         <v>23</v>
       </c>
       <c r="H113" s="9" t="s">
-        <v>431</v>
+        <v>439</v>
       </c>
       <c r="I113" s="7" t="s">
         <v>24</v>
@@ -7790,22 +7824,22 @@
         <v>24</v>
       </c>
       <c r="L113" s="1" t="s">
-        <v>432</v>
+        <v>440</v>
       </c>
       <c r="M113" s="1" t="s">
-        <v>433</v>
+        <v>441</v>
       </c>
       <c r="O113" s="1" t="s">
         <v>333</v>
       </c>
       <c r="P113" s="1" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
       <c r="Q113" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R113" s="1" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="Z113" s="1"/>
       <c r="AA113" s="1"/>
@@ -7825,7 +7859,7 @@
         <v>326</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>435</v>
+        <v>443</v>
       </c>
       <c r="C114" s="9"/>
       <c r="D114" s="9"/>
@@ -7849,22 +7883,22 @@
         <v>24</v>
       </c>
       <c r="L114" s="1" t="s">
-        <v>436</v>
+        <v>444</v>
       </c>
       <c r="M114" s="1" t="s">
-        <v>437</v>
+        <v>445</v>
       </c>
       <c r="O114" s="1" t="s">
         <v>333</v>
       </c>
       <c r="P114" s="1" t="s">
-        <v>438</v>
+        <v>446</v>
       </c>
       <c r="Q114" s="1" t="n">
         <v>3</v>
       </c>
       <c r="R114" s="1" t="s">
-        <v>439</v>
+        <v>447</v>
       </c>
       <c r="Z114" s="1"/>
       <c r="AA114" s="1"/>
@@ -7890,7 +7924,7 @@
         <v>326</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>440</v>
+        <v>448</v>
       </c>
       <c r="C115" s="9"/>
       <c r="D115" s="9"/>
@@ -7902,7 +7936,7 @@
         <v>23</v>
       </c>
       <c r="H115" s="9" t="s">
-        <v>441</v>
+        <v>449</v>
       </c>
       <c r="I115" s="7" t="s">
         <v>23</v>
@@ -7914,22 +7948,22 @@
         <v>24</v>
       </c>
       <c r="L115" s="1" t="s">
-        <v>442</v>
+        <v>450</v>
       </c>
       <c r="M115" s="1" t="s">
-        <v>443</v>
+        <v>451</v>
       </c>
       <c r="O115" s="1" t="s">
         <v>333</v>
       </c>
       <c r="P115" s="1" t="s">
-        <v>444</v>
+        <v>452</v>
       </c>
       <c r="Q115" s="1" t="n">
         <v>3</v>
       </c>
       <c r="R115" s="1" t="s">
-        <v>439</v>
+        <v>447</v>
       </c>
       <c r="Z115" s="1"/>
       <c r="AA115" s="1"/>
@@ -7955,7 +7989,7 @@
         <v>326</v>
       </c>
       <c r="B116" s="9" t="s">
-        <v>445</v>
+        <v>453</v>
       </c>
       <c r="C116" s="9"/>
       <c r="D116" s="9"/>
@@ -7967,7 +8001,7 @@
         <v>23</v>
       </c>
       <c r="H116" s="9" t="s">
-        <v>446</v>
+        <v>454</v>
       </c>
       <c r="I116" s="7" t="s">
         <v>23</v>
@@ -7979,16 +8013,16 @@
         <v>24</v>
       </c>
       <c r="L116" s="1" t="s">
-        <v>447</v>
+        <v>455</v>
       </c>
       <c r="M116" s="1" t="s">
-        <v>448</v>
+        <v>456</v>
       </c>
       <c r="O116" s="1" t="s">
         <v>333</v>
       </c>
       <c r="P116" s="1" t="s">
-        <v>449</v>
+        <v>457</v>
       </c>
       <c r="Q116" s="1" t="n">
         <v>3</v>
@@ -8017,7 +8051,7 @@
         <v>326</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>450</v>
+        <v>458</v>
       </c>
       <c r="C117" s="9"/>
       <c r="D117" s="9"/>
@@ -8029,7 +8063,7 @@
         <v>23</v>
       </c>
       <c r="H117" s="9" t="s">
-        <v>451</v>
+        <v>459</v>
       </c>
       <c r="I117" s="7" t="s">
         <v>23</v>
@@ -8041,22 +8075,22 @@
         <v>24</v>
       </c>
       <c r="L117" s="1" t="s">
-        <v>452</v>
+        <v>460</v>
       </c>
       <c r="M117" s="1" t="s">
-        <v>453</v>
+        <v>461</v>
       </c>
       <c r="O117" s="1" t="s">
         <v>333</v>
       </c>
       <c r="P117" s="1" t="s">
-        <v>454</v>
+        <v>462</v>
       </c>
       <c r="Q117" s="1" t="n">
         <v>3</v>
       </c>
       <c r="R117" s="1" t="s">
-        <v>439</v>
+        <v>447</v>
       </c>
       <c r="Z117" s="1"/>
       <c r="AA117" s="1"/>
@@ -8106,7 +8140,7 @@
         <v>23</v>
       </c>
       <c r="L118" s="1" t="s">
-        <v>455</v>
+        <v>463</v>
       </c>
       <c r="N118" s="1" t="s">
         <v>158</v>
@@ -8162,7 +8196,7 @@
         <v>23</v>
       </c>
       <c r="L119" s="1" t="s">
-        <v>456</v>
+        <v>464</v>
       </c>
       <c r="N119" s="1" t="s">
         <v>161</v>
@@ -8218,7 +8252,7 @@
         <v>23</v>
       </c>
       <c r="L120" s="1" t="s">
-        <v>457</v>
+        <v>465</v>
       </c>
       <c r="N120" s="1" t="s">
         <v>164</v>
@@ -8248,11 +8282,11 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="121">
       <c r="A121" s="9"/>
       <c r="B121" s="9" t="s">
-        <v>458</v>
+        <v>466</v>
       </c>
       <c r="C121" s="9"/>
       <c r="D121" s="9" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
       <c r="E121" s="9" t="s">
         <v>23</v>
@@ -8262,7 +8296,7 @@
         <v>23</v>
       </c>
       <c r="H121" s="9" t="s">
-        <v>459</v>
+        <v>467</v>
       </c>
       <c r="I121" s="7" t="s">
         <v>23</v>
@@ -8274,22 +8308,22 @@
         <v>24</v>
       </c>
       <c r="L121" s="1" t="s">
-        <v>460</v>
+        <v>468</v>
       </c>
       <c r="M121" s="1" t="s">
-        <v>461</v>
+        <v>469</v>
       </c>
       <c r="O121" s="1" t="s">
         <v>333</v>
       </c>
       <c r="P121" s="1" t="s">
-        <v>462</v>
+        <v>470</v>
       </c>
       <c r="Q121" s="1" t="n">
         <v>3</v>
       </c>
       <c r="R121" s="1" t="s">
-        <v>439</v>
+        <v>447</v>
       </c>
       <c r="Z121" s="1"/>
       <c r="AA121" s="1"/>
@@ -8318,7 +8352,7 @@
         <v>143</v>
       </c>
       <c r="C122" s="9" t="s">
-        <v>463</v>
+        <v>471</v>
       </c>
       <c r="D122" s="9"/>
       <c r="E122" s="9" t="s">
@@ -8337,34 +8371,34 @@
         <v>23</v>
       </c>
       <c r="J122" s="13" t="s">
-        <v>464</v>
+        <v>472</v>
       </c>
       <c r="K122" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L122" s="1" t="s">
-        <v>465</v>
+        <v>473</v>
       </c>
       <c r="M122" s="1" t="s">
-        <v>466</v>
+        <v>474</v>
       </c>
       <c r="N122" s="1" t="s">
-        <v>467</v>
+        <v>475</v>
       </c>
       <c r="O122" s="1" t="s">
-        <v>468</v>
+        <v>476</v>
       </c>
       <c r="P122" s="1" t="s">
-        <v>469</v>
+        <v>477</v>
       </c>
       <c r="Q122" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R122" s="1" t="s">
-        <v>470</v>
+        <v>478</v>
       </c>
       <c r="S122" s="1" t="s">
-        <v>471</v>
+        <v>479</v>
       </c>
       <c r="Z122" s="1"/>
       <c r="AA122" s="1"/>
@@ -8393,7 +8427,7 @@
         <v>306</v>
       </c>
       <c r="C123" s="9" t="s">
-        <v>472</v>
+        <v>480</v>
       </c>
       <c r="D123" s="9"/>
       <c r="E123" s="9" t="s">
@@ -8412,31 +8446,31 @@
         <v>23</v>
       </c>
       <c r="J123" s="13" t="s">
-        <v>464</v>
+        <v>472</v>
       </c>
       <c r="K123" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L123" s="1" t="s">
-        <v>473</v>
+        <v>481</v>
       </c>
       <c r="M123" s="1" t="s">
-        <v>474</v>
+        <v>482</v>
       </c>
       <c r="N123" s="1" t="s">
-        <v>475</v>
+        <v>483</v>
       </c>
       <c r="O123" s="1" t="s">
-        <v>468</v>
+        <v>476</v>
       </c>
       <c r="P123" s="1" t="s">
-        <v>476</v>
+        <v>484</v>
       </c>
       <c r="Q123" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R123" s="1" t="s">
-        <v>477</v>
+        <v>485</v>
       </c>
       <c r="Z123" s="1"/>
       <c r="AA123" s="1"/>
@@ -8462,7 +8496,7 @@
         <v>265</v>
       </c>
       <c r="B124" s="9" t="s">
-        <v>478</v>
+        <v>486</v>
       </c>
       <c r="C124" s="9"/>
       <c r="D124" s="9"/>
@@ -8482,37 +8516,37 @@
         <v>23</v>
       </c>
       <c r="J124" s="13" t="s">
-        <v>464</v>
+        <v>472</v>
       </c>
       <c r="K124" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L124" s="1" t="s">
-        <v>479</v>
+        <v>487</v>
       </c>
       <c r="M124" s="1" t="s">
-        <v>480</v>
+        <v>488</v>
       </c>
       <c r="O124" s="1" t="s">
-        <v>468</v>
+        <v>476</v>
       </c>
       <c r="P124" s="1" t="s">
-        <v>481</v>
+        <v>489</v>
       </c>
       <c r="Q124" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R124" s="1" t="s">
-        <v>482</v>
+        <v>490</v>
       </c>
       <c r="S124" s="1" t="s">
-        <v>471</v>
+        <v>479</v>
       </c>
       <c r="T124" s="1" t="s">
-        <v>483</v>
+        <v>491</v>
       </c>
       <c r="U124" s="1" t="s">
-        <v>484</v>
+        <v>492</v>
       </c>
       <c r="Z124" s="1"/>
       <c r="AA124" s="1"/>
@@ -8538,7 +8572,7 @@
         <v>265</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>485</v>
+        <v>493</v>
       </c>
       <c r="C125" s="9"/>
       <c r="D125" s="9"/>
@@ -8558,40 +8592,40 @@
         <v>23</v>
       </c>
       <c r="J125" s="13" t="s">
-        <v>464</v>
+        <v>472</v>
       </c>
       <c r="K125" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L125" s="1" t="s">
-        <v>486</v>
+        <v>494</v>
       </c>
       <c r="M125" s="1" t="s">
-        <v>487</v>
+        <v>495</v>
       </c>
       <c r="N125" s="1" t="s">
-        <v>488</v>
+        <v>496</v>
       </c>
       <c r="O125" s="1" t="s">
-        <v>468</v>
+        <v>476</v>
       </c>
       <c r="P125" s="1" t="s">
-        <v>489</v>
+        <v>497</v>
       </c>
       <c r="Q125" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R125" s="1" t="s">
-        <v>490</v>
+        <v>498</v>
       </c>
       <c r="S125" s="1" t="s">
-        <v>471</v>
+        <v>479</v>
       </c>
       <c r="T125" s="1" t="s">
-        <v>491</v>
+        <v>499</v>
       </c>
       <c r="U125" s="1" t="s">
-        <v>484</v>
+        <v>492</v>
       </c>
       <c r="Z125" s="1"/>
       <c r="AA125" s="1"/>
@@ -8617,7 +8651,7 @@
         <v>265</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="C126" s="9"/>
       <c r="D126" s="9"/>
@@ -8637,28 +8671,28 @@
         <v>23</v>
       </c>
       <c r="J126" s="13" t="s">
-        <v>464</v>
+        <v>472</v>
       </c>
       <c r="K126" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L126" s="1" t="s">
-        <v>492</v>
+        <v>500</v>
       </c>
       <c r="M126" s="1" t="s">
-        <v>493</v>
+        <v>501</v>
       </c>
       <c r="O126" s="1" t="s">
         <v>333</v>
       </c>
       <c r="P126" s="1" t="s">
-        <v>494</v>
+        <v>502</v>
       </c>
       <c r="Q126" s="1" t="n">
         <v>1</v>
       </c>
       <c r="T126" s="1" t="s">
-        <v>495</v>
+        <v>503</v>
       </c>
       <c r="Z126" s="1"/>
       <c r="AA126" s="1"/>
@@ -8684,7 +8718,7 @@
         <v>265</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="C127" s="9"/>
       <c r="D127" s="9"/>
@@ -8704,28 +8738,28 @@
         <v>23</v>
       </c>
       <c r="J127" s="13" t="s">
-        <v>464</v>
+        <v>472</v>
       </c>
       <c r="K127" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L127" s="1" t="s">
-        <v>496</v>
+        <v>504</v>
       </c>
       <c r="M127" s="1" t="s">
-        <v>497</v>
+        <v>505</v>
       </c>
       <c r="O127" s="1" t="s">
         <v>333</v>
       </c>
       <c r="P127" s="1" t="s">
-        <v>498</v>
+        <v>506</v>
       </c>
       <c r="Q127" s="1" t="n">
         <v>1</v>
       </c>
       <c r="T127" s="1" t="s">
-        <v>499</v>
+        <v>507</v>
       </c>
       <c r="Z127" s="1"/>
       <c r="AA127" s="1"/>
@@ -8751,7 +8785,7 @@
         <v>265</v>
       </c>
       <c r="B128" s="9" t="s">
-        <v>500</v>
+        <v>508</v>
       </c>
       <c r="C128" s="9"/>
       <c r="D128" s="9"/>
@@ -8771,31 +8805,31 @@
         <v>23</v>
       </c>
       <c r="J128" s="13" t="s">
-        <v>464</v>
+        <v>472</v>
       </c>
       <c r="K128" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L128" s="1" t="s">
-        <v>501</v>
+        <v>509</v>
       </c>
       <c r="M128" s="1" t="s">
-        <v>502</v>
+        <v>510</v>
       </c>
       <c r="O128" s="1" t="s">
         <v>333</v>
       </c>
       <c r="P128" s="1" t="s">
-        <v>503</v>
+        <v>511</v>
       </c>
       <c r="Q128" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R128" s="1" t="s">
-        <v>504</v>
+        <v>512</v>
       </c>
       <c r="T128" s="1" t="s">
-        <v>505</v>
+        <v>513</v>
       </c>
       <c r="Z128" s="1"/>
       <c r="AA128" s="1"/>
@@ -8821,7 +8855,7 @@
         <v>265</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>506</v>
+        <v>514</v>
       </c>
       <c r="C129" s="9"/>
       <c r="D129" s="9"/>
@@ -8839,37 +8873,37 @@
         <v>23</v>
       </c>
       <c r="J129" s="13" t="s">
-        <v>464</v>
+        <v>472</v>
       </c>
       <c r="K129" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L129" s="1" t="s">
-        <v>507</v>
+        <v>515</v>
       </c>
       <c r="M129" s="1" t="s">
-        <v>508</v>
+        <v>516</v>
       </c>
       <c r="O129" s="1" t="s">
-        <v>468</v>
+        <v>476</v>
       </c>
       <c r="P129" s="1" t="s">
-        <v>509</v>
+        <v>517</v>
       </c>
       <c r="Q129" s="1" t="n">
         <v>2</v>
       </c>
       <c r="R129" s="1" t="s">
-        <v>510</v>
+        <v>518</v>
       </c>
       <c r="S129" s="1" t="s">
-        <v>511</v>
+        <v>519</v>
       </c>
       <c r="T129" s="1" t="s">
-        <v>512</v>
+        <v>520</v>
       </c>
       <c r="U129" s="1" t="s">
-        <v>513</v>
+        <v>521</v>
       </c>
       <c r="Z129" s="1"/>
       <c r="AA129" s="1"/>
@@ -8895,7 +8929,7 @@
         <v>265</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>514</v>
+        <v>522</v>
       </c>
       <c r="C130" s="9"/>
       <c r="D130" s="9"/>
@@ -8913,37 +8947,37 @@
         <v>23</v>
       </c>
       <c r="J130" s="13" t="s">
-        <v>464</v>
+        <v>472</v>
       </c>
       <c r="K130" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L130" s="1" t="s">
-        <v>515</v>
+        <v>523</v>
       </c>
       <c r="M130" s="1" t="s">
-        <v>516</v>
+        <v>524</v>
       </c>
       <c r="O130" s="1" t="s">
-        <v>468</v>
+        <v>476</v>
       </c>
       <c r="P130" s="1" t="s">
-        <v>517</v>
+        <v>525</v>
       </c>
       <c r="Q130" s="1" t="n">
         <v>2</v>
       </c>
       <c r="R130" s="1" t="s">
-        <v>518</v>
+        <v>526</v>
       </c>
       <c r="S130" s="1" t="s">
-        <v>519</v>
+        <v>527</v>
       </c>
       <c r="T130" s="1" t="s">
-        <v>520</v>
+        <v>528</v>
       </c>
       <c r="U130" s="1" t="s">
-        <v>521</v>
+        <v>529</v>
       </c>
       <c r="Z130" s="1"/>
       <c r="AA130" s="1"/>
@@ -8969,7 +9003,7 @@
         <v>265</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>522</v>
+        <v>530</v>
       </c>
       <c r="C131" s="9"/>
       <c r="D131" s="9"/>
@@ -8987,34 +9021,34 @@
         <v>23</v>
       </c>
       <c r="J131" s="13" t="s">
-        <v>464</v>
+        <v>472</v>
       </c>
       <c r="K131" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L131" s="1" t="s">
-        <v>523</v>
+        <v>531</v>
       </c>
       <c r="M131" s="1" t="s">
-        <v>524</v>
+        <v>532</v>
       </c>
       <c r="O131" s="1" t="s">
-        <v>468</v>
+        <v>476</v>
       </c>
       <c r="P131" s="1" t="s">
-        <v>525</v>
+        <v>533</v>
       </c>
       <c r="Q131" s="1" t="n">
         <v>2</v>
       </c>
       <c r="S131" s="1" t="s">
-        <v>526</v>
+        <v>534</v>
       </c>
       <c r="T131" s="1" t="s">
-        <v>527</v>
+        <v>535</v>
       </c>
       <c r="U131" s="1" t="s">
-        <v>521</v>
+        <v>529</v>
       </c>
       <c r="Z131" s="1"/>
       <c r="AA131" s="1"/>
@@ -9040,7 +9074,7 @@
         <v>265</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>528</v>
+        <v>536</v>
       </c>
       <c r="C132" s="9"/>
       <c r="D132" s="9"/>
@@ -9058,34 +9092,34 @@
         <v>23</v>
       </c>
       <c r="J132" s="13" t="s">
-        <v>464</v>
+        <v>472</v>
       </c>
       <c r="K132" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L132" s="1" t="s">
-        <v>529</v>
+        <v>537</v>
       </c>
       <c r="M132" s="1" t="s">
-        <v>530</v>
+        <v>538</v>
       </c>
       <c r="O132" s="1" t="s">
         <v>333</v>
       </c>
       <c r="P132" s="1" t="s">
-        <v>531</v>
+        <v>539</v>
       </c>
       <c r="Q132" s="1" t="n">
         <v>1</v>
       </c>
       <c r="S132" s="1" t="s">
-        <v>532</v>
+        <v>540</v>
       </c>
       <c r="T132" s="1" t="s">
-        <v>533</v>
+        <v>541</v>
       </c>
       <c r="U132" s="1" t="s">
-        <v>534</v>
+        <v>542</v>
       </c>
       <c r="Z132" s="1"/>
       <c r="AA132" s="1"/>
@@ -9111,7 +9145,7 @@
         <v>265</v>
       </c>
       <c r="B133" s="9" t="s">
-        <v>535</v>
+        <v>543</v>
       </c>
       <c r="C133" s="9"/>
       <c r="D133" s="9"/>
@@ -9129,37 +9163,37 @@
         <v>23</v>
       </c>
       <c r="J133" s="13" t="s">
-        <v>464</v>
+        <v>472</v>
       </c>
       <c r="K133" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L133" s="1" t="s">
-        <v>536</v>
+        <v>544</v>
       </c>
       <c r="M133" s="1" t="s">
-        <v>537</v>
+        <v>545</v>
       </c>
       <c r="O133" s="1" t="s">
         <v>333</v>
       </c>
       <c r="P133" s="1" t="s">
-        <v>538</v>
+        <v>546</v>
       </c>
       <c r="Q133" s="1" t="n">
         <v>2</v>
       </c>
       <c r="R133" s="1" t="s">
-        <v>539</v>
+        <v>547</v>
       </c>
       <c r="S133" s="1" t="s">
-        <v>532</v>
+        <v>540</v>
       </c>
       <c r="T133" s="1" t="s">
-        <v>540</v>
+        <v>548</v>
       </c>
       <c r="U133" s="1" t="s">
-        <v>534</v>
+        <v>542</v>
       </c>
       <c r="Z133" s="1"/>
       <c r="AA133" s="1"/>
@@ -9185,7 +9219,7 @@
         <v>265</v>
       </c>
       <c r="B134" s="9" t="s">
-        <v>541</v>
+        <v>549</v>
       </c>
       <c r="C134" s="9"/>
       <c r="D134" s="9"/>
@@ -9203,37 +9237,37 @@
         <v>23</v>
       </c>
       <c r="J134" s="13" t="s">
-        <v>464</v>
+        <v>472</v>
       </c>
       <c r="K134" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L134" s="1" t="s">
-        <v>542</v>
+        <v>550</v>
       </c>
       <c r="M134" s="1" t="s">
-        <v>543</v>
+        <v>551</v>
       </c>
       <c r="O134" s="1" t="s">
         <v>333</v>
       </c>
       <c r="P134" s="1" t="s">
-        <v>544</v>
+        <v>552</v>
       </c>
       <c r="Q134" s="1" t="n">
         <v>2</v>
       </c>
       <c r="R134" s="1" t="s">
-        <v>545</v>
+        <v>553</v>
       </c>
       <c r="S134" s="1" t="s">
-        <v>532</v>
+        <v>540</v>
       </c>
       <c r="T134" s="1" t="s">
-        <v>546</v>
+        <v>554</v>
       </c>
       <c r="U134" s="1" t="s">
-        <v>534</v>
+        <v>542</v>
       </c>
       <c r="Z134" s="1"/>
       <c r="AA134" s="1"/>
@@ -9259,7 +9293,7 @@
         <v>265</v>
       </c>
       <c r="B135" s="9" t="s">
-        <v>547</v>
+        <v>555</v>
       </c>
       <c r="C135" s="9"/>
       <c r="D135" s="9"/>
@@ -9277,37 +9311,37 @@
         <v>23</v>
       </c>
       <c r="J135" s="13" t="s">
-        <v>464</v>
+        <v>472</v>
       </c>
       <c r="K135" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L135" s="1" t="s">
-        <v>548</v>
+        <v>556</v>
       </c>
       <c r="M135" s="1" t="s">
-        <v>549</v>
+        <v>557</v>
       </c>
       <c r="O135" s="1" t="s">
-        <v>468</v>
+        <v>476</v>
       </c>
       <c r="P135" s="1" t="s">
-        <v>550</v>
+        <v>558</v>
       </c>
       <c r="Q135" s="1" t="s">
-        <v>551</v>
+        <v>559</v>
       </c>
       <c r="R135" s="1" t="s">
-        <v>552</v>
+        <v>560</v>
       </c>
       <c r="S135" s="1" t="s">
-        <v>553</v>
+        <v>561</v>
       </c>
       <c r="T135" s="1" t="s">
-        <v>554</v>
+        <v>562</v>
       </c>
       <c r="U135" s="1" t="s">
-        <v>555</v>
+        <v>563</v>
       </c>
       <c r="Z135" s="1"/>
       <c r="AA135" s="1"/>
@@ -9333,7 +9367,7 @@
         <v>265</v>
       </c>
       <c r="B136" s="9" t="s">
-        <v>556</v>
+        <v>564</v>
       </c>
       <c r="C136" s="9"/>
       <c r="D136" s="9"/>
@@ -9351,37 +9385,37 @@
         <v>23</v>
       </c>
       <c r="J136" s="13" t="s">
-        <v>464</v>
+        <v>472</v>
       </c>
       <c r="K136" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L136" s="1" t="s">
-        <v>557</v>
+        <v>565</v>
       </c>
       <c r="M136" s="1" t="s">
-        <v>558</v>
+        <v>566</v>
       </c>
       <c r="O136" s="1" t="s">
-        <v>468</v>
+        <v>476</v>
       </c>
       <c r="P136" s="1" t="s">
-        <v>559</v>
+        <v>567</v>
       </c>
       <c r="Q136" s="1" t="n">
         <v>2</v>
       </c>
       <c r="R136" s="1" t="s">
-        <v>545</v>
+        <v>553</v>
       </c>
       <c r="S136" s="1" t="s">
-        <v>471</v>
+        <v>479</v>
       </c>
       <c r="T136" s="1" t="s">
-        <v>560</v>
+        <v>568</v>
       </c>
       <c r="U136" s="1" t="s">
-        <v>484</v>
+        <v>492</v>
       </c>
       <c r="Z136" s="1"/>
       <c r="AA136" s="1"/>
@@ -9407,7 +9441,7 @@
         <v>265</v>
       </c>
       <c r="B137" s="9" t="s">
-        <v>561</v>
+        <v>569</v>
       </c>
       <c r="C137" s="9"/>
       <c r="D137" s="9"/>
@@ -9425,37 +9459,37 @@
         <v>23</v>
       </c>
       <c r="J137" s="13" t="s">
-        <v>464</v>
+        <v>472</v>
       </c>
       <c r="K137" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L137" s="1" t="s">
-        <v>562</v>
+        <v>570</v>
       </c>
       <c r="M137" s="1" t="s">
-        <v>563</v>
+        <v>571</v>
       </c>
       <c r="O137" s="1" t="s">
-        <v>468</v>
+        <v>476</v>
       </c>
       <c r="P137" s="1" t="s">
-        <v>564</v>
+        <v>572</v>
       </c>
       <c r="Q137" s="1" t="n">
         <v>3</v>
       </c>
       <c r="R137" s="1" t="s">
-        <v>565</v>
+        <v>573</v>
       </c>
       <c r="S137" s="1" t="s">
-        <v>566</v>
+        <v>574</v>
       </c>
       <c r="T137" s="1" t="s">
-        <v>567</v>
+        <v>575</v>
       </c>
       <c r="U137" s="1" t="s">
-        <v>568</v>
+        <v>576</v>
       </c>
       <c r="Z137" s="1"/>
       <c r="AA137" s="1"/>
@@ -9481,7 +9515,7 @@
         <v>265</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>569</v>
+        <v>577</v>
       </c>
       <c r="C138" s="9"/>
       <c r="D138" s="9"/>
@@ -9499,34 +9533,34 @@
         <v>23</v>
       </c>
       <c r="J138" s="13" t="s">
-        <v>464</v>
+        <v>472</v>
       </c>
       <c r="K138" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L138" s="1" t="s">
-        <v>570</v>
+        <v>578</v>
       </c>
       <c r="M138" s="1" t="s">
-        <v>571</v>
+        <v>579</v>
       </c>
       <c r="O138" s="1" t="s">
         <v>333</v>
       </c>
       <c r="P138" s="1" t="s">
-        <v>572</v>
+        <v>580</v>
       </c>
       <c r="Q138" s="1" t="n">
         <v>2</v>
       </c>
       <c r="S138" s="1" t="s">
-        <v>573</v>
+        <v>581</v>
       </c>
       <c r="T138" s="1" t="s">
-        <v>574</v>
+        <v>582</v>
       </c>
       <c r="U138" s="1" t="s">
-        <v>575</v>
+        <v>583</v>
       </c>
       <c r="Z138" s="1"/>
       <c r="AA138" s="1"/>
@@ -9552,7 +9586,7 @@
         <v>265</v>
       </c>
       <c r="B139" s="9" t="s">
-        <v>576</v>
+        <v>584</v>
       </c>
       <c r="C139" s="9"/>
       <c r="D139" s="9"/>
@@ -9570,31 +9604,31 @@
         <v>23</v>
       </c>
       <c r="J139" s="13" t="s">
-        <v>464</v>
+        <v>472</v>
       </c>
       <c r="K139" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L139" s="1" t="s">
-        <v>577</v>
+        <v>585</v>
       </c>
       <c r="M139" s="1" t="s">
-        <v>578</v>
+        <v>586</v>
       </c>
       <c r="P139" s="1" t="s">
-        <v>579</v>
+        <v>587</v>
       </c>
       <c r="Q139" s="1" t="n">
         <v>2</v>
       </c>
       <c r="S139" s="1" t="s">
-        <v>580</v>
+        <v>588</v>
       </c>
       <c r="T139" s="1" t="s">
-        <v>581</v>
+        <v>589</v>
       </c>
       <c r="U139" s="1" t="s">
-        <v>582</v>
+        <v>590</v>
       </c>
       <c r="Z139" s="1"/>
       <c r="AA139" s="1"/>
@@ -9618,11 +9652,11 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="140">
       <c r="A140" s="9"/>
       <c r="B140" s="9" t="s">
-        <v>583</v>
+        <v>591</v>
       </c>
       <c r="C140" s="9"/>
       <c r="D140" s="9" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
       <c r="E140" s="9"/>
       <c r="F140" s="9"/>
@@ -9636,34 +9670,34 @@
         <v>23</v>
       </c>
       <c r="J140" s="13" t="s">
-        <v>464</v>
+        <v>472</v>
       </c>
       <c r="K140" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L140" s="1" t="s">
-        <v>584</v>
+        <v>592</v>
       </c>
       <c r="M140" s="1" t="s">
-        <v>585</v>
+        <v>593</v>
       </c>
       <c r="O140" s="1" t="s">
-        <v>586</v>
+        <v>594</v>
       </c>
       <c r="P140" s="1" t="s">
-        <v>587</v>
+        <v>595</v>
       </c>
       <c r="Q140" s="1" t="n">
         <v>1</v>
       </c>
       <c r="S140" s="1" t="s">
-        <v>532</v>
+        <v>540</v>
       </c>
       <c r="T140" s="1" t="s">
-        <v>588</v>
+        <v>596</v>
       </c>
       <c r="U140" s="1" t="s">
-        <v>534</v>
+        <v>542</v>
       </c>
       <c r="Z140" s="1"/>
       <c r="AA140" s="1"/>
@@ -9687,11 +9721,11 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="141">
       <c r="A141" s="9"/>
       <c r="B141" s="9" t="s">
-        <v>589</v>
+        <v>597</v>
       </c>
       <c r="C141" s="9"/>
       <c r="D141" s="9" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
       <c r="E141" s="9"/>
       <c r="F141" s="9"/>
@@ -9705,34 +9739,34 @@
         <v>23</v>
       </c>
       <c r="J141" s="13" t="s">
-        <v>464</v>
+        <v>472</v>
       </c>
       <c r="K141" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L141" s="1" t="s">
-        <v>590</v>
+        <v>598</v>
       </c>
       <c r="M141" s="1" t="s">
-        <v>591</v>
+        <v>599</v>
       </c>
       <c r="O141" s="1" t="s">
-        <v>586</v>
+        <v>594</v>
       </c>
       <c r="P141" s="1" t="s">
-        <v>592</v>
+        <v>600</v>
       </c>
       <c r="Q141" s="1" t="n">
         <v>1</v>
       </c>
       <c r="S141" s="1" t="s">
-        <v>532</v>
+        <v>540</v>
       </c>
       <c r="T141" s="1" t="s">
-        <v>593</v>
+        <v>601</v>
       </c>
       <c r="U141" s="1" t="s">
-        <v>534</v>
+        <v>542</v>
       </c>
       <c r="Z141" s="1"/>
       <c r="AA141" s="1"/>
@@ -9761,7 +9795,7 @@
         <v>143</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>594</v>
+        <v>602</v>
       </c>
       <c r="E142" s="9" t="s">
         <v>23</v>
@@ -9779,46 +9813,46 @@
         <v>23</v>
       </c>
       <c r="J142" s="9" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="K142" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L142" s="1" t="s">
-        <v>596</v>
+        <v>604</v>
       </c>
       <c r="M142" s="1" t="s">
-        <v>597</v>
+        <v>605</v>
       </c>
       <c r="N142" s="1" t="s">
-        <v>598</v>
+        <v>606</v>
       </c>
       <c r="O142" s="1" t="s">
-        <v>599</v>
+        <v>607</v>
       </c>
       <c r="P142" s="1" t="s">
-        <v>600</v>
+        <v>608</v>
       </c>
       <c r="Q142" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R142" s="1" t="s">
-        <v>601</v>
+        <v>609</v>
       </c>
       <c r="S142" s="1" t="s">
-        <v>602</v>
+        <v>610</v>
       </c>
       <c r="V142" s="1" t="s">
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="W142" s="1" t="s">
-        <v>604</v>
+        <v>612</v>
       </c>
       <c r="X142" s="1" t="s">
-        <v>605</v>
+        <v>613</v>
       </c>
       <c r="Y142" s="1" t="s">
-        <v>606</v>
+        <v>614</v>
       </c>
       <c r="Z142" s="1"/>
       <c r="AA142" s="1"/>
@@ -9844,7 +9878,7 @@
         <v>262</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>607</v>
+        <v>615</v>
       </c>
       <c r="E143" s="9" t="s">
         <v>24</v>
@@ -9862,31 +9896,31 @@
         <v>23</v>
       </c>
       <c r="J143" s="9" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="K143" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L143" s="1" t="s">
-        <v>608</v>
+        <v>616</v>
       </c>
       <c r="M143" s="1" t="s">
-        <v>609</v>
+        <v>617</v>
       </c>
       <c r="N143" s="1" t="s">
-        <v>610</v>
+        <v>618</v>
       </c>
       <c r="O143" s="1" t="s">
-        <v>599</v>
+        <v>607</v>
       </c>
       <c r="P143" s="1" t="s">
-        <v>476</v>
+        <v>484</v>
       </c>
       <c r="Q143" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R143" s="1" t="s">
-        <v>611</v>
+        <v>619</v>
       </c>
       <c r="Z143" s="1"/>
       <c r="AA143" s="1"/>
@@ -9912,7 +9946,7 @@
         <v>262</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>485</v>
+        <v>493</v>
       </c>
       <c r="E144" s="9" t="s">
         <v>23</v>
@@ -9930,31 +9964,31 @@
         <v>23</v>
       </c>
       <c r="J144" s="9" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="K144" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L144" s="1" t="s">
-        <v>612</v>
+        <v>620</v>
       </c>
       <c r="M144" s="1" t="s">
-        <v>613</v>
+        <v>621</v>
       </c>
       <c r="N144" s="1" t="s">
-        <v>488</v>
+        <v>496</v>
       </c>
       <c r="O144" s="1" t="s">
-        <v>599</v>
+        <v>607</v>
       </c>
       <c r="P144" s="1" t="s">
-        <v>614</v>
+        <v>622</v>
       </c>
       <c r="Q144" s="1" t="n">
         <v>2</v>
       </c>
       <c r="R144" s="1" t="s">
-        <v>615</v>
+        <v>623</v>
       </c>
       <c r="Z144" s="1"/>
       <c r="AA144" s="1"/>
@@ -9980,7 +10014,7 @@
         <v>262</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>616</v>
+        <v>624</v>
       </c>
       <c r="E145" s="9" t="s">
         <v>23</v>
@@ -9995,28 +10029,28 @@
         <v>23</v>
       </c>
       <c r="J145" s="9" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="K145" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L145" s="1" t="s">
-        <v>617</v>
+        <v>625</v>
       </c>
       <c r="M145" s="1" t="s">
-        <v>618</v>
+        <v>626</v>
       </c>
       <c r="O145" s="1" t="s">
-        <v>599</v>
+        <v>607</v>
       </c>
       <c r="P145" s="1" t="s">
-        <v>619</v>
+        <v>627</v>
       </c>
       <c r="Q145" s="1" t="n">
         <v>2</v>
       </c>
       <c r="R145" s="1" t="s">
-        <v>620</v>
+        <v>628</v>
       </c>
       <c r="Z145" s="1"/>
       <c r="AA145" s="1"/>
@@ -10042,7 +10076,7 @@
         <v>262</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>621</v>
+        <v>629</v>
       </c>
       <c r="E146" s="9" t="s">
         <v>23</v>
@@ -10057,25 +10091,25 @@
         <v>23</v>
       </c>
       <c r="J146" s="9" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="K146" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L146" s="1" t="s">
-        <v>622</v>
+        <v>630</v>
       </c>
       <c r="M146" s="1" t="s">
-        <v>623</v>
+        <v>631</v>
       </c>
       <c r="O146" s="1" t="s">
-        <v>624</v>
+        <v>632</v>
       </c>
       <c r="Q146" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R146" s="1" t="s">
-        <v>625</v>
+        <v>633</v>
       </c>
       <c r="Z146" s="1"/>
       <c r="AA146" s="1"/>
@@ -10104,7 +10138,7 @@
         <v>102</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>626</v>
+        <v>634</v>
       </c>
       <c r="E147" s="9" t="s">
         <v>23</v>
@@ -10122,31 +10156,31 @@
         <v>23</v>
       </c>
       <c r="J147" s="9" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="K147" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L147" s="1" t="s">
-        <v>627</v>
+        <v>635</v>
       </c>
       <c r="M147" s="1" t="s">
-        <v>628</v>
+        <v>636</v>
       </c>
       <c r="N147" s="1" t="s">
-        <v>629</v>
+        <v>637</v>
       </c>
       <c r="O147" s="1" t="s">
-        <v>624</v>
+        <v>632</v>
       </c>
       <c r="P147" s="1" t="s">
-        <v>630</v>
+        <v>638</v>
       </c>
       <c r="Q147" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R147" s="1" t="s">
-        <v>631</v>
+        <v>639</v>
       </c>
       <c r="Z147" s="1"/>
       <c r="AA147" s="1"/>
@@ -10172,7 +10206,7 @@
         <v>262</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>632</v>
+        <v>640</v>
       </c>
       <c r="E148" s="9" t="s">
         <v>23</v>
@@ -10187,43 +10221,43 @@
         <v>23</v>
       </c>
       <c r="J148" s="9" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="K148" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L148" s="1" t="s">
-        <v>633</v>
+        <v>641</v>
       </c>
       <c r="M148" s="1" t="s">
-        <v>634</v>
+        <v>642</v>
       </c>
       <c r="O148" s="1" t="s">
-        <v>635</v>
+        <v>643</v>
       </c>
       <c r="P148" s="1" t="s">
-        <v>636</v>
+        <v>644</v>
       </c>
       <c r="Q148" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R148" s="1" t="s">
-        <v>637</v>
+        <v>645</v>
       </c>
       <c r="S148" s="1" t="s">
-        <v>638</v>
+        <v>646</v>
       </c>
       <c r="V148" s="1" t="s">
-        <v>639</v>
+        <v>647</v>
       </c>
       <c r="W148" s="1" t="s">
-        <v>640</v>
+        <v>648</v>
       </c>
       <c r="X148" s="1" t="s">
-        <v>641</v>
+        <v>649</v>
       </c>
       <c r="Y148" s="1" t="s">
-        <v>642</v>
+        <v>650</v>
       </c>
       <c r="Z148" s="1"/>
       <c r="AA148" s="1"/>
@@ -10249,7 +10283,7 @@
         <v>262</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="E149" s="9" t="s">
         <v>23</v>
@@ -10264,31 +10298,31 @@
         <v>23</v>
       </c>
       <c r="J149" s="9" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="K149" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L149" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="M149" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="O149" s="1" t="s">
         <v>643</v>
       </c>
-      <c r="M149" s="1" t="s">
-        <v>644</v>
-      </c>
-      <c r="O149" s="1" t="s">
-        <v>635</v>
-      </c>
       <c r="P149" s="1" t="s">
-        <v>645</v>
+        <v>653</v>
       </c>
       <c r="Q149" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R149" s="1" t="s">
-        <v>646</v>
+        <v>654</v>
       </c>
       <c r="W149" s="1" t="s">
-        <v>647</v>
+        <v>655</v>
       </c>
       <c r="Z149" s="1"/>
       <c r="AA149" s="1"/>
@@ -10314,7 +10348,7 @@
         <v>262</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>500</v>
+        <v>508</v>
       </c>
       <c r="E150" s="9" t="s">
         <v>23</v>
@@ -10329,31 +10363,31 @@
         <v>23</v>
       </c>
       <c r="J150" s="9" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="K150" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L150" s="1" t="s">
-        <v>648</v>
+        <v>656</v>
       </c>
       <c r="M150" s="1" t="s">
-        <v>649</v>
+        <v>657</v>
       </c>
       <c r="O150" s="1" t="s">
-        <v>635</v>
+        <v>643</v>
       </c>
       <c r="P150" s="1" t="s">
-        <v>650</v>
+        <v>658</v>
       </c>
       <c r="Q150" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R150" s="1" t="s">
-        <v>651</v>
+        <v>659</v>
       </c>
       <c r="U150" s="1" t="s">
-        <v>652</v>
+        <v>660</v>
       </c>
       <c r="Z150" s="1"/>
       <c r="AA150" s="1"/>
@@ -10379,7 +10413,7 @@
         <v>262</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>653</v>
+        <v>661</v>
       </c>
       <c r="E151" s="9" t="s">
         <v>23</v>
@@ -10397,37 +10431,37 @@
         <v>23</v>
       </c>
       <c r="J151" s="9" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="K151" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L151" s="1" t="s">
-        <v>654</v>
+        <v>662</v>
       </c>
       <c r="M151" s="1" t="s">
-        <v>655</v>
+        <v>663</v>
       </c>
       <c r="O151" s="1" t="s">
-        <v>599</v>
+        <v>607</v>
       </c>
       <c r="P151" s="1" t="s">
-        <v>656</v>
+        <v>664</v>
       </c>
       <c r="Q151" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R151" s="1" t="s">
-        <v>657</v>
+        <v>665</v>
       </c>
       <c r="S151" s="1" t="s">
-        <v>658</v>
+        <v>666</v>
       </c>
       <c r="T151" s="1" t="s">
-        <v>659</v>
+        <v>667</v>
       </c>
       <c r="V151" s="1" t="s">
-        <v>660</v>
+        <v>668</v>
       </c>
       <c r="Z151" s="1"/>
       <c r="AA151" s="1"/>
@@ -10453,7 +10487,7 @@
         <v>262</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>661</v>
+        <v>669</v>
       </c>
       <c r="E152" s="9" t="s">
         <v>23</v>
@@ -10471,31 +10505,31 @@
         <v>23</v>
       </c>
       <c r="J152" s="9" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="K152" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L152" s="1" t="s">
-        <v>662</v>
+        <v>670</v>
       </c>
       <c r="M152" s="1" t="s">
-        <v>663</v>
+        <v>671</v>
       </c>
       <c r="O152" s="1" t="s">
-        <v>599</v>
+        <v>607</v>
       </c>
       <c r="P152" s="1" t="s">
-        <v>664</v>
+        <v>672</v>
       </c>
       <c r="Q152" s="1" t="n">
         <v>1</v>
       </c>
       <c r="S152" s="1" t="s">
-        <v>665</v>
+        <v>673</v>
       </c>
       <c r="T152" s="1" t="s">
-        <v>666</v>
+        <v>674</v>
       </c>
       <c r="Z152" s="1"/>
       <c r="AA152" s="1"/>
@@ -10521,7 +10555,7 @@
         <v>262</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>667</v>
+        <v>675</v>
       </c>
       <c r="E153" s="9" t="s">
         <v>23</v>
@@ -10539,46 +10573,46 @@
         <v>23</v>
       </c>
       <c r="J153" s="9" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="K153" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L153" s="1" t="s">
-        <v>668</v>
+        <v>676</v>
       </c>
       <c r="M153" s="1" t="s">
-        <v>669</v>
+        <v>677</v>
       </c>
       <c r="O153" s="1" t="s">
-        <v>599</v>
+        <v>607</v>
       </c>
       <c r="P153" s="1" t="s">
-        <v>670</v>
+        <v>678</v>
       </c>
       <c r="Q153" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R153" s="1" t="s">
-        <v>671</v>
+        <v>679</v>
       </c>
       <c r="S153" s="1" t="s">
-        <v>665</v>
+        <v>673</v>
       </c>
       <c r="T153" s="1" t="s">
-        <v>666</v>
+        <v>674</v>
       </c>
       <c r="V153" s="1" t="s">
-        <v>672</v>
+        <v>680</v>
       </c>
       <c r="W153" s="1" t="s">
-        <v>673</v>
+        <v>681</v>
       </c>
       <c r="X153" s="1" t="s">
-        <v>674</v>
+        <v>682</v>
       </c>
       <c r="Y153" s="1" t="s">
-        <v>675</v>
+        <v>683</v>
       </c>
       <c r="Z153" s="1"/>
       <c r="AA153" s="1"/>
@@ -10604,7 +10638,7 @@
         <v>262</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>676</v>
+        <v>684</v>
       </c>
       <c r="E154" s="9" t="s">
         <v>23</v>
@@ -10622,40 +10656,40 @@
         <v>23</v>
       </c>
       <c r="J154" s="9" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="K154" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L154" s="1" t="s">
-        <v>677</v>
+        <v>685</v>
       </c>
       <c r="M154" s="1" t="s">
-        <v>678</v>
+        <v>686</v>
       </c>
       <c r="O154" s="1" t="s">
-        <v>599</v>
+        <v>607</v>
       </c>
       <c r="P154" s="1" t="s">
-        <v>679</v>
+        <v>687</v>
       </c>
       <c r="Q154" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R154" s="1" t="s">
-        <v>680</v>
+        <v>688</v>
       </c>
       <c r="S154" s="1" t="s">
-        <v>681</v>
+        <v>689</v>
       </c>
       <c r="T154" s="1" t="s">
-        <v>682</v>
+        <v>690</v>
       </c>
       <c r="U154" s="1" t="s">
-        <v>683</v>
+        <v>691</v>
       </c>
       <c r="W154" s="1" t="s">
-        <v>684</v>
+        <v>692</v>
       </c>
       <c r="Z154" s="1"/>
       <c r="AA154" s="1"/>
@@ -10681,7 +10715,7 @@
         <v>262</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>685</v>
+        <v>693</v>
       </c>
       <c r="E155" s="9" t="s">
         <v>23</v>
@@ -10696,31 +10730,31 @@
         <v>23</v>
       </c>
       <c r="J155" s="9" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="K155" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L155" s="1" t="s">
-        <v>686</v>
+        <v>694</v>
       </c>
       <c r="M155" s="1" t="s">
-        <v>687</v>
+        <v>695</v>
       </c>
       <c r="O155" s="1" t="s">
-        <v>688</v>
+        <v>696</v>
       </c>
       <c r="P155" s="1" t="s">
-        <v>689</v>
+        <v>697</v>
       </c>
       <c r="Q155" s="1" t="n">
         <v>2</v>
       </c>
       <c r="R155" s="1" t="s">
-        <v>690</v>
+        <v>698</v>
       </c>
       <c r="U155" s="1" t="s">
-        <v>691</v>
+        <v>699</v>
       </c>
       <c r="Z155" s="1"/>
       <c r="AA155" s="1"/>
@@ -10746,7 +10780,7 @@
         <v>262</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>692</v>
+        <v>700</v>
       </c>
       <c r="E156" s="9" t="s">
         <v>23</v>
@@ -10764,46 +10798,46 @@
         <v>23</v>
       </c>
       <c r="J156" s="9" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="K156" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L156" s="1" t="s">
-        <v>693</v>
+        <v>701</v>
       </c>
       <c r="M156" s="1" t="s">
-        <v>694</v>
+        <v>702</v>
       </c>
       <c r="O156" s="1" t="s">
-        <v>599</v>
+        <v>607</v>
       </c>
       <c r="P156" s="1" t="s">
-        <v>695</v>
+        <v>703</v>
       </c>
       <c r="Q156" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R156" s="1" t="s">
-        <v>696</v>
+        <v>704</v>
       </c>
       <c r="S156" s="1" t="s">
-        <v>697</v>
+        <v>705</v>
       </c>
       <c r="T156" s="1" t="s">
-        <v>698</v>
+        <v>706</v>
       </c>
       <c r="U156" s="1" t="s">
-        <v>699</v>
+        <v>707</v>
       </c>
       <c r="V156" s="1" t="s">
-        <v>700</v>
+        <v>708</v>
       </c>
       <c r="W156" s="1" t="s">
-        <v>701</v>
+        <v>709</v>
       </c>
       <c r="Y156" s="1" t="s">
-        <v>702</v>
+        <v>710</v>
       </c>
       <c r="Z156" s="1"/>
       <c r="AA156" s="1"/>
@@ -10829,7 +10863,7 @@
         <v>262</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>703</v>
+        <v>711</v>
       </c>
       <c r="E157" s="9" t="s">
         <v>23</v>
@@ -10844,34 +10878,34 @@
         <v>23</v>
       </c>
       <c r="J157" s="9" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="K157" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L157" s="1" t="s">
-        <v>704</v>
+        <v>712</v>
       </c>
       <c r="M157" s="1" t="s">
-        <v>705</v>
+        <v>713</v>
       </c>
       <c r="O157" s="1" t="s">
-        <v>599</v>
+        <v>607</v>
       </c>
       <c r="P157" s="1" t="s">
-        <v>706</v>
+        <v>714</v>
       </c>
       <c r="Q157" s="1" t="n">
         <v>2</v>
       </c>
       <c r="R157" s="1" t="s">
-        <v>707</v>
+        <v>715</v>
       </c>
       <c r="S157" s="1" t="s">
-        <v>708</v>
+        <v>716</v>
       </c>
       <c r="U157" s="1" t="s">
-        <v>709</v>
+        <v>717</v>
       </c>
       <c r="Z157" s="1"/>
       <c r="AA157" s="1"/>
@@ -10897,7 +10931,7 @@
         <v>262</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>710</v>
+        <v>718</v>
       </c>
       <c r="E158" s="9" t="s">
         <v>23</v>
@@ -10912,43 +10946,43 @@
         <v>23</v>
       </c>
       <c r="J158" s="9" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="K158" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L158" s="1" t="s">
-        <v>711</v>
+        <v>719</v>
       </c>
       <c r="M158" s="1" t="s">
-        <v>712</v>
+        <v>720</v>
       </c>
       <c r="O158" s="1" t="s">
-        <v>599</v>
+        <v>607</v>
       </c>
       <c r="P158" s="1" t="s">
-        <v>713</v>
+        <v>721</v>
       </c>
       <c r="Q158" s="1" t="n">
         <v>1</v>
       </c>
       <c r="S158" s="14" t="s">
-        <v>714</v>
+        <v>722</v>
       </c>
       <c r="T158" s="1" t="s">
-        <v>534</v>
+        <v>542</v>
       </c>
       <c r="U158" s="1" t="s">
-        <v>715</v>
+        <v>723</v>
       </c>
       <c r="V158" s="1" t="s">
-        <v>716</v>
+        <v>724</v>
       </c>
       <c r="W158" s="1" t="s">
-        <v>717</v>
+        <v>725</v>
       </c>
       <c r="Y158" s="1" t="s">
-        <v>718</v>
+        <v>726</v>
       </c>
       <c r="Z158" s="1"/>
       <c r="AA158" s="1"/>
@@ -10974,7 +11008,7 @@
         <v>262</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>719</v>
+        <v>727</v>
       </c>
       <c r="E159" s="9" t="s">
         <v>23</v>
@@ -10989,37 +11023,37 @@
         <v>23</v>
       </c>
       <c r="J159" s="9" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="K159" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L159" s="1" t="s">
-        <v>720</v>
+        <v>728</v>
       </c>
       <c r="M159" s="1" t="s">
-        <v>721</v>
+        <v>729</v>
       </c>
       <c r="O159" s="1" t="s">
-        <v>599</v>
+        <v>607</v>
       </c>
       <c r="P159" s="1" t="s">
-        <v>722</v>
+        <v>730</v>
       </c>
       <c r="Q159" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R159" s="1" t="s">
-        <v>723</v>
+        <v>731</v>
       </c>
       <c r="S159" s="14" t="s">
-        <v>724</v>
+        <v>732</v>
       </c>
       <c r="T159" s="1" t="s">
-        <v>534</v>
+        <v>542</v>
       </c>
       <c r="U159" s="1" t="s">
-        <v>725</v>
+        <v>733</v>
       </c>
       <c r="Z159" s="1"/>
       <c r="AA159" s="1"/>
@@ -11045,7 +11079,7 @@
         <v>262</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>726</v>
+        <v>734</v>
       </c>
       <c r="E160" s="9" t="s">
         <v>23</v>
@@ -11060,37 +11094,37 @@
         <v>23</v>
       </c>
       <c r="J160" s="9" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="K160" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L160" s="1" t="s">
-        <v>727</v>
+        <v>735</v>
       </c>
       <c r="M160" s="1" t="s">
-        <v>728</v>
+        <v>736</v>
       </c>
       <c r="O160" s="1" t="s">
-        <v>599</v>
+        <v>607</v>
       </c>
       <c r="P160" s="1" t="s">
-        <v>729</v>
+        <v>737</v>
       </c>
       <c r="Q160" s="1" t="n">
         <v>2</v>
       </c>
       <c r="R160" s="1" t="s">
-        <v>730</v>
+        <v>738</v>
       </c>
       <c r="S160" s="1" t="s">
-        <v>731</v>
+        <v>739</v>
       </c>
       <c r="U160" s="1" t="s">
-        <v>652</v>
+        <v>660</v>
       </c>
       <c r="V160" s="1" t="s">
-        <v>732</v>
+        <v>740</v>
       </c>
       <c r="Z160" s="1"/>
       <c r="AA160" s="1"/>
@@ -11116,7 +11150,7 @@
         <v>262</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>733</v>
+        <v>741</v>
       </c>
       <c r="E161" s="9" t="s">
         <v>23</v>
@@ -11131,40 +11165,40 @@
         <v>23</v>
       </c>
       <c r="J161" s="9" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="K161" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L161" s="1" t="s">
-        <v>734</v>
+        <v>742</v>
       </c>
       <c r="M161" s="1" t="s">
-        <v>735</v>
+        <v>743</v>
       </c>
       <c r="O161" s="1" t="s">
-        <v>599</v>
+        <v>607</v>
       </c>
       <c r="P161" s="1" t="s">
-        <v>736</v>
+        <v>744</v>
       </c>
       <c r="Q161" s="1" t="n">
         <v>2</v>
       </c>
       <c r="R161" s="1" t="s">
-        <v>737</v>
+        <v>745</v>
       </c>
       <c r="S161" s="14" t="s">
-        <v>738</v>
+        <v>746</v>
       </c>
       <c r="T161" s="1" t="s">
-        <v>534</v>
+        <v>542</v>
       </c>
       <c r="U161" s="1" t="s">
-        <v>739</v>
+        <v>747</v>
       </c>
       <c r="Y161" s="1" t="s">
-        <v>740</v>
+        <v>748</v>
       </c>
       <c r="Z161" s="1"/>
       <c r="AA161" s="1"/>
@@ -11190,7 +11224,7 @@
         <v>262</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>741</v>
+        <v>749</v>
       </c>
       <c r="E162" s="9" t="s">
         <v>23</v>
@@ -11205,37 +11239,37 @@
         <v>23</v>
       </c>
       <c r="J162" s="9" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="K162" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L162" s="1" t="s">
-        <v>742</v>
+        <v>750</v>
       </c>
       <c r="M162" s="1" t="s">
-        <v>743</v>
+        <v>751</v>
       </c>
       <c r="O162" s="1" t="s">
-        <v>635</v>
+        <v>643</v>
       </c>
       <c r="P162" s="1" t="s">
-        <v>744</v>
+        <v>752</v>
       </c>
       <c r="Q162" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R162" s="1" t="s">
-        <v>745</v>
+        <v>753</v>
       </c>
       <c r="S162" s="1" t="s">
-        <v>746</v>
+        <v>754</v>
       </c>
       <c r="U162" s="1" t="s">
-        <v>747</v>
+        <v>755</v>
       </c>
       <c r="W162" s="1" t="s">
-        <v>748</v>
+        <v>756</v>
       </c>
       <c r="Z162" s="1"/>
       <c r="AA162" s="1"/>
@@ -11261,7 +11295,7 @@
         <v>262</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>749</v>
+        <v>757</v>
       </c>
       <c r="E163" s="9" t="s">
         <v>23</v>
@@ -11276,31 +11310,31 @@
         <v>23</v>
       </c>
       <c r="J163" s="9" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="K163" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L163" s="1" t="s">
-        <v>750</v>
+        <v>758</v>
       </c>
       <c r="M163" s="1" t="s">
-        <v>751</v>
+        <v>759</v>
       </c>
       <c r="O163" s="1" t="s">
-        <v>599</v>
+        <v>607</v>
       </c>
       <c r="P163" s="1" t="s">
-        <v>752</v>
+        <v>760</v>
       </c>
       <c r="Q163" s="1" t="n">
         <v>2</v>
       </c>
       <c r="R163" s="1" t="s">
-        <v>753</v>
+        <v>761</v>
       </c>
       <c r="U163" s="1" t="s">
-        <v>754</v>
+        <v>762</v>
       </c>
       <c r="Z163" s="1"/>
       <c r="AA163" s="1"/>
@@ -11326,7 +11360,7 @@
         <v>262</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>755</v>
+        <v>763</v>
       </c>
       <c r="E164" s="9" t="s">
         <v>23</v>
@@ -11341,37 +11375,37 @@
         <v>23</v>
       </c>
       <c r="J164" s="9" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="K164" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L164" s="1" t="s">
-        <v>756</v>
+        <v>764</v>
       </c>
       <c r="M164" s="1" t="s">
-        <v>757</v>
+        <v>765</v>
       </c>
       <c r="O164" s="1" t="s">
-        <v>599</v>
+        <v>607</v>
       </c>
       <c r="P164" s="1" t="s">
-        <v>758</v>
+        <v>766</v>
       </c>
       <c r="Q164" s="1" t="n">
         <v>1</v>
       </c>
       <c r="R164" s="1" t="s">
-        <v>759</v>
+        <v>767</v>
       </c>
       <c r="S164" s="1" t="s">
-        <v>760</v>
+        <v>768</v>
       </c>
       <c r="T164" s="1" t="s">
-        <v>761</v>
+        <v>769</v>
       </c>
       <c r="U164" s="1" t="s">
-        <v>762</v>
+        <v>770</v>
       </c>
       <c r="Z164" s="1"/>
       <c r="AA164" s="1"/>
@@ -11397,7 +11431,7 @@
         <v>262</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>763</v>
+        <v>771</v>
       </c>
       <c r="E165" s="9" t="s">
         <v>23</v>
@@ -11406,46 +11440,46 @@
         <v>23</v>
       </c>
       <c r="H165" s="9" t="s">
-        <v>441</v>
+        <v>449</v>
       </c>
       <c r="I165" s="7" t="s">
         <v>23</v>
       </c>
       <c r="J165" s="9" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="K165" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L165" s="1" t="s">
-        <v>764</v>
+        <v>772</v>
       </c>
       <c r="M165" s="1" t="s">
-        <v>765</v>
+        <v>773</v>
       </c>
       <c r="O165" s="1" t="s">
-        <v>599</v>
+        <v>607</v>
       </c>
       <c r="P165" s="1" t="s">
-        <v>766</v>
+        <v>774</v>
       </c>
       <c r="Q165" s="1" t="n">
         <v>2</v>
       </c>
       <c r="R165" s="1" t="s">
-        <v>767</v>
+        <v>775</v>
       </c>
       <c r="S165" s="1" t="s">
-        <v>768</v>
+        <v>776</v>
       </c>
       <c r="T165" s="1" t="s">
-        <v>484</v>
+        <v>492</v>
       </c>
       <c r="U165" s="1" t="s">
-        <v>769</v>
+        <v>777</v>
       </c>
       <c r="V165" s="1" t="s">
-        <v>770</v>
+        <v>778</v>
       </c>
       <c r="Z165" s="1"/>
       <c r="AA165" s="1"/>
@@ -11471,7 +11505,7 @@
         <v>262</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>771</v>
+        <v>779</v>
       </c>
       <c r="E166" s="9" t="s">
         <v>23</v>
@@ -11480,46 +11514,46 @@
         <v>23</v>
       </c>
       <c r="H166" s="9" t="s">
-        <v>446</v>
+        <v>454</v>
       </c>
       <c r="I166" s="7" t="s">
         <v>23</v>
       </c>
       <c r="J166" s="9" t="s">
-        <v>595</v>
+        <v>603</v>
       </c>
       <c r="K166" s="13" t="s">
         <v>23</v>
       </c>
       <c r="L166" s="1" t="s">
-        <v>772</v>
+        <v>780</v>
       </c>
       <c r="M166" s="1" t="s">
-        <v>773</v>
+        <v>781</v>
       </c>
       <c r="O166" s="1" t="s">
-        <v>599</v>
+        <v>607</v>
       </c>
       <c r="P166" s="1" t="s">
-        <v>774</v>
+        <v>782</v>
       </c>
       <c r="Q166" s="1" t="n">
         <v>2</v>
       </c>
       <c r="R166" s="1" t="s">
-        <v>775</v>
+        <v>783</v>
       </c>
       <c r="S166" s="1" t="s">
-        <v>776</v>
+        <v>784</v>
       </c>
       <c r="U166" s="1" t="s">
-        <v>777</v>
+        <v>785</v>
       </c>
       <c r="V166" s="1" t="s">
-        <v>778</v>
+        <v>786</v>
       </c>
       <c r="Y166" s="1" t="s">
-        <v>779</v>
+        <v>787</v>
       </c>
       <c r="Z166" s="1"/>
       <c r="AA166" s="1"/>

</xml_diff>

<commit_message>
implement Antibody and OtherReagent working group types - implements issue #189
</commit_message>
<xml_diff>
--- a/sampledata/fieldinformation.xlsx
+++ b/sampledata/fieldinformation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2027" uniqueCount="788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2432" uniqueCount="917">
   <si>
     <t>table</t>
   </si>
@@ -2384,6 +2384,393 @@
   </si>
   <si>
     <t>Patient Gender</t>
+  </si>
+  <si>
+    <t>antibody</t>
+  </si>
+  <si>
+    <t>2012-10-12</t>
+  </si>
+  <si>
+    <t>AR:1</t>
+  </si>
+  <si>
+    <t>AR_Name</t>
+  </si>
+  <si>
+    <t>Antibody Name</t>
+  </si>
+  <si>
+    <t>The primary name of the antibody as chosen by LINCS</t>
+  </si>
+  <si>
+    <t>AR:2</t>
+  </si>
+  <si>
+    <t>AR_ID</t>
+  </si>
+  <si>
+    <t>Antibody LINCS ID</t>
+  </si>
+  <si>
+    <t>Unique identifier of antibody reagent</t>
+  </si>
+  <si>
+    <t>AR:3</t>
+  </si>
+  <si>
+    <t>AR_Alternative_Name</t>
+  </si>
+  <si>
+    <t>List of synonymous antibody names, including the primary name</t>
+  </si>
+  <si>
+    <t>AR:4</t>
+  </si>
+  <si>
+    <t>AR_Center_ID</t>
+  </si>
+  <si>
+    <t>Antibody Facility ID</t>
+  </si>
+  <si>
+    <t>Center specific ID for antibody</t>
+  </si>
+  <si>
+    <t>target_protein_name</t>
+  </si>
+  <si>
+    <t>AR:8</t>
+  </si>
+  <si>
+    <t>AR_Target_Protein</t>
+  </si>
+  <si>
+    <t>The name of the protein (target), which is the recommended name from the UniProt database. If the name of a related entity is used instead, this should be documented explicitly in AR_Immunogen.</t>
+  </si>
+  <si>
+    <t>target_protein_uniprot_id</t>
+  </si>
+  <si>
+    <t>AR:9</t>
+  </si>
+  <si>
+    <t>AR_Target_Protein_ID</t>
+  </si>
+  <si>
+    <t>The UniProt ID of the protein targeted by the antibody, if available. If the UniProt ID of a related entity is used instead, this should be documented explicitly.</t>
+  </si>
+  <si>
+    <t>target_gene_name</t>
+  </si>
+  <si>
+    <t>AR:10</t>
+  </si>
+  <si>
+    <t>AR_Target_Gene</t>
+  </si>
+  <si>
+    <t>The NCBI gene name. In cases where the protein is modified (the protein sequence differs from the sequence encoded by the gene listed), it should be described in AR_Immunogen.</t>
+  </si>
+  <si>
+    <t>target_gene_id</t>
+  </si>
+  <si>
+    <t>AR:11</t>
+  </si>
+  <si>
+    <t>AR_Target_Gene ID</t>
+  </si>
+  <si>
+    <t>target_organism</t>
+  </si>
+  <si>
+    <t>AR:12</t>
+  </si>
+  <si>
+    <t>AR_Target_Organism</t>
+  </si>
+  <si>
+    <t>The organism of the target protein/gene described in AR:7-AR:10; NCBI nomenclature (e.g. Homo sapiens).</t>
+  </si>
+  <si>
+    <t>immunogen</t>
+  </si>
+  <si>
+    <t>AR:13</t>
+  </si>
+  <si>
+    <t>AR_Immunogen</t>
+  </si>
+  <si>
+    <t>A complete description of the immunogen used to make the antibody (text). This description should include the source of the immunogen (e.g. recombinantly expressed in E. coli, purified from canine pancreas, etc.). Any references relevant to the immunogen or making of the antibody can be listed in AR_Relevant_Reference.</t>
+  </si>
+  <si>
+    <t>immunogen_sequence</t>
+  </si>
+  <si>
+    <t>AR:14</t>
+  </si>
+  <si>
+    <t>AR_Immunogen_Sequence</t>
+  </si>
+  <si>
+    <t>If the immunogen is a peptide, protein fragment, or small protein, the amino acid sequence should be provided.</t>
+  </si>
+  <si>
+    <t>antibody_clonality</t>
+  </si>
+  <si>
+    <t>AR:15</t>
+  </si>
+  <si>
+    <t>AR_AntibodyClonality</t>
+  </si>
+  <si>
+    <t>A controlled vocabulary specifying whether the antibody is polyclonal or monoclonal.</t>
+  </si>
+  <si>
+    <t>AR:16</t>
+  </si>
+  <si>
+    <t>AR_Source_Organism</t>
+  </si>
+  <si>
+    <t>A controlled vocabulary describing the source of the antibody (e.g. mouse, rabbit, horse, goat, etc.)</t>
+  </si>
+  <si>
+    <t>antibody_isotype</t>
+  </si>
+  <si>
+    <t>AR:17</t>
+  </si>
+  <si>
+    <t>AR_Antibody_Isotype</t>
+  </si>
+  <si>
+    <t>A controlled vocabulary describing the antibody isotype (e.g. IgG, IgM, etc.)</t>
+  </si>
+  <si>
+    <t>engineering</t>
+  </si>
+  <si>
+    <t>AR:18</t>
+  </si>
+  <si>
+    <t>AR_Engineering</t>
+  </si>
+  <si>
+    <t>Is the antibody engineered/produced in an animal? Yes/No. If yes, then information should be provided about the engineering method and the production method (produced in mammalian cells, insect cells, yeast, bacteria, etc.).</t>
+  </si>
+  <si>
+    <t>antibody_purity</t>
+  </si>
+  <si>
+    <t>AR:19</t>
+  </si>
+  <si>
+    <t>AR_Antibody_Purity</t>
+  </si>
+  <si>
+    <t>A description of the antibody's level of purity (e.g., if it was purified, affinity purified, etc.)--a controlled vocabulary should be developed.</t>
+  </si>
+  <si>
+    <t>antibody_labeling</t>
+  </si>
+  <si>
+    <t>AR:20</t>
+  </si>
+  <si>
+    <t>AR_Antibody_Labeling</t>
+  </si>
+  <si>
+    <t>It should be indicated (Yes/No) whether the antibody is labeled or conjugated; If yes, with what fluor or enzyme (horseradish peroxidase)</t>
+  </si>
+  <si>
+    <t>recommended_experiment_type</t>
+  </si>
+  <si>
+    <t>AR:21</t>
+  </si>
+  <si>
+    <t>AR_Recommended_Experiment_Type</t>
+  </si>
+  <si>
+    <t>The type of experiment in which the antibody is useful, e.g., western blot, ELISA, immunostaining, etc. This depends on the ability of the antibody to recognize the native (non-denatured) or denatured target protein.</t>
+  </si>
+  <si>
+    <t>relevant_reference</t>
+  </si>
+  <si>
+    <t>AR:22</t>
+  </si>
+  <si>
+    <t>AR_Relevant_Reference</t>
+  </si>
+  <si>
+    <t>specificity</t>
+  </si>
+  <si>
+    <t>AR:23</t>
+  </si>
+  <si>
+    <t>AR_Specificity</t>
+  </si>
+  <si>
+    <t>Proteins other than the intended target with which the antibody cross-reacts. This includes homologues of the target protein from other organisms (text field; appropriate references should be provided if available).</t>
+  </si>
+  <si>
+    <t>antibodybatch</t>
+  </si>
+  <si>
+    <t>AR:5</t>
+  </si>
+  <si>
+    <t>AR_Provider</t>
+  </si>
+  <si>
+    <t>Vendor or lab that supplied the antibody</t>
+  </si>
+  <si>
+    <t>AR:6</t>
+  </si>
+  <si>
+    <t>AR_Provider_Catalog_ ID</t>
+  </si>
+  <si>
+    <t>ID or catalogue number assigned to the antibody by the vendor or provider</t>
+  </si>
+  <si>
+    <t>AR:7</t>
+  </si>
+  <si>
+    <t>AR_Batch_ID</t>
+  </si>
+  <si>
+    <t>Batch or lot number assigned to the antibody by the vendor or provider</t>
+  </si>
+  <si>
+    <t>otherreagent</t>
+  </si>
+  <si>
+    <t>2012-11-07</t>
+  </si>
+  <si>
+    <t>OR:2</t>
+  </si>
+  <si>
+    <t>OR_ID</t>
+  </si>
+  <si>
+    <t>Reagent LINCS ID</t>
+  </si>
+  <si>
+    <t>canonical</t>
+  </si>
+  <si>
+    <t>LINCS internal ID; this is a batch independent ID</t>
+  </si>
+  <si>
+    <t>OR:99</t>
+  </si>
+  <si>
+    <t>Reagent Facility ID</t>
+  </si>
+  <si>
+    <t>Facility ID</t>
+  </si>
+  <si>
+    <t>OR:5</t>
+  </si>
+  <si>
+    <t>OR_Alternate_ID</t>
+  </si>
+  <si>
+    <t>Other relevant IDs for reagents</t>
+  </si>
+  <si>
+    <t>OR:1</t>
+  </si>
+  <si>
+    <t>OR_Primary_Name</t>
+  </si>
+  <si>
+    <t>Reagent Name</t>
+  </si>
+  <si>
+    <t>The name of the reagent</t>
+  </si>
+  <si>
+    <t>Should correspond to existing names as much as possible; batch independent name</t>
+  </si>
+  <si>
+    <t>OR:3</t>
+  </si>
+  <si>
+    <t>OR_Alternate_Name</t>
+  </si>
+  <si>
+    <t>synonymous or alternative names; but only significant difference</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>OR:4</t>
+  </si>
+  <si>
+    <t>OR_Role</t>
+  </si>
+  <si>
+    <t>Role of reagent</t>
+  </si>
+  <si>
+    <t>Text field, ideally including some controlled vocabulary from BAO and ChEBI</t>
+  </si>
+  <si>
+    <t>OR:9</t>
+  </si>
+  <si>
+    <t>OR_Reference</t>
+  </si>
+  <si>
+    <t>A literature reference for the reagent if relevant/available.</t>
+  </si>
+  <si>
+    <t>otherreagentbatch</t>
+  </si>
+  <si>
+    <t>OR:6</t>
+  </si>
+  <si>
+    <t>OR_Provider_Name</t>
+  </si>
+  <si>
+    <t>Name of vendor (provider) that supplied the reagent</t>
+  </si>
+  <si>
+    <t>Vendor(s) or provider</t>
+  </si>
+  <si>
+    <t>OR:7</t>
+  </si>
+  <si>
+    <t>OR_Provider_Catalog_ID</t>
+  </si>
+  <si>
+    <t>ID or catalog number assigned to the reagent by the vendor or provider</t>
+  </si>
+  <si>
+    <t>Reagent provider's ID</t>
+  </si>
+  <si>
+    <t>OR:8</t>
+  </si>
+  <si>
+    <t>OR_Batch_ID</t>
+  </si>
+  <si>
+    <t>Vendor/Provider Batch ID number; Batch or lot number assigned to the reagent by the vendor or provider</t>
   </si>
 </sst>
 </file>
@@ -2545,7 +2932,7 @@
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -2555,32 +2942,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AQ166"/>
+  <dimension ref="A1:AQ199"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <pane activePane="bottomRight" topLeftCell="A80" xSplit="3560" ySplit="1881"/>
+      <pane activePane="bottomRight" topLeftCell="A162" xSplit="3934" ySplit="1837"/>
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
       <selection activeCell="A1" activeCellId="0" pane="topRight" sqref="A1"/>
-      <selection activeCell="A80" activeCellId="0" pane="bottomLeft" sqref="A80"/>
-      <selection activeCell="C101" activeCellId="0" pane="bottomRight" sqref="C101"/>
+      <selection activeCell="A162" activeCellId="0" pane="bottomLeft" sqref="A162"/>
+      <selection activeCell="A191" activeCellId="0" pane="bottomRight" sqref="A191"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.0588235294118"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.6627450980392"/>
-    <col collapsed="false" hidden="false" max="9" min="3" style="1" width="12.0196078431373"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="2" width="12.0196078431373"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.0196078431373"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="31.0862745098039"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="1" width="28.6235294117647"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="61.6117647058824"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="16.7333333333333"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="49.5803921568627"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="15.4549019607843"/>
-    <col collapsed="false" hidden="false" max="21" min="20" style="1" width="23.9058823529412"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="23.7882352941176"/>
-    <col collapsed="false" hidden="false" max="25" min="23" style="1" width="10.3843137254902"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="8.77254901960784"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.4196078431373"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.878431372549"/>
+    <col collapsed="false" hidden="false" max="9" min="3" style="1" width="12.2"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="2" width="12.2"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.2"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="31.5450980392157"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="1" width="29.0509803921569"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="62.5333333333333"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="16.9843137254902"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="50.321568627451"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="15.6901960784314"/>
+    <col collapsed="false" hidden="false" max="21" min="20" style="1" width="24.2666666666667"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="24.1490196078431"/>
+    <col collapsed="false" hidden="false" max="25" min="23" style="1" width="10.5372549019608"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="8.90980392156863"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="67.5" outlineLevel="0" r="1" s="6">
@@ -6781,7 +7168,7 @@
       <c r="AJ95" s="1"/>
       <c r="AK95" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="96">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="96">
       <c r="A96" s="9" t="s">
         <v>296</v>
       </c>
@@ -6844,7 +7231,7 @@
       <c r="AJ96" s="1"/>
       <c r="AK96" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="97">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="97">
       <c r="A97" s="9" t="s">
         <v>296</v>
       </c>
@@ -6907,7 +7294,7 @@
       <c r="AJ97" s="1"/>
       <c r="AK97" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="98">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="98">
       <c r="A98" s="9" t="s">
         <v>296</v>
       </c>
@@ -6971,7 +7358,7 @@
       <c r="AJ98" s="1"/>
       <c r="AK98" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="99">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="99">
       <c r="A99" s="9" t="s">
         <v>296</v>
       </c>
@@ -7035,7 +7422,7 @@
       <c r="AJ99" s="1"/>
       <c r="AK99" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="100">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="100">
       <c r="A100" s="9" t="s">
         <v>296</v>
       </c>
@@ -10926,7 +11313,7 @@
       <c r="AP157" s="1"/>
       <c r="AQ157" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="95.55" outlineLevel="0" r="158">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.4" outlineLevel="0" r="158">
       <c r="A158" s="1" t="s">
         <v>262</v>
       </c>
@@ -11003,7 +11390,7 @@
       <c r="AP158" s="1"/>
       <c r="AQ158" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="177.9" outlineLevel="0" r="159">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.4" outlineLevel="0" r="159">
       <c r="A159" s="1" t="s">
         <v>262</v>
       </c>
@@ -11145,7 +11532,7 @@
       <c r="AP160" s="1"/>
       <c r="AQ160" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="107.35" outlineLevel="0" r="161">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="161">
       <c r="A161" s="1" t="s">
         <v>262</v>
       </c>
@@ -11574,6 +11961,1360 @@
       <c r="AP166" s="1"/>
       <c r="AQ166" s="1"/>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="167">
+      <c r="A167" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E167" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F167" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G167" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H167" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I167" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J167" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="K167" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L167" s="10" t="s">
+        <v>790</v>
+      </c>
+      <c r="M167" s="10" t="s">
+        <v>791</v>
+      </c>
+      <c r="N167" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="P167" s="10" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="168">
+      <c r="A168" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="E168" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F168" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G168" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H168" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I168" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J168" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="K168" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L168" s="10" t="s">
+        <v>794</v>
+      </c>
+      <c r="M168" s="10" t="s">
+        <v>795</v>
+      </c>
+      <c r="N168" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="P168" s="10" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="169">
+      <c r="A169" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F169" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G169" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H169" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I169" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J169" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="K169" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L169" s="10" t="s">
+        <v>798</v>
+      </c>
+      <c r="M169" s="10" t="s">
+        <v>799</v>
+      </c>
+      <c r="P169" s="10" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="170">
+      <c r="A170" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C170" s="10"/>
+      <c r="D170" s="10"/>
+      <c r="E170" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F170" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G170" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H170" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I170" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J170" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="K170" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L170" s="10" t="s">
+        <v>801</v>
+      </c>
+      <c r="M170" s="10" t="s">
+        <v>802</v>
+      </c>
+      <c r="N170" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="P170" s="10" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="171">
+      <c r="A171" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B171" s="10" t="s">
+        <v>805</v>
+      </c>
+      <c r="C171" s="10"/>
+      <c r="D171" s="10"/>
+      <c r="E171" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F171" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G171" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H171" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I171" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J171" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="K171" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L171" s="10" t="s">
+        <v>806</v>
+      </c>
+      <c r="M171" s="10" t="s">
+        <v>807</v>
+      </c>
+      <c r="P171" s="10" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="172">
+      <c r="A172" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="C172" s="10"/>
+      <c r="D172" s="10"/>
+      <c r="E172" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F172" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G172" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H172" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I172" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J172" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="K172" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L172" s="10" t="s">
+        <v>810</v>
+      </c>
+      <c r="M172" s="10" t="s">
+        <v>811</v>
+      </c>
+      <c r="P172" s="10" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="173">
+      <c r="A173" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="C173" s="10"/>
+      <c r="D173" s="10"/>
+      <c r="E173" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F173" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G173" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H173" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I173" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J173" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="K173" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L173" s="10" t="s">
+        <v>814</v>
+      </c>
+      <c r="M173" s="10" t="s">
+        <v>815</v>
+      </c>
+      <c r="P173" s="10" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="174">
+      <c r="A174" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="C174" s="10"/>
+      <c r="D174" s="10"/>
+      <c r="E174" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F174" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G174" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H174" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I174" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J174" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="K174" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L174" s="10" t="s">
+        <v>818</v>
+      </c>
+      <c r="M174" s="10" t="s">
+        <v>819</v>
+      </c>
+      <c r="P174" s="10" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="175">
+      <c r="A175" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="C175" s="10"/>
+      <c r="D175" s="10"/>
+      <c r="E175" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F175" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G175" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H175" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I175" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J175" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="K175" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L175" s="10" t="s">
+        <v>821</v>
+      </c>
+      <c r="M175" s="10" t="s">
+        <v>822</v>
+      </c>
+      <c r="P175" s="10" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="176">
+      <c r="A176" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="C176" s="10"/>
+      <c r="D176" s="10"/>
+      <c r="E176" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F176" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G176" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H176" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I176" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J176" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="K176" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L176" s="10" t="s">
+        <v>825</v>
+      </c>
+      <c r="M176" s="10" t="s">
+        <v>826</v>
+      </c>
+      <c r="P176" s="10" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="177">
+      <c r="A177" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="C177" s="10"/>
+      <c r="D177" s="10"/>
+      <c r="E177" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G177" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H177" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I177" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J177" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="K177" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L177" s="10" t="s">
+        <v>829</v>
+      </c>
+      <c r="M177" s="10" t="s">
+        <v>830</v>
+      </c>
+      <c r="P177" s="10" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="178">
+      <c r="A178" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>832</v>
+      </c>
+      <c r="C178" s="10"/>
+      <c r="D178" s="10"/>
+      <c r="E178" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F178" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G178" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H178" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I178" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J178" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="K178" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L178" s="10" t="s">
+        <v>833</v>
+      </c>
+      <c r="M178" s="10" t="s">
+        <v>834</v>
+      </c>
+      <c r="P178" s="10" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="179">
+      <c r="A179" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="C179" s="10"/>
+      <c r="D179" s="10"/>
+      <c r="E179" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F179" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G179" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H179" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I179" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J179" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="K179" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L179" s="10" t="s">
+        <v>836</v>
+      </c>
+      <c r="M179" s="10" t="s">
+        <v>837</v>
+      </c>
+      <c r="P179" s="10" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="180">
+      <c r="A180" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>839</v>
+      </c>
+      <c r="C180" s="10"/>
+      <c r="D180" s="10"/>
+      <c r="E180" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F180" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G180" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H180" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I180" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J180" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="K180" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L180" s="10" t="s">
+        <v>840</v>
+      </c>
+      <c r="M180" s="10" t="s">
+        <v>841</v>
+      </c>
+      <c r="P180" s="10" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="181">
+      <c r="A181" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="C181" s="10"/>
+      <c r="D181" s="10"/>
+      <c r="E181" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G181" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H181" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I181" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J181" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="K181" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L181" s="10" t="s">
+        <v>844</v>
+      </c>
+      <c r="M181" s="10" t="s">
+        <v>845</v>
+      </c>
+      <c r="P181" s="10" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="182">
+      <c r="A182" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>847</v>
+      </c>
+      <c r="C182" s="10"/>
+      <c r="D182" s="10"/>
+      <c r="E182" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G182" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H182" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I182" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J182" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="K182" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L182" s="10" t="s">
+        <v>848</v>
+      </c>
+      <c r="M182" s="10" t="s">
+        <v>849</v>
+      </c>
+      <c r="P182" s="10" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="183">
+      <c r="A183" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="C183" s="10"/>
+      <c r="D183" s="10"/>
+      <c r="E183" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G183" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H183" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I183" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J183" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="K183" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L183" s="10" t="s">
+        <v>852</v>
+      </c>
+      <c r="M183" s="10" t="s">
+        <v>853</v>
+      </c>
+      <c r="P183" s="10" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="184">
+      <c r="A184" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="C184" s="10"/>
+      <c r="D184" s="10"/>
+      <c r="E184" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G184" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H184" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I184" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J184" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="K184" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L184" s="10" t="s">
+        <v>856</v>
+      </c>
+      <c r="M184" s="10" t="s">
+        <v>857</v>
+      </c>
+      <c r="P184" s="10" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="185">
+      <c r="A185" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="C185" s="10"/>
+      <c r="D185" s="10"/>
+      <c r="E185" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G185" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H185" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I185" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J185" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="K185" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L185" s="10" t="s">
+        <v>860</v>
+      </c>
+      <c r="M185" s="10" t="s">
+        <v>861</v>
+      </c>
+      <c r="P185" s="10" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="186">
+      <c r="A186" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="C186" s="10"/>
+      <c r="D186" s="10"/>
+      <c r="E186" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F186" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G186" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H186" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I186" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J186" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="K186" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L186" s="10" t="s">
+        <v>863</v>
+      </c>
+      <c r="M186" s="10" t="s">
+        <v>864</v>
+      </c>
+      <c r="P186" s="10" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="187">
+      <c r="A187" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="C187" s="10"/>
+      <c r="D187" s="10"/>
+      <c r="E187" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G187" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H187" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I187" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J187" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="K187" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L187" s="10" t="s">
+        <v>867</v>
+      </c>
+      <c r="M187" s="10" t="s">
+        <v>868</v>
+      </c>
+      <c r="P187" s="10" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="188">
+      <c r="A188" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="C188" s="10"/>
+      <c r="D188" s="10"/>
+      <c r="E188" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G188" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H188" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="I188" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J188" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="K188" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L188" s="10" t="s">
+        <v>870</v>
+      </c>
+      <c r="M188" s="10" t="s">
+        <v>871</v>
+      </c>
+      <c r="P188" s="10" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="189">
+      <c r="A189" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="C189" s="10"/>
+      <c r="D189" s="10"/>
+      <c r="E189" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G189" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H189" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="I189" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J189" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="K189" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L189" s="10" t="s">
+        <v>873</v>
+      </c>
+      <c r="M189" s="10" t="s">
+        <v>874</v>
+      </c>
+      <c r="P189" s="10" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="190">
+      <c r="A190" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="E190" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F190" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G190" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H190" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I190" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J190" s="2" t="s">
+        <v>877</v>
+      </c>
+      <c r="K190" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L190" s="10" t="s">
+        <v>878</v>
+      </c>
+      <c r="M190" s="10" t="s">
+        <v>879</v>
+      </c>
+      <c r="N190" s="1" t="s">
+        <v>880</v>
+      </c>
+      <c r="O190" s="10" t="s">
+        <v>881</v>
+      </c>
+      <c r="P190" s="10" t="s">
+        <v>484</v>
+      </c>
+      <c r="Q190" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="R190" s="10" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="191">
+      <c r="A191" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E191" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F191" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G191" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H191" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I191" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J191" s="2" t="s">
+        <v>877</v>
+      </c>
+      <c r="K191" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L191" s="10" t="s">
+        <v>883</v>
+      </c>
+      <c r="M191" s="10"/>
+      <c r="N191" s="1" t="s">
+        <v>884</v>
+      </c>
+      <c r="O191" s="10" t="s">
+        <v>881</v>
+      </c>
+      <c r="P191" s="10" t="s">
+        <v>885</v>
+      </c>
+      <c r="Q191" s="10" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="192">
+      <c r="A192" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="E192" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F192" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G192" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H192" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I192" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J192" s="2" t="s">
+        <v>877</v>
+      </c>
+      <c r="K192" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L192" s="10" t="s">
+        <v>886</v>
+      </c>
+      <c r="M192" s="10" t="s">
+        <v>887</v>
+      </c>
+      <c r="O192" s="10" t="s">
+        <v>881</v>
+      </c>
+      <c r="P192" s="10" t="s">
+        <v>888</v>
+      </c>
+      <c r="Q192" s="10" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="193">
+      <c r="A193" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E193" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F193" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G193" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H193" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I193" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J193" s="2" t="s">
+        <v>877</v>
+      </c>
+      <c r="K193" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L193" s="10" t="s">
+        <v>889</v>
+      </c>
+      <c r="M193" s="10" t="s">
+        <v>890</v>
+      </c>
+      <c r="N193" s="1" t="s">
+        <v>891</v>
+      </c>
+      <c r="O193" s="10" t="s">
+        <v>881</v>
+      </c>
+      <c r="P193" s="10" t="s">
+        <v>892</v>
+      </c>
+      <c r="Q193" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="R193" s="10" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="194">
+      <c r="A194" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="E194" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F194" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G194" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H194" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I194" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J194" s="2" t="s">
+        <v>877</v>
+      </c>
+      <c r="K194" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L194" s="10" t="s">
+        <v>894</v>
+      </c>
+      <c r="M194" s="10" t="s">
+        <v>895</v>
+      </c>
+      <c r="O194" s="10" t="s">
+        <v>881</v>
+      </c>
+      <c r="P194" s="10" t="s">
+        <v>622</v>
+      </c>
+      <c r="Q194" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="R194" s="10" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="195">
+      <c r="A195" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>897</v>
+      </c>
+      <c r="E195" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F195" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G195" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H195" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I195" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J195" s="2" t="s">
+        <v>877</v>
+      </c>
+      <c r="K195" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L195" s="10" t="s">
+        <v>898</v>
+      </c>
+      <c r="M195" s="10" t="s">
+        <v>899</v>
+      </c>
+      <c r="O195" s="10" t="s">
+        <v>881</v>
+      </c>
+      <c r="P195" s="10" t="s">
+        <v>900</v>
+      </c>
+      <c r="Q195" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="R195" s="10" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="196">
+      <c r="A196" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="E196" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F196" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G196" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H196" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I196" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J196" s="2" t="s">
+        <v>877</v>
+      </c>
+      <c r="K196" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L196" s="10" t="s">
+        <v>902</v>
+      </c>
+      <c r="M196" s="10" t="s">
+        <v>903</v>
+      </c>
+      <c r="O196" s="10" t="s">
+        <v>881</v>
+      </c>
+      <c r="P196" s="10" t="s">
+        <v>904</v>
+      </c>
+      <c r="Q196" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="R196" s="10"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="197">
+      <c r="A197" s="1" t="s">
+        <v>905</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="E197" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G197" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H197" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I197" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J197" s="2" t="s">
+        <v>877</v>
+      </c>
+      <c r="K197" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L197" s="10" t="s">
+        <v>906</v>
+      </c>
+      <c r="M197" s="10" t="s">
+        <v>907</v>
+      </c>
+      <c r="O197" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="P197" s="10" t="s">
+        <v>908</v>
+      </c>
+      <c r="Q197" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="R197" s="10" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="198">
+      <c r="A198" s="1" t="s">
+        <v>905</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="E198" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G198" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H198" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I198" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J198" s="2" t="s">
+        <v>877</v>
+      </c>
+      <c r="K198" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L198" s="10" t="s">
+        <v>910</v>
+      </c>
+      <c r="M198" s="10" t="s">
+        <v>911</v>
+      </c>
+      <c r="O198" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="P198" s="10" t="s">
+        <v>912</v>
+      </c>
+      <c r="Q198" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="R198" s="10" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="199">
+      <c r="A199" s="1" t="s">
+        <v>905</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="E199" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G199" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H199" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I199" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J199" s="2" t="s">
+        <v>877</v>
+      </c>
+      <c r="K199" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L199" s="10" t="s">
+        <v>914</v>
+      </c>
+      <c r="M199" s="10" t="s">
+        <v>915</v>
+      </c>
+      <c r="O199" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="P199" s="10" t="s">
+        <v>916</v>
+      </c>
+      <c r="Q199" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="R199" s="10"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink display="The version of the LINCS Data Working Group Standards Document from which this column definition was taken.  See https://sites.google.com/site/lincsdwgdevelopment/standards-and-use" ref="P11" r:id="rId1"/>

</xml_diff>

<commit_message>
fix typo error causing load fail
</commit_message>
<xml_diff>
--- a/sampledata/fieldinformation.xlsx
+++ b/sampledata/fieldinformation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2441" uniqueCount="925">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2432" uniqueCount="916">
   <si>
     <t>table</t>
   </si>
@@ -2768,33 +2768,6 @@
   </si>
   <si>
     <t>Vendor/Provider Batch ID number; Batch or lot number assigned to the reagent by the vendor or provider</t>
-  </si>
-  <si>
-    <t>The KINOMEscan dataset type</t>
-  </si>
-  <si>
-    <t>KiNativ dataset type</t>
-  </si>
-  <si>
-    <t>MGH/CMT Growth Inhibition dataset type</t>
-  </si>
-  <si>
-    <t>Microfluidics" (Yale) dataset type</t>
-  </si>
-  <si>
-    <t>Microscopy/Imaging dataset type</t>
-  </si>
-  <si>
-    <t>ELISA dataset type</t>
-  </si>
-  <si>
-    <t>Analysis dataset type</t>
-  </si>
-  <si>
-    <t>Other dataset type</t>
-  </si>
-  <si>
-    <t>Datasets that have been published by LINCS Centers</t>
   </si>
 </sst>
 </file>
@@ -2956,7 +2929,7 @@
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -2966,31 +2939,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AQ208"/>
+  <dimension ref="A1:AQ199"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="K1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <pane activePane="bottomLeft" topLeftCell="A188" xSplit="4338" ySplit="1793"/>
-      <selection activeCell="K1" activeCellId="0" pane="topLeft" sqref="K1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <pane activePane="bottomLeft" topLeftCell="A179" xSplit="4487" ySplit="1778"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
       <selection activeCell="A1" activeCellId="0" pane="topRight" sqref="A1"/>
-      <selection activeCell="B200" activeCellId="0" pane="bottomLeft" sqref="B200:L208"/>
-      <selection activeCell="A188" activeCellId="0" pane="bottomRight" sqref="A188"/>
+      <selection activeCell="A199" activeCellId="0" pane="bottomLeft" sqref="A199"/>
+      <selection activeCell="A179" activeCellId="0" pane="bottomRight" sqref="A179"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.7725490196078"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.1058823529412"/>
-    <col collapsed="false" hidden="false" max="9" min="3" style="1" width="12.3803921568627"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="2" width="12.3803921568627"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.3803921568627"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="32.0156862745098"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="1" width="29.4862745098039"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="63.4823529411765"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="17.2313725490196"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="51.0823529411765"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="15.9254901960784"/>
-    <col collapsed="false" hidden="false" max="21" min="20" style="1" width="24.6196078431373"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="24.5019607843137"/>
-    <col collapsed="false" hidden="false" max="25" min="23" style="1" width="10.6980392156863"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.8901960784314"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.1843137254902"/>
+    <col collapsed="false" hidden="false" max="9" min="3" style="1" width="12.443137254902"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="2" width="12.443137254902"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.443137254902"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="32.1725490196078"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="1" width="29.6274509803922"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="63.8"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="17.321568627451"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="51.3372549019608"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="16"/>
+    <col collapsed="false" hidden="false" max="21" min="20" style="1" width="24.7372549019608"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="24.6196078431373"/>
+    <col collapsed="false" hidden="false" max="25" min="23" style="1" width="10.7529411764706"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="8.54509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="67.5" outlineLevel="0" r="1" s="6">
@@ -4520,7 +4494,7 @@
       <c r="AF35" s="1"/>
       <c r="AG35" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="36">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="36">
       <c r="A36" s="9" t="s">
         <v>101</v>
       </c>
@@ -13338,150 +13312,6 @@
       </c>
       <c r="R199" s="10"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="200">
-      <c r="B200" s="0"/>
-      <c r="C200" s="0"/>
-      <c r="D200" s="0"/>
-      <c r="E200" s="0"/>
-      <c r="F200" s="0"/>
-      <c r="G200" s="0"/>
-      <c r="H200" s="0"/>
-      <c r="I200" s="0"/>
-      <c r="J200" s="0"/>
-      <c r="K200" s="0"/>
-      <c r="L200" s="0"/>
-      <c r="P200" s="1" t="s">
-        <v>916</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="201">
-      <c r="B201" s="0"/>
-      <c r="C201" s="0"/>
-      <c r="D201" s="0"/>
-      <c r="E201" s="0"/>
-      <c r="F201" s="0"/>
-      <c r="G201" s="0"/>
-      <c r="H201" s="0"/>
-      <c r="I201" s="0"/>
-      <c r="J201" s="0"/>
-      <c r="K201" s="0"/>
-      <c r="L201" s="0"/>
-      <c r="P201" s="10" t="s">
-        <v>917</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="202">
-      <c r="B202" s="0"/>
-      <c r="C202" s="0"/>
-      <c r="D202" s="0"/>
-      <c r="E202" s="0"/>
-      <c r="F202" s="0"/>
-      <c r="G202" s="0"/>
-      <c r="H202" s="0"/>
-      <c r="I202" s="0"/>
-      <c r="J202" s="0"/>
-      <c r="K202" s="0"/>
-      <c r="L202" s="0"/>
-      <c r="P202" s="10" t="s">
-        <v>918</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="203">
-      <c r="B203" s="0"/>
-      <c r="C203" s="0"/>
-      <c r="D203" s="0"/>
-      <c r="E203" s="0"/>
-      <c r="F203" s="0"/>
-      <c r="G203" s="0"/>
-      <c r="H203" s="0"/>
-      <c r="I203" s="0"/>
-      <c r="J203" s="0"/>
-      <c r="K203" s="0"/>
-      <c r="L203" s="0"/>
-      <c r="P203" s="10" t="s">
-        <v>919</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="204">
-      <c r="B204" s="0"/>
-      <c r="C204" s="0"/>
-      <c r="D204" s="0"/>
-      <c r="E204" s="0"/>
-      <c r="F204" s="0"/>
-      <c r="G204" s="0"/>
-      <c r="H204" s="0"/>
-      <c r="I204" s="0"/>
-      <c r="J204" s="0"/>
-      <c r="K204" s="0"/>
-      <c r="L204" s="0"/>
-      <c r="P204" s="10" t="s">
-        <v>920</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="205">
-      <c r="B205" s="0"/>
-      <c r="C205" s="0"/>
-      <c r="D205" s="0"/>
-      <c r="E205" s="0"/>
-      <c r="F205" s="0"/>
-      <c r="G205" s="0"/>
-      <c r="H205" s="0"/>
-      <c r="I205" s="0"/>
-      <c r="J205" s="0"/>
-      <c r="K205" s="0"/>
-      <c r="L205" s="0"/>
-      <c r="P205" s="10" t="s">
-        <v>921</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="206">
-      <c r="B206" s="0"/>
-      <c r="C206" s="0"/>
-      <c r="D206" s="0"/>
-      <c r="E206" s="0"/>
-      <c r="F206" s="0"/>
-      <c r="G206" s="0"/>
-      <c r="H206" s="0"/>
-      <c r="I206" s="0"/>
-      <c r="J206" s="0"/>
-      <c r="K206" s="0"/>
-      <c r="L206" s="0"/>
-      <c r="P206" s="10" t="s">
-        <v>922</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="207">
-      <c r="B207" s="0"/>
-      <c r="C207" s="0"/>
-      <c r="D207" s="0"/>
-      <c r="E207" s="0"/>
-      <c r="F207" s="0"/>
-      <c r="G207" s="0"/>
-      <c r="H207" s="0"/>
-      <c r="I207" s="0"/>
-      <c r="J207" s="0"/>
-      <c r="K207" s="0"/>
-      <c r="L207" s="0"/>
-      <c r="P207" s="1" t="s">
-        <v>923</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="208">
-      <c r="B208" s="0"/>
-      <c r="C208" s="0"/>
-      <c r="D208" s="0"/>
-      <c r="E208" s="0"/>
-      <c r="F208" s="0"/>
-      <c r="G208" s="0"/>
-      <c r="H208" s="0"/>
-      <c r="I208" s="0"/>
-      <c r="J208" s="0"/>
-      <c r="K208" s="0"/>
-      <c r="L208" s="0"/>
-      <c r="P208" s="10" t="s">
-        <v>924</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink display="The version of the LINCS Data Working Group Standards Document from which this column definition was taken.  See https://sites.google.com/site/lincsdwgdevelopment/standards-and-use" ref="P11" r:id="rId1"/>

</xml_diff>

<commit_message>
visible columns and column widths
</commit_message>
<xml_diff>
--- a/sampledata/fieldinformation.xlsx
+++ b/sampledata/fieldinformation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2455" uniqueCount="925">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2456" uniqueCount="925">
   <si>
     <t>table</t>
   </si>
@@ -2956,7 +2956,7 @@
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -2968,30 +2968,30 @@
   </sheetPr>
   <dimension ref="A1:AR201"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <pane activePane="bottomRight" topLeftCell="B83" xSplit="4802" ySplit="1749"/>
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="E1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <pane activePane="bottomLeft" topLeftCell="B2" xSplit="4966" ySplit="1734"/>
+      <selection activeCell="E1" activeCellId="0" pane="topLeft" sqref="E1"/>
       <selection activeCell="B1" activeCellId="0" pane="topRight" sqref="B1"/>
-      <selection activeCell="A83" activeCellId="0" pane="bottomLeft" sqref="A83"/>
-      <selection activeCell="G108" activeCellId="0" pane="bottomRight" sqref="G108"/>
+      <selection activeCell="G37" activeCellId="0" pane="bottomLeft" sqref="G37"/>
+      <selection activeCell="B2" activeCellId="0" pane="bottomRight" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.1333333333333"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.3372549019608"/>
-    <col collapsed="false" hidden="false" max="10" min="3" style="1" width="12.5725490196078"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="2" width="12.5725490196078"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.5725490196078"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="32.4980392156863"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="1" width="29.9176470588235"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="64.4313725490196"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="17.5019607843137"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="51.843137254902"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="16.1607843137255"/>
-    <col collapsed="false" hidden="false" max="22" min="21" style="1" width="24.9882352941176"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="24.8627450980392"/>
-    <col collapsed="false" hidden="false" max="26" min="24" style="1" width="10.8627450980392"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.63921568627451"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.2627450980392"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.4117647058824"/>
+    <col collapsed="false" hidden="false" max="10" min="3" style="1" width="12.6352941176471"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="2" width="12.6352941176471"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.6352941176471"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="32.6588235294118"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="1" width="30.0627450980392"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="64.756862745098"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="17.5921568627451"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="52.1058823529412"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="16.243137254902"/>
+    <col collapsed="false" hidden="false" max="22" min="21" style="1" width="25.1176470588235"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="24.9882352941176"/>
+    <col collapsed="false" hidden="false" max="26" min="24" style="1" width="10.9176470588235"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.68235294117647"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="67.5" outlineLevel="0" r="1" s="6">
@@ -3076,7 +3076,7 @@
       <c r="AG1" s="3"/>
       <c r="AH1" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="2">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
@@ -3122,7 +3122,7 @@
       <c r="AG2" s="1"/>
       <c r="AH2" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="3">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -3168,7 +3168,7 @@
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="4">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -3214,7 +3214,7 @@
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="5">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -3260,7 +3260,7 @@
       <c r="AG5" s="1"/>
       <c r="AH5" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="6">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -3303,7 +3303,7 @@
       <c r="AG6" s="1"/>
       <c r="AH6" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="7">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -3343,7 +3343,7 @@
       <c r="AG7" s="1"/>
       <c r="AH7" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="8">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -3383,7 +3383,7 @@
       <c r="AG8" s="1"/>
       <c r="AH8" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="9">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -3423,7 +3423,7 @@
       <c r="AG9" s="1"/>
       <c r="AH9" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="10">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -3463,7 +3463,7 @@
       <c r="AG10" s="1"/>
       <c r="AH10" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="11">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -3546,7 +3546,7 @@
       <c r="AG12" s="1"/>
       <c r="AH12" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="13">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -3592,7 +3592,7 @@
       <c r="AG13" s="1"/>
       <c r="AH13" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="14">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="14">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -3635,7 +3635,7 @@
       <c r="AG14" s="1"/>
       <c r="AH14" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="15">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="15">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -3678,7 +3678,7 @@
       <c r="AG15" s="1"/>
       <c r="AH15" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="16">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -3721,7 +3721,7 @@
       <c r="AG16" s="1"/>
       <c r="AH16" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="17">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -3764,7 +3764,7 @@
       <c r="AG17" s="1"/>
       <c r="AH17" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="18">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="18">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
@@ -3807,7 +3807,7 @@
       <c r="AG18" s="1"/>
       <c r="AH18" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="19">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="19">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
@@ -3850,7 +3850,7 @@
       <c r="AG19" s="1"/>
       <c r="AH19" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="20">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="20">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -3893,7 +3893,7 @@
       <c r="AG20" s="1"/>
       <c r="AH20" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="21">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="21">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -3933,7 +3933,7 @@
       <c r="AG21" s="1"/>
       <c r="AH21" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="22">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="22">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -3973,7 +3973,7 @@
       <c r="AG22" s="1"/>
       <c r="AH22" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="23">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="23">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -4103,7 +4103,7 @@
       <c r="AG25" s="1"/>
       <c r="AH25" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="26">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="26">
       <c r="A26" s="9" t="s">
         <v>106</v>
       </c>
@@ -4145,7 +4145,7 @@
       <c r="AG26" s="1"/>
       <c r="AH26" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="27">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="27">
       <c r="A27" s="9" t="s">
         <v>106</v>
       </c>
@@ -4273,7 +4273,7 @@
       <c r="AG29" s="1"/>
       <c r="AH29" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="30">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="30">
       <c r="A30" s="9" t="s">
         <v>106</v>
       </c>
@@ -4315,7 +4315,7 @@
       <c r="AG30" s="1"/>
       <c r="AH30" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="31">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="31">
       <c r="A31" s="9" t="s">
         <v>106</v>
       </c>
@@ -4587,9 +4587,11 @@
         <v>24</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G37" s="7"/>
+        <v>24</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="H37" s="1" t="s">
         <v>25</v>
       </c>
@@ -4992,7 +4994,7 @@
       <c r="AG46" s="1"/>
       <c r="AH46" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="47">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="47">
       <c r="A47" s="1" t="s">
         <v>174</v>
       </c>
@@ -5035,7 +5037,7 @@
       <c r="AG47" s="1"/>
       <c r="AH47" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="48">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="48">
       <c r="A48" s="1" t="s">
         <v>174</v>
       </c>
@@ -5078,7 +5080,7 @@
       <c r="AG48" s="1"/>
       <c r="AH48" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="49">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="49">
       <c r="A49" s="1" t="s">
         <v>174</v>
       </c>
@@ -5121,7 +5123,7 @@
       <c r="AG49" s="1"/>
       <c r="AH49" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="50">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="50">
       <c r="A50" s="9" t="s">
         <v>174</v>
       </c>
@@ -5164,7 +5166,7 @@
       <c r="AG50" s="1"/>
       <c r="AH50" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="51">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="51">
       <c r="A51" s="9" t="s">
         <v>174</v>
       </c>
@@ -5289,7 +5291,7 @@
       <c r="AG53" s="1"/>
       <c r="AH53" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="54">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="54">
       <c r="A54" s="9"/>
       <c r="B54" s="1" t="s">
         <v>196</v>
@@ -5328,7 +5330,7 @@
       <c r="AG54" s="1"/>
       <c r="AH54" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="55">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="55">
       <c r="A55" s="9"/>
       <c r="B55" s="1" t="s">
         <v>199</v>
@@ -5369,7 +5371,7 @@
       <c r="AG55" s="1"/>
       <c r="AH55" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="56">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="56">
       <c r="A56" s="10" t="s">
         <v>202</v>
       </c>
@@ -5412,7 +5414,7 @@
       <c r="AG56" s="1"/>
       <c r="AH56" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="57">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="57">
       <c r="A57" s="10" t="s">
         <v>202</v>
       </c>
@@ -5455,7 +5457,7 @@
       <c r="AG57" s="1"/>
       <c r="AH57" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="58">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="58">
       <c r="A58" s="1" t="s">
         <v>202</v>
       </c>
@@ -5495,7 +5497,7 @@
       <c r="AG58" s="1"/>
       <c r="AH58" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="59">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="59">
       <c r="A59" s="1" t="s">
         <v>202</v>
       </c>
@@ -5535,7 +5537,7 @@
       <c r="AG59" s="1"/>
       <c r="AH59" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="60">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="60">
       <c r="A60" s="1" t="s">
         <v>202</v>
       </c>
@@ -5575,7 +5577,7 @@
       <c r="AG60" s="1"/>
       <c r="AH60" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="61">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="61">
       <c r="A61" s="1" t="s">
         <v>202</v>
       </c>
@@ -5615,7 +5617,7 @@
       <c r="AG61" s="1"/>
       <c r="AH61" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="62">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="62">
       <c r="A62" s="1" t="s">
         <v>202</v>
       </c>
@@ -5658,7 +5660,7 @@
       <c r="AG62" s="1"/>
       <c r="AH62" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="63">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="63">
       <c r="A63" s="1" t="s">
         <v>202</v>
       </c>
@@ -5701,7 +5703,7 @@
       <c r="AG63" s="1"/>
       <c r="AH63" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="64">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="64">
       <c r="A64" s="1" t="s">
         <v>224</v>
       </c>
@@ -5744,7 +5746,7 @@
       <c r="AG64" s="1"/>
       <c r="AH64" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="65">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="65">
       <c r="A65" s="1" t="s">
         <v>224</v>
       </c>
@@ -5787,7 +5789,7 @@
       <c r="AG65" s="1"/>
       <c r="AH65" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="66">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="66">
       <c r="A66" s="1" t="s">
         <v>224</v>
       </c>
@@ -5830,7 +5832,7 @@
       <c r="AG66" s="1"/>
       <c r="AH66" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="67">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="67">
       <c r="A67" s="1" t="s">
         <v>224</v>
       </c>
@@ -5873,7 +5875,7 @@
       <c r="AG67" s="1"/>
       <c r="AH67" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="68">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="68">
       <c r="A68" s="1" t="s">
         <v>235</v>
       </c>
@@ -5919,7 +5921,7 @@
       <c r="AG68" s="1"/>
       <c r="AH68" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="69">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="69">
       <c r="A69" s="1" t="s">
         <v>235</v>
       </c>
@@ -5965,7 +5967,7 @@
       <c r="AG69" s="1"/>
       <c r="AH69" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="70">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="70">
       <c r="A70" s="1" t="s">
         <v>235</v>
       </c>
@@ -6008,7 +6010,7 @@
       <c r="AG70" s="1"/>
       <c r="AH70" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="71">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="71">
       <c r="A71" s="1" t="s">
         <v>235</v>
       </c>
@@ -6051,7 +6053,7 @@
       <c r="AG71" s="1"/>
       <c r="AH71" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="72">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="72">
       <c r="A72" s="1" t="s">
         <v>235</v>
       </c>
@@ -6094,7 +6096,7 @@
       <c r="AG72" s="1"/>
       <c r="AH72" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="73">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="73">
       <c r="A73" s="1" t="s">
         <v>235</v>
       </c>
@@ -6137,7 +6139,7 @@
       <c r="AG73" s="1"/>
       <c r="AH73" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="74">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="74">
       <c r="A74" s="1" t="s">
         <v>235</v>
       </c>
@@ -6180,7 +6182,7 @@
       <c r="AG74" s="1"/>
       <c r="AH74" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="75">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="75">
       <c r="A75" s="1" t="s">
         <v>235</v>
       </c>
@@ -6223,7 +6225,7 @@
       <c r="AG75" s="1"/>
       <c r="AH75" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="76">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="76">
       <c r="A76" s="1" t="s">
         <v>235</v>
       </c>
@@ -6266,7 +6268,7 @@
       <c r="AG76" s="1"/>
       <c r="AH76" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="77">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="77">
       <c r="A77" s="1" t="s">
         <v>235</v>
       </c>
@@ -6309,7 +6311,7 @@
       <c r="AG77" s="1"/>
       <c r="AH77" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="78">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="78">
       <c r="A78" s="1" t="s">
         <v>235</v>
       </c>
@@ -6352,7 +6354,7 @@
       <c r="AG78" s="1"/>
       <c r="AH78" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="79">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="79">
       <c r="A79" s="1" t="s">
         <v>235</v>
       </c>
@@ -6395,7 +6397,7 @@
       <c r="AG79" s="1"/>
       <c r="AH79" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="80">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="80">
       <c r="A80" s="1" t="s">
         <v>235</v>
       </c>
@@ -6438,7 +6440,7 @@
       <c r="AG80" s="1"/>
       <c r="AH80" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="81">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="81">
       <c r="B81" s="1" t="s">
         <v>272</v>
       </c>
@@ -6481,7 +6483,7 @@
       <c r="AG81" s="1"/>
       <c r="AH81" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="82">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="82">
       <c r="B82" s="1" t="s">
         <v>276</v>
       </c>
@@ -6516,7 +6518,7 @@
         <v>278</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="83">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="83">
       <c r="B83" s="1" t="s">
         <v>279</v>
       </c>
@@ -6551,7 +6553,7 @@
         <v>281</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="84">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="84">
       <c r="B84" s="1" t="s">
         <v>282</v>
       </c>
@@ -6586,7 +6588,7 @@
         <v>285</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="85">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="85">
       <c r="B85" s="1" t="s">
         <v>286</v>
       </c>
@@ -6621,7 +6623,7 @@
         <v>289</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="86">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="86">
       <c r="B86" s="1" t="s">
         <v>290</v>
       </c>
@@ -6656,7 +6658,7 @@
         <v>293</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="87">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="87">
       <c r="B87" s="1" t="s">
         <v>294</v>
       </c>
@@ -6691,7 +6693,7 @@
         <v>298</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="88">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="88">
       <c r="A88" s="9" t="s">
         <v>299</v>
       </c>
@@ -6760,7 +6762,7 @@
       <c r="AK88" s="1"/>
       <c r="AL88" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="89">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="89">
       <c r="A89" s="9" t="s">
         <v>299</v>
       </c>
@@ -6818,7 +6820,7 @@
       <c r="AK89" s="1"/>
       <c r="AL89" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="90">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="90">
       <c r="A90" s="9" t="s">
         <v>299</v>
       </c>
@@ -6884,7 +6886,7 @@
       <c r="AK90" s="1"/>
       <c r="AL90" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="91">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="91">
       <c r="A91" s="9" t="s">
         <v>299</v>
       </c>
@@ -6945,7 +6947,7 @@
       <c r="AK91" s="1"/>
       <c r="AL91" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="92">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="92">
       <c r="A92" s="9"/>
       <c r="B92" s="9" t="s">
         <v>324</v>
@@ -6995,7 +6997,7 @@
       <c r="AK92" s="1"/>
       <c r="AL92" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="93">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="93">
       <c r="B93" s="9" t="s">
         <v>328</v>
       </c>
@@ -7043,7 +7045,7 @@
       <c r="AK93" s="1"/>
       <c r="AL93" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="94">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="94">
       <c r="A94" s="9" t="s">
         <v>299</v>
       </c>
@@ -7110,7 +7112,7 @@
       <c r="AK94" s="1"/>
       <c r="AL94" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="95">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="95">
       <c r="A95" s="9" t="s">
         <v>299</v>
       </c>
@@ -7181,7 +7183,7 @@
       <c r="AK95" s="1"/>
       <c r="AL95" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="96">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="96">
       <c r="A96" s="9" t="s">
         <v>299</v>
       </c>
@@ -7249,7 +7251,7 @@
       <c r="AK96" s="1"/>
       <c r="AL96" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="97">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="97">
       <c r="A97" s="9" t="s">
         <v>299</v>
       </c>
@@ -7313,7 +7315,7 @@
       <c r="AK97" s="1"/>
       <c r="AL97" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="98">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="98">
       <c r="A98" s="9" t="s">
         <v>299</v>
       </c>
@@ -7377,7 +7379,7 @@
       <c r="AK98" s="1"/>
       <c r="AL98" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="99">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="99">
       <c r="A99" s="9" t="s">
         <v>299</v>
       </c>
@@ -7442,7 +7444,7 @@
       <c r="AK99" s="1"/>
       <c r="AL99" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="100">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="100">
       <c r="A100" s="9" t="s">
         <v>299</v>
       </c>
@@ -7507,7 +7509,7 @@
       <c r="AK100" s="1"/>
       <c r="AL100" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="101">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="101">
       <c r="A101" s="9" t="s">
         <v>299</v>
       </c>
@@ -7572,7 +7574,7 @@
       <c r="AK101" s="1"/>
       <c r="AL101" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="102">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="102">
       <c r="A102" s="9" t="s">
         <v>299</v>
       </c>
@@ -7733,7 +7735,7 @@
       <c r="AK104" s="1"/>
       <c r="AL104" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="105">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="105">
       <c r="A105" s="9" t="s">
         <v>299</v>
       </c>
@@ -7790,7 +7792,7 @@
       <c r="AK105" s="1"/>
       <c r="AL105" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="106">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="106">
       <c r="A106" s="9" t="s">
         <v>299</v>
       </c>
@@ -7847,7 +7849,7 @@
       <c r="AK106" s="1"/>
       <c r="AL106" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="107">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="107">
       <c r="A107" s="9"/>
       <c r="B107" s="9" t="s">
         <v>405</v>
@@ -7910,7 +7912,7 @@
       <c r="AK107" s="1"/>
       <c r="AL107" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="108">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="108">
       <c r="B108" s="9" t="s">
         <v>411</v>
       </c>
@@ -7962,7 +7964,7 @@
       <c r="AK108" s="1"/>
       <c r="AL108" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="109">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="109">
       <c r="A109" s="9" t="s">
         <v>329</v>
       </c>
@@ -8028,7 +8030,7 @@
       <c r="AK109" s="1"/>
       <c r="AL109" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="110">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="110">
       <c r="A110" s="9" t="s">
         <v>329</v>
       </c>
@@ -8089,7 +8091,7 @@
       <c r="AK110" s="1"/>
       <c r="AL110" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="111">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="111">
       <c r="A111" s="9" t="s">
         <v>329</v>
       </c>
@@ -8147,7 +8149,7 @@
       <c r="AK111" s="1"/>
       <c r="AL111" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="112">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="112">
       <c r="A112" s="9" t="s">
         <v>329</v>
       </c>
@@ -8208,7 +8210,7 @@
       <c r="AK112" s="1"/>
       <c r="AL112" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="113">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="113">
       <c r="A113" s="9" t="s">
         <v>329</v>
       </c>
@@ -8268,7 +8270,7 @@
       <c r="AK113" s="1"/>
       <c r="AL113" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="114">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="114">
       <c r="A114" s="9" t="s">
         <v>329</v>
       </c>
@@ -8328,7 +8330,7 @@
       <c r="AK114" s="1"/>
       <c r="AL114" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="115">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="115">
       <c r="A115" s="9" t="s">
         <v>329</v>
       </c>
@@ -8388,7 +8390,7 @@
       <c r="AK115" s="1"/>
       <c r="AL115" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="116">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="116">
       <c r="A116" s="9" t="s">
         <v>329</v>
       </c>
@@ -8454,7 +8456,7 @@
       <c r="AQ116" s="1"/>
       <c r="AR116" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="117">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="117">
       <c r="A117" s="9" t="s">
         <v>329</v>
       </c>
@@ -8520,7 +8522,7 @@
       <c r="AQ117" s="1"/>
       <c r="AR117" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="118">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="118">
       <c r="A118" s="9" t="s">
         <v>329</v>
       </c>
@@ -8583,7 +8585,7 @@
       <c r="AQ118" s="1"/>
       <c r="AR118" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="119">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="119">
       <c r="A119" s="9" t="s">
         <v>329</v>
       </c>
@@ -8649,7 +8651,7 @@
       <c r="AQ119" s="1"/>
       <c r="AR119" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="120">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="120">
       <c r="A120" s="9" t="s">
         <v>329</v>
       </c>
@@ -8705,7 +8707,7 @@
       <c r="AQ120" s="1"/>
       <c r="AR120" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="121">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="121">
       <c r="A121" s="9" t="s">
         <v>329</v>
       </c>
@@ -8761,7 +8763,7 @@
       <c r="AQ121" s="1"/>
       <c r="AR121" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="122">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="122">
       <c r="A122" s="9" t="s">
         <v>329</v>
       </c>
@@ -8817,7 +8819,7 @@
       <c r="AQ122" s="1"/>
       <c r="AR122" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="123">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="123">
       <c r="A123" s="9"/>
       <c r="B123" s="9" t="s">
         <v>474</v>
@@ -8883,7 +8885,7 @@
       <c r="AQ123" s="1"/>
       <c r="AR123" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="124">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="124">
       <c r="A124" s="9" t="s">
         <v>269</v>
       </c>
@@ -8958,7 +8960,7 @@
       <c r="AQ124" s="1"/>
       <c r="AR124" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="125">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="125">
       <c r="A125" s="9" t="s">
         <v>269</v>
       </c>
@@ -9030,7 +9032,7 @@
       <c r="AQ125" s="1"/>
       <c r="AR125" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="126">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="126">
       <c r="A126" s="9" t="s">
         <v>269</v>
       </c>
@@ -9106,7 +9108,7 @@
       <c r="AQ126" s="1"/>
       <c r="AR126" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="127">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="127">
       <c r="A127" s="9" t="s">
         <v>269</v>
       </c>
@@ -9252,7 +9254,7 @@
       <c r="AQ128" s="1"/>
       <c r="AR128" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="129">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="129">
       <c r="A129" s="9" t="s">
         <v>269</v>
       </c>
@@ -9389,7 +9391,7 @@
       <c r="AQ130" s="1"/>
       <c r="AR130" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="131">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="131">
       <c r="A131" s="9" t="s">
         <v>269</v>
       </c>
@@ -9464,7 +9466,7 @@
       <c r="AQ131" s="1"/>
       <c r="AR131" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="132">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="132">
       <c r="A132" s="9" t="s">
         <v>269</v>
       </c>
@@ -9539,7 +9541,7 @@
       <c r="AQ132" s="1"/>
       <c r="AR132" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="133">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="133">
       <c r="A133" s="9" t="s">
         <v>269</v>
       </c>
@@ -9611,7 +9613,7 @@
       <c r="AQ133" s="1"/>
       <c r="AR133" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="134">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="134">
       <c r="A134" s="9" t="s">
         <v>269</v>
       </c>
@@ -9683,7 +9685,7 @@
       <c r="AQ134" s="1"/>
       <c r="AR134" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="135">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="135">
       <c r="A135" s="9" t="s">
         <v>269</v>
       </c>
@@ -9758,7 +9760,7 @@
       <c r="AQ135" s="1"/>
       <c r="AR135" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="136">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="136">
       <c r="A136" s="9" t="s">
         <v>269</v>
       </c>
@@ -9833,7 +9835,7 @@
       <c r="AQ136" s="1"/>
       <c r="AR136" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="137">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="137">
       <c r="A137" s="9" t="s">
         <v>269</v>
       </c>
@@ -9908,7 +9910,7 @@
       <c r="AQ137" s="1"/>
       <c r="AR137" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="138">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="138">
       <c r="A138" s="9" t="s">
         <v>269</v>
       </c>
@@ -9983,7 +9985,7 @@
       <c r="AQ138" s="1"/>
       <c r="AR138" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="139">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="139">
       <c r="A139" s="9" t="s">
         <v>269</v>
       </c>
@@ -10058,7 +10060,7 @@
       <c r="AQ139" s="1"/>
       <c r="AR139" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="140">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="140">
       <c r="A140" s="9" t="s">
         <v>269</v>
       </c>
@@ -10130,7 +10132,7 @@
       <c r="AQ140" s="1"/>
       <c r="AR140" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="141">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="141">
       <c r="A141" s="9" t="s">
         <v>269</v>
       </c>
@@ -10199,7 +10201,7 @@
       <c r="AQ141" s="1"/>
       <c r="AR141" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="142">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="142">
       <c r="A142" s="9"/>
       <c r="B142" s="9" t="s">
         <v>599</v>
@@ -10269,7 +10271,7 @@
       <c r="AQ142" s="1"/>
       <c r="AR142" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="143">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="143">
       <c r="A143" s="9"/>
       <c r="B143" s="9" t="s">
         <v>605</v>
@@ -10339,7 +10341,7 @@
       <c r="AQ143" s="1"/>
       <c r="AR143" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="144">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="144">
       <c r="A144" s="1" t="s">
         <v>266</v>
       </c>
@@ -10682,7 +10684,7 @@
       <c r="AQ148" s="1"/>
       <c r="AR148" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="149">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="149">
       <c r="A149" s="1" t="s">
         <v>266</v>
       </c>
@@ -10753,7 +10755,7 @@
       <c r="AQ149" s="1"/>
       <c r="AR149" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="150">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="150">
       <c r="A150" s="1" t="s">
         <v>266</v>
       </c>
@@ -10830,7 +10832,7 @@
       <c r="AQ150" s="1"/>
       <c r="AR150" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="151">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="151">
       <c r="A151" s="1" t="s">
         <v>266</v>
       </c>
@@ -10960,7 +10962,7 @@
       <c r="AQ152" s="1"/>
       <c r="AR152" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="153">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="153">
       <c r="A153" s="1" t="s">
         <v>266</v>
       </c>
@@ -11034,7 +11036,7 @@
       <c r="AQ153" s="1"/>
       <c r="AR153" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="154">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="154">
       <c r="A154" s="1" t="s">
         <v>266</v>
       </c>
@@ -11102,7 +11104,7 @@
       <c r="AQ154" s="1"/>
       <c r="AR154" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="155">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="155">
       <c r="A155" s="1" t="s">
         <v>266</v>
       </c>
@@ -11185,7 +11187,7 @@
       <c r="AQ155" s="1"/>
       <c r="AR155" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="156">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="156">
       <c r="A156" s="1" t="s">
         <v>266</v>
       </c>
@@ -11327,7 +11329,7 @@
       <c r="AQ157" s="1"/>
       <c r="AR157" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="158">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="158">
       <c r="A158" s="1" t="s">
         <v>266</v>
       </c>
@@ -11626,7 +11628,7 @@
       <c r="AQ161" s="1"/>
       <c r="AR161" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="162">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="162">
       <c r="A162" s="1" t="s">
         <v>266</v>
       </c>
@@ -11907,7 +11909,7 @@
       <c r="AQ165" s="1"/>
       <c r="AR165" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="166">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="166">
       <c r="A166" s="1" t="s">
         <v>266</v>
       </c>
@@ -11978,7 +11980,7 @@
       <c r="AQ166" s="1"/>
       <c r="AR166" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="167">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="167">
       <c r="A167" s="1" t="s">
         <v>266</v>
       </c>
@@ -12167,7 +12169,7 @@
         <v>801</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="170">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="170">
       <c r="A170" s="1" t="s">
         <v>796</v>
       </c>
@@ -12289,7 +12291,7 @@
         <v>812</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="173">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="173">
       <c r="A173" s="1" t="s">
         <v>796</v>
       </c>
@@ -12329,7 +12331,7 @@
         <v>816</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="174">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="174">
       <c r="A174" s="1" t="s">
         <v>796</v>
       </c>
@@ -12369,7 +12371,7 @@
         <v>820</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="175">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="175">
       <c r="A175" s="1" t="s">
         <v>796</v>
       </c>
@@ -12409,7 +12411,7 @@
         <v>824</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="176">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="176">
       <c r="A176" s="1" t="s">
         <v>796</v>
       </c>
@@ -12449,7 +12451,7 @@
         <v>541</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="177">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="177">
       <c r="A177" s="1" t="s">
         <v>796</v>
       </c>
@@ -12489,7 +12491,7 @@
         <v>831</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="178">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="178">
       <c r="A178" s="1" t="s">
         <v>796</v>
       </c>
@@ -12529,7 +12531,7 @@
         <v>835</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="179">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="179">
       <c r="A179" s="1" t="s">
         <v>796</v>
       </c>
@@ -12566,7 +12568,7 @@
         <v>839</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="180">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="180">
       <c r="A180" s="1" t="s">
         <v>796</v>
       </c>
@@ -12606,7 +12608,7 @@
         <v>843</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="181">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="181">
       <c r="A181" s="1" t="s">
         <v>796</v>
       </c>
@@ -12646,7 +12648,7 @@
         <v>846</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="182">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="182">
       <c r="A182" s="1" t="s">
         <v>796</v>
       </c>
@@ -12723,7 +12725,7 @@
         <v>854</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="184">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="184">
       <c r="A184" s="1" t="s">
         <v>796</v>
       </c>
@@ -12760,7 +12762,7 @@
         <v>858</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="185">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="185">
       <c r="A185" s="1" t="s">
         <v>796</v>
       </c>
@@ -12797,7 +12799,7 @@
         <v>862</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="186">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="186">
       <c r="A186" s="1" t="s">
         <v>796</v>
       </c>
@@ -12871,7 +12873,7 @@
         <v>595</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="188">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="188">
       <c r="A188" s="1" t="s">
         <v>796</v>
       </c>
@@ -12911,7 +12913,7 @@
         <v>873</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="189">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="189">
       <c r="A189" s="1" t="s">
         <v>874</v>
       </c>
@@ -12948,7 +12950,7 @@
         <v>877</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="190">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="190">
       <c r="A190" s="1" t="s">
         <v>874</v>
       </c>
@@ -12985,7 +12987,7 @@
         <v>880</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="191">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="191">
       <c r="A191" s="1" t="s">
         <v>874</v>
       </c>
@@ -13022,7 +13024,7 @@
         <v>883</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="192">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="192">
       <c r="A192" s="1" t="s">
         <v>884</v>
       </c>
@@ -13072,7 +13074,7 @@
         <v>890</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="193">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="193">
       <c r="A193" s="1" t="s">
         <v>884</v>
       </c>
@@ -13117,7 +13119,7 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="194">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="194">
       <c r="A194" s="1" t="s">
         <v>884</v>
       </c>
@@ -13161,7 +13163,7 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="195">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="195">
       <c r="A195" s="1" t="s">
         <v>884</v>
       </c>
@@ -13211,7 +13213,7 @@
         <v>901</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="196">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="196">
       <c r="A196" s="1" t="s">
         <v>884</v>
       </c>
@@ -13258,7 +13260,7 @@
         <v>904</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="197">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="197">
       <c r="A197" s="1" t="s">
         <v>884</v>
       </c>
@@ -13305,7 +13307,7 @@
         <v>909</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="198">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="198">
       <c r="A198" s="1" t="s">
         <v>884</v>
       </c>
@@ -13350,7 +13352,7 @@
       </c>
       <c r="S198" s="10"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="199">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="199">
       <c r="A199" s="1" t="s">
         <v>913</v>
       </c>
@@ -13394,7 +13396,7 @@
         <v>917</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="200">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="200">
       <c r="A200" s="1" t="s">
         <v>913</v>
       </c>
@@ -13438,7 +13440,7 @@
         <v>921</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="201">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="201">
       <c r="A201" s="1" t="s">
         <v>913</v>
       </c>

</xml_diff>

<commit_message>
add a label to the filter results
</commit_message>
<xml_diff>
--- a/sampledata/fieldinformation.xlsx
+++ b/sampledata/fieldinformation.xlsx
@@ -2956,7 +2956,7 @@
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -2968,30 +2968,30 @@
   </sheetPr>
   <dimension ref="A1:AR201"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <pane activePane="bottomRight" topLeftCell="C88" xSplit="4966" ySplit="1734"/>
-      <selection activeCell="B1" activeCellId="0" pane="topLeft" sqref="B1"/>
-      <selection activeCell="C1" activeCellId="0" pane="topRight" sqref="C1"/>
-      <selection activeCell="B88" activeCellId="0" pane="bottomLeft" sqref="B88"/>
-      <selection activeCell="O109" activeCellId="0" pane="bottomRight" sqref="O109"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <pane activePane="bottomRight" topLeftCell="A139" xSplit="5131" ySplit="1719"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="A1" activeCellId="0" pane="topRight" sqref="A1"/>
+      <selection activeCell="A139" activeCellId="0" pane="bottomLeft" sqref="A139"/>
+      <selection activeCell="I158" activeCellId="0" pane="bottomRight" sqref="I158"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.2627450980392"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.4117647058824"/>
-    <col collapsed="false" hidden="false" max="10" min="3" style="1" width="12.6352941176471"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="2" width="12.6352941176471"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.6352941176471"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="32.6588235294118"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="1" width="30.0627450980392"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="64.756862745098"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="17.5921568627451"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="52.1058823529412"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="16.243137254902"/>
-    <col collapsed="false" hidden="false" max="22" min="21" style="1" width="25.1176470588235"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="24.9882352941176"/>
-    <col collapsed="false" hidden="false" max="26" min="24" style="1" width="10.9176470588235"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.68235294117647"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.3882352941176"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.4941176470588"/>
+    <col collapsed="false" hidden="false" max="10" min="3" style="1" width="12.6980392156863"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="2" width="12.6980392156863"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.6980392156863"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="32.8235294117647"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="1" width="30.2078431372549"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="65.0745098039216"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="17.6823529411765"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="52.3686274509804"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="16.3254901960784"/>
+    <col collapsed="false" hidden="false" max="22" min="21" style="1" width="25.243137254902"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="25.1176470588235"/>
+    <col collapsed="false" hidden="false" max="26" min="24" style="1" width="10.9725490196078"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.72941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="67.5" outlineLevel="0" r="1" s="6">
@@ -4574,7 +4574,7 @@
       <c r="AG36" s="1"/>
       <c r="AH36" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="37">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="37">
       <c r="A37" s="9" t="s">
         <v>106</v>
       </c>
@@ -7910,7 +7910,7 @@
       <c r="AK107" s="1"/>
       <c r="AL107" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="108">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="108">
       <c r="B108" s="9" t="s">
         <v>411</v>
       </c>
@@ -10508,7 +10508,7 @@
         <v>24</v>
       </c>
       <c r="I146" s="9" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="J146" s="7" t="s">
         <v>24</v>
@@ -11117,7 +11117,7 @@
         <v>24</v>
       </c>
       <c r="I155" s="9" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="J155" s="7" t="s">
         <v>24</v>
@@ -11274,7 +11274,7 @@
         <v>24</v>
       </c>
       <c r="I157" s="9" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="J157" s="7" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
change Bioassay Type to Dataset Type for #209
</commit_message>
<xml_diff>
--- a/sampledata/fieldinformation.xlsx
+++ b/sampledata/fieldinformation.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2514" uniqueCount="931">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2513" uniqueCount="931">
   <si>
     <t>table</t>
   </si>
@@ -440,7 +440,7 @@
     <t>dataset_type</t>
   </si>
   <si>
-    <t>BioAssay Type</t>
+    <t>Dataset Type</t>
   </si>
   <si>
     <t>Distinguishes datasets that are used elsewhere, such as the Nominal Targets dataset.</t>
@@ -1259,10 +1259,10 @@
     <t>SMQ:1</t>
   </si>
   <si>
-    <t>BioAssay Types</t>
-  </si>
-  <si>
-    <t>Types of bioassays studying this entity.</t>
+    <t>Dataset types</t>
+  </si>
+  <si>
+    <t>Types of datasets studying this entity.</t>
   </si>
   <si>
     <t>facility_batch_id</t>
@@ -2974,7 +2974,7 @@
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -2987,11 +2987,11 @@
   <dimension ref="A1:AR205"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <pane activePane="bottomRight" state="split" topLeftCell="M193" xSplit="4814" ySplit="1725"/>
+      <pane activePane="bottomRight" state="split" topLeftCell="O96" xSplit="4509" ySplit="1725"/>
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-      <selection activeCell="M1" activeCellId="0" pane="topRight" sqref="M1"/>
-      <selection activeCell="A193" activeCellId="0" pane="bottomLeft" sqref="A193"/>
-      <selection activeCell="O205" activeCellId="0" pane="bottomRight" sqref="O205"/>
+      <selection activeCell="O1" activeCellId="0" pane="topRight" sqref="O1"/>
+      <selection activeCell="A96" activeCellId="0" pane="bottomLeft" sqref="A96"/>
+      <selection activeCell="O109" activeCellId="0" pane="bottomRight" sqref="O109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4593,7 +4593,7 @@
       <c r="AG36" s="1"/>
       <c r="AH36" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="37">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
       <c r="A37" s="6" t="s">
         <v>106</v>
       </c>
@@ -4623,9 +4623,6 @@
       </c>
       <c r="M37" s="1" t="n">
         <v>35</v>
-      </c>
-      <c r="N37" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="O37" s="1" t="s">
         <v>141</v>
@@ -7929,7 +7926,7 @@
       <c r="AK107" s="1"/>
       <c r="AL107" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="108">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="108">
       <c r="B108" s="6" t="s">
         <v>411</v>
       </c>

</xml_diff>

<commit_message>
modify #215, show bioassay field only in SAF output
</commit_message>
<xml_diff>
--- a/sampledata/fieldinformation.xlsx
+++ b/sampledata/fieldinformation.xlsx
@@ -440,10 +440,10 @@
     <t>dataset_type</t>
   </si>
   <si>
-    <t>Dataset Type</t>
-  </si>
-  <si>
-    <t>Distinguishes datasets that are used elsewhere, such as the Nominal Targets dataset.</t>
+    <t>HMS Dataset Type</t>
+  </si>
+  <si>
+    <t>HMS Dataset category</t>
   </si>
   <si>
     <t>bioassay</t>
@@ -3043,7 +3043,7 @@
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal" xfId="20"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -3056,11 +3056,11 @@
   <dimension ref="A1:AR212"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <pane activePane="bottomRight" state="split" topLeftCell="A128" xSplit="3726" ySplit="1725"/>
+      <pane activePane="bottomRight" state="split" topLeftCell="P20" xSplit="3494" ySplit="1725"/>
       <selection activeCell="B1" activeCellId="0" pane="topLeft" sqref="B1"/>
-      <selection activeCell="A1" activeCellId="0" pane="topRight" sqref="A1"/>
-      <selection activeCell="B128" activeCellId="0" pane="bottomLeft" sqref="B128"/>
-      <selection activeCell="B142" activeCellId="0" pane="bottomRight" sqref="B142"/>
+      <selection activeCell="P1" activeCellId="0" pane="topRight" sqref="P1"/>
+      <selection activeCell="B20" activeCellId="0" pane="bottomLeft" sqref="B20"/>
+      <selection activeCell="Q38" activeCellId="0" pane="bottomRight" sqref="Q38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4718,7 +4718,7 @@
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F38" s="6" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
QC Events updates: remove qc outcome from batch detail:  - from discussion:  - remove "QC Outcome" from the batch information table  - may replace with a manually curated "current status" field  - change QC title to include "HMS"
</commit_message>
<xml_diff>
--- a/sampledata/fieldinformation.xlsx
+++ b/sampledata/fieldinformation.xlsx
@@ -2933,7 +2933,7 @@
     <t>QC:3</t>
   </si>
   <si>
-    <t>Outcome</t>
+    <t>HMS QC Outcome</t>
   </si>
   <si>
     <t>Outcome of the QC test: PASS/FAIL</t>
@@ -3142,11 +3142,11 @@
   <dimension ref="A1:AR224"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="P209" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="N200" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="P1" activeCellId="0" sqref="P1"/>
-      <selection pane="bottomLeft" activeCell="A209" activeCellId="0" sqref="A209"/>
-      <selection pane="bottomRight" activeCell="Q220" activeCellId="0" sqref="Q220"/>
+      <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="bottomLeft" activeCell="A200" activeCellId="0" sqref="A200"/>
+      <selection pane="bottomRight" activeCell="O219" activeCellId="0" sqref="O219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
QC event implementation final UI adjustments - show datasets above batch info - don't show datasets when batch detail is displayed - omit type from qc attached file import' - add up to 5 attached qc files in the import file - add 'HMS' to batch qc section title
add import statement

add import statement
</commit_message>
<xml_diff>
--- a/sampledata/fieldinformation.xlsx
+++ b/sampledata/fieldinformation.xlsx
@@ -2948,7 +2948,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Date effective</t>
+    <t>Event date</t>
   </si>
   <si>
     <t>comment</t>
@@ -3146,7 +3146,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="A200" activeCellId="0" sqref="A200"/>
-      <selection pane="bottomRight" activeCell="O219" activeCellId="0" sqref="O219"/>
+      <selection pane="bottomRight" activeCell="Q219" activeCellId="0" sqref="Q219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>